<commit_message>
Update in ResetPassword and FYP_Test_Plan
- Update in ResetPassword with DynamoDB and Cognito
- Check the Android Monitor Log
If Success it will show 'Success------------------------------------------'
If Fail it will show 'Fail---------------------------------------'
</commit_message>
<xml_diff>
--- a/FYP documentation/FYP_Test_Plan.xlsx
+++ b/FYP documentation/FYP_Test_Plan.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18326"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Durrah\UOW- Year 3\CSCI 321 - FYP\Extra\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6940"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6936"/>
   </bookViews>
   <sheets>
     <sheet name="Test Plan" sheetId="3" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="72">
   <si>
     <t>Expected Result</t>
   </si>
@@ -234,11 +229,42 @@
     <t>1. Enter valid phone number with country code 
 2. Click on 'SIGN UP' button</t>
   </si>
+  <si>
+    <t>TC-011</t>
+  </si>
+  <si>
+    <t>S3 TOKEN GET NULL when start the app</t>
+  </si>
+  <si>
+    <t>TC-012</t>
+  </si>
+  <si>
+    <t>Reset Password</t>
+  </si>
+  <si>
+    <t>Initialize App</t>
+  </si>
+  <si>
+    <t>Check whether the encrypted file by old password open correctly after change password</t>
+  </si>
+  <si>
+    <t>1. Delete the previous account data in DynamoDB 
+2. Delete the previous account data in Cognito 
+3. Uninstall the existed App in phone 
+4. Reinstall the app</t>
+  </si>
+  <si>
+    <t>1. Create Account
+2. Create new area and new file
+3. Change Password via Reset Password
+4. Relogin the account with new password
+5. Open the created area and file and check whetehr it opens correctly</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -385,7 +411,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -421,6 +447,33 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -430,28 +483,10 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="표준" xfId="0" builtinId="0"/>
+    <cellStyle name="하이퍼링크" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -486,7 +521,7 @@
         <xdr:cNvPr id="2061" name="AutoShape 13">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{30BA1063-A16B-4C68-A743-4B420C5465C1}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{30BA1063-A16B-4C68-A743-4B420C5465C1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -534,7 +569,7 @@
         <xdr:cNvPr id="2060" name="Picture 12" descr="out">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DF567FBA-98D6-41F8-887E-3AB62EFCE5E8}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DF567FBA-98D6-41F8-887E-3AB62EFCE5E8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -595,7 +630,7 @@
         <xdr:cNvPr id="2059" name="Picture 11" descr="out">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{63E93150-DA75-4658-ACF7-D189E05151A8}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{63E93150-DA75-4658-ACF7-D189E05151A8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -656,7 +691,7 @@
         <xdr:cNvPr id="2058" name="AutoShape 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{31457A75-25A1-4182-A274-BF0A57FF81ED}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{31457A75-25A1-4182-A274-BF0A57FF81ED}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -704,7 +739,7 @@
         <xdr:cNvPr id="2057" name="AutoShape 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FD5E9B17-BBE9-4F3F-8C7B-720ECD2D681E}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FD5E9B17-BBE9-4F3F-8C7B-720ECD2D681E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -752,7 +787,7 @@
         <xdr:cNvPr id="2056" name="AutoShape 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ACF2AA01-B252-4B3A-A375-0E01973F5F28}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ACF2AA01-B252-4B3A-A375-0E01973F5F28}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -800,7 +835,7 @@
         <xdr:cNvPr id="2055" name="Picture 7" descr="out">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{65879D11-6224-4C7F-89C2-EB96196F1A0F}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{65879D11-6224-4C7F-89C2-EB96196F1A0F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -861,7 +896,7 @@
         <xdr:cNvPr id="2054" name="Picture 6" descr="out">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5CF822E1-047C-4A3B-84DC-EC8AC8269EFF}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5CF822E1-047C-4A3B-84DC-EC8AC8269EFF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -922,7 +957,7 @@
         <xdr:cNvPr id="2053" name="Picture 5" descr="out">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{04925A52-F4C6-4CD2-894B-53641F217E98}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{04925A52-F4C6-4CD2-894B-53641F217E98}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -983,7 +1018,7 @@
         <xdr:cNvPr id="2052" name="Picture 4" descr="out">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ABFA5086-6E08-48C0-9ACC-F28827F67131}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ABFA5086-6E08-48C0-9ACC-F28827F67131}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1044,7 +1079,7 @@
         <xdr:cNvPr id="2051" name="Picture 3" descr="out">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{57E4935A-4571-48AC-8BC5-8DE7A584B4D3}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{57E4935A-4571-48AC-8BC5-8DE7A584B4D3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1105,7 +1140,7 @@
         <xdr:cNvPr id="2050" name="Picture 2" descr="out">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{73C78A6D-821A-410B-9678-567D6BA6A13D}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{73C78A6D-821A-410B-9678-567D6BA6A13D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1166,7 +1201,7 @@
         <xdr:cNvPr id="2049" name="Picture 1" descr="out?google_nid=adroll5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0583EF1F-95CC-4F68-83EF-C3E41E3B377C}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0583EF1F-95CC-4F68-83EF-C3E41E3B377C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1501,7 +1536,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1509,40 +1544,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:I24"/>
+  <dimension ref="A4:I27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.6328125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="13.6640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="10" style="1" customWidth="1"/>
-    <col min="3" max="3" width="15.90625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="20.453125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="24.54296875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="26.453125" style="16" customWidth="1"/>
-    <col min="7" max="7" width="16.6328125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="12.81640625" style="2" customWidth="1"/>
-    <col min="9" max="9" width="12.90625" style="2" customWidth="1"/>
-    <col min="10" max="16384" width="8.7265625" style="2"/>
+    <col min="3" max="3" width="15.88671875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="20.44140625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="24.5546875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="26.44140625" style="13" customWidth="1"/>
+    <col min="7" max="7" width="16.6640625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="12.77734375" style="2" customWidth="1"/>
+    <col min="9" max="9" width="12.88671875" style="2" customWidth="1"/>
+    <col min="10" max="16384" width="8.77734375" style="2"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A4" s="13" t="s">
+    <row r="4" spans="1:9" ht="18.45" x14ac:dyDescent="0.45">
+      <c r="A4" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="14"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
-      <c r="I4" s="15"/>
+      <c r="B4" s="23"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="23"/>
+      <c r="H4" s="23"/>
+      <c r="I4" s="24"/>
     </row>
-    <row r="5" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" s="4" customFormat="1" ht="14.55" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
@@ -1558,7 +1593,7 @@
       <c r="E5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="17" t="s">
+      <c r="F5" s="14" t="s">
         <v>14</v>
       </c>
       <c r="G5" s="3" t="s">
@@ -1571,7 +1606,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:9" s="1" customFormat="1" ht="29.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" s="1" customFormat="1" ht="29.55" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="6">
         <v>1</v>
       </c>
@@ -1592,7 +1627,7 @@
       <c r="H6" s="9"/>
       <c r="I6" s="9"/>
     </row>
-    <row r="7" spans="1:9" s="1" customFormat="1" ht="43" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" s="1" customFormat="1" ht="43.05" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="6">
         <v>2</v>
       </c>
@@ -1608,7 +1643,7 @@
       <c r="E7" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="F7" s="18" t="s">
+      <c r="F7" s="15" t="s">
         <v>18</v>
       </c>
       <c r="G7" s="8"/>
@@ -1638,7 +1673,7 @@
       <c r="H8" s="9"/>
       <c r="I8" s="9"/>
     </row>
-    <row r="9" spans="1:9" s="1" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" s="1" customFormat="1" ht="58.05" x14ac:dyDescent="0.35">
       <c r="A9" s="6">
         <v>4</v>
       </c>
@@ -1654,25 +1689,25 @@
       <c r="E9" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="F9" s="18"/>
+      <c r="F9" s="15"/>
       <c r="G9" s="9"/>
       <c r="H9" s="9"/>
       <c r="I9" s="9"/>
     </row>
-    <row r="13" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A13" s="13" t="s">
+    <row r="13" spans="1:9" ht="18.45" x14ac:dyDescent="0.45">
+      <c r="A13" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="14"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
-      <c r="I13" s="15"/>
+      <c r="B13" s="23"/>
+      <c r="C13" s="23"/>
+      <c r="D13" s="23"/>
+      <c r="E13" s="23"/>
+      <c r="F13" s="23"/>
+      <c r="G13" s="23"/>
+      <c r="H13" s="23"/>
+      <c r="I13" s="24"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" ht="14.55" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
         <v>3</v>
       </c>
@@ -1688,7 +1723,7 @@
       <c r="E14" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F14" s="17" t="s">
+      <c r="F14" s="14" t="s">
         <v>14</v>
       </c>
       <c r="G14" s="3" t="s">
@@ -1701,7 +1736,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="62" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" ht="61.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="6">
         <v>1</v>
       </c>
@@ -1724,7 +1759,7 @@
       <c r="H15" s="9"/>
       <c r="I15" s="9"/>
     </row>
-    <row r="16" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" ht="28.95" x14ac:dyDescent="0.35">
       <c r="A16" s="6">
         <v>2</v>
       </c>
@@ -1740,14 +1775,14 @@
       <c r="E16" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="F16" s="19" t="s">
+      <c r="F16" s="16" t="s">
         <v>25</v>
       </c>
       <c r="G16" s="8"/>
       <c r="H16" s="9"/>
       <c r="I16" s="9"/>
     </row>
-    <row r="17" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" ht="58.05" x14ac:dyDescent="0.35">
       <c r="A17" s="6">
         <v>3</v>
       </c>
@@ -1763,12 +1798,12 @@
       <c r="E17" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="F17" s="20"/>
+      <c r="F17" s="17"/>
       <c r="G17" s="8"/>
       <c r="H17" s="9"/>
       <c r="I17" s="9"/>
     </row>
-    <row r="18" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" ht="72.45" x14ac:dyDescent="0.35">
       <c r="A18" s="6">
         <v>4</v>
       </c>
@@ -1784,14 +1819,14 @@
       <c r="E18" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="F18" s="21" t="s">
+      <c r="F18" s="18" t="s">
         <v>33</v>
       </c>
       <c r="G18" s="9"/>
       <c r="H18" s="9"/>
       <c r="I18" s="9"/>
     </row>
-    <row r="19" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A19" s="6">
         <v>5</v>
       </c>
@@ -1814,7 +1849,7 @@
       <c r="H19" s="9"/>
       <c r="I19" s="9"/>
     </row>
-    <row r="20" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A20" s="6">
         <v>6</v>
       </c>
@@ -1830,14 +1865,14 @@
       <c r="E20" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="F20" s="21" t="s">
+      <c r="F20" s="18" t="s">
         <v>36</v>
       </c>
       <c r="G20" s="9"/>
       <c r="H20" s="9"/>
       <c r="I20" s="9"/>
     </row>
-    <row r="21" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A21" s="6">
         <v>7</v>
       </c>
@@ -1860,7 +1895,7 @@
       <c r="H21" s="9"/>
       <c r="I21" s="9"/>
     </row>
-    <row r="22" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A22" s="7">
         <v>8</v>
       </c>
@@ -1883,7 +1918,7 @@
       <c r="H22" s="8"/>
       <c r="I22" s="8"/>
     </row>
-    <row r="23" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A23" s="7">
         <v>9</v>
       </c>
@@ -1906,7 +1941,7 @@
       <c r="H23" s="8"/>
       <c r="I23" s="8"/>
     </row>
-    <row r="24" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A24" s="7">
         <v>10</v>
       </c>
@@ -1928,6 +1963,40 @@
       <c r="G24" s="8"/>
       <c r="H24" s="8"/>
       <c r="I24" s="8"/>
+    </row>
+    <row r="26" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A26" s="1">
+        <v>11</v>
+      </c>
+      <c r="B26" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="C26" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="D26" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="E26" s="21" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="144" x14ac:dyDescent="0.3">
+      <c r="A27" s="1">
+        <v>12</v>
+      </c>
+      <c r="B27" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="C27" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="D27" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="E27" s="21" t="s">
+        <v>71</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Added search function and restmap to searched area.
</commit_message>
<xml_diff>
--- a/FYP documentation/FYP_Test_Plan.xlsx
+++ b/FYP documentation/FYP_Test_Plan.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18326"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Durrah\UOW- Year 3\CSCI 321 - FYP\Extra\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Class_notes\BSS_FYP_TEAM173D\FYP documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6940"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6936" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Plan" sheetId="3" r:id="rId1"/>
@@ -238,7 +238,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -251,6 +251,14 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -274,14 +282,6 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="14"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -385,68 +385,59 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1508,426 +1499,426 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A4:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13:I14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.6328125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10" style="1" customWidth="1"/>
-    <col min="3" max="3" width="15.90625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="20.453125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="24.54296875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="26.453125" style="16" customWidth="1"/>
-    <col min="7" max="7" width="16.6328125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="12.81640625" style="2" customWidth="1"/>
-    <col min="9" max="9" width="12.90625" style="2" customWidth="1"/>
-    <col min="10" max="16384" width="8.7265625" style="2"/>
+    <col min="1" max="1" width="13.6640625" style="13" customWidth="1"/>
+    <col min="2" max="2" width="10" style="13" customWidth="1"/>
+    <col min="3" max="3" width="15.88671875" style="13" customWidth="1"/>
+    <col min="4" max="4" width="20.44140625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="24.5546875" style="4" customWidth="1"/>
+    <col min="6" max="6" width="26.44140625" style="18" customWidth="1"/>
+    <col min="7" max="7" width="16.6640625" style="4" customWidth="1"/>
+    <col min="8" max="8" width="12.77734375" style="4" customWidth="1"/>
+    <col min="9" max="9" width="12.88671875" style="4" customWidth="1"/>
+    <col min="10" max="16384" width="8.77734375" style="4"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A4" s="13" t="s">
+    <row r="4" spans="1:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="14"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
-      <c r="I4" s="15"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="3"/>
     </row>
-    <row r="5" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="3" t="s">
+    <row r="5" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="17" t="s">
+      <c r="F5" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="G5" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="H5" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="I5" s="3" t="s">
+      <c r="I5" s="5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:9" s="1" customFormat="1" ht="29.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="6">
+    <row r="6" spans="1:9" s="13" customFormat="1" ht="29.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="8">
         <v>1</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="12" t="s">
+      <c r="E6" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="F6" s="12"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="9"/>
-      <c r="I6" s="9"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="12"/>
+      <c r="I6" s="12"/>
     </row>
-    <row r="7" spans="1:9" s="1" customFormat="1" ht="43" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="6">
+    <row r="7" spans="1:9" s="13" customFormat="1" ht="43.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="8">
         <v>2</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="F7" s="18" t="s">
+      <c r="F7" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="G7" s="8"/>
-      <c r="H7" s="9"/>
-      <c r="I7" s="9"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="12"/>
     </row>
-    <row r="8" spans="1:9" s="1" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="6">
+    <row r="8" spans="1:9" s="13" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A8" s="8">
         <v>3</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="E8" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="F8" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="G8" s="8"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="9"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="12"/>
     </row>
-    <row r="9" spans="1:9" s="1" customFormat="1" ht="58" x14ac:dyDescent="0.35">
-      <c r="A9" s="6">
+    <row r="9" spans="1:9" s="13" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A9" s="8">
         <v>4</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D9" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="E9" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="F9" s="18"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="9"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12"/>
+      <c r="I9" s="12"/>
     </row>
-    <row r="13" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A13" s="13" t="s">
+    <row r="13" spans="1:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="14"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
-      <c r="I13" s="15"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="3"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A14" s="3" t="s">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="D14" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E14" s="3" t="s">
+      <c r="E14" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F14" s="17" t="s">
+      <c r="F14" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="G14" s="3" t="s">
+      <c r="G14" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="H14" s="3" t="s">
+      <c r="H14" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="I14" s="3" t="s">
+      <c r="I14" s="5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="62" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="6">
+    <row r="15" spans="1:9" ht="61.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="8">
         <v>1</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="B15" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C15" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="D15" s="7" t="s">
+      <c r="D15" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="E15" s="5" t="s">
+      <c r="E15" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="F15" s="5" t="s">
+      <c r="F15" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="G15" s="8"/>
-      <c r="H15" s="9"/>
-      <c r="I15" s="9"/>
+      <c r="G15" s="11"/>
+      <c r="H15" s="12"/>
+      <c r="I15" s="12"/>
     </row>
-    <row r="16" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A16" s="6">
+    <row r="16" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A16" s="8">
         <v>2</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="B16" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="D16" s="7" t="s">
+      <c r="D16" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="E16" s="5" t="s">
+      <c r="E16" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="F16" s="19" t="s">
+      <c r="F16" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="G16" s="8"/>
-      <c r="H16" s="9"/>
-      <c r="I16" s="9"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="12"/>
+      <c r="I16" s="12"/>
     </row>
-    <row r="17" spans="1:9" ht="58" x14ac:dyDescent="0.35">
-      <c r="A17" s="6">
+    <row r="17" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A17" s="8">
         <v>3</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B17" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="C17" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="D17" s="7" t="s">
+      <c r="D17" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="E17" s="5" t="s">
+      <c r="E17" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="F17" s="20"/>
-      <c r="G17" s="8"/>
-      <c r="H17" s="9"/>
-      <c r="I17" s="9"/>
+      <c r="F17" s="16"/>
+      <c r="G17" s="11"/>
+      <c r="H17" s="12"/>
+      <c r="I17" s="12"/>
     </row>
-    <row r="18" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A18" s="6">
+    <row r="18" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A18" s="8">
         <v>4</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="B18" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C18" s="7" t="s">
+      <c r="C18" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="D18" s="10" t="s">
+      <c r="D18" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="E18" s="5" t="s">
+      <c r="E18" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="F18" s="21" t="s">
+      <c r="F18" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="G18" s="9"/>
-      <c r="H18" s="9"/>
-      <c r="I18" s="9"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="12"/>
+      <c r="I18" s="12"/>
     </row>
-    <row r="19" spans="1:9" ht="58" x14ac:dyDescent="0.35">
-      <c r="A19" s="6">
+    <row r="19" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A19" s="8">
         <v>5</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="B19" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="C19" s="7" t="s">
+      <c r="C19" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="D19" s="11" t="s">
+      <c r="D19" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="E19" s="5" t="s">
+      <c r="E19" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="F19" s="5" t="s">
+      <c r="F19" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="G19" s="9"/>
-      <c r="H19" s="9"/>
-      <c r="I19" s="9"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="12"/>
+      <c r="I19" s="12"/>
     </row>
-    <row r="20" spans="1:9" ht="58" x14ac:dyDescent="0.35">
-      <c r="A20" s="6">
+    <row r="20" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A20" s="8">
         <v>6</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="B20" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="C20" s="7" t="s">
+      <c r="C20" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="D20" s="11" t="s">
+      <c r="D20" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="E20" s="5" t="s">
+      <c r="E20" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="F20" s="21" t="s">
+      <c r="F20" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="G20" s="9"/>
-      <c r="H20" s="9"/>
-      <c r="I20" s="9"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="12"/>
+      <c r="I20" s="12"/>
     </row>
-    <row r="21" spans="1:9" ht="58" x14ac:dyDescent="0.35">
-      <c r="A21" s="6">
+    <row r="21" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A21" s="8">
         <v>7</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="B21" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="C21" s="11" t="s">
+      <c r="C21" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="D21" s="11" t="s">
+      <c r="D21" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="E21" s="5" t="s">
+      <c r="E21" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="F21" s="5" t="s">
+      <c r="F21" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="G21" s="9"/>
-      <c r="H21" s="9"/>
-      <c r="I21" s="9"/>
+      <c r="G21" s="12"/>
+      <c r="H21" s="12"/>
+      <c r="I21" s="12"/>
     </row>
-    <row r="22" spans="1:9" ht="58" x14ac:dyDescent="0.35">
-      <c r="A22" s="7">
+    <row r="22" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A22" s="9">
         <v>8</v>
       </c>
-      <c r="B22" s="7" t="s">
+      <c r="B22" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="C22" s="11" t="s">
+      <c r="C22" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="D22" s="11" t="s">
+      <c r="D22" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="E22" s="5" t="s">
+      <c r="E22" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="F22" s="5" t="s">
+      <c r="F22" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="G22" s="8"/>
-      <c r="H22" s="8"/>
-      <c r="I22" s="8"/>
+      <c r="G22" s="11"/>
+      <c r="H22" s="11"/>
+      <c r="I22" s="11"/>
     </row>
-    <row r="23" spans="1:9" ht="58" x14ac:dyDescent="0.35">
-      <c r="A23" s="7">
+    <row r="23" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A23" s="9">
         <v>9</v>
       </c>
-      <c r="B23" s="7" t="s">
+      <c r="B23" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="C23" s="11" t="s">
+      <c r="C23" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="D23" s="11" t="s">
+      <c r="D23" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="E23" s="5" t="s">
+      <c r="E23" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="F23" s="5" t="s">
+      <c r="F23" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="G23" s="8"/>
-      <c r="H23" s="8"/>
-      <c r="I23" s="8"/>
+      <c r="G23" s="11"/>
+      <c r="H23" s="11"/>
+      <c r="I23" s="11"/>
     </row>
-    <row r="24" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A24" s="7">
+    <row r="24" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A24" s="9">
         <v>10</v>
       </c>
-      <c r="B24" s="7" t="s">
+      <c r="B24" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="C24" s="11" t="s">
+      <c r="C24" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="D24" s="11" t="s">
+      <c r="D24" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="E24" s="5" t="s">
+      <c r="E24" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="F24" s="5" t="s">
+      <c r="F24" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="G24" s="8"/>
-      <c r="H24" s="8"/>
-      <c r="I24" s="8"/>
+      <c r="G24" s="11"/>
+      <c r="H24" s="11"/>
+      <c r="I24" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1935,8 +1926,8 @@
     <mergeCell ref="A13:I13"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="F8" r:id="rId1" display="testingfyp2017@gmail.com_x000a_testingfyp"/>
-    <hyperlink ref="F16" r:id="rId2"/>
+    <hyperlink ref="F8" r:id="rId1" display="testingfyp2017@gmail.com_x000a_testingfyp" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="F16" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>

</xml_diff>

<commit_message>
Made changes to test plan excel file
</commit_message>
<xml_diff>
--- a/FYP documentation/FYP_Test_Plan.xlsx
+++ b/FYP documentation/FYP_Test_Plan.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18528"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6936" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6936" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Plan" sheetId="3" r:id="rId1"/>
+    <sheet name="Test Plan Final" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="86">
   <si>
     <t>Expected Result</t>
   </si>
@@ -233,13 +234,80 @@
   <si>
     <t>1. Enter valid phone number with country code 
 2. Click on 'SIGN UP' button</t>
+  </si>
+  <si>
+    <t>Test Plan</t>
+  </si>
+  <si>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>Objective</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Classification </t>
+  </si>
+  <si>
+    <t>Pre-requisite (if any)</t>
+  </si>
+  <si>
+    <t>Action</t>
+  </si>
+  <si>
+    <t>Expected result</t>
+  </si>
+  <si>
+    <t>Actual Result</t>
+  </si>
+  <si>
+    <t>All resposnd</t>
+  </si>
+  <si>
+    <t>Pass/Fail/Others</t>
+  </si>
+  <si>
+    <t>Tester Name</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>Case No</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test plan for login </t>
+  </si>
+  <si>
+    <t>Ther user should have already signed up previously</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The error messages for repective should appear </t>
+  </si>
+  <si>
+    <t>Login successfully</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Enter invalid values in required fields 
+2. Click on 'LOG IN' button  </t>
+  </si>
+  <si>
+    <t>Login fail</t>
+  </si>
+  <si>
+    <t>Sign up</t>
+  </si>
+  <si>
+    <t>Test plan for Signup</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -286,8 +354,46 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="TimesNewRomanPS-BoldMT"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="TimesNewRomanPSMT"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="TimesNewRomanPS-BoldMT"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -306,8 +412,25 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -380,22 +503,125 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color theme="4"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thick">
+        <color theme="4"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color theme="4"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -439,10 +665,151 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="6" xfId="3" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="5" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="7" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="8" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="12" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="13" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="15" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="6">
+    <cellStyle name="20% - Accent3" xfId="5" builtinId="38"/>
+    <cellStyle name="Accent1" xfId="4" builtinId="29"/>
+    <cellStyle name="Heading 1" xfId="3" builtinId="16"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Title" xfId="2" builtinId="15" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1502,423 +1869,423 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A4:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:I14"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="13.6640625" style="13" customWidth="1"/>
-    <col min="2" max="2" width="10" style="13" customWidth="1"/>
-    <col min="3" max="3" width="15.88671875" style="13" customWidth="1"/>
-    <col min="4" max="4" width="20.44140625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="24.5546875" style="4" customWidth="1"/>
-    <col min="6" max="6" width="26.44140625" style="18" customWidth="1"/>
-    <col min="7" max="7" width="16.6640625" style="4" customWidth="1"/>
-    <col min="8" max="8" width="12.77734375" style="4" customWidth="1"/>
-    <col min="9" max="9" width="12.88671875" style="4" customWidth="1"/>
-    <col min="10" max="16384" width="8.77734375" style="4"/>
+    <col min="1" max="1" width="13.6640625" style="10" customWidth="1"/>
+    <col min="2" max="2" width="10" style="10" customWidth="1"/>
+    <col min="3" max="3" width="15.88671875" style="10" customWidth="1"/>
+    <col min="4" max="4" width="20.44140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="24.5546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="26.44140625" style="15" customWidth="1"/>
+    <col min="7" max="7" width="16.6640625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="12.77734375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="12.88671875" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.77734375" style="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:9" ht="18">
+      <c r="A4" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="3"/>
-    </row>
-    <row r="5" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="5" t="s">
+      <c r="B4" s="17"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="18"/>
+    </row>
+    <row r="5" spans="1:9" s="4" customFormat="1">
+      <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="G5" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="H5" s="5" t="s">
+      <c r="H5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="I5" s="5" t="s">
+      <c r="I5" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:9" s="13" customFormat="1" ht="29.55" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="8">
+    <row r="6" spans="1:9" s="10" customFormat="1" ht="29.55" customHeight="1">
+      <c r="A6" s="5">
         <v>1</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="D6" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="E6" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="F6" s="10"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
-    </row>
-    <row r="7" spans="1:9" s="13" customFormat="1" ht="43.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="8">
+      <c r="F6" s="7"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+    </row>
+    <row r="7" spans="1:9" s="10" customFormat="1" ht="43.05" customHeight="1">
+      <c r="A7" s="5">
         <v>2</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="D7" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="E7" s="46" t="s">
         <v>50</v>
       </c>
-      <c r="F7" s="14" t="s">
+      <c r="F7" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="G7" s="11"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="12"/>
-    </row>
-    <row r="8" spans="1:9" s="13" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A8" s="8">
+      <c r="G7" s="8"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+    </row>
+    <row r="8" spans="1:9" s="10" customFormat="1" ht="43.2">
+      <c r="A8" s="5">
         <v>3</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="D8" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="E8" s="10" t="s">
+      <c r="E8" s="46" t="s">
         <v>49</v>
       </c>
-      <c r="F8" s="10" t="s">
+      <c r="F8" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="G8" s="11"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="12"/>
-    </row>
-    <row r="9" spans="1:9" s="13" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A9" s="8">
+      <c r="G8" s="8"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
+    </row>
+    <row r="9" spans="1:9" s="10" customFormat="1" ht="43.2">
+      <c r="A9" s="5">
         <v>4</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="9" t="s">
+      <c r="D9" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="E9" s="10" t="s">
+      <c r="E9" s="46" t="s">
         <v>51</v>
       </c>
-      <c r="F9" s="14"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12"/>
-      <c r="I9" s="12"/>
-    </row>
-    <row r="13" spans="1:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="A13" s="1" t="s">
+      <c r="F9" s="11"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+    </row>
+    <row r="13" spans="1:9" ht="18">
+      <c r="A13" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="3"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="5" t="s">
+      <c r="B13" s="17"/>
+      <c r="C13" s="17"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="17"/>
+      <c r="G13" s="17"/>
+      <c r="H13" s="17"/>
+      <c r="I13" s="18"/>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="D14" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E14" s="5" t="s">
+      <c r="E14" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F14" s="6" t="s">
+      <c r="F14" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G14" s="5" t="s">
+      <c r="G14" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="H14" s="5" t="s">
+      <c r="H14" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="I14" s="5" t="s">
+      <c r="I14" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="61.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="8">
+    <row r="15" spans="1:9" ht="61.95" customHeight="1">
+      <c r="A15" s="5">
         <v>1</v>
       </c>
-      <c r="B15" s="9" t="s">
+      <c r="B15" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C15" s="8" t="s">
+      <c r="C15" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D15" s="9" t="s">
+      <c r="D15" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E15" s="10" t="s">
+      <c r="E15" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="F15" s="10" t="s">
+      <c r="F15" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="G15" s="11"/>
-      <c r="H15" s="12"/>
-      <c r="I15" s="12"/>
-    </row>
-    <row r="16" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A16" s="8">
+      <c r="G15" s="8"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
+    </row>
+    <row r="16" spans="1:9" ht="28.8">
+      <c r="A16" s="5">
         <v>2</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C16" s="8" t="s">
+      <c r="C16" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D16" s="9" t="s">
+      <c r="D16" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="E16" s="10" t="s">
+      <c r="E16" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="F16" s="15" t="s">
+      <c r="F16" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="G16" s="11"/>
-      <c r="H16" s="12"/>
-      <c r="I16" s="12"/>
-    </row>
-    <row r="17" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A17" s="8">
+      <c r="G16" s="8"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="9"/>
+    </row>
+    <row r="17" spans="1:9" ht="57.6">
+      <c r="A17" s="5">
         <v>3</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="B17" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C17" s="8" t="s">
+      <c r="C17" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D17" s="9" t="s">
+      <c r="D17" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="E17" s="10" t="s">
+      <c r="E17" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="F17" s="16"/>
-      <c r="G17" s="11"/>
-      <c r="H17" s="12"/>
-      <c r="I17" s="12"/>
-    </row>
-    <row r="18" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A18" s="8">
+      <c r="F17" s="13"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="9"/>
+    </row>
+    <row r="18" spans="1:9" ht="57.6">
+      <c r="A18" s="5">
         <v>4</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C18" s="9" t="s">
+      <c r="C18" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D18" s="17" t="s">
+      <c r="D18" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="E18" s="10" t="s">
+      <c r="E18" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="F18" s="14" t="s">
+      <c r="F18" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="G18" s="12"/>
-      <c r="H18" s="12"/>
-      <c r="I18" s="12"/>
-    </row>
-    <row r="19" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A19" s="8">
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="9"/>
+    </row>
+    <row r="19" spans="1:9" ht="57.6">
+      <c r="A19" s="5">
         <v>5</v>
       </c>
-      <c r="B19" s="8" t="s">
+      <c r="B19" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C19" s="9" t="s">
+      <c r="C19" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D19" s="9" t="s">
+      <c r="D19" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="E19" s="10" t="s">
+      <c r="E19" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="F19" s="10" t="s">
+      <c r="F19" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="G19" s="12"/>
-      <c r="H19" s="12"/>
-      <c r="I19" s="12"/>
-    </row>
-    <row r="20" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A20" s="8">
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
+    </row>
+    <row r="20" spans="1:9" ht="57.6">
+      <c r="A20" s="5">
         <v>6</v>
       </c>
-      <c r="B20" s="8" t="s">
+      <c r="B20" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C20" s="9" t="s">
+      <c r="C20" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D20" s="9" t="s">
+      <c r="D20" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="E20" s="10" t="s">
+      <c r="E20" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="F20" s="14" t="s">
+      <c r="F20" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="G20" s="12"/>
-      <c r="H20" s="12"/>
-      <c r="I20" s="12"/>
-    </row>
-    <row r="21" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A21" s="8">
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="9"/>
+    </row>
+    <row r="21" spans="1:9" ht="57.6">
+      <c r="A21" s="5">
         <v>7</v>
       </c>
-      <c r="B21" s="8" t="s">
+      <c r="B21" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C21" s="9" t="s">
+      <c r="C21" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D21" s="9" t="s">
+      <c r="D21" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="E21" s="10" t="s">
+      <c r="E21" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="F21" s="10" t="s">
+      <c r="F21" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="G21" s="12"/>
-      <c r="H21" s="12"/>
-      <c r="I21" s="12"/>
-    </row>
-    <row r="22" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A22" s="9">
+      <c r="G21" s="9"/>
+      <c r="H21" s="9"/>
+      <c r="I21" s="9"/>
+    </row>
+    <row r="22" spans="1:9" ht="57.6">
+      <c r="A22" s="6">
         <v>8</v>
       </c>
-      <c r="B22" s="9" t="s">
+      <c r="B22" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="C22" s="9" t="s">
+      <c r="C22" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="D22" s="9" t="s">
+      <c r="D22" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="E22" s="10" t="s">
+      <c r="E22" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="F22" s="10" t="s">
+      <c r="F22" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="G22" s="11"/>
-      <c r="H22" s="11"/>
-      <c r="I22" s="11"/>
-    </row>
-    <row r="23" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A23" s="9">
+      <c r="G22" s="8"/>
+      <c r="H22" s="8"/>
+      <c r="I22" s="8"/>
+    </row>
+    <row r="23" spans="1:9" ht="57.6">
+      <c r="A23" s="6">
         <v>9</v>
       </c>
-      <c r="B23" s="9" t="s">
+      <c r="B23" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C23" s="9" t="s">
+      <c r="C23" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="D23" s="9" t="s">
+      <c r="D23" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="E23" s="10" t="s">
+      <c r="E23" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="F23" s="10" t="s">
+      <c r="F23" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="G23" s="11"/>
-      <c r="H23" s="11"/>
-      <c r="I23" s="11"/>
-    </row>
-    <row r="24" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A24" s="9">
+      <c r="G23" s="8"/>
+      <c r="H23" s="8"/>
+      <c r="I23" s="8"/>
+    </row>
+    <row r="24" spans="1:9" ht="43.2">
+      <c r="A24" s="6">
         <v>10</v>
       </c>
-      <c r="B24" s="9" t="s">
+      <c r="B24" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="C24" s="9" t="s">
+      <c r="C24" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="D24" s="9" t="s">
+      <c r="D24" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="E24" s="10" t="s">
+      <c r="E24" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="F24" s="10" t="s">
+      <c r="F24" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="G24" s="11"/>
-      <c r="H24" s="11"/>
-      <c r="I24" s="11"/>
+      <c r="G24" s="8"/>
+      <c r="H24" s="8"/>
+      <c r="I24" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1930,7 +2297,505 @@
     <hyperlink ref="F16" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="landscape" r:id="rId3"/>
   <drawing r:id="rId4"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93F0FCE8-3BDA-4408-86A1-FE4757BC6CF8}">
+  <dimension ref="A1:I45"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="9.88671875" customWidth="1"/>
+    <col min="2" max="2" width="13.5546875" customWidth="1"/>
+    <col min="3" max="3" width="13.109375" customWidth="1"/>
+    <col min="4" max="4" width="15.109375" customWidth="1"/>
+    <col min="5" max="5" width="8.6640625" customWidth="1"/>
+    <col min="6" max="6" width="41.6640625" customWidth="1"/>
+    <col min="7" max="7" width="15.44140625" customWidth="1"/>
+    <col min="8" max="8" width="10.5546875" customWidth="1"/>
+    <col min="9" max="9" width="7.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="40.799999999999997" customHeight="1">
+      <c r="A1" s="55" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" s="20"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="22"/>
+    </row>
+    <row r="3" spans="1:9" ht="31.2" customHeight="1" thickBot="1">
+      <c r="A3" s="23" t="s">
+        <v>84</v>
+      </c>
+      <c r="B3" s="23"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+    </row>
+    <row r="4" spans="1:9" ht="18.600000000000001" customHeight="1" thickTop="1">
+      <c r="A4" s="34" t="s">
+        <v>66</v>
+      </c>
+      <c r="B4" s="35"/>
+      <c r="C4" s="29" t="s">
+        <v>85</v>
+      </c>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="31"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+    </row>
+    <row r="5" spans="1:9" ht="14.4" customHeight="1">
+      <c r="A5" s="34" t="s">
+        <v>67</v>
+      </c>
+      <c r="B5" s="35"/>
+      <c r="C5" s="26"/>
+      <c r="D5" s="27"/>
+      <c r="E5" s="27"/>
+      <c r="F5" s="27"/>
+      <c r="G5" s="28"/>
+      <c r="H5" s="19"/>
+      <c r="I5" s="19"/>
+    </row>
+    <row r="6" spans="1:9" ht="14.4" customHeight="1">
+      <c r="A6" s="34" t="s">
+        <v>68</v>
+      </c>
+      <c r="B6" s="35"/>
+      <c r="C6" s="52"/>
+      <c r="D6" s="53"/>
+      <c r="E6" s="53"/>
+      <c r="F6" s="53"/>
+      <c r="G6" s="54"/>
+      <c r="H6" s="20"/>
+      <c r="I6" s="21"/>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="36"/>
+      <c r="B7" s="32"/>
+      <c r="C7" s="32"/>
+      <c r="D7" s="32"/>
+      <c r="E7" s="32"/>
+      <c r="F7" s="32"/>
+      <c r="G7" s="33"/>
+      <c r="H7" s="21"/>
+      <c r="I7" s="21"/>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" s="40" t="s">
+        <v>77</v>
+      </c>
+      <c r="B8" s="37" t="s">
+        <v>69</v>
+      </c>
+      <c r="C8" s="38"/>
+      <c r="D8" s="37" t="s">
+        <v>70</v>
+      </c>
+      <c r="E8" s="38"/>
+      <c r="F8" s="39" t="s">
+        <v>71</v>
+      </c>
+      <c r="G8" s="40" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="27" customHeight="1">
+      <c r="A9" s="41"/>
+      <c r="B9" s="47"/>
+      <c r="C9" s="48"/>
+      <c r="D9" s="47"/>
+      <c r="E9" s="48"/>
+      <c r="F9" s="25"/>
+      <c r="G9" s="25"/>
+    </row>
+    <row r="10" spans="1:9" ht="29.4" customHeight="1">
+      <c r="A10" s="41"/>
+      <c r="B10" s="49"/>
+      <c r="C10" s="50"/>
+      <c r="D10" s="49"/>
+      <c r="E10" s="50"/>
+      <c r="F10" s="25"/>
+      <c r="G10" s="25"/>
+    </row>
+    <row r="11" spans="1:9" ht="40.200000000000003" customHeight="1">
+      <c r="A11" s="41"/>
+      <c r="B11" s="49"/>
+      <c r="C11" s="50"/>
+      <c r="D11" s="49"/>
+      <c r="E11" s="50"/>
+      <c r="F11" s="25"/>
+      <c r="G11" s="25"/>
+    </row>
+    <row r="12" spans="1:9" ht="24" customHeight="1">
+      <c r="A12" s="41"/>
+      <c r="B12" s="49"/>
+      <c r="C12" s="50"/>
+      <c r="D12" s="49"/>
+      <c r="E12" s="50"/>
+      <c r="F12" s="25"/>
+      <c r="G12" s="25"/>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" s="37" t="s">
+        <v>74</v>
+      </c>
+      <c r="B13" s="38"/>
+      <c r="C13" s="42"/>
+      <c r="D13" s="24"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="24"/>
+      <c r="G13" s="43"/>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" s="37" t="s">
+        <v>75</v>
+      </c>
+      <c r="B14" s="38"/>
+      <c r="C14" s="42"/>
+      <c r="D14" s="24"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="24"/>
+      <c r="G14" s="43"/>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" s="44" t="s">
+        <v>76</v>
+      </c>
+      <c r="B15" s="38"/>
+      <c r="C15" s="42"/>
+      <c r="D15" s="24"/>
+      <c r="E15" s="24"/>
+      <c r="F15" s="24"/>
+      <c r="G15" s="43"/>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" s="44" t="s">
+        <v>73</v>
+      </c>
+      <c r="B16" s="45"/>
+      <c r="C16" s="42"/>
+      <c r="D16" s="24"/>
+      <c r="E16" s="24"/>
+      <c r="F16" s="24"/>
+      <c r="G16" s="43"/>
+    </row>
+    <row r="17" spans="1:7" ht="26.4" customHeight="1">
+      <c r="A17" s="21"/>
+      <c r="B17" s="21"/>
+      <c r="C17" s="21"/>
+      <c r="D17" s="21"/>
+      <c r="E17" s="21"/>
+      <c r="F17" s="21"/>
+      <c r="G17" s="21"/>
+    </row>
+    <row r="18" spans="1:7" ht="36" customHeight="1">
+      <c r="A18" s="21"/>
+      <c r="B18" s="21"/>
+      <c r="C18" s="21"/>
+      <c r="D18" s="21"/>
+      <c r="E18" s="21"/>
+      <c r="F18" s="21"/>
+      <c r="G18" s="21"/>
+    </row>
+    <row r="19" spans="1:7" ht="25.2" customHeight="1">
+      <c r="A19" s="21"/>
+      <c r="B19" s="21"/>
+      <c r="C19" s="21"/>
+      <c r="D19" s="21"/>
+      <c r="E19" s="21"/>
+      <c r="F19" s="21"/>
+      <c r="G19" s="21"/>
+    </row>
+    <row r="20" spans="1:7" ht="19.8" customHeight="1">
+      <c r="A20" s="21"/>
+      <c r="B20" s="21"/>
+      <c r="C20" s="21"/>
+      <c r="D20" s="21"/>
+      <c r="E20" s="21"/>
+      <c r="F20" s="21"/>
+      <c r="G20" s="21"/>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" s="21"/>
+      <c r="B21" s="21"/>
+      <c r="C21" s="21"/>
+      <c r="D21" s="21"/>
+      <c r="E21" s="21"/>
+      <c r="F21" s="21"/>
+      <c r="G21" s="21"/>
+    </row>
+    <row r="22" spans="1:7" ht="25.8" customHeight="1"/>
+    <row r="23" spans="1:7" ht="20.399999999999999" thickBot="1">
+      <c r="A23" s="23" t="s">
+        <v>65</v>
+      </c>
+      <c r="B23" s="23"/>
+      <c r="C23" s="23"/>
+      <c r="D23" s="23"/>
+      <c r="E23" s="23"/>
+      <c r="F23" s="23"/>
+      <c r="G23" s="23"/>
+    </row>
+    <row r="24" spans="1:7" ht="15" thickTop="1">
+      <c r="A24" s="61" t="s">
+        <v>66</v>
+      </c>
+      <c r="B24" s="62"/>
+      <c r="C24" s="58" t="s">
+        <v>78</v>
+      </c>
+      <c r="D24" s="59"/>
+      <c r="E24" s="59"/>
+      <c r="F24" s="59"/>
+      <c r="G24" s="60"/>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" s="34" t="s">
+        <v>67</v>
+      </c>
+      <c r="B25" s="35"/>
+      <c r="C25" s="26"/>
+      <c r="D25" s="27"/>
+      <c r="E25" s="27"/>
+      <c r="F25" s="27"/>
+      <c r="G25" s="28"/>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26" s="34" t="s">
+        <v>68</v>
+      </c>
+      <c r="B26" s="35"/>
+      <c r="C26" s="52" t="s">
+        <v>79</v>
+      </c>
+      <c r="D26" s="63"/>
+      <c r="E26" s="63"/>
+      <c r="F26" s="63"/>
+      <c r="G26" s="64"/>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27" s="42"/>
+      <c r="B27" s="24"/>
+      <c r="C27" s="24"/>
+      <c r="D27" s="24"/>
+      <c r="E27" s="24"/>
+      <c r="F27" s="24"/>
+      <c r="G27" s="43"/>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28" s="40" t="s">
+        <v>77</v>
+      </c>
+      <c r="B28" s="37" t="s">
+        <v>69</v>
+      </c>
+      <c r="C28" s="38"/>
+      <c r="D28" s="37" t="s">
+        <v>70</v>
+      </c>
+      <c r="E28" s="38"/>
+      <c r="F28" s="39" t="s">
+        <v>71</v>
+      </c>
+      <c r="G28" s="40" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="18" customHeight="1">
+      <c r="A29" s="41" t="s">
+        <v>5</v>
+      </c>
+      <c r="B29" s="49" t="s">
+        <v>17</v>
+      </c>
+      <c r="C29" s="50"/>
+      <c r="D29" s="47" t="s">
+        <v>72</v>
+      </c>
+      <c r="E29" s="48"/>
+      <c r="F29" s="25"/>
+      <c r="G29" s="25"/>
+    </row>
+    <row r="30" spans="1:7" ht="46.8" customHeight="1">
+      <c r="A30" s="41" t="s">
+        <v>6</v>
+      </c>
+      <c r="B30" s="49" t="s">
+        <v>50</v>
+      </c>
+      <c r="C30" s="50"/>
+      <c r="D30" s="49" t="s">
+        <v>80</v>
+      </c>
+      <c r="E30" s="50"/>
+      <c r="F30" s="25"/>
+      <c r="G30" s="25"/>
+    </row>
+    <row r="31" spans="1:7" ht="45.6" customHeight="1">
+      <c r="A31" s="41" t="s">
+        <v>7</v>
+      </c>
+      <c r="B31" s="49" t="s">
+        <v>49</v>
+      </c>
+      <c r="C31" s="50"/>
+      <c r="D31" s="49" t="s">
+        <v>81</v>
+      </c>
+      <c r="E31" s="50"/>
+      <c r="F31" s="25"/>
+      <c r="G31" s="25"/>
+    </row>
+    <row r="32" spans="1:7" ht="48" customHeight="1">
+      <c r="A32" s="41" t="s">
+        <v>8</v>
+      </c>
+      <c r="B32" s="49" t="s">
+        <v>82</v>
+      </c>
+      <c r="C32" s="50"/>
+      <c r="D32" s="49" t="s">
+        <v>83</v>
+      </c>
+      <c r="E32" s="50"/>
+      <c r="F32" s="25"/>
+      <c r="G32" s="25"/>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="A33" s="37" t="s">
+        <v>74</v>
+      </c>
+      <c r="B33" s="38"/>
+      <c r="C33" s="42"/>
+      <c r="D33" s="24"/>
+      <c r="E33" s="24"/>
+      <c r="F33" s="24"/>
+      <c r="G33" s="43"/>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="A34" s="37" t="s">
+        <v>75</v>
+      </c>
+      <c r="B34" s="38"/>
+      <c r="C34" s="42"/>
+      <c r="D34" s="24"/>
+      <c r="E34" s="24"/>
+      <c r="F34" s="24"/>
+      <c r="G34" s="43"/>
+    </row>
+    <row r="35" spans="1:7">
+      <c r="A35" s="44" t="s">
+        <v>76</v>
+      </c>
+      <c r="B35" s="45"/>
+      <c r="C35" s="42"/>
+      <c r="D35" s="24"/>
+      <c r="E35" s="24"/>
+      <c r="F35" s="24"/>
+      <c r="G35" s="43"/>
+    </row>
+    <row r="36" spans="1:7">
+      <c r="A36" s="44" t="s">
+        <v>73</v>
+      </c>
+      <c r="B36" s="45"/>
+      <c r="C36" s="42"/>
+      <c r="D36" s="24"/>
+      <c r="E36" s="24"/>
+      <c r="F36" s="24"/>
+      <c r="G36" s="43"/>
+    </row>
+    <row r="44" spans="1:7" ht="31.8" customHeight="1"/>
+    <row r="45" spans="1:7" ht="63" customHeight="1"/>
+  </sheetData>
+  <mergeCells count="53">
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="C34:G34"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="C35:G35"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="C36:G36"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="C33:G33"/>
+    <mergeCell ref="A27:G27"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="A23:G23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="C24:G24"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="C25:G25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="C26:G26"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="C15:G15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="C16:G16"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="C13:G13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="C14:G14"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="A3:G3"/>
+    <mergeCell ref="A7:G7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:G6"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:G4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:G5"/>
+    <mergeCell ref="A1:G1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added instanse ID test case  to test plan
</commit_message>
<xml_diff>
--- a/FYP documentation/FYP_Test_Plan.xlsx
+++ b/FYP documentation/FYP_Test_Plan.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18528"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Durrah\UOW- Year 3\CSCI 321 - FYP\GitRepo\BSS_FYP_TEAM173D\FYP documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Class_notes\BSS_FYP_TEAM173D\FYP documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6940"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6936" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Plan Final" sheetId="4" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="110">
   <si>
     <t>Expected Result</t>
   </si>
@@ -352,11 +352,44 @@
     <t>1) Enter valid phone number with country code 
 2) Click on 'SIGN UP' button</t>
   </si>
+  <si>
+    <t>Test Instance ID verification</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The user must be logged in </t>
+  </si>
+  <si>
+    <t>The first device should log out</t>
+  </si>
+  <si>
+    <t>Instance ID Verification</t>
+  </si>
+  <si>
+    <t>1. Login to first device.               2. Login to second device</t>
+  </si>
+  <si>
+    <t>Password Recovery</t>
+  </si>
+  <si>
+    <t>The user should have previously signed up</t>
+  </si>
+  <si>
+    <t>Test if the user can recover password and forms work perfectly.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. click forget password                 2. Enter password1   in current password field             </t>
+  </si>
+  <si>
+    <t>1. Enter invalid email                      2. Click forget password</t>
+  </si>
+  <si>
+    <t>There should be a error message and no verificationemail sent over to client.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="12">
     <font>
       <sz val="11"/>
@@ -735,6 +768,131 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="6" xfId="3" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="13" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="15" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="7" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="8" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="12" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -743,131 +901,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="6" xfId="3" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="13" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="15" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="7" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="8" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="12" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -1933,36 +1966,36 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I51"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18:E18"/>
+    <sheetView tabSelected="1" topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D66" sqref="D66:E66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="9.90625" customWidth="1"/>
-    <col min="2" max="2" width="13.54296875" customWidth="1"/>
-    <col min="3" max="3" width="13.08984375" customWidth="1"/>
-    <col min="4" max="4" width="15.08984375" customWidth="1"/>
-    <col min="5" max="5" width="8.6328125" customWidth="1"/>
-    <col min="6" max="6" width="41.6328125" customWidth="1"/>
-    <col min="7" max="7" width="15.453125" customWidth="1"/>
-    <col min="8" max="8" width="10.54296875" customWidth="1"/>
-    <col min="9" max="9" width="7.1796875" customWidth="1"/>
+    <col min="1" max="1" width="9.88671875" customWidth="1"/>
+    <col min="2" max="2" width="13.5546875" customWidth="1"/>
+    <col min="3" max="3" width="13.109375" customWidth="1"/>
+    <col min="4" max="4" width="15.109375" customWidth="1"/>
+    <col min="5" max="5" width="8.6640625" customWidth="1"/>
+    <col min="6" max="6" width="41.6640625" customWidth="1"/>
+    <col min="7" max="7" width="15.44140625" customWidth="1"/>
+    <col min="8" max="8" width="10.5546875" customWidth="1"/>
+    <col min="9" max="9" width="7.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="40.75" customHeight="1">
-      <c r="A1" s="62" t="s">
+    <row r="1" spans="1:9" ht="40.799999999999997" customHeight="1">
+      <c r="A1" s="66" t="s">
         <v>64</v>
       </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
-      <c r="F1" s="63"/>
-      <c r="G1" s="64"/>
+      <c r="B1" s="67"/>
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
+      <c r="F1" s="67"/>
+      <c r="G1" s="68"/>
       <c r="H1" s="16"/>
       <c r="I1" s="16"/>
     </row>
@@ -1977,68 +2010,68 @@
       <c r="H2" s="19"/>
       <c r="I2" s="19"/>
     </row>
-    <row r="3" spans="1:9" ht="31.25" customHeight="1" thickBot="1">
-      <c r="A3" s="40" t="s">
+    <row r="3" spans="1:9" ht="31.2" customHeight="1" thickBot="1">
+      <c r="A3" s="46" t="s">
         <v>83</v>
       </c>
-      <c r="B3" s="40"/>
-      <c r="C3" s="40"/>
-      <c r="D3" s="40"/>
-      <c r="E3" s="40"/>
-      <c r="F3" s="40"/>
-      <c r="G3" s="40"/>
+      <c r="B3" s="46"/>
+      <c r="C3" s="46"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="46"/>
+      <c r="F3" s="46"/>
+      <c r="G3" s="46"/>
       <c r="H3" s="16"/>
       <c r="I3" s="16"/>
     </row>
-    <row r="4" spans="1:9" ht="18.649999999999999" customHeight="1" thickTop="1">
-      <c r="A4" s="46" t="s">
+    <row r="4" spans="1:9" ht="18.600000000000001" customHeight="1" thickTop="1">
+      <c r="A4" s="38" t="s">
         <v>66</v>
       </c>
-      <c r="B4" s="47"/>
-      <c r="C4" s="59" t="s">
+      <c r="B4" s="39"/>
+      <c r="C4" s="47" t="s">
         <v>84</v>
       </c>
-      <c r="D4" s="60"/>
-      <c r="E4" s="60"/>
-      <c r="F4" s="60"/>
-      <c r="G4" s="61"/>
+      <c r="D4" s="48"/>
+      <c r="E4" s="48"/>
+      <c r="F4" s="48"/>
+      <c r="G4" s="49"/>
       <c r="H4" s="17"/>
       <c r="I4" s="17"/>
     </row>
     <row r="5" spans="1:9" ht="14.4" customHeight="1">
-      <c r="A5" s="46" t="s">
+      <c r="A5" s="38" t="s">
         <v>67</v>
       </c>
-      <c r="B5" s="47"/>
-      <c r="C5" s="48"/>
-      <c r="D5" s="49"/>
-      <c r="E5" s="49"/>
-      <c r="F5" s="49"/>
-      <c r="G5" s="50"/>
+      <c r="B5" s="39"/>
+      <c r="C5" s="50"/>
+      <c r="D5" s="51"/>
+      <c r="E5" s="51"/>
+      <c r="F5" s="51"/>
+      <c r="G5" s="52"/>
       <c r="H5" s="16"/>
       <c r="I5" s="16"/>
     </row>
     <row r="6" spans="1:9" ht="14.4" customHeight="1">
-      <c r="A6" s="46" t="s">
+      <c r="A6" s="38" t="s">
         <v>68</v>
       </c>
-      <c r="B6" s="47"/>
-      <c r="C6" s="51"/>
-      <c r="D6" s="57"/>
-      <c r="E6" s="57"/>
-      <c r="F6" s="57"/>
-      <c r="G6" s="58"/>
+      <c r="B6" s="39"/>
+      <c r="C6" s="40"/>
+      <c r="D6" s="41"/>
+      <c r="E6" s="41"/>
+      <c r="F6" s="41"/>
+      <c r="G6" s="42"/>
       <c r="H6" s="17"/>
       <c r="I6" s="18"/>
     </row>
     <row r="7" spans="1:9">
-      <c r="A7" s="54"/>
-      <c r="B7" s="55"/>
-      <c r="C7" s="55"/>
-      <c r="D7" s="55"/>
-      <c r="E7" s="55"/>
-      <c r="F7" s="55"/>
-      <c r="G7" s="56"/>
+      <c r="A7" s="43"/>
+      <c r="B7" s="44"/>
+      <c r="C7" s="44"/>
+      <c r="D7" s="44"/>
+      <c r="E7" s="44"/>
+      <c r="F7" s="44"/>
+      <c r="G7" s="45"/>
       <c r="H7" s="18"/>
       <c r="I7" s="18"/>
     </row>
@@ -2046,11 +2079,11 @@
       <c r="A8" s="22" t="s">
         <v>77</v>
       </c>
-      <c r="B8" s="29" t="s">
+      <c r="B8" s="35" t="s">
         <v>69</v>
       </c>
       <c r="C8" s="30"/>
-      <c r="D8" s="29" t="s">
+      <c r="D8" s="35" t="s">
         <v>70</v>
       </c>
       <c r="E8" s="30"/>
@@ -2062,157 +2095,157 @@
       </c>
     </row>
     <row r="9" spans="1:9" ht="34.5" customHeight="1">
-      <c r="A9" s="68" t="s">
+      <c r="A9" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="66" t="s">
+      <c r="B9" s="36" t="s">
         <v>85</v>
       </c>
-      <c r="C9" s="65"/>
-      <c r="D9" s="66" t="s">
+      <c r="C9" s="37"/>
+      <c r="D9" s="36" t="s">
         <v>90</v>
       </c>
-      <c r="E9" s="65"/>
+      <c r="E9" s="37"/>
       <c r="F9" s="20"/>
       <c r="G9" s="20"/>
     </row>
     <row r="10" spans="1:9" ht="29.4" customHeight="1">
-      <c r="A10" s="68" t="s">
+      <c r="A10" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="66" t="s">
+      <c r="B10" s="36" t="s">
         <v>88</v>
       </c>
-      <c r="C10" s="65"/>
-      <c r="D10" s="66" t="s">
+      <c r="C10" s="37"/>
+      <c r="D10" s="36" t="s">
         <v>91</v>
       </c>
-      <c r="E10" s="67"/>
+      <c r="E10" s="55"/>
       <c r="F10" s="20"/>
       <c r="G10" s="20"/>
     </row>
-    <row r="11" spans="1:9" ht="40.25" customHeight="1">
-      <c r="A11" s="68" t="s">
+    <row r="11" spans="1:9" ht="40.200000000000003" customHeight="1">
+      <c r="A11" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="66" t="s">
+      <c r="B11" s="36" t="s">
         <v>89</v>
       </c>
-      <c r="C11" s="65"/>
-      <c r="D11" s="66" t="s">
+      <c r="C11" s="37"/>
+      <c r="D11" s="36" t="s">
         <v>87</v>
       </c>
-      <c r="E11" s="65"/>
+      <c r="E11" s="37"/>
       <c r="F11" s="20"/>
       <c r="G11" s="20"/>
     </row>
     <row r="12" spans="1:9" ht="58.5" customHeight="1">
-      <c r="A12" s="68" t="s">
+      <c r="A12" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="66" t="s">
+      <c r="B12" s="36" t="s">
         <v>92</v>
       </c>
-      <c r="C12" s="67"/>
-      <c r="D12" s="66" t="s">
+      <c r="C12" s="55"/>
+      <c r="D12" s="36" t="s">
         <v>87</v>
       </c>
-      <c r="E12" s="65"/>
+      <c r="E12" s="37"/>
       <c r="F12" s="20"/>
       <c r="G12" s="20"/>
     </row>
     <row r="13" spans="1:9" ht="57" customHeight="1">
-      <c r="A13" s="68" t="s">
+      <c r="A13" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="B13" s="66" t="s">
+      <c r="B13" s="36" t="s">
         <v>94</v>
       </c>
-      <c r="C13" s="67"/>
-      <c r="D13" s="66" t="s">
+      <c r="C13" s="55"/>
+      <c r="D13" s="36" t="s">
         <v>87</v>
       </c>
-      <c r="E13" s="65"/>
+      <c r="E13" s="37"/>
       <c r="F13" s="20"/>
       <c r="G13" s="20"/>
     </row>
-    <row r="14" spans="1:9" ht="56" customHeight="1">
-      <c r="A14" s="68" t="s">
+    <row r="14" spans="1:9" ht="55.95" customHeight="1">
+      <c r="A14" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="B14" s="66" t="s">
+      <c r="B14" s="36" t="s">
         <v>93</v>
       </c>
-      <c r="C14" s="65"/>
-      <c r="D14" s="66" t="s">
+      <c r="C14" s="37"/>
+      <c r="D14" s="36" t="s">
         <v>87</v>
       </c>
-      <c r="E14" s="65"/>
+      <c r="E14" s="37"/>
       <c r="F14" s="20"/>
       <c r="G14" s="20"/>
     </row>
-    <row r="15" spans="1:9" ht="56" customHeight="1">
-      <c r="A15" s="68" t="s">
+    <row r="15" spans="1:9" ht="55.95" customHeight="1">
+      <c r="A15" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="B15" s="71" t="s">
+      <c r="B15" s="56" t="s">
         <v>95</v>
       </c>
-      <c r="C15" s="71"/>
-      <c r="D15" s="66" t="s">
+      <c r="C15" s="56"/>
+      <c r="D15" s="36" t="s">
         <v>91</v>
       </c>
-      <c r="E15" s="67"/>
-      <c r="F15" s="69"/>
-      <c r="G15" s="70"/>
-    </row>
-    <row r="16" spans="1:9" ht="45.5" customHeight="1">
-      <c r="A16" s="68" t="s">
+      <c r="E15" s="55"/>
+      <c r="F15" s="27"/>
+      <c r="G15" s="28"/>
+    </row>
+    <row r="16" spans="1:9" ht="45.45" customHeight="1">
+      <c r="A16" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="B16" s="71" t="s">
+      <c r="B16" s="56" t="s">
         <v>96</v>
       </c>
-      <c r="C16" s="71"/>
-      <c r="D16" s="66" t="s">
+      <c r="C16" s="56"/>
+      <c r="D16" s="36" t="s">
         <v>87</v>
       </c>
-      <c r="E16" s="65"/>
-      <c r="F16" s="69"/>
-      <c r="G16" s="70"/>
-    </row>
-    <row r="17" spans="1:7" ht="45.5" customHeight="1">
-      <c r="A17" s="68" t="s">
+      <c r="E16" s="37"/>
+      <c r="F16" s="27"/>
+      <c r="G16" s="28"/>
+    </row>
+    <row r="17" spans="1:7" ht="45.45" customHeight="1">
+      <c r="A17" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="B17" s="71" t="s">
+      <c r="B17" s="56" t="s">
         <v>97</v>
       </c>
-      <c r="C17" s="71"/>
-      <c r="D17" s="66" t="s">
+      <c r="C17" s="56"/>
+      <c r="D17" s="36" t="s">
         <v>87</v>
       </c>
-      <c r="E17" s="65"/>
-      <c r="F17" s="69"/>
-      <c r="G17" s="70"/>
-    </row>
-    <row r="18" spans="1:7" ht="45.5" customHeight="1">
-      <c r="A18" s="68" t="s">
+      <c r="E17" s="37"/>
+      <c r="F17" s="27"/>
+      <c r="G17" s="28"/>
+    </row>
+    <row r="18" spans="1:7" ht="45.45" customHeight="1">
+      <c r="A18" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="B18" s="71" t="s">
+      <c r="B18" s="56" t="s">
         <v>98</v>
       </c>
-      <c r="C18" s="71"/>
-      <c r="D18" s="66" t="s">
+      <c r="C18" s="56"/>
+      <c r="D18" s="36" t="s">
         <v>91</v>
       </c>
-      <c r="E18" s="67"/>
-      <c r="F18" s="69"/>
-      <c r="G18" s="70"/>
+      <c r="E18" s="55"/>
+      <c r="F18" s="27"/>
+      <c r="G18" s="28"/>
     </row>
     <row r="19" spans="1:7">
-      <c r="A19" s="29" t="s">
+      <c r="A19" s="35" t="s">
         <v>74</v>
       </c>
       <c r="B19" s="30"/>
@@ -2223,7 +2256,7 @@
       <c r="G19" s="33"/>
     </row>
     <row r="20" spans="1:7">
-      <c r="A20" s="29" t="s">
+      <c r="A20" s="35" t="s">
         <v>75</v>
       </c>
       <c r="B20" s="30"/>
@@ -2234,7 +2267,7 @@
       <c r="G20" s="33"/>
     </row>
     <row r="21" spans="1:7">
-      <c r="A21" s="34" t="s">
+      <c r="A21" s="29" t="s">
         <v>76</v>
       </c>
       <c r="B21" s="30"/>
@@ -2245,10 +2278,10 @@
       <c r="G21" s="33"/>
     </row>
     <row r="22" spans="1:7">
-      <c r="A22" s="34" t="s">
+      <c r="A22" s="29" t="s">
         <v>73</v>
       </c>
-      <c r="B22" s="35"/>
+      <c r="B22" s="34"/>
       <c r="C22" s="31"/>
       <c r="D22" s="32"/>
       <c r="E22" s="32"/>
@@ -2273,7 +2306,7 @@
       <c r="F24" s="18"/>
       <c r="G24" s="18"/>
     </row>
-    <row r="25" spans="1:7" ht="25.25" customHeight="1">
+    <row r="25" spans="1:7" ht="25.2" customHeight="1">
       <c r="A25" s="18"/>
       <c r="B25" s="18"/>
       <c r="C25" s="18"/>
@@ -2282,7 +2315,7 @@
       <c r="F25" s="18"/>
       <c r="G25" s="18"/>
     </row>
-    <row r="26" spans="1:7" ht="19.75" customHeight="1">
+    <row r="26" spans="1:7" ht="19.8" customHeight="1">
       <c r="A26" s="18"/>
       <c r="B26" s="18"/>
       <c r="C26" s="18"/>
@@ -2300,54 +2333,54 @@
       <c r="F27" s="18"/>
       <c r="G27" s="18"/>
     </row>
-    <row r="28" spans="1:7" ht="25.75" customHeight="1"/>
-    <row r="29" spans="1:7" ht="20" thickBot="1">
-      <c r="A29" s="40" t="s">
+    <row r="28" spans="1:7" ht="25.8" customHeight="1"/>
+    <row r="29" spans="1:7" ht="20.399999999999999" thickBot="1">
+      <c r="A29" s="46" t="s">
         <v>65</v>
       </c>
-      <c r="B29" s="40"/>
-      <c r="C29" s="40"/>
-      <c r="D29" s="40"/>
-      <c r="E29" s="40"/>
-      <c r="F29" s="40"/>
-      <c r="G29" s="40"/>
+      <c r="B29" s="46"/>
+      <c r="C29" s="46"/>
+      <c r="D29" s="46"/>
+      <c r="E29" s="46"/>
+      <c r="F29" s="46"/>
+      <c r="G29" s="46"/>
     </row>
     <row r="30" spans="1:7" ht="15" thickTop="1">
-      <c r="A30" s="41" t="s">
+      <c r="A30" s="57" t="s">
         <v>66</v>
       </c>
-      <c r="B30" s="42"/>
-      <c r="C30" s="43" t="s">
+      <c r="B30" s="58"/>
+      <c r="C30" s="59" t="s">
         <v>78</v>
       </c>
-      <c r="D30" s="44"/>
-      <c r="E30" s="44"/>
-      <c r="F30" s="44"/>
-      <c r="G30" s="45"/>
+      <c r="D30" s="60"/>
+      <c r="E30" s="60"/>
+      <c r="F30" s="60"/>
+      <c r="G30" s="61"/>
     </row>
     <row r="31" spans="1:7">
-      <c r="A31" s="46" t="s">
+      <c r="A31" s="38" t="s">
         <v>67</v>
       </c>
-      <c r="B31" s="47"/>
-      <c r="C31" s="48"/>
-      <c r="D31" s="49"/>
-      <c r="E31" s="49"/>
-      <c r="F31" s="49"/>
-      <c r="G31" s="50"/>
+      <c r="B31" s="39"/>
+      <c r="C31" s="50"/>
+      <c r="D31" s="51"/>
+      <c r="E31" s="51"/>
+      <c r="F31" s="51"/>
+      <c r="G31" s="52"/>
     </row>
     <row r="32" spans="1:7">
-      <c r="A32" s="46" t="s">
+      <c r="A32" s="38" t="s">
         <v>68</v>
       </c>
-      <c r="B32" s="47"/>
-      <c r="C32" s="51" t="s">
+      <c r="B32" s="39"/>
+      <c r="C32" s="40" t="s">
         <v>79</v>
       </c>
-      <c r="D32" s="52"/>
-      <c r="E32" s="52"/>
-      <c r="F32" s="52"/>
-      <c r="G32" s="53"/>
+      <c r="D32" s="62"/>
+      <c r="E32" s="62"/>
+      <c r="F32" s="62"/>
+      <c r="G32" s="63"/>
     </row>
     <row r="33" spans="1:7">
       <c r="A33" s="31"/>
@@ -2362,11 +2395,11 @@
       <c r="A34" s="22" t="s">
         <v>77</v>
       </c>
-      <c r="B34" s="29" t="s">
+      <c r="B34" s="35" t="s">
         <v>69</v>
       </c>
       <c r="C34" s="30"/>
-      <c r="D34" s="29" t="s">
+      <c r="D34" s="35" t="s">
         <v>70</v>
       </c>
       <c r="E34" s="30"/>
@@ -2381,64 +2414,64 @@
       <c r="A35" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="B35" s="36" t="s">
+      <c r="B35" s="53" t="s">
         <v>17</v>
       </c>
-      <c r="C35" s="37"/>
-      <c r="D35" s="38" t="s">
+      <c r="C35" s="54"/>
+      <c r="D35" s="64" t="s">
         <v>72</v>
       </c>
-      <c r="E35" s="39"/>
+      <c r="E35" s="65"/>
       <c r="F35" s="20"/>
       <c r="G35" s="20"/>
     </row>
-    <row r="36" spans="1:7" ht="46.75" customHeight="1">
-      <c r="A36" s="68" t="s">
+    <row r="36" spans="1:7" ht="46.8" customHeight="1">
+      <c r="A36" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="B36" s="36" t="s">
+      <c r="B36" s="53" t="s">
         <v>50</v>
       </c>
-      <c r="C36" s="37"/>
-      <c r="D36" s="66" t="s">
+      <c r="C36" s="54"/>
+      <c r="D36" s="36" t="s">
         <v>86</v>
       </c>
-      <c r="E36" s="67"/>
+      <c r="E36" s="55"/>
       <c r="F36" s="20"/>
       <c r="G36" s="20"/>
     </row>
-    <row r="37" spans="1:7" ht="45.65" customHeight="1">
-      <c r="A37" s="68" t="s">
+    <row r="37" spans="1:7" ht="45.6" customHeight="1">
+      <c r="A37" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="B37" s="36" t="s">
+      <c r="B37" s="53" t="s">
         <v>49</v>
       </c>
-      <c r="C37" s="37"/>
-      <c r="D37" s="66" t="s">
+      <c r="C37" s="54"/>
+      <c r="D37" s="36" t="s">
         <v>80</v>
       </c>
-      <c r="E37" s="67"/>
+      <c r="E37" s="55"/>
       <c r="F37" s="20"/>
       <c r="G37" s="20"/>
     </row>
     <row r="38" spans="1:7" ht="48" customHeight="1">
-      <c r="A38" s="68" t="s">
+      <c r="A38" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="B38" s="36" t="s">
+      <c r="B38" s="53" t="s">
         <v>81</v>
       </c>
-      <c r="C38" s="37"/>
-      <c r="D38" s="66" t="s">
+      <c r="C38" s="54"/>
+      <c r="D38" s="36" t="s">
         <v>82</v>
       </c>
-      <c r="E38" s="67"/>
+      <c r="E38" s="55"/>
       <c r="F38" s="20"/>
       <c r="G38" s="20"/>
     </row>
     <row r="39" spans="1:7">
-      <c r="A39" s="29" t="s">
+      <c r="A39" s="35" t="s">
         <v>74</v>
       </c>
       <c r="B39" s="30"/>
@@ -2449,7 +2482,7 @@
       <c r="G39" s="33"/>
     </row>
     <row r="40" spans="1:7">
-      <c r="A40" s="29" t="s">
+      <c r="A40" s="35" t="s">
         <v>75</v>
       </c>
       <c r="B40" s="30"/>
@@ -2460,10 +2493,10 @@
       <c r="G40" s="33"/>
     </row>
     <row r="41" spans="1:7">
-      <c r="A41" s="34" t="s">
+      <c r="A41" s="29" t="s">
         <v>76</v>
       </c>
-      <c r="B41" s="35"/>
+      <c r="B41" s="34"/>
       <c r="C41" s="31"/>
       <c r="D41" s="32"/>
       <c r="E41" s="32"/>
@@ -2471,20 +2504,323 @@
       <c r="G41" s="33"/>
     </row>
     <row r="42" spans="1:7">
-      <c r="A42" s="34" t="s">
+      <c r="A42" s="29" t="s">
         <v>73</v>
       </c>
-      <c r="B42" s="35"/>
+      <c r="B42" s="34"/>
       <c r="C42" s="31"/>
       <c r="D42" s="32"/>
       <c r="E42" s="32"/>
       <c r="F42" s="32"/>
       <c r="G42" s="33"/>
     </row>
-    <row r="50" ht="31.75" customHeight="1"/>
-    <row r="51" ht="63" customHeight="1"/>
+    <row r="46" spans="1:7" ht="20.399999999999999" thickBot="1">
+      <c r="A46" s="46" t="s">
+        <v>102</v>
+      </c>
+      <c r="B46" s="46"/>
+      <c r="C46" s="46"/>
+      <c r="D46" s="46"/>
+      <c r="E46" s="46"/>
+      <c r="F46" s="46"/>
+      <c r="G46" s="46"/>
+    </row>
+    <row r="47" spans="1:7" ht="15" thickTop="1">
+      <c r="A47" s="38" t="s">
+        <v>66</v>
+      </c>
+      <c r="B47" s="39"/>
+      <c r="C47" s="47" t="s">
+        <v>99</v>
+      </c>
+      <c r="D47" s="48"/>
+      <c r="E47" s="48"/>
+      <c r="F47" s="48"/>
+      <c r="G47" s="49"/>
+    </row>
+    <row r="48" spans="1:7">
+      <c r="A48" s="38" t="s">
+        <v>67</v>
+      </c>
+      <c r="B48" s="39"/>
+      <c r="C48" s="50"/>
+      <c r="D48" s="51"/>
+      <c r="E48" s="51"/>
+      <c r="F48" s="51"/>
+      <c r="G48" s="52"/>
+    </row>
+    <row r="49" spans="1:7">
+      <c r="A49" s="38" t="s">
+        <v>68</v>
+      </c>
+      <c r="B49" s="39"/>
+      <c r="C49" s="40" t="s">
+        <v>100</v>
+      </c>
+      <c r="D49" s="41"/>
+      <c r="E49" s="41"/>
+      <c r="F49" s="41"/>
+      <c r="G49" s="42"/>
+    </row>
+    <row r="50" spans="1:7" ht="31.8" customHeight="1">
+      <c r="A50" s="43"/>
+      <c r="B50" s="44"/>
+      <c r="C50" s="44"/>
+      <c r="D50" s="44"/>
+      <c r="E50" s="44"/>
+      <c r="F50" s="44"/>
+      <c r="G50" s="45"/>
+    </row>
+    <row r="51" spans="1:7" ht="63" customHeight="1">
+      <c r="A51" s="22" t="s">
+        <v>77</v>
+      </c>
+      <c r="B51" s="35" t="s">
+        <v>69</v>
+      </c>
+      <c r="C51" s="30"/>
+      <c r="D51" s="35" t="s">
+        <v>70</v>
+      </c>
+      <c r="E51" s="30"/>
+      <c r="F51" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="G51" s="22" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" ht="54" customHeight="1">
+      <c r="A52" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="B52" s="36" t="s">
+        <v>103</v>
+      </c>
+      <c r="C52" s="37"/>
+      <c r="D52" s="36" t="s">
+        <v>101</v>
+      </c>
+      <c r="E52" s="37"/>
+      <c r="F52" s="20"/>
+      <c r="G52" s="20"/>
+    </row>
+    <row r="53" spans="1:7" ht="27" customHeight="1">
+      <c r="A53" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="B53" s="30"/>
+      <c r="C53" s="31"/>
+      <c r="D53" s="32"/>
+      <c r="E53" s="32"/>
+      <c r="F53" s="32"/>
+      <c r="G53" s="33"/>
+    </row>
+    <row r="54" spans="1:7" ht="34.799999999999997" customHeight="1">
+      <c r="A54" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="B54" s="30"/>
+      <c r="C54" s="31"/>
+      <c r="D54" s="32"/>
+      <c r="E54" s="32"/>
+      <c r="F54" s="32"/>
+      <c r="G54" s="33"/>
+    </row>
+    <row r="55" spans="1:7" ht="25.2" customHeight="1">
+      <c r="A55" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="B55" s="30"/>
+      <c r="C55" s="31"/>
+      <c r="D55" s="32"/>
+      <c r="E55" s="32"/>
+      <c r="F55" s="32"/>
+      <c r="G55" s="33"/>
+    </row>
+    <row r="56" spans="1:7">
+      <c r="A56" s="29" t="s">
+        <v>73</v>
+      </c>
+      <c r="B56" s="34"/>
+      <c r="C56" s="31"/>
+      <c r="D56" s="32"/>
+      <c r="E56" s="32"/>
+      <c r="F56" s="32"/>
+      <c r="G56" s="33"/>
+    </row>
+    <row r="59" spans="1:7" ht="20.399999999999999" thickBot="1">
+      <c r="A59" s="46" t="s">
+        <v>104</v>
+      </c>
+      <c r="B59" s="46"/>
+      <c r="C59" s="46"/>
+      <c r="D59" s="46"/>
+      <c r="E59" s="46"/>
+      <c r="F59" s="46"/>
+      <c r="G59" s="46"/>
+    </row>
+    <row r="60" spans="1:7" ht="15" thickTop="1">
+      <c r="A60" s="38" t="s">
+        <v>66</v>
+      </c>
+      <c r="B60" s="39"/>
+      <c r="C60" s="47" t="s">
+        <v>106</v>
+      </c>
+      <c r="D60" s="48"/>
+      <c r="E60" s="48"/>
+      <c r="F60" s="48"/>
+      <c r="G60" s="49"/>
+    </row>
+    <row r="61" spans="1:7">
+      <c r="A61" s="38" t="s">
+        <v>67</v>
+      </c>
+      <c r="B61" s="39"/>
+      <c r="C61" s="50"/>
+      <c r="D61" s="51"/>
+      <c r="E61" s="51"/>
+      <c r="F61" s="51"/>
+      <c r="G61" s="52"/>
+    </row>
+    <row r="62" spans="1:7">
+      <c r="A62" s="38" t="s">
+        <v>68</v>
+      </c>
+      <c r="B62" s="39"/>
+      <c r="C62" s="40" t="s">
+        <v>105</v>
+      </c>
+      <c r="D62" s="41"/>
+      <c r="E62" s="41"/>
+      <c r="F62" s="41"/>
+      <c r="G62" s="42"/>
+    </row>
+    <row r="63" spans="1:7">
+      <c r="A63" s="43"/>
+      <c r="B63" s="44"/>
+      <c r="C63" s="44"/>
+      <c r="D63" s="44"/>
+      <c r="E63" s="44"/>
+      <c r="F63" s="44"/>
+      <c r="G63" s="45"/>
+    </row>
+    <row r="64" spans="1:7">
+      <c r="A64" s="22" t="s">
+        <v>77</v>
+      </c>
+      <c r="B64" s="35" t="s">
+        <v>69</v>
+      </c>
+      <c r="C64" s="30"/>
+      <c r="D64" s="35" t="s">
+        <v>70</v>
+      </c>
+      <c r="E64" s="30"/>
+      <c r="F64" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="G64" s="22" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" ht="82.2" customHeight="1">
+      <c r="A65" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="B65" s="36" t="s">
+        <v>108</v>
+      </c>
+      <c r="C65" s="37"/>
+      <c r="D65" s="36" t="s">
+        <v>109</v>
+      </c>
+      <c r="E65" s="37"/>
+      <c r="F65" s="20"/>
+      <c r="G65" s="20"/>
+    </row>
+    <row r="66" spans="1:7" ht="56.4" customHeight="1">
+      <c r="A66" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="B66" s="36" t="s">
+        <v>107</v>
+      </c>
+      <c r="C66" s="37"/>
+      <c r="D66" s="36"/>
+      <c r="E66" s="37"/>
+      <c r="F66" s="20"/>
+      <c r="G66" s="20"/>
+    </row>
+    <row r="67" spans="1:7">
+      <c r="A67" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="B67" s="30"/>
+      <c r="C67" s="31"/>
+      <c r="D67" s="32"/>
+      <c r="E67" s="32"/>
+      <c r="F67" s="32"/>
+      <c r="G67" s="33"/>
+    </row>
+    <row r="68" spans="1:7">
+      <c r="A68" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="B68" s="30"/>
+      <c r="C68" s="31"/>
+      <c r="D68" s="32"/>
+      <c r="E68" s="32"/>
+      <c r="F68" s="32"/>
+      <c r="G68" s="33"/>
+    </row>
+    <row r="69" spans="1:7">
+      <c r="A69" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="B69" s="30"/>
+      <c r="C69" s="31"/>
+      <c r="D69" s="32"/>
+      <c r="E69" s="32"/>
+      <c r="F69" s="32"/>
+      <c r="G69" s="33"/>
+    </row>
+    <row r="70" spans="1:7">
+      <c r="A70" s="29" t="s">
+        <v>73</v>
+      </c>
+      <c r="B70" s="34"/>
+      <c r="C70" s="31"/>
+      <c r="D70" s="32"/>
+      <c r="E70" s="32"/>
+      <c r="F70" s="32"/>
+      <c r="G70" s="33"/>
+    </row>
   </sheetData>
-  <mergeCells count="65">
+  <mergeCells count="107">
+    <mergeCell ref="A68:B68"/>
+    <mergeCell ref="C68:G68"/>
+    <mergeCell ref="A69:B69"/>
+    <mergeCell ref="C69:G69"/>
+    <mergeCell ref="A70:B70"/>
+    <mergeCell ref="C70:G70"/>
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="D64:E64"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="D65:E65"/>
+    <mergeCell ref="A67:B67"/>
+    <mergeCell ref="C67:G67"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="D66:E66"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="C61:G61"/>
+    <mergeCell ref="A62:B62"/>
+    <mergeCell ref="C62:G62"/>
+    <mergeCell ref="A63:G63"/>
+    <mergeCell ref="A59:G59"/>
+    <mergeCell ref="A60:B60"/>
+    <mergeCell ref="C60:G60"/>
     <mergeCell ref="D17:E17"/>
     <mergeCell ref="D18:E18"/>
     <mergeCell ref="B18:C18"/>
@@ -2550,6 +2886,26 @@
     <mergeCell ref="C41:G41"/>
     <mergeCell ref="A42:B42"/>
     <mergeCell ref="C42:G42"/>
+    <mergeCell ref="A46:G46"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="C47:G47"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="C48:G48"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="D52:E52"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="C49:G49"/>
+    <mergeCell ref="A50:G50"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="D51:E51"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="C55:G55"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="C56:G56"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="C53:G53"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="C54:G54"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
@@ -2557,39 +2913,39 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A4:I24"/>
   <sheetViews>
     <sheetView topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="13.6328125" style="10" customWidth="1"/>
+    <col min="1" max="1" width="13.6640625" style="10" customWidth="1"/>
     <col min="2" max="2" width="10" style="10" customWidth="1"/>
-    <col min="3" max="3" width="15.90625" style="10" customWidth="1"/>
-    <col min="4" max="4" width="20.453125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="24.54296875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="26.453125" style="15" customWidth="1"/>
-    <col min="7" max="7" width="16.6328125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="12.81640625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="12.90625" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="8.81640625" style="1"/>
+    <col min="3" max="3" width="15.88671875" style="10" customWidth="1"/>
+    <col min="4" max="4" width="20.44140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="24.5546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="26.44140625" style="15" customWidth="1"/>
+    <col min="7" max="7" width="16.6640625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="12.77734375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="12.88671875" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.77734375" style="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:9" ht="18.5">
-      <c r="A4" s="26" t="s">
+    <row r="4" spans="1:9" ht="18">
+      <c r="A4" s="69" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
-      <c r="I4" s="28"/>
+      <c r="B4" s="70"/>
+      <c r="C4" s="70"/>
+      <c r="D4" s="70"/>
+      <c r="E4" s="70"/>
+      <c r="F4" s="70"/>
+      <c r="G4" s="70"/>
+      <c r="H4" s="70"/>
+      <c r="I4" s="71"/>
     </row>
     <row r="5" spans="1:9" s="4" customFormat="1">
       <c r="A5" s="2" t="s">
@@ -2620,7 +2976,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:9" s="10" customFormat="1" ht="29.5" customHeight="1">
+    <row r="6" spans="1:9" s="10" customFormat="1" ht="29.55" customHeight="1">
       <c r="A6" s="5">
         <v>1</v>
       </c>
@@ -2641,7 +2997,7 @@
       <c r="H6" s="9"/>
       <c r="I6" s="9"/>
     </row>
-    <row r="7" spans="1:9" s="10" customFormat="1" ht="43" customHeight="1">
+    <row r="7" spans="1:9" s="10" customFormat="1" ht="43.05" customHeight="1">
       <c r="A7" s="5">
         <v>2</v>
       </c>
@@ -2664,7 +3020,7 @@
       <c r="H7" s="9"/>
       <c r="I7" s="9"/>
     </row>
-    <row r="8" spans="1:9" s="10" customFormat="1" ht="43.5">
+    <row r="8" spans="1:9" s="10" customFormat="1" ht="43.2">
       <c r="A8" s="5">
         <v>3</v>
       </c>
@@ -2687,7 +3043,7 @@
       <c r="H8" s="9"/>
       <c r="I8" s="9"/>
     </row>
-    <row r="9" spans="1:9" s="10" customFormat="1" ht="43.5">
+    <row r="9" spans="1:9" s="10" customFormat="1" ht="43.2">
       <c r="A9" s="5">
         <v>4</v>
       </c>
@@ -2708,18 +3064,18 @@
       <c r="H9" s="9"/>
       <c r="I9" s="9"/>
     </row>
-    <row r="13" spans="1:9" ht="18.5">
-      <c r="A13" s="26" t="s">
+    <row r="13" spans="1:9" ht="18">
+      <c r="A13" s="69" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="27"/>
-      <c r="C13" s="27"/>
-      <c r="D13" s="27"/>
-      <c r="E13" s="27"/>
-      <c r="F13" s="27"/>
-      <c r="G13" s="27"/>
-      <c r="H13" s="27"/>
-      <c r="I13" s="28"/>
+      <c r="B13" s="70"/>
+      <c r="C13" s="70"/>
+      <c r="D13" s="70"/>
+      <c r="E13" s="70"/>
+      <c r="F13" s="70"/>
+      <c r="G13" s="70"/>
+      <c r="H13" s="70"/>
+      <c r="I13" s="71"/>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="2" t="s">
@@ -2750,7 +3106,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="62" customHeight="1">
+    <row r="15" spans="1:9" ht="61.95" customHeight="1">
       <c r="A15" s="5">
         <v>1</v>
       </c>
@@ -2773,7 +3129,7 @@
       <c r="H15" s="9"/>
       <c r="I15" s="9"/>
     </row>
-    <row r="16" spans="1:9" ht="29">
+    <row r="16" spans="1:9" ht="28.8">
       <c r="A16" s="5">
         <v>2</v>
       </c>
@@ -2796,7 +3152,7 @@
       <c r="H16" s="9"/>
       <c r="I16" s="9"/>
     </row>
-    <row r="17" spans="1:9" ht="58">
+    <row r="17" spans="1:9" ht="57.6">
       <c r="A17" s="5">
         <v>3</v>
       </c>
@@ -2817,7 +3173,7 @@
       <c r="H17" s="9"/>
       <c r="I17" s="9"/>
     </row>
-    <row r="18" spans="1:9" ht="58">
+    <row r="18" spans="1:9" ht="57.6">
       <c r="A18" s="5">
         <v>4</v>
       </c>
@@ -2840,7 +3196,7 @@
       <c r="H18" s="9"/>
       <c r="I18" s="9"/>
     </row>
-    <row r="19" spans="1:9" ht="58">
+    <row r="19" spans="1:9" ht="57.6">
       <c r="A19" s="5">
         <v>5</v>
       </c>
@@ -2863,7 +3219,7 @@
       <c r="H19" s="9"/>
       <c r="I19" s="9"/>
     </row>
-    <row r="20" spans="1:9" ht="58">
+    <row r="20" spans="1:9" ht="57.6">
       <c r="A20" s="5">
         <v>6</v>
       </c>
@@ -2886,7 +3242,7 @@
       <c r="H20" s="9"/>
       <c r="I20" s="9"/>
     </row>
-    <row r="21" spans="1:9" ht="58">
+    <row r="21" spans="1:9" ht="57.6">
       <c r="A21" s="5">
         <v>7</v>
       </c>
@@ -2909,7 +3265,7 @@
       <c r="H21" s="9"/>
       <c r="I21" s="9"/>
     </row>
-    <row r="22" spans="1:9" ht="58">
+    <row r="22" spans="1:9" ht="57.6">
       <c r="A22" s="6">
         <v>8</v>
       </c>
@@ -2932,7 +3288,7 @@
       <c r="H22" s="8"/>
       <c r="I22" s="8"/>
     </row>
-    <row r="23" spans="1:9" ht="58">
+    <row r="23" spans="1:9" ht="57.6">
       <c r="A23" s="6">
         <v>9</v>
       </c>
@@ -2955,7 +3311,7 @@
       <c r="H23" s="8"/>
       <c r="I23" s="8"/>
     </row>
-    <row r="24" spans="1:9" ht="43.5">
+    <row r="24" spans="1:9" ht="43.2">
       <c r="A24" s="6">
         <v>10</v>
       </c>
@@ -2984,8 +3340,8 @@
     <mergeCell ref="A13:I13"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="F8" r:id="rId1" display="testingfyp2017@gmail.com_x000a_testingfyp"/>
-    <hyperlink ref="F16" r:id="rId2"/>
+    <hyperlink ref="F8" r:id="rId1" display="testingfyp2017@gmail.com_x000a_testingfyp" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="F16" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId3"/>

</xml_diff>

<commit_message>
did small changes to the home page activity and did login test
</commit_message>
<xml_diff>
--- a/FYP documentation/FYP_Test_Plan.xlsx
+++ b/FYP documentation/FYP_Test_Plan.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6936" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6936" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Plan Final" sheetId="4" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="118">
   <si>
     <t>Expected Result</t>
   </si>
@@ -368,22 +368,46 @@
     <t>1. Login to first device.               2. Login to second device</t>
   </si>
   <si>
-    <t>Password Recovery</t>
-  </si>
-  <si>
     <t>The user should have previously signed up</t>
   </si>
   <si>
-    <t>Test if the user can recover password and forms work perfectly.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. click forget password                 2. Enter password1   in current password field             </t>
-  </si>
-  <si>
-    <t>1. Enter invalid email                      2. Click forget password</t>
-  </si>
-  <si>
-    <t>There should be a error message and no verificationemail sent over to client.</t>
+    <t>Home page</t>
+  </si>
+  <si>
+    <t>Test if home page is functional</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Perform Login                          2. Switch gps off and network off.                                                     3. Move the map around                                                     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">A message should be displayed to ask the user to witch on network. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.  Switch of the gps and turn on the network.         </t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>Login fail message</t>
+  </si>
+  <si>
+    <t>Error message appear above the edittext field</t>
+  </si>
+  <si>
+    <t>Login sussesfull home screen displayed</t>
+  </si>
+  <si>
+    <t>All respond</t>
+  </si>
+  <si>
+    <t>1. Click on the fields</t>
+  </si>
+  <si>
+    <t>Abhi Jay Krishnan</t>
+  </si>
+  <si>
+    <t>1842hrs</t>
   </si>
 </sst>
 </file>
@@ -703,7 +727,7 @@
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -772,7 +796,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -794,18 +817,36 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -827,36 +868,33 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="6" xfId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="7" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="8" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="12" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="13" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -878,21 +916,6 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="7" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="8" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="12" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -901,6 +924,15 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -1969,8 +2001,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D66" sqref="D66:E66"/>
+    <sheetView topLeftCell="A61" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C67" sqref="C67:G67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1987,15 +2019,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="40.799999999999997" customHeight="1">
-      <c r="A1" s="66" t="s">
+      <c r="A1" s="58" t="s">
         <v>64</v>
       </c>
-      <c r="B1" s="67"/>
-      <c r="C1" s="67"/>
-      <c r="D1" s="67"/>
-      <c r="E1" s="67"/>
-      <c r="F1" s="67"/>
-      <c r="G1" s="68"/>
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
+      <c r="F1" s="59"/>
+      <c r="G1" s="60"/>
       <c r="H1" s="16"/>
       <c r="I1" s="16"/>
     </row>
@@ -2011,67 +2043,67 @@
       <c r="I2" s="19"/>
     </row>
     <row r="3" spans="1:9" ht="31.2" customHeight="1" thickBot="1">
-      <c r="A3" s="46" t="s">
+      <c r="A3" s="51" t="s">
         <v>83</v>
       </c>
-      <c r="B3" s="46"/>
-      <c r="C3" s="46"/>
-      <c r="D3" s="46"/>
-      <c r="E3" s="46"/>
-      <c r="F3" s="46"/>
-      <c r="G3" s="46"/>
+      <c r="B3" s="51"/>
+      <c r="C3" s="51"/>
+      <c r="D3" s="51"/>
+      <c r="E3" s="51"/>
+      <c r="F3" s="51"/>
+      <c r="G3" s="51"/>
       <c r="H3" s="16"/>
       <c r="I3" s="16"/>
     </row>
     <row r="4" spans="1:9" ht="18.600000000000001" customHeight="1" thickTop="1">
-      <c r="A4" s="38" t="s">
+      <c r="A4" s="35" t="s">
         <v>66</v>
       </c>
-      <c r="B4" s="39"/>
-      <c r="C4" s="47" t="s">
+      <c r="B4" s="36"/>
+      <c r="C4" s="37" t="s">
         <v>84</v>
       </c>
-      <c r="D4" s="48"/>
-      <c r="E4" s="48"/>
-      <c r="F4" s="48"/>
-      <c r="G4" s="49"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="39"/>
       <c r="H4" s="17"/>
       <c r="I4" s="17"/>
     </row>
     <row r="5" spans="1:9" ht="14.4" customHeight="1">
-      <c r="A5" s="38" t="s">
+      <c r="A5" s="35" t="s">
         <v>67</v>
       </c>
-      <c r="B5" s="39"/>
-      <c r="C5" s="50"/>
-      <c r="D5" s="51"/>
-      <c r="E5" s="51"/>
-      <c r="F5" s="51"/>
-      <c r="G5" s="52"/>
+      <c r="B5" s="36"/>
+      <c r="C5" s="40"/>
+      <c r="D5" s="41"/>
+      <c r="E5" s="41"/>
+      <c r="F5" s="41"/>
+      <c r="G5" s="42"/>
       <c r="H5" s="16"/>
       <c r="I5" s="16"/>
     </row>
     <row r="6" spans="1:9" ht="14.4" customHeight="1">
-      <c r="A6" s="38" t="s">
+      <c r="A6" s="35" t="s">
         <v>68</v>
       </c>
-      <c r="B6" s="39"/>
-      <c r="C6" s="40"/>
-      <c r="D6" s="41"/>
-      <c r="E6" s="41"/>
-      <c r="F6" s="41"/>
-      <c r="G6" s="42"/>
+      <c r="B6" s="36"/>
+      <c r="C6" s="45"/>
+      <c r="D6" s="46"/>
+      <c r="E6" s="46"/>
+      <c r="F6" s="46"/>
+      <c r="G6" s="47"/>
       <c r="H6" s="17"/>
       <c r="I6" s="18"/>
     </row>
     <row r="7" spans="1:9">
-      <c r="A7" s="43"/>
-      <c r="B7" s="44"/>
-      <c r="C7" s="44"/>
-      <c r="D7" s="44"/>
-      <c r="E7" s="44"/>
-      <c r="F7" s="44"/>
-      <c r="G7" s="45"/>
+      <c r="A7" s="48"/>
+      <c r="B7" s="49"/>
+      <c r="C7" s="49"/>
+      <c r="D7" s="49"/>
+      <c r="E7" s="49"/>
+      <c r="F7" s="49"/>
+      <c r="G7" s="50"/>
       <c r="H7" s="18"/>
       <c r="I7" s="18"/>
     </row>
@@ -2079,14 +2111,14 @@
       <c r="A8" s="22" t="s">
         <v>77</v>
       </c>
-      <c r="B8" s="35" t="s">
+      <c r="B8" s="34" t="s">
         <v>69</v>
       </c>
-      <c r="C8" s="30"/>
-      <c r="D8" s="35" t="s">
+      <c r="C8" s="29"/>
+      <c r="D8" s="34" t="s">
         <v>70</v>
       </c>
-      <c r="E8" s="30"/>
+      <c r="E8" s="29"/>
       <c r="F8" s="21" t="s">
         <v>71</v>
       </c>
@@ -2098,14 +2130,14 @@
       <c r="A9" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="36" t="s">
+      <c r="B9" s="43" t="s">
         <v>85</v>
       </c>
-      <c r="C9" s="37"/>
-      <c r="D9" s="36" t="s">
+      <c r="C9" s="44"/>
+      <c r="D9" s="43" t="s">
         <v>90</v>
       </c>
-      <c r="E9" s="37"/>
+      <c r="E9" s="44"/>
       <c r="F9" s="20"/>
       <c r="G9" s="20"/>
     </row>
@@ -2113,14 +2145,14 @@
       <c r="A10" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="36" t="s">
+      <c r="B10" s="43" t="s">
         <v>88</v>
       </c>
-      <c r="C10" s="37"/>
-      <c r="D10" s="36" t="s">
+      <c r="C10" s="44"/>
+      <c r="D10" s="43" t="s">
         <v>91</v>
       </c>
-      <c r="E10" s="55"/>
+      <c r="E10" s="56"/>
       <c r="F10" s="20"/>
       <c r="G10" s="20"/>
     </row>
@@ -2128,14 +2160,14 @@
       <c r="A11" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="36" t="s">
+      <c r="B11" s="43" t="s">
         <v>89</v>
       </c>
-      <c r="C11" s="37"/>
-      <c r="D11" s="36" t="s">
+      <c r="C11" s="44"/>
+      <c r="D11" s="43" t="s">
         <v>87</v>
       </c>
-      <c r="E11" s="37"/>
+      <c r="E11" s="44"/>
       <c r="F11" s="20"/>
       <c r="G11" s="20"/>
     </row>
@@ -2143,14 +2175,14 @@
       <c r="A12" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="36" t="s">
+      <c r="B12" s="43" t="s">
         <v>92</v>
       </c>
-      <c r="C12" s="55"/>
-      <c r="D12" s="36" t="s">
+      <c r="C12" s="56"/>
+      <c r="D12" s="43" t="s">
         <v>87</v>
       </c>
-      <c r="E12" s="37"/>
+      <c r="E12" s="44"/>
       <c r="F12" s="20"/>
       <c r="G12" s="20"/>
     </row>
@@ -2158,14 +2190,14 @@
       <c r="A13" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="B13" s="36" t="s">
+      <c r="B13" s="43" t="s">
         <v>94</v>
       </c>
-      <c r="C13" s="55"/>
-      <c r="D13" s="36" t="s">
+      <c r="C13" s="56"/>
+      <c r="D13" s="43" t="s">
         <v>87</v>
       </c>
-      <c r="E13" s="37"/>
+      <c r="E13" s="44"/>
       <c r="F13" s="20"/>
       <c r="G13" s="20"/>
     </row>
@@ -2173,120 +2205,120 @@
       <c r="A14" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="B14" s="36" t="s">
+      <c r="B14" s="43" t="s">
         <v>93</v>
       </c>
-      <c r="C14" s="37"/>
-      <c r="D14" s="36" t="s">
+      <c r="C14" s="44"/>
+      <c r="D14" s="43" t="s">
         <v>87</v>
       </c>
-      <c r="E14" s="37"/>
+      <c r="E14" s="44"/>
       <c r="F14" s="20"/>
       <c r="G14" s="20"/>
     </row>
     <row r="15" spans="1:9" ht="55.95" customHeight="1">
-      <c r="A15" s="26" t="s">
+      <c r="A15" s="73" t="s">
         <v>30</v>
       </c>
-      <c r="B15" s="56" t="s">
+      <c r="B15" s="57" t="s">
         <v>95</v>
       </c>
-      <c r="C15" s="56"/>
-      <c r="D15" s="36" t="s">
+      <c r="C15" s="57"/>
+      <c r="D15" s="43" t="s">
         <v>91</v>
       </c>
-      <c r="E15" s="55"/>
+      <c r="E15" s="56"/>
       <c r="F15" s="27"/>
-      <c r="G15" s="28"/>
+      <c r="G15" s="20"/>
     </row>
     <row r="16" spans="1:9" ht="45.45" customHeight="1">
-      <c r="A16" s="26" t="s">
+      <c r="A16" s="73" t="s">
         <v>39</v>
       </c>
-      <c r="B16" s="56" t="s">
+      <c r="B16" s="57" t="s">
         <v>96</v>
       </c>
-      <c r="C16" s="56"/>
-      <c r="D16" s="36" t="s">
+      <c r="C16" s="57"/>
+      <c r="D16" s="43" t="s">
         <v>87</v>
       </c>
-      <c r="E16" s="37"/>
+      <c r="E16" s="44"/>
       <c r="F16" s="27"/>
-      <c r="G16" s="28"/>
+      <c r="G16" s="20"/>
     </row>
     <row r="17" spans="1:7" ht="45.45" customHeight="1">
-      <c r="A17" s="26" t="s">
+      <c r="A17" s="73" t="s">
         <v>40</v>
       </c>
-      <c r="B17" s="56" t="s">
+      <c r="B17" s="57" t="s">
         <v>97</v>
       </c>
-      <c r="C17" s="56"/>
-      <c r="D17" s="36" t="s">
+      <c r="C17" s="57"/>
+      <c r="D17" s="43" t="s">
         <v>87</v>
       </c>
-      <c r="E17" s="37"/>
+      <c r="E17" s="44"/>
       <c r="F17" s="27"/>
-      <c r="G17" s="28"/>
+      <c r="G17" s="20"/>
     </row>
     <row r="18" spans="1:7" ht="45.45" customHeight="1">
-      <c r="A18" s="26" t="s">
+      <c r="A18" s="73" t="s">
         <v>41</v>
       </c>
-      <c r="B18" s="56" t="s">
+      <c r="B18" s="57" t="s">
         <v>98</v>
       </c>
-      <c r="C18" s="56"/>
-      <c r="D18" s="36" t="s">
+      <c r="C18" s="57"/>
+      <c r="D18" s="43" t="s">
         <v>91</v>
       </c>
-      <c r="E18" s="55"/>
+      <c r="E18" s="56"/>
       <c r="F18" s="27"/>
-      <c r="G18" s="28"/>
+      <c r="G18" s="20"/>
     </row>
     <row r="19" spans="1:7">
-      <c r="A19" s="35" t="s">
+      <c r="A19" s="34" t="s">
         <v>74</v>
       </c>
-      <c r="B19" s="30"/>
-      <c r="C19" s="31"/>
-      <c r="D19" s="32"/>
-      <c r="E19" s="32"/>
-      <c r="F19" s="32"/>
-      <c r="G19" s="33"/>
+      <c r="B19" s="29"/>
+      <c r="C19" s="30"/>
+      <c r="D19" s="31"/>
+      <c r="E19" s="31"/>
+      <c r="F19" s="31"/>
+      <c r="G19" s="32"/>
     </row>
     <row r="20" spans="1:7">
-      <c r="A20" s="35" t="s">
+      <c r="A20" s="34" t="s">
         <v>75</v>
       </c>
-      <c r="B20" s="30"/>
-      <c r="C20" s="31"/>
-      <c r="D20" s="32"/>
-      <c r="E20" s="32"/>
-      <c r="F20" s="32"/>
-      <c r="G20" s="33"/>
+      <c r="B20" s="29"/>
+      <c r="C20" s="30"/>
+      <c r="D20" s="31"/>
+      <c r="E20" s="31"/>
+      <c r="F20" s="31"/>
+      <c r="G20" s="32"/>
     </row>
     <row r="21" spans="1:7">
-      <c r="A21" s="29" t="s">
+      <c r="A21" s="28" t="s">
         <v>76</v>
       </c>
-      <c r="B21" s="30"/>
-      <c r="C21" s="31"/>
-      <c r="D21" s="32"/>
-      <c r="E21" s="32"/>
-      <c r="F21" s="32"/>
-      <c r="G21" s="33"/>
+      <c r="B21" s="29"/>
+      <c r="C21" s="30"/>
+      <c r="D21" s="31"/>
+      <c r="E21" s="31"/>
+      <c r="F21" s="31"/>
+      <c r="G21" s="32"/>
     </row>
     <row r="22" spans="1:7">
-      <c r="A22" s="29" t="s">
+      <c r="A22" s="28" t="s">
         <v>73</v>
       </c>
-      <c r="B22" s="34"/>
-      <c r="C22" s="31"/>
-      <c r="D22" s="32"/>
-      <c r="E22" s="32"/>
-      <c r="F22" s="32"/>
-      <c r="G22" s="33"/>
+      <c r="B22" s="33"/>
+      <c r="C22" s="30"/>
+      <c r="D22" s="31"/>
+      <c r="E22" s="31"/>
+      <c r="F22" s="31"/>
+      <c r="G22" s="32"/>
     </row>
     <row r="23" spans="1:7" ht="26.4" customHeight="1">
       <c r="A23" s="18"/>
@@ -2335,74 +2367,74 @@
     </row>
     <row r="28" spans="1:7" ht="25.8" customHeight="1"/>
     <row r="29" spans="1:7" ht="20.399999999999999" thickBot="1">
-      <c r="A29" s="46" t="s">
+      <c r="A29" s="51" t="s">
         <v>65</v>
       </c>
-      <c r="B29" s="46"/>
-      <c r="C29" s="46"/>
-      <c r="D29" s="46"/>
-      <c r="E29" s="46"/>
-      <c r="F29" s="46"/>
-      <c r="G29" s="46"/>
+      <c r="B29" s="51"/>
+      <c r="C29" s="51"/>
+      <c r="D29" s="51"/>
+      <c r="E29" s="51"/>
+      <c r="F29" s="51"/>
+      <c r="G29" s="51"/>
     </row>
     <row r="30" spans="1:7" ht="15" thickTop="1">
-      <c r="A30" s="57" t="s">
+      <c r="A30" s="61" t="s">
         <v>66</v>
       </c>
-      <c r="B30" s="58"/>
-      <c r="C30" s="59" t="s">
+      <c r="B30" s="62"/>
+      <c r="C30" s="63" t="s">
         <v>78</v>
       </c>
-      <c r="D30" s="60"/>
-      <c r="E30" s="60"/>
-      <c r="F30" s="60"/>
-      <c r="G30" s="61"/>
+      <c r="D30" s="64"/>
+      <c r="E30" s="64"/>
+      <c r="F30" s="64"/>
+      <c r="G30" s="65"/>
     </row>
     <row r="31" spans="1:7">
-      <c r="A31" s="38" t="s">
+      <c r="A31" s="35" t="s">
         <v>67</v>
       </c>
-      <c r="B31" s="39"/>
-      <c r="C31" s="50"/>
-      <c r="D31" s="51"/>
-      <c r="E31" s="51"/>
-      <c r="F31" s="51"/>
-      <c r="G31" s="52"/>
+      <c r="B31" s="36"/>
+      <c r="C31" s="40"/>
+      <c r="D31" s="41"/>
+      <c r="E31" s="41"/>
+      <c r="F31" s="41"/>
+      <c r="G31" s="42"/>
     </row>
     <row r="32" spans="1:7">
-      <c r="A32" s="38" t="s">
+      <c r="A32" s="35" t="s">
         <v>68</v>
       </c>
-      <c r="B32" s="39"/>
-      <c r="C32" s="40" t="s">
+      <c r="B32" s="36"/>
+      <c r="C32" s="45" t="s">
         <v>79</v>
       </c>
-      <c r="D32" s="62"/>
-      <c r="E32" s="62"/>
-      <c r="F32" s="62"/>
-      <c r="G32" s="63"/>
+      <c r="D32" s="66"/>
+      <c r="E32" s="66"/>
+      <c r="F32" s="66"/>
+      <c r="G32" s="67"/>
     </row>
     <row r="33" spans="1:7">
-      <c r="A33" s="31"/>
-      <c r="B33" s="32"/>
-      <c r="C33" s="32"/>
-      <c r="D33" s="32"/>
-      <c r="E33" s="32"/>
-      <c r="F33" s="32"/>
-      <c r="G33" s="33"/>
+      <c r="A33" s="30"/>
+      <c r="B33" s="31"/>
+      <c r="C33" s="31"/>
+      <c r="D33" s="31"/>
+      <c r="E33" s="31"/>
+      <c r="F33" s="31"/>
+      <c r="G33" s="32"/>
     </row>
     <row r="34" spans="1:7">
       <c r="A34" s="22" t="s">
         <v>77</v>
       </c>
-      <c r="B34" s="35" t="s">
+      <c r="B34" s="34" t="s">
         <v>69</v>
       </c>
-      <c r="C34" s="30"/>
-      <c r="D34" s="35" t="s">
+      <c r="C34" s="29"/>
+      <c r="D34" s="34" t="s">
         <v>70</v>
       </c>
-      <c r="E34" s="30"/>
+      <c r="E34" s="29"/>
       <c r="F34" s="21" t="s">
         <v>71</v>
       </c>
@@ -2414,175 +2446,199 @@
       <c r="A35" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="B35" s="53" t="s">
-        <v>17</v>
-      </c>
-      <c r="C35" s="54"/>
-      <c r="D35" s="64" t="s">
+      <c r="B35" s="52" t="s">
+        <v>115</v>
+      </c>
+      <c r="C35" s="53"/>
+      <c r="D35" s="54" t="s">
         <v>72</v>
       </c>
-      <c r="E35" s="65"/>
-      <c r="F35" s="20"/>
-      <c r="G35" s="20"/>
+      <c r="E35" s="55"/>
+      <c r="F35" s="20" t="s">
+        <v>114</v>
+      </c>
+      <c r="G35" s="20" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="36" spans="1:7" ht="46.8" customHeight="1">
       <c r="A36" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="B36" s="53" t="s">
+      <c r="B36" s="52" t="s">
         <v>50</v>
       </c>
-      <c r="C36" s="54"/>
-      <c r="D36" s="36" t="s">
+      <c r="C36" s="53"/>
+      <c r="D36" s="43" t="s">
         <v>86</v>
       </c>
-      <c r="E36" s="55"/>
-      <c r="F36" s="20"/>
-      <c r="G36" s="20"/>
+      <c r="E36" s="56"/>
+      <c r="F36" s="20" t="s">
+        <v>112</v>
+      </c>
+      <c r="G36" s="20" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="37" spans="1:7" ht="45.6" customHeight="1">
       <c r="A37" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="B37" s="53" t="s">
+      <c r="B37" s="52" t="s">
         <v>49</v>
       </c>
-      <c r="C37" s="54"/>
-      <c r="D37" s="36" t="s">
+      <c r="C37" s="53"/>
+      <c r="D37" s="43" t="s">
         <v>80</v>
       </c>
-      <c r="E37" s="55"/>
-      <c r="F37" s="20"/>
-      <c r="G37" s="20"/>
+      <c r="E37" s="56"/>
+      <c r="F37" s="20" t="s">
+        <v>113</v>
+      </c>
+      <c r="G37" s="20" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="38" spans="1:7" ht="48" customHeight="1">
       <c r="A38" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="B38" s="53" t="s">
+      <c r="B38" s="52" t="s">
         <v>81</v>
       </c>
-      <c r="C38" s="54"/>
-      <c r="D38" s="36" t="s">
+      <c r="C38" s="53"/>
+      <c r="D38" s="43" t="s">
         <v>82</v>
       </c>
-      <c r="E38" s="55"/>
-      <c r="F38" s="20"/>
-      <c r="G38" s="20"/>
+      <c r="E38" s="56"/>
+      <c r="F38" s="20" t="s">
+        <v>111</v>
+      </c>
+      <c r="G38" s="20" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="39" spans="1:7">
-      <c r="A39" s="35" t="s">
+      <c r="A39" s="34" t="s">
         <v>74</v>
       </c>
-      <c r="B39" s="30"/>
-      <c r="C39" s="31"/>
-      <c r="D39" s="32"/>
-      <c r="E39" s="32"/>
-      <c r="F39" s="32"/>
-      <c r="G39" s="33"/>
+      <c r="B39" s="29"/>
+      <c r="C39" s="54" t="s">
+        <v>116</v>
+      </c>
+      <c r="D39" s="71"/>
+      <c r="E39" s="71"/>
+      <c r="F39" s="71"/>
+      <c r="G39" s="55"/>
     </row>
     <row r="40" spans="1:7">
-      <c r="A40" s="35" t="s">
+      <c r="A40" s="34" t="s">
         <v>75</v>
       </c>
-      <c r="B40" s="30"/>
-      <c r="C40" s="31"/>
-      <c r="D40" s="32"/>
-      <c r="E40" s="32"/>
-      <c r="F40" s="32"/>
-      <c r="G40" s="33"/>
+      <c r="B40" s="29"/>
+      <c r="C40" s="72">
+        <v>43042</v>
+      </c>
+      <c r="D40" s="71"/>
+      <c r="E40" s="71"/>
+      <c r="F40" s="71"/>
+      <c r="G40" s="55"/>
     </row>
     <row r="41" spans="1:7">
-      <c r="A41" s="29" t="s">
+      <c r="A41" s="28" t="s">
         <v>76</v>
       </c>
-      <c r="B41" s="34"/>
-      <c r="C41" s="31"/>
-      <c r="D41" s="32"/>
-      <c r="E41" s="32"/>
-      <c r="F41" s="32"/>
-      <c r="G41" s="33"/>
+      <c r="B41" s="33"/>
+      <c r="C41" s="54" t="s">
+        <v>117</v>
+      </c>
+      <c r="D41" s="71"/>
+      <c r="E41" s="71"/>
+      <c r="F41" s="71"/>
+      <c r="G41" s="55"/>
     </row>
     <row r="42" spans="1:7">
-      <c r="A42" s="29" t="s">
+      <c r="A42" s="28" t="s">
         <v>73</v>
       </c>
-      <c r="B42" s="34"/>
-      <c r="C42" s="31"/>
-      <c r="D42" s="32"/>
-      <c r="E42" s="32"/>
-      <c r="F42" s="32"/>
-      <c r="G42" s="33"/>
+      <c r="B42" s="33"/>
+      <c r="C42" s="54" t="s">
+        <v>110</v>
+      </c>
+      <c r="D42" s="71"/>
+      <c r="E42" s="71"/>
+      <c r="F42" s="71"/>
+      <c r="G42" s="55"/>
     </row>
     <row r="46" spans="1:7" ht="20.399999999999999" thickBot="1">
-      <c r="A46" s="46" t="s">
+      <c r="A46" s="51" t="s">
         <v>102</v>
       </c>
-      <c r="B46" s="46"/>
-      <c r="C46" s="46"/>
-      <c r="D46" s="46"/>
-      <c r="E46" s="46"/>
-      <c r="F46" s="46"/>
-      <c r="G46" s="46"/>
+      <c r="B46" s="51"/>
+      <c r="C46" s="51"/>
+      <c r="D46" s="51"/>
+      <c r="E46" s="51"/>
+      <c r="F46" s="51"/>
+      <c r="G46" s="51"/>
     </row>
     <row r="47" spans="1:7" ht="15" thickTop="1">
-      <c r="A47" s="38" t="s">
+      <c r="A47" s="35" t="s">
         <v>66</v>
       </c>
-      <c r="B47" s="39"/>
-      <c r="C47" s="47" t="s">
+      <c r="B47" s="36"/>
+      <c r="C47" s="37" t="s">
         <v>99</v>
       </c>
-      <c r="D47" s="48"/>
-      <c r="E47" s="48"/>
-      <c r="F47" s="48"/>
-      <c r="G47" s="49"/>
+      <c r="D47" s="38"/>
+      <c r="E47" s="38"/>
+      <c r="F47" s="38"/>
+      <c r="G47" s="39"/>
     </row>
     <row r="48" spans="1:7">
-      <c r="A48" s="38" t="s">
+      <c r="A48" s="35" t="s">
         <v>67</v>
       </c>
-      <c r="B48" s="39"/>
-      <c r="C48" s="50"/>
-      <c r="D48" s="51"/>
-      <c r="E48" s="51"/>
-      <c r="F48" s="51"/>
-      <c r="G48" s="52"/>
+      <c r="B48" s="36"/>
+      <c r="C48" s="40"/>
+      <c r="D48" s="41"/>
+      <c r="E48" s="41"/>
+      <c r="F48" s="41"/>
+      <c r="G48" s="42"/>
     </row>
     <row r="49" spans="1:7">
-      <c r="A49" s="38" t="s">
+      <c r="A49" s="35" t="s">
         <v>68</v>
       </c>
-      <c r="B49" s="39"/>
-      <c r="C49" s="40" t="s">
+      <c r="B49" s="36"/>
+      <c r="C49" s="45" t="s">
         <v>100</v>
       </c>
-      <c r="D49" s="41"/>
-      <c r="E49" s="41"/>
-      <c r="F49" s="41"/>
-      <c r="G49" s="42"/>
+      <c r="D49" s="46"/>
+      <c r="E49" s="46"/>
+      <c r="F49" s="46"/>
+      <c r="G49" s="47"/>
     </row>
     <row r="50" spans="1:7" ht="31.8" customHeight="1">
-      <c r="A50" s="43"/>
-      <c r="B50" s="44"/>
-      <c r="C50" s="44"/>
-      <c r="D50" s="44"/>
-      <c r="E50" s="44"/>
-      <c r="F50" s="44"/>
-      <c r="G50" s="45"/>
+      <c r="A50" s="48"/>
+      <c r="B50" s="49"/>
+      <c r="C50" s="49"/>
+      <c r="D50" s="49"/>
+      <c r="E50" s="49"/>
+      <c r="F50" s="49"/>
+      <c r="G50" s="50"/>
     </row>
     <row r="51" spans="1:7" ht="63" customHeight="1">
       <c r="A51" s="22" t="s">
         <v>77</v>
       </c>
-      <c r="B51" s="35" t="s">
+      <c r="B51" s="34" t="s">
         <v>69</v>
       </c>
-      <c r="C51" s="30"/>
-      <c r="D51" s="35" t="s">
+      <c r="C51" s="29"/>
+      <c r="D51" s="34" t="s">
         <v>70</v>
       </c>
-      <c r="E51" s="30"/>
+      <c r="E51" s="29"/>
       <c r="F51" s="21" t="s">
         <v>71</v>
       </c>
@@ -2594,130 +2650,132 @@
       <c r="A52" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="B52" s="36" t="s">
+      <c r="B52" s="43" t="s">
         <v>103</v>
       </c>
-      <c r="C52" s="37"/>
-      <c r="D52" s="36" t="s">
+      <c r="C52" s="44"/>
+      <c r="D52" s="43" t="s">
         <v>101</v>
       </c>
-      <c r="E52" s="37"/>
+      <c r="E52" s="44"/>
       <c r="F52" s="20"/>
       <c r="G52" s="20"/>
     </row>
     <row r="53" spans="1:7" ht="27" customHeight="1">
-      <c r="A53" s="29" t="s">
+      <c r="A53" s="28" t="s">
         <v>74</v>
       </c>
-      <c r="B53" s="30"/>
-      <c r="C53" s="31"/>
-      <c r="D53" s="32"/>
-      <c r="E53" s="32"/>
-      <c r="F53" s="32"/>
-      <c r="G53" s="33"/>
+      <c r="B53" s="29"/>
+      <c r="C53" s="54" t="s">
+        <v>116</v>
+      </c>
+      <c r="D53" s="71"/>
+      <c r="E53" s="71"/>
+      <c r="F53" s="71"/>
+      <c r="G53" s="55"/>
     </row>
     <row r="54" spans="1:7" ht="34.799999999999997" customHeight="1">
-      <c r="A54" s="35" t="s">
+      <c r="A54" s="34" t="s">
         <v>75</v>
       </c>
-      <c r="B54" s="30"/>
-      <c r="C54" s="31"/>
-      <c r="D54" s="32"/>
-      <c r="E54" s="32"/>
-      <c r="F54" s="32"/>
-      <c r="G54" s="33"/>
+      <c r="B54" s="29"/>
+      <c r="C54" s="30"/>
+      <c r="D54" s="31"/>
+      <c r="E54" s="31"/>
+      <c r="F54" s="31"/>
+      <c r="G54" s="32"/>
     </row>
     <row r="55" spans="1:7" ht="25.2" customHeight="1">
-      <c r="A55" s="29" t="s">
+      <c r="A55" s="28" t="s">
         <v>76</v>
       </c>
-      <c r="B55" s="30"/>
-      <c r="C55" s="31"/>
-      <c r="D55" s="32"/>
-      <c r="E55" s="32"/>
-      <c r="F55" s="32"/>
-      <c r="G55" s="33"/>
+      <c r="B55" s="29"/>
+      <c r="C55" s="30"/>
+      <c r="D55" s="31"/>
+      <c r="E55" s="31"/>
+      <c r="F55" s="31"/>
+      <c r="G55" s="32"/>
     </row>
     <row r="56" spans="1:7">
-      <c r="A56" s="29" t="s">
+      <c r="A56" s="28" t="s">
         <v>73</v>
       </c>
-      <c r="B56" s="34"/>
-      <c r="C56" s="31"/>
-      <c r="D56" s="32"/>
-      <c r="E56" s="32"/>
-      <c r="F56" s="32"/>
-      <c r="G56" s="33"/>
+      <c r="B56" s="33"/>
+      <c r="C56" s="30"/>
+      <c r="D56" s="31"/>
+      <c r="E56" s="31"/>
+      <c r="F56" s="31"/>
+      <c r="G56" s="32"/>
     </row>
     <row r="59" spans="1:7" ht="20.399999999999999" thickBot="1">
-      <c r="A59" s="46" t="s">
+      <c r="A59" s="51" t="s">
+        <v>105</v>
+      </c>
+      <c r="B59" s="51"/>
+      <c r="C59" s="51"/>
+      <c r="D59" s="51"/>
+      <c r="E59" s="51"/>
+      <c r="F59" s="51"/>
+      <c r="G59" s="51"/>
+    </row>
+    <row r="60" spans="1:7" ht="15" thickTop="1">
+      <c r="A60" s="35" t="s">
+        <v>66</v>
+      </c>
+      <c r="B60" s="36"/>
+      <c r="C60" s="37" t="s">
+        <v>106</v>
+      </c>
+      <c r="D60" s="38"/>
+      <c r="E60" s="38"/>
+      <c r="F60" s="38"/>
+      <c r="G60" s="39"/>
+    </row>
+    <row r="61" spans="1:7">
+      <c r="A61" s="35" t="s">
+        <v>67</v>
+      </c>
+      <c r="B61" s="36"/>
+      <c r="C61" s="40"/>
+      <c r="D61" s="41"/>
+      <c r="E61" s="41"/>
+      <c r="F61" s="41"/>
+      <c r="G61" s="42"/>
+    </row>
+    <row r="62" spans="1:7">
+      <c r="A62" s="35" t="s">
+        <v>68</v>
+      </c>
+      <c r="B62" s="36"/>
+      <c r="C62" s="45" t="s">
         <v>104</v>
       </c>
-      <c r="B59" s="46"/>
-      <c r="C59" s="46"/>
-      <c r="D59" s="46"/>
-      <c r="E59" s="46"/>
-      <c r="F59" s="46"/>
-      <c r="G59" s="46"/>
-    </row>
-    <row r="60" spans="1:7" ht="15" thickTop="1">
-      <c r="A60" s="38" t="s">
-        <v>66</v>
-      </c>
-      <c r="B60" s="39"/>
-      <c r="C60" s="47" t="s">
-        <v>106</v>
-      </c>
-      <c r="D60" s="48"/>
-      <c r="E60" s="48"/>
-      <c r="F60" s="48"/>
-      <c r="G60" s="49"/>
-    </row>
-    <row r="61" spans="1:7">
-      <c r="A61" s="38" t="s">
-        <v>67</v>
-      </c>
-      <c r="B61" s="39"/>
-      <c r="C61" s="50"/>
-      <c r="D61" s="51"/>
-      <c r="E61" s="51"/>
-      <c r="F61" s="51"/>
-      <c r="G61" s="52"/>
-    </row>
-    <row r="62" spans="1:7">
-      <c r="A62" s="38" t="s">
-        <v>68</v>
-      </c>
-      <c r="B62" s="39"/>
-      <c r="C62" s="40" t="s">
-        <v>105</v>
-      </c>
-      <c r="D62" s="41"/>
-      <c r="E62" s="41"/>
-      <c r="F62" s="41"/>
-      <c r="G62" s="42"/>
+      <c r="D62" s="46"/>
+      <c r="E62" s="46"/>
+      <c r="F62" s="46"/>
+      <c r="G62" s="47"/>
     </row>
     <row r="63" spans="1:7">
-      <c r="A63" s="43"/>
-      <c r="B63" s="44"/>
-      <c r="C63" s="44"/>
-      <c r="D63" s="44"/>
-      <c r="E63" s="44"/>
-      <c r="F63" s="44"/>
-      <c r="G63" s="45"/>
+      <c r="A63" s="48"/>
+      <c r="B63" s="49"/>
+      <c r="C63" s="49"/>
+      <c r="D63" s="49"/>
+      <c r="E63" s="49"/>
+      <c r="F63" s="49"/>
+      <c r="G63" s="50"/>
     </row>
     <row r="64" spans="1:7">
       <c r="A64" s="22" t="s">
         <v>77</v>
       </c>
-      <c r="B64" s="35" t="s">
+      <c r="B64" s="34" t="s">
         <v>69</v>
       </c>
-      <c r="C64" s="30"/>
-      <c r="D64" s="35" t="s">
+      <c r="C64" s="29"/>
+      <c r="D64" s="34" t="s">
         <v>70</v>
       </c>
-      <c r="E64" s="30"/>
+      <c r="E64" s="29"/>
       <c r="F64" s="21" t="s">
         <v>71</v>
       </c>
@@ -2729,14 +2787,14 @@
       <c r="A65" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="B65" s="36" t="s">
+      <c r="B65" s="43" t="s">
+        <v>107</v>
+      </c>
+      <c r="C65" s="44"/>
+      <c r="D65" s="43" t="s">
         <v>108</v>
       </c>
-      <c r="C65" s="37"/>
-      <c r="D65" s="36" t="s">
-        <v>109</v>
-      </c>
-      <c r="E65" s="37"/>
+      <c r="E65" s="44"/>
       <c r="F65" s="20"/>
       <c r="G65" s="20"/>
     </row>
@@ -2744,58 +2802,58 @@
       <c r="A66" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="B66" s="36" t="s">
-        <v>107</v>
-      </c>
-      <c r="C66" s="37"/>
-      <c r="D66" s="36"/>
-      <c r="E66" s="37"/>
+      <c r="B66" s="43" t="s">
+        <v>109</v>
+      </c>
+      <c r="C66" s="44"/>
+      <c r="D66" s="43"/>
+      <c r="E66" s="44"/>
       <c r="F66" s="20"/>
       <c r="G66" s="20"/>
     </row>
     <row r="67" spans="1:7">
-      <c r="A67" s="29" t="s">
+      <c r="A67" s="28" t="s">
         <v>74</v>
       </c>
-      <c r="B67" s="30"/>
-      <c r="C67" s="31"/>
-      <c r="D67" s="32"/>
-      <c r="E67" s="32"/>
-      <c r="F67" s="32"/>
-      <c r="G67" s="33"/>
+      <c r="B67" s="29"/>
+      <c r="C67" s="30"/>
+      <c r="D67" s="31"/>
+      <c r="E67" s="31"/>
+      <c r="F67" s="31"/>
+      <c r="G67" s="32"/>
     </row>
     <row r="68" spans="1:7">
-      <c r="A68" s="35" t="s">
+      <c r="A68" s="34" t="s">
         <v>75</v>
       </c>
-      <c r="B68" s="30"/>
-      <c r="C68" s="31"/>
-      <c r="D68" s="32"/>
-      <c r="E68" s="32"/>
-      <c r="F68" s="32"/>
-      <c r="G68" s="33"/>
+      <c r="B68" s="29"/>
+      <c r="C68" s="30"/>
+      <c r="D68" s="31"/>
+      <c r="E68" s="31"/>
+      <c r="F68" s="31"/>
+      <c r="G68" s="32"/>
     </row>
     <row r="69" spans="1:7">
-      <c r="A69" s="29" t="s">
+      <c r="A69" s="28" t="s">
         <v>76</v>
       </c>
-      <c r="B69" s="30"/>
-      <c r="C69" s="31"/>
-      <c r="D69" s="32"/>
-      <c r="E69" s="32"/>
-      <c r="F69" s="32"/>
-      <c r="G69" s="33"/>
+      <c r="B69" s="29"/>
+      <c r="C69" s="30"/>
+      <c r="D69" s="31"/>
+      <c r="E69" s="31"/>
+      <c r="F69" s="31"/>
+      <c r="G69" s="32"/>
     </row>
     <row r="70" spans="1:7">
-      <c r="A70" s="29" t="s">
+      <c r="A70" s="28" t="s">
         <v>73</v>
       </c>
-      <c r="B70" s="34"/>
-      <c r="C70" s="31"/>
-      <c r="D70" s="32"/>
-      <c r="E70" s="32"/>
-      <c r="F70" s="32"/>
-      <c r="G70" s="33"/>
+      <c r="B70" s="33"/>
+      <c r="C70" s="30"/>
+      <c r="D70" s="31"/>
+      <c r="E70" s="31"/>
+      <c r="F70" s="31"/>
+      <c r="G70" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="107">
@@ -2824,6 +2882,19 @@
     <mergeCell ref="D17:E17"/>
     <mergeCell ref="D18:E18"/>
     <mergeCell ref="B18:C18"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="C22:G22"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="A29:G29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="C30:G30"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="C32:G32"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="B13:C13"/>
     <mergeCell ref="B12:C12"/>
@@ -2844,10 +2915,6 @@
     <mergeCell ref="D10:E10"/>
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="D11:E11"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="C21:G21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="C22:G22"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="D13:E13"/>
     <mergeCell ref="A19:B19"/>
@@ -2860,15 +2927,6 @@
     <mergeCell ref="B16:C16"/>
     <mergeCell ref="D16:E16"/>
     <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="A29:G29"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="C30:G30"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="C31:G31"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="C32:G32"/>
     <mergeCell ref="A33:G33"/>
     <mergeCell ref="B34:C34"/>
     <mergeCell ref="D34:E34"/>
@@ -2887,6 +2945,14 @@
     <mergeCell ref="A42:B42"/>
     <mergeCell ref="C42:G42"/>
     <mergeCell ref="A46:G46"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="C55:G55"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="C56:G56"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="C53:G53"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="C54:G54"/>
     <mergeCell ref="A47:B47"/>
     <mergeCell ref="C47:G47"/>
     <mergeCell ref="A48:B48"/>
@@ -2898,14 +2964,6 @@
     <mergeCell ref="A50:G50"/>
     <mergeCell ref="B51:C51"/>
     <mergeCell ref="D51:E51"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="C55:G55"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="C56:G56"/>
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="C53:G53"/>
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="C54:G54"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
@@ -2916,7 +2974,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A4:I24"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
@@ -2935,17 +2993,17 @@
   </cols>
   <sheetData>
     <row r="4" spans="1:9" ht="18">
-      <c r="A4" s="69" t="s">
+      <c r="A4" s="68" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="70"/>
-      <c r="C4" s="70"/>
-      <c r="D4" s="70"/>
-      <c r="E4" s="70"/>
-      <c r="F4" s="70"/>
-      <c r="G4" s="70"/>
-      <c r="H4" s="70"/>
-      <c r="I4" s="71"/>
+      <c r="B4" s="69"/>
+      <c r="C4" s="69"/>
+      <c r="D4" s="69"/>
+      <c r="E4" s="69"/>
+      <c r="F4" s="69"/>
+      <c r="G4" s="69"/>
+      <c r="H4" s="69"/>
+      <c r="I4" s="70"/>
     </row>
     <row r="5" spans="1:9" s="4" customFormat="1">
       <c r="A5" s="2" t="s">
@@ -3065,17 +3123,17 @@
       <c r="I9" s="9"/>
     </row>
     <row r="13" spans="1:9" ht="18">
-      <c r="A13" s="69" t="s">
+      <c r="A13" s="68" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="70"/>
-      <c r="C13" s="70"/>
-      <c r="D13" s="70"/>
-      <c r="E13" s="70"/>
-      <c r="F13" s="70"/>
-      <c r="G13" s="70"/>
-      <c r="H13" s="70"/>
-      <c r="I13" s="71"/>
+      <c r="B13" s="69"/>
+      <c r="C13" s="69"/>
+      <c r="D13" s="69"/>
+      <c r="E13" s="69"/>
+      <c r="F13" s="69"/>
+      <c r="G13" s="69"/>
+      <c r="H13" s="69"/>
+      <c r="I13" s="70"/>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="2" t="s">

</xml_diff>

<commit_message>
Chnged UI layout and color of 3 bottom fragments
1. Add new area
2. Import document
3. Change radius
</commit_message>
<xml_diff>
--- a/FYP documentation/FYP_Test_Plan.xlsx
+++ b/FYP documentation/FYP_Test_Plan.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6936" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6936" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Plan Final" sheetId="4" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="124">
   <si>
     <t>Expected Result</t>
   </si>
@@ -383,9 +383,6 @@
     <t xml:space="preserve">A message should be displayed to ask the user to witch on network. </t>
   </si>
   <si>
-    <t xml:space="preserve">1.  Switch of the gps and turn on the network.         </t>
-  </si>
-  <si>
     <t>Pass</t>
   </si>
   <si>
@@ -408,6 +405,27 @@
   </si>
   <si>
     <t>1842hrs</t>
+  </si>
+  <si>
+    <t>1.  Move around a radius of 100m</t>
+  </si>
+  <si>
+    <t>The current location should be updated realtime.</t>
+  </si>
+  <si>
+    <t>1. click the three line icon on the lefty hand corner of the screen (toolbar)</t>
+  </si>
+  <si>
+    <t>1.  Click the location search icon on the right corner of toolbar</t>
+  </si>
+  <si>
+    <t>The menu should be inflated from the left hand side</t>
+  </si>
+  <si>
+    <t>The location search should be infalted on the tool bar.</t>
+  </si>
+  <si>
+    <t>1.  On loading the screen there should be 3</t>
   </si>
 </sst>
 </file>
@@ -796,26 +814,35 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -823,6 +850,36 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="6" xfId="3" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -832,41 +889,11 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="6" xfId="3" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -874,47 +901,47 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="13" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="15" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="7" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="8" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="12" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="7" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="8" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="12" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="13" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="15" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -924,15 +951,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -1999,10 +2017,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I70"/>
+  <dimension ref="A1:I73"/>
   <sheetViews>
-    <sheetView topLeftCell="A61" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C67" sqref="C67:G67"/>
+    <sheetView tabSelected="1" topLeftCell="A61" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B69" sqref="B69:C69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2019,15 +2037,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="40.799999999999997" customHeight="1">
-      <c r="A1" s="58" t="s">
+      <c r="A1" s="64" t="s">
         <v>64</v>
       </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
-      <c r="E1" s="59"/>
-      <c r="F1" s="59"/>
-      <c r="G1" s="60"/>
+      <c r="B1" s="65"/>
+      <c r="C1" s="65"/>
+      <c r="D1" s="65"/>
+      <c r="E1" s="65"/>
+      <c r="F1" s="65"/>
+      <c r="G1" s="66"/>
       <c r="H1" s="16"/>
       <c r="I1" s="16"/>
     </row>
@@ -2043,38 +2061,38 @@
       <c r="I2" s="19"/>
     </row>
     <row r="3" spans="1:9" ht="31.2" customHeight="1" thickBot="1">
-      <c r="A3" s="51" t="s">
+      <c r="A3" s="49" t="s">
         <v>83</v>
       </c>
-      <c r="B3" s="51"/>
-      <c r="C3" s="51"/>
-      <c r="D3" s="51"/>
-      <c r="E3" s="51"/>
-      <c r="F3" s="51"/>
-      <c r="G3" s="51"/>
+      <c r="B3" s="49"/>
+      <c r="C3" s="49"/>
+      <c r="D3" s="49"/>
+      <c r="E3" s="49"/>
+      <c r="F3" s="49"/>
+      <c r="G3" s="49"/>
       <c r="H3" s="16"/>
       <c r="I3" s="16"/>
     </row>
     <row r="4" spans="1:9" ht="18.600000000000001" customHeight="1" thickTop="1">
-      <c r="A4" s="35" t="s">
+      <c r="A4" s="38" t="s">
         <v>66</v>
       </c>
-      <c r="B4" s="36"/>
-      <c r="C4" s="37" t="s">
+      <c r="B4" s="39"/>
+      <c r="C4" s="50" t="s">
         <v>84</v>
       </c>
-      <c r="D4" s="38"/>
-      <c r="E4" s="38"/>
-      <c r="F4" s="38"/>
-      <c r="G4" s="39"/>
+      <c r="D4" s="51"/>
+      <c r="E4" s="51"/>
+      <c r="F4" s="51"/>
+      <c r="G4" s="52"/>
       <c r="H4" s="17"/>
       <c r="I4" s="17"/>
     </row>
     <row r="5" spans="1:9" ht="14.4" customHeight="1">
-      <c r="A5" s="35" t="s">
+      <c r="A5" s="38" t="s">
         <v>67</v>
       </c>
-      <c r="B5" s="36"/>
+      <c r="B5" s="39"/>
       <c r="C5" s="40"/>
       <c r="D5" s="41"/>
       <c r="E5" s="41"/>
@@ -2084,26 +2102,26 @@
       <c r="I5" s="16"/>
     </row>
     <row r="6" spans="1:9" ht="14.4" customHeight="1">
-      <c r="A6" s="35" t="s">
+      <c r="A6" s="38" t="s">
         <v>68</v>
       </c>
-      <c r="B6" s="36"/>
-      <c r="C6" s="45"/>
-      <c r="D6" s="46"/>
-      <c r="E6" s="46"/>
-      <c r="F6" s="46"/>
-      <c r="G6" s="47"/>
+      <c r="B6" s="39"/>
+      <c r="C6" s="43"/>
+      <c r="D6" s="44"/>
+      <c r="E6" s="44"/>
+      <c r="F6" s="44"/>
+      <c r="G6" s="45"/>
       <c r="H6" s="17"/>
       <c r="I6" s="18"/>
     </row>
     <row r="7" spans="1:9">
-      <c r="A7" s="48"/>
-      <c r="B7" s="49"/>
-      <c r="C7" s="49"/>
-      <c r="D7" s="49"/>
-      <c r="E7" s="49"/>
-      <c r="F7" s="49"/>
-      <c r="G7" s="50"/>
+      <c r="A7" s="46"/>
+      <c r="B7" s="47"/>
+      <c r="C7" s="47"/>
+      <c r="D7" s="47"/>
+      <c r="E7" s="47"/>
+      <c r="F7" s="47"/>
+      <c r="G7" s="48"/>
       <c r="H7" s="18"/>
       <c r="I7" s="18"/>
     </row>
@@ -2111,14 +2129,14 @@
       <c r="A8" s="22" t="s">
         <v>77</v>
       </c>
-      <c r="B8" s="34" t="s">
+      <c r="B8" s="29" t="s">
         <v>69</v>
       </c>
-      <c r="C8" s="29"/>
-      <c r="D8" s="34" t="s">
+      <c r="C8" s="30"/>
+      <c r="D8" s="29" t="s">
         <v>70</v>
       </c>
-      <c r="E8" s="29"/>
+      <c r="E8" s="30"/>
       <c r="F8" s="21" t="s">
         <v>71</v>
       </c>
@@ -2130,14 +2148,14 @@
       <c r="A9" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="43" t="s">
+      <c r="B9" s="36" t="s">
         <v>85</v>
       </c>
-      <c r="C9" s="44"/>
-      <c r="D9" s="43" t="s">
+      <c r="C9" s="37"/>
+      <c r="D9" s="36" t="s">
         <v>90</v>
       </c>
-      <c r="E9" s="44"/>
+      <c r="E9" s="37"/>
       <c r="F9" s="20"/>
       <c r="G9" s="20"/>
     </row>
@@ -2145,14 +2163,14 @@
       <c r="A10" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="43" t="s">
+      <c r="B10" s="36" t="s">
         <v>88</v>
       </c>
-      <c r="C10" s="44"/>
-      <c r="D10" s="43" t="s">
+      <c r="C10" s="37"/>
+      <c r="D10" s="36" t="s">
         <v>91</v>
       </c>
-      <c r="E10" s="56"/>
+      <c r="E10" s="53"/>
       <c r="F10" s="20"/>
       <c r="G10" s="20"/>
     </row>
@@ -2160,14 +2178,14 @@
       <c r="A11" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="43" t="s">
+      <c r="B11" s="36" t="s">
         <v>89</v>
       </c>
-      <c r="C11" s="44"/>
-      <c r="D11" s="43" t="s">
+      <c r="C11" s="37"/>
+      <c r="D11" s="36" t="s">
         <v>87</v>
       </c>
-      <c r="E11" s="44"/>
+      <c r="E11" s="37"/>
       <c r="F11" s="20"/>
       <c r="G11" s="20"/>
     </row>
@@ -2175,14 +2193,14 @@
       <c r="A12" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="43" t="s">
+      <c r="B12" s="36" t="s">
         <v>92</v>
       </c>
-      <c r="C12" s="56"/>
-      <c r="D12" s="43" t="s">
+      <c r="C12" s="53"/>
+      <c r="D12" s="36" t="s">
         <v>87</v>
       </c>
-      <c r="E12" s="44"/>
+      <c r="E12" s="37"/>
       <c r="F12" s="20"/>
       <c r="G12" s="20"/>
     </row>
@@ -2190,14 +2208,14 @@
       <c r="A13" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="B13" s="43" t="s">
+      <c r="B13" s="36" t="s">
         <v>94</v>
       </c>
-      <c r="C13" s="56"/>
-      <c r="D13" s="43" t="s">
+      <c r="C13" s="53"/>
+      <c r="D13" s="36" t="s">
         <v>87</v>
       </c>
-      <c r="E13" s="44"/>
+      <c r="E13" s="37"/>
       <c r="F13" s="20"/>
       <c r="G13" s="20"/>
     </row>
@@ -2205,120 +2223,120 @@
       <c r="A14" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="B14" s="43" t="s">
+      <c r="B14" s="36" t="s">
         <v>93</v>
       </c>
-      <c r="C14" s="44"/>
-      <c r="D14" s="43" t="s">
+      <c r="C14" s="37"/>
+      <c r="D14" s="36" t="s">
         <v>87</v>
       </c>
-      <c r="E14" s="44"/>
+      <c r="E14" s="37"/>
       <c r="F14" s="20"/>
       <c r="G14" s="20"/>
     </row>
     <row r="15" spans="1:9" ht="55.95" customHeight="1">
-      <c r="A15" s="73" t="s">
+      <c r="A15" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="B15" s="57" t="s">
+      <c r="B15" s="54" t="s">
         <v>95</v>
       </c>
-      <c r="C15" s="57"/>
-      <c r="D15" s="43" t="s">
+      <c r="C15" s="54"/>
+      <c r="D15" s="36" t="s">
         <v>91</v>
       </c>
-      <c r="E15" s="56"/>
+      <c r="E15" s="53"/>
       <c r="F15" s="27"/>
       <c r="G15" s="20"/>
     </row>
     <row r="16" spans="1:9" ht="45.45" customHeight="1">
-      <c r="A16" s="73" t="s">
+      <c r="A16" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="B16" s="57" t="s">
+      <c r="B16" s="54" t="s">
         <v>96</v>
       </c>
-      <c r="C16" s="57"/>
-      <c r="D16" s="43" t="s">
+      <c r="C16" s="54"/>
+      <c r="D16" s="36" t="s">
         <v>87</v>
       </c>
-      <c r="E16" s="44"/>
+      <c r="E16" s="37"/>
       <c r="F16" s="27"/>
       <c r="G16" s="20"/>
     </row>
     <row r="17" spans="1:7" ht="45.45" customHeight="1">
-      <c r="A17" s="73" t="s">
+      <c r="A17" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="B17" s="57" t="s">
+      <c r="B17" s="54" t="s">
         <v>97</v>
       </c>
-      <c r="C17" s="57"/>
-      <c r="D17" s="43" t="s">
+      <c r="C17" s="54"/>
+      <c r="D17" s="36" t="s">
         <v>87</v>
       </c>
-      <c r="E17" s="44"/>
+      <c r="E17" s="37"/>
       <c r="F17" s="27"/>
       <c r="G17" s="20"/>
     </row>
     <row r="18" spans="1:7" ht="45.45" customHeight="1">
-      <c r="A18" s="73" t="s">
+      <c r="A18" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="B18" s="57" t="s">
+      <c r="B18" s="54" t="s">
         <v>98</v>
       </c>
-      <c r="C18" s="57"/>
-      <c r="D18" s="43" t="s">
+      <c r="C18" s="54"/>
+      <c r="D18" s="36" t="s">
         <v>91</v>
       </c>
-      <c r="E18" s="56"/>
+      <c r="E18" s="53"/>
       <c r="F18" s="27"/>
       <c r="G18" s="20"/>
     </row>
     <row r="19" spans="1:7">
-      <c r="A19" s="34" t="s">
+      <c r="A19" s="29" t="s">
         <v>74</v>
       </c>
-      <c r="B19" s="29"/>
-      <c r="C19" s="30"/>
-      <c r="D19" s="31"/>
-      <c r="E19" s="31"/>
-      <c r="F19" s="31"/>
-      <c r="G19" s="32"/>
+      <c r="B19" s="30"/>
+      <c r="C19" s="31"/>
+      <c r="D19" s="32"/>
+      <c r="E19" s="32"/>
+      <c r="F19" s="32"/>
+      <c r="G19" s="33"/>
     </row>
     <row r="20" spans="1:7">
-      <c r="A20" s="34" t="s">
+      <c r="A20" s="29" t="s">
         <v>75</v>
       </c>
-      <c r="B20" s="29"/>
-      <c r="C20" s="30"/>
-      <c r="D20" s="31"/>
-      <c r="E20" s="31"/>
-      <c r="F20" s="31"/>
-      <c r="G20" s="32"/>
+      <c r="B20" s="30"/>
+      <c r="C20" s="31"/>
+      <c r="D20" s="32"/>
+      <c r="E20" s="32"/>
+      <c r="F20" s="32"/>
+      <c r="G20" s="33"/>
     </row>
     <row r="21" spans="1:7">
-      <c r="A21" s="28" t="s">
+      <c r="A21" s="34" t="s">
         <v>76</v>
       </c>
-      <c r="B21" s="29"/>
-      <c r="C21" s="30"/>
-      <c r="D21" s="31"/>
-      <c r="E21" s="31"/>
-      <c r="F21" s="31"/>
-      <c r="G21" s="32"/>
+      <c r="B21" s="30"/>
+      <c r="C21" s="31"/>
+      <c r="D21" s="32"/>
+      <c r="E21" s="32"/>
+      <c r="F21" s="32"/>
+      <c r="G21" s="33"/>
     </row>
     <row r="22" spans="1:7">
-      <c r="A22" s="28" t="s">
+      <c r="A22" s="34" t="s">
         <v>73</v>
       </c>
-      <c r="B22" s="33"/>
-      <c r="C22" s="30"/>
-      <c r="D22" s="31"/>
-      <c r="E22" s="31"/>
-      <c r="F22" s="31"/>
-      <c r="G22" s="32"/>
+      <c r="B22" s="35"/>
+      <c r="C22" s="31"/>
+      <c r="D22" s="32"/>
+      <c r="E22" s="32"/>
+      <c r="F22" s="32"/>
+      <c r="G22" s="33"/>
     </row>
     <row r="23" spans="1:7" ht="26.4" customHeight="1">
       <c r="A23" s="18"/>
@@ -2367,34 +2385,34 @@
     </row>
     <row r="28" spans="1:7" ht="25.8" customHeight="1"/>
     <row r="29" spans="1:7" ht="20.399999999999999" thickBot="1">
-      <c r="A29" s="51" t="s">
+      <c r="A29" s="49" t="s">
         <v>65</v>
       </c>
-      <c r="B29" s="51"/>
-      <c r="C29" s="51"/>
-      <c r="D29" s="51"/>
-      <c r="E29" s="51"/>
-      <c r="F29" s="51"/>
-      <c r="G29" s="51"/>
+      <c r="B29" s="49"/>
+      <c r="C29" s="49"/>
+      <c r="D29" s="49"/>
+      <c r="E29" s="49"/>
+      <c r="F29" s="49"/>
+      <c r="G29" s="49"/>
     </row>
     <row r="30" spans="1:7" ht="15" thickTop="1">
-      <c r="A30" s="61" t="s">
+      <c r="A30" s="57" t="s">
         <v>66</v>
       </c>
-      <c r="B30" s="62"/>
-      <c r="C30" s="63" t="s">
+      <c r="B30" s="58"/>
+      <c r="C30" s="59" t="s">
         <v>78</v>
       </c>
-      <c r="D30" s="64"/>
-      <c r="E30" s="64"/>
-      <c r="F30" s="64"/>
-      <c r="G30" s="65"/>
+      <c r="D30" s="60"/>
+      <c r="E30" s="60"/>
+      <c r="F30" s="60"/>
+      <c r="G30" s="61"/>
     </row>
     <row r="31" spans="1:7">
-      <c r="A31" s="35" t="s">
+      <c r="A31" s="38" t="s">
         <v>67</v>
       </c>
-      <c r="B31" s="36"/>
+      <c r="B31" s="39"/>
       <c r="C31" s="40"/>
       <c r="D31" s="41"/>
       <c r="E31" s="41"/>
@@ -2402,39 +2420,39 @@
       <c r="G31" s="42"/>
     </row>
     <row r="32" spans="1:7">
-      <c r="A32" s="35" t="s">
+      <c r="A32" s="38" t="s">
         <v>68</v>
       </c>
-      <c r="B32" s="36"/>
-      <c r="C32" s="45" t="s">
+      <c r="B32" s="39"/>
+      <c r="C32" s="43" t="s">
         <v>79</v>
       </c>
-      <c r="D32" s="66"/>
-      <c r="E32" s="66"/>
-      <c r="F32" s="66"/>
-      <c r="G32" s="67"/>
+      <c r="D32" s="62"/>
+      <c r="E32" s="62"/>
+      <c r="F32" s="62"/>
+      <c r="G32" s="63"/>
     </row>
     <row r="33" spans="1:7">
-      <c r="A33" s="30"/>
-      <c r="B33" s="31"/>
-      <c r="C33" s="31"/>
-      <c r="D33" s="31"/>
-      <c r="E33" s="31"/>
-      <c r="F33" s="31"/>
-      <c r="G33" s="32"/>
+      <c r="A33" s="31"/>
+      <c r="B33" s="32"/>
+      <c r="C33" s="32"/>
+      <c r="D33" s="32"/>
+      <c r="E33" s="32"/>
+      <c r="F33" s="32"/>
+      <c r="G33" s="33"/>
     </row>
     <row r="34" spans="1:7">
       <c r="A34" s="22" t="s">
         <v>77</v>
       </c>
-      <c r="B34" s="34" t="s">
+      <c r="B34" s="29" t="s">
         <v>69</v>
       </c>
-      <c r="C34" s="29"/>
-      <c r="D34" s="34" t="s">
+      <c r="C34" s="30"/>
+      <c r="D34" s="29" t="s">
         <v>70</v>
       </c>
-      <c r="E34" s="29"/>
+      <c r="E34" s="30"/>
       <c r="F34" s="21" t="s">
         <v>71</v>
       </c>
@@ -2446,159 +2464,159 @@
       <c r="A35" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="B35" s="52" t="s">
-        <v>115</v>
-      </c>
-      <c r="C35" s="53"/>
-      <c r="D35" s="54" t="s">
+      <c r="B35" s="55" t="s">
+        <v>114</v>
+      </c>
+      <c r="C35" s="56"/>
+      <c r="D35" s="67" t="s">
         <v>72</v>
       </c>
-      <c r="E35" s="55"/>
+      <c r="E35" s="68"/>
       <c r="F35" s="20" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G35" s="20" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="46.8" customHeight="1">
       <c r="A36" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="B36" s="52" t="s">
+      <c r="B36" s="55" t="s">
         <v>50</v>
       </c>
-      <c r="C36" s="53"/>
-      <c r="D36" s="43" t="s">
+      <c r="C36" s="56"/>
+      <c r="D36" s="36" t="s">
         <v>86</v>
       </c>
-      <c r="E36" s="56"/>
+      <c r="E36" s="53"/>
       <c r="F36" s="20" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G36" s="20" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="45.6" customHeight="1">
       <c r="A37" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="B37" s="52" t="s">
+      <c r="B37" s="55" t="s">
         <v>49</v>
       </c>
-      <c r="C37" s="53"/>
-      <c r="D37" s="43" t="s">
+      <c r="C37" s="56"/>
+      <c r="D37" s="36" t="s">
         <v>80</v>
       </c>
-      <c r="E37" s="56"/>
+      <c r="E37" s="53"/>
       <c r="F37" s="20" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G37" s="20" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="48" customHeight="1">
       <c r="A38" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="B38" s="52" t="s">
+      <c r="B38" s="55" t="s">
         <v>81</v>
       </c>
-      <c r="C38" s="53"/>
-      <c r="D38" s="43" t="s">
+      <c r="C38" s="56"/>
+      <c r="D38" s="36" t="s">
         <v>82</v>
       </c>
-      <c r="E38" s="56"/>
+      <c r="E38" s="53"/>
       <c r="F38" s="20" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G38" s="20" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="39" spans="1:7">
-      <c r="A39" s="34" t="s">
+      <c r="A39" s="29" t="s">
         <v>74</v>
       </c>
-      <c r="B39" s="29"/>
-      <c r="C39" s="54" t="s">
+      <c r="B39" s="30"/>
+      <c r="C39" s="67" t="s">
+        <v>115</v>
+      </c>
+      <c r="D39" s="69"/>
+      <c r="E39" s="69"/>
+      <c r="F39" s="69"/>
+      <c r="G39" s="68"/>
+    </row>
+    <row r="40" spans="1:7">
+      <c r="A40" s="29" t="s">
+        <v>75</v>
+      </c>
+      <c r="B40" s="30"/>
+      <c r="C40" s="70">
+        <v>43042</v>
+      </c>
+      <c r="D40" s="69"/>
+      <c r="E40" s="69"/>
+      <c r="F40" s="69"/>
+      <c r="G40" s="68"/>
+    </row>
+    <row r="41" spans="1:7">
+      <c r="A41" s="34" t="s">
+        <v>76</v>
+      </c>
+      <c r="B41" s="35"/>
+      <c r="C41" s="67" t="s">
         <v>116</v>
       </c>
-      <c r="D39" s="71"/>
-      <c r="E39" s="71"/>
-      <c r="F39" s="71"/>
-      <c r="G39" s="55"/>
-    </row>
-    <row r="40" spans="1:7">
-      <c r="A40" s="34" t="s">
-        <v>75</v>
-      </c>
-      <c r="B40" s="29"/>
-      <c r="C40" s="72">
-        <v>43042</v>
-      </c>
-      <c r="D40" s="71"/>
-      <c r="E40" s="71"/>
-      <c r="F40" s="71"/>
-      <c r="G40" s="55"/>
-    </row>
-    <row r="41" spans="1:7">
-      <c r="A41" s="28" t="s">
-        <v>76</v>
-      </c>
-      <c r="B41" s="33"/>
-      <c r="C41" s="54" t="s">
-        <v>117</v>
-      </c>
-      <c r="D41" s="71"/>
-      <c r="E41" s="71"/>
-      <c r="F41" s="71"/>
-      <c r="G41" s="55"/>
+      <c r="D41" s="69"/>
+      <c r="E41" s="69"/>
+      <c r="F41" s="69"/>
+      <c r="G41" s="68"/>
     </row>
     <row r="42" spans="1:7">
-      <c r="A42" s="28" t="s">
+      <c r="A42" s="34" t="s">
         <v>73</v>
       </c>
-      <c r="B42" s="33"/>
-      <c r="C42" s="54" t="s">
-        <v>110</v>
-      </c>
-      <c r="D42" s="71"/>
-      <c r="E42" s="71"/>
-      <c r="F42" s="71"/>
-      <c r="G42" s="55"/>
+      <c r="B42" s="35"/>
+      <c r="C42" s="67" t="s">
+        <v>109</v>
+      </c>
+      <c r="D42" s="69"/>
+      <c r="E42" s="69"/>
+      <c r="F42" s="69"/>
+      <c r="G42" s="68"/>
     </row>
     <row r="46" spans="1:7" ht="20.399999999999999" thickBot="1">
-      <c r="A46" s="51" t="s">
+      <c r="A46" s="49" t="s">
         <v>102</v>
       </c>
-      <c r="B46" s="51"/>
-      <c r="C46" s="51"/>
-      <c r="D46" s="51"/>
-      <c r="E46" s="51"/>
-      <c r="F46" s="51"/>
-      <c r="G46" s="51"/>
+      <c r="B46" s="49"/>
+      <c r="C46" s="49"/>
+      <c r="D46" s="49"/>
+      <c r="E46" s="49"/>
+      <c r="F46" s="49"/>
+      <c r="G46" s="49"/>
     </row>
     <row r="47" spans="1:7" ht="15" thickTop="1">
-      <c r="A47" s="35" t="s">
+      <c r="A47" s="38" t="s">
         <v>66</v>
       </c>
-      <c r="B47" s="36"/>
-      <c r="C47" s="37" t="s">
+      <c r="B47" s="39"/>
+      <c r="C47" s="50" t="s">
         <v>99</v>
       </c>
-      <c r="D47" s="38"/>
-      <c r="E47" s="38"/>
-      <c r="F47" s="38"/>
-      <c r="G47" s="39"/>
+      <c r="D47" s="51"/>
+      <c r="E47" s="51"/>
+      <c r="F47" s="51"/>
+      <c r="G47" s="52"/>
     </row>
     <row r="48" spans="1:7">
-      <c r="A48" s="35" t="s">
+      <c r="A48" s="38" t="s">
         <v>67</v>
       </c>
-      <c r="B48" s="36"/>
+      <c r="B48" s="39"/>
       <c r="C48" s="40"/>
       <c r="D48" s="41"/>
       <c r="E48" s="41"/>
@@ -2606,39 +2624,39 @@
       <c r="G48" s="42"/>
     </row>
     <row r="49" spans="1:7">
-      <c r="A49" s="35" t="s">
+      <c r="A49" s="38" t="s">
         <v>68</v>
       </c>
-      <c r="B49" s="36"/>
-      <c r="C49" s="45" t="s">
+      <c r="B49" s="39"/>
+      <c r="C49" s="43" t="s">
         <v>100</v>
       </c>
-      <c r="D49" s="46"/>
-      <c r="E49" s="46"/>
-      <c r="F49" s="46"/>
-      <c r="G49" s="47"/>
+      <c r="D49" s="44"/>
+      <c r="E49" s="44"/>
+      <c r="F49" s="44"/>
+      <c r="G49" s="45"/>
     </row>
     <row r="50" spans="1:7" ht="31.8" customHeight="1">
-      <c r="A50" s="48"/>
-      <c r="B50" s="49"/>
-      <c r="C50" s="49"/>
-      <c r="D50" s="49"/>
-      <c r="E50" s="49"/>
-      <c r="F50" s="49"/>
-      <c r="G50" s="50"/>
+      <c r="A50" s="46"/>
+      <c r="B50" s="47"/>
+      <c r="C50" s="47"/>
+      <c r="D50" s="47"/>
+      <c r="E50" s="47"/>
+      <c r="F50" s="47"/>
+      <c r="G50" s="48"/>
     </row>
     <row r="51" spans="1:7" ht="63" customHeight="1">
       <c r="A51" s="22" t="s">
         <v>77</v>
       </c>
-      <c r="B51" s="34" t="s">
+      <c r="B51" s="29" t="s">
         <v>69</v>
       </c>
-      <c r="C51" s="29"/>
-      <c r="D51" s="34" t="s">
+      <c r="C51" s="30"/>
+      <c r="D51" s="29" t="s">
         <v>70</v>
       </c>
-      <c r="E51" s="29"/>
+      <c r="E51" s="30"/>
       <c r="F51" s="21" t="s">
         <v>71</v>
       </c>
@@ -2650,92 +2668,92 @@
       <c r="A52" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="B52" s="43" t="s">
+      <c r="B52" s="36" t="s">
         <v>103</v>
       </c>
-      <c r="C52" s="44"/>
-      <c r="D52" s="43" t="s">
+      <c r="C52" s="37"/>
+      <c r="D52" s="36" t="s">
         <v>101</v>
       </c>
-      <c r="E52" s="44"/>
+      <c r="E52" s="37"/>
       <c r="F52" s="20"/>
       <c r="G52" s="20"/>
     </row>
     <row r="53" spans="1:7" ht="27" customHeight="1">
-      <c r="A53" s="28" t="s">
+      <c r="A53" s="34" t="s">
         <v>74</v>
       </c>
-      <c r="B53" s="29"/>
-      <c r="C53" s="54" t="s">
-        <v>116</v>
-      </c>
-      <c r="D53" s="71"/>
-      <c r="E53" s="71"/>
-      <c r="F53" s="71"/>
-      <c r="G53" s="55"/>
+      <c r="B53" s="30"/>
+      <c r="C53" s="67" t="s">
+        <v>115</v>
+      </c>
+      <c r="D53" s="69"/>
+      <c r="E53" s="69"/>
+      <c r="F53" s="69"/>
+      <c r="G53" s="68"/>
     </row>
     <row r="54" spans="1:7" ht="34.799999999999997" customHeight="1">
-      <c r="A54" s="34" t="s">
+      <c r="A54" s="29" t="s">
         <v>75</v>
       </c>
-      <c r="B54" s="29"/>
-      <c r="C54" s="30"/>
-      <c r="D54" s="31"/>
-      <c r="E54" s="31"/>
-      <c r="F54" s="31"/>
-      <c r="G54" s="32"/>
+      <c r="B54" s="30"/>
+      <c r="C54" s="31"/>
+      <c r="D54" s="32"/>
+      <c r="E54" s="32"/>
+      <c r="F54" s="32"/>
+      <c r="G54" s="33"/>
     </row>
     <row r="55" spans="1:7" ht="25.2" customHeight="1">
-      <c r="A55" s="28" t="s">
+      <c r="A55" s="34" t="s">
         <v>76</v>
       </c>
-      <c r="B55" s="29"/>
-      <c r="C55" s="30"/>
-      <c r="D55" s="31"/>
-      <c r="E55" s="31"/>
-      <c r="F55" s="31"/>
-      <c r="G55" s="32"/>
+      <c r="B55" s="30"/>
+      <c r="C55" s="31"/>
+      <c r="D55" s="32"/>
+      <c r="E55" s="32"/>
+      <c r="F55" s="32"/>
+      <c r="G55" s="33"/>
     </row>
     <row r="56" spans="1:7">
-      <c r="A56" s="28" t="s">
+      <c r="A56" s="34" t="s">
         <v>73</v>
       </c>
-      <c r="B56" s="33"/>
-      <c r="C56" s="30"/>
-      <c r="D56" s="31"/>
-      <c r="E56" s="31"/>
-      <c r="F56" s="31"/>
-      <c r="G56" s="32"/>
+      <c r="B56" s="35"/>
+      <c r="C56" s="31"/>
+      <c r="D56" s="32"/>
+      <c r="E56" s="32"/>
+      <c r="F56" s="32"/>
+      <c r="G56" s="33"/>
     </row>
     <row r="59" spans="1:7" ht="20.399999999999999" thickBot="1">
-      <c r="A59" s="51" t="s">
+      <c r="A59" s="49" t="s">
         <v>105</v>
       </c>
-      <c r="B59" s="51"/>
-      <c r="C59" s="51"/>
-      <c r="D59" s="51"/>
-      <c r="E59" s="51"/>
-      <c r="F59" s="51"/>
-      <c r="G59" s="51"/>
+      <c r="B59" s="49"/>
+      <c r="C59" s="49"/>
+      <c r="D59" s="49"/>
+      <c r="E59" s="49"/>
+      <c r="F59" s="49"/>
+      <c r="G59" s="49"/>
     </row>
     <row r="60" spans="1:7" ht="15" thickTop="1">
-      <c r="A60" s="35" t="s">
+      <c r="A60" s="38" t="s">
         <v>66</v>
       </c>
-      <c r="B60" s="36"/>
-      <c r="C60" s="37" t="s">
+      <c r="B60" s="39"/>
+      <c r="C60" s="50" t="s">
         <v>106</v>
       </c>
-      <c r="D60" s="38"/>
-      <c r="E60" s="38"/>
-      <c r="F60" s="38"/>
-      <c r="G60" s="39"/>
+      <c r="D60" s="51"/>
+      <c r="E60" s="51"/>
+      <c r="F60" s="51"/>
+      <c r="G60" s="52"/>
     </row>
     <row r="61" spans="1:7">
-      <c r="A61" s="35" t="s">
+      <c r="A61" s="38" t="s">
         <v>67</v>
       </c>
-      <c r="B61" s="36"/>
+      <c r="B61" s="39"/>
       <c r="C61" s="40"/>
       <c r="D61" s="41"/>
       <c r="E61" s="41"/>
@@ -2743,39 +2761,39 @@
       <c r="G61" s="42"/>
     </row>
     <row r="62" spans="1:7">
-      <c r="A62" s="35" t="s">
+      <c r="A62" s="38" t="s">
         <v>68</v>
       </c>
-      <c r="B62" s="36"/>
-      <c r="C62" s="45" t="s">
+      <c r="B62" s="39"/>
+      <c r="C62" s="43" t="s">
         <v>104</v>
       </c>
-      <c r="D62" s="46"/>
-      <c r="E62" s="46"/>
-      <c r="F62" s="46"/>
-      <c r="G62" s="47"/>
+      <c r="D62" s="44"/>
+      <c r="E62" s="44"/>
+      <c r="F62" s="44"/>
+      <c r="G62" s="45"/>
     </row>
     <row r="63" spans="1:7">
-      <c r="A63" s="48"/>
-      <c r="B63" s="49"/>
-      <c r="C63" s="49"/>
-      <c r="D63" s="49"/>
-      <c r="E63" s="49"/>
-      <c r="F63" s="49"/>
-      <c r="G63" s="50"/>
+      <c r="A63" s="46"/>
+      <c r="B63" s="47"/>
+      <c r="C63" s="47"/>
+      <c r="D63" s="47"/>
+      <c r="E63" s="47"/>
+      <c r="F63" s="47"/>
+      <c r="G63" s="48"/>
     </row>
     <row r="64" spans="1:7">
       <c r="A64" s="22" t="s">
         <v>77</v>
       </c>
-      <c r="B64" s="34" t="s">
+      <c r="B64" s="29" t="s">
         <v>69</v>
       </c>
-      <c r="C64" s="29"/>
-      <c r="D64" s="34" t="s">
+      <c r="C64" s="30"/>
+      <c r="D64" s="29" t="s">
         <v>70</v>
       </c>
-      <c r="E64" s="29"/>
+      <c r="E64" s="30"/>
       <c r="F64" s="21" t="s">
         <v>71</v>
       </c>
@@ -2787,14 +2805,14 @@
       <c r="A65" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="B65" s="43" t="s">
+      <c r="B65" s="36" t="s">
         <v>107</v>
       </c>
-      <c r="C65" s="44"/>
-      <c r="D65" s="43" t="s">
+      <c r="C65" s="37"/>
+      <c r="D65" s="36" t="s">
         <v>108</v>
       </c>
-      <c r="E65" s="44"/>
+      <c r="E65" s="37"/>
       <c r="F65" s="20"/>
       <c r="G65" s="20"/>
     </row>
@@ -2802,75 +2820,177 @@
       <c r="A66" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="B66" s="43" t="s">
-        <v>109</v>
-      </c>
-      <c r="C66" s="44"/>
-      <c r="D66" s="43"/>
-      <c r="E66" s="44"/>
+      <c r="B66" s="36" t="s">
+        <v>117</v>
+      </c>
+      <c r="C66" s="37"/>
+      <c r="D66" s="36" t="s">
+        <v>118</v>
+      </c>
+      <c r="E66" s="37"/>
       <c r="F66" s="20"/>
       <c r="G66" s="20"/>
     </row>
-    <row r="67" spans="1:7">
-      <c r="A67" s="28" t="s">
+    <row r="67" spans="1:7" ht="49.8" customHeight="1">
+      <c r="A67" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="B67" s="36" t="s">
+        <v>119</v>
+      </c>
+      <c r="C67" s="37"/>
+      <c r="D67" s="36" t="s">
+        <v>121</v>
+      </c>
+      <c r="E67" s="37"/>
+      <c r="F67" s="20"/>
+      <c r="G67" s="20"/>
+    </row>
+    <row r="68" spans="1:7" ht="41.4" customHeight="1">
+      <c r="A68" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="B68" s="36" t="s">
+        <v>120</v>
+      </c>
+      <c r="C68" s="37"/>
+      <c r="D68" s="36" t="s">
+        <v>122</v>
+      </c>
+      <c r="E68" s="37"/>
+      <c r="F68" s="20"/>
+      <c r="G68" s="20"/>
+    </row>
+    <row r="69" spans="1:7" ht="46.8" customHeight="1">
+      <c r="A69" s="26" t="s">
+        <v>28</v>
+      </c>
+      <c r="B69" s="36" t="s">
+        <v>123</v>
+      </c>
+      <c r="C69" s="37"/>
+      <c r="D69" s="36" t="s">
+        <v>122</v>
+      </c>
+      <c r="E69" s="37"/>
+      <c r="F69" s="20"/>
+      <c r="G69" s="20"/>
+    </row>
+    <row r="70" spans="1:7">
+      <c r="A70" s="34" t="s">
         <v>74</v>
       </c>
-      <c r="B67" s="29"/>
-      <c r="C67" s="30"/>
-      <c r="D67" s="31"/>
-      <c r="E67" s="31"/>
-      <c r="F67" s="31"/>
-      <c r="G67" s="32"/>
-    </row>
-    <row r="68" spans="1:7">
-      <c r="A68" s="34" t="s">
+      <c r="B70" s="30"/>
+      <c r="C70" s="31"/>
+      <c r="D70" s="32"/>
+      <c r="E70" s="32"/>
+      <c r="F70" s="32"/>
+      <c r="G70" s="33"/>
+    </row>
+    <row r="71" spans="1:7">
+      <c r="A71" s="29" t="s">
         <v>75</v>
       </c>
-      <c r="B68" s="29"/>
-      <c r="C68" s="30"/>
-      <c r="D68" s="31"/>
-      <c r="E68" s="31"/>
-      <c r="F68" s="31"/>
-      <c r="G68" s="32"/>
-    </row>
-    <row r="69" spans="1:7">
-      <c r="A69" s="28" t="s">
+      <c r="B71" s="30"/>
+      <c r="C71" s="31"/>
+      <c r="D71" s="32"/>
+      <c r="E71" s="32"/>
+      <c r="F71" s="32"/>
+      <c r="G71" s="33"/>
+    </row>
+    <row r="72" spans="1:7">
+      <c r="A72" s="34" t="s">
         <v>76</v>
       </c>
-      <c r="B69" s="29"/>
-      <c r="C69" s="30"/>
-      <c r="D69" s="31"/>
-      <c r="E69" s="31"/>
-      <c r="F69" s="31"/>
-      <c r="G69" s="32"/>
-    </row>
-    <row r="70" spans="1:7">
-      <c r="A70" s="28" t="s">
+      <c r="B72" s="30"/>
+      <c r="C72" s="31"/>
+      <c r="D72" s="32"/>
+      <c r="E72" s="32"/>
+      <c r="F72" s="32"/>
+      <c r="G72" s="33"/>
+    </row>
+    <row r="73" spans="1:7">
+      <c r="A73" s="34" t="s">
         <v>73</v>
       </c>
-      <c r="B70" s="33"/>
-      <c r="C70" s="30"/>
-      <c r="D70" s="31"/>
-      <c r="E70" s="31"/>
-      <c r="F70" s="31"/>
-      <c r="G70" s="32"/>
+      <c r="B73" s="35"/>
+      <c r="C73" s="31"/>
+      <c r="D73" s="32"/>
+      <c r="E73" s="32"/>
+      <c r="F73" s="32"/>
+      <c r="G73" s="33"/>
     </row>
   </sheetData>
-  <mergeCells count="107">
-    <mergeCell ref="A68:B68"/>
-    <mergeCell ref="C68:G68"/>
-    <mergeCell ref="A69:B69"/>
-    <mergeCell ref="C69:G69"/>
-    <mergeCell ref="A70:B70"/>
-    <mergeCell ref="C70:G70"/>
-    <mergeCell ref="B64:C64"/>
-    <mergeCell ref="D64:E64"/>
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="D65:E65"/>
-    <mergeCell ref="A67:B67"/>
-    <mergeCell ref="C67:G67"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="D66:E66"/>
+  <mergeCells count="113">
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="C55:G55"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="C56:G56"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="C53:G53"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="C54:G54"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="C47:G47"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="C48:G48"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="D52:E52"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="C49:G49"/>
+    <mergeCell ref="A50:G50"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="D51:E51"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="C39:G39"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="C40:G40"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="C41:G41"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="C42:G42"/>
+    <mergeCell ref="A46:G46"/>
+    <mergeCell ref="A33:G33"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A3:G3"/>
+    <mergeCell ref="A7:G7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:G6"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:G4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:G5"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D11:E11"/>
     <mergeCell ref="A61:B61"/>
     <mergeCell ref="C61:G61"/>
     <mergeCell ref="A62:B62"/>
@@ -2895,75 +3015,26 @@
     <mergeCell ref="C31:G31"/>
     <mergeCell ref="A32:B32"/>
     <mergeCell ref="C32:G32"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A3:G3"/>
-    <mergeCell ref="A7:G7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:G6"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:G4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:G5"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="C20:G20"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="A33:G33"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="C39:G39"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="C40:G40"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="C41:G41"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="C42:G42"/>
-    <mergeCell ref="A46:G46"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="C55:G55"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="C56:G56"/>
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="C53:G53"/>
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="C54:G54"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="C47:G47"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="C48:G48"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="D52:E52"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="C49:G49"/>
-    <mergeCell ref="A50:G50"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="D51:E51"/>
+    <mergeCell ref="A71:B71"/>
+    <mergeCell ref="C71:G71"/>
+    <mergeCell ref="A72:B72"/>
+    <mergeCell ref="C72:G72"/>
+    <mergeCell ref="A73:B73"/>
+    <mergeCell ref="C73:G73"/>
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="D64:E64"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="D65:E65"/>
+    <mergeCell ref="A70:B70"/>
+    <mergeCell ref="C70:G70"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="D66:E66"/>
+    <mergeCell ref="B67:C67"/>
+    <mergeCell ref="D67:E67"/>
+    <mergeCell ref="B68:C68"/>
+    <mergeCell ref="D68:E68"/>
+    <mergeCell ref="B69:C69"/>
+    <mergeCell ref="D69:E69"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
@@ -2974,7 +3045,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A4:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
@@ -2993,17 +3064,17 @@
   </cols>
   <sheetData>
     <row r="4" spans="1:9" ht="18">
-      <c r="A4" s="68" t="s">
+      <c r="A4" s="71" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="69"/>
-      <c r="C4" s="69"/>
-      <c r="D4" s="69"/>
-      <c r="E4" s="69"/>
-      <c r="F4" s="69"/>
-      <c r="G4" s="69"/>
-      <c r="H4" s="69"/>
-      <c r="I4" s="70"/>
+      <c r="B4" s="72"/>
+      <c r="C4" s="72"/>
+      <c r="D4" s="72"/>
+      <c r="E4" s="72"/>
+      <c r="F4" s="72"/>
+      <c r="G4" s="72"/>
+      <c r="H4" s="72"/>
+      <c r="I4" s="73"/>
     </row>
     <row r="5" spans="1:9" s="4" customFormat="1">
       <c r="A5" s="2" t="s">
@@ -3123,17 +3194,17 @@
       <c r="I9" s="9"/>
     </row>
     <row r="13" spans="1:9" ht="18">
-      <c r="A13" s="68" t="s">
+      <c r="A13" s="71" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="69"/>
-      <c r="C13" s="69"/>
-      <c r="D13" s="69"/>
-      <c r="E13" s="69"/>
-      <c r="F13" s="69"/>
-      <c r="G13" s="69"/>
-      <c r="H13" s="69"/>
-      <c r="I13" s="70"/>
+      <c r="B13" s="72"/>
+      <c r="C13" s="72"/>
+      <c r="D13" s="72"/>
+      <c r="E13" s="72"/>
+      <c r="F13" s="72"/>
+      <c r="G13" s="72"/>
+      <c r="H13" s="72"/>
+      <c r="I13" s="73"/>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="2" t="s">

</xml_diff>

<commit_message>
Did test on signup, homepage and login
</commit_message>
<xml_diff>
--- a/FYP documentation/FYP_Test_Plan.xlsx
+++ b/FYP documentation/FYP_Test_Plan.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="134">
   <si>
     <t>Expected Result</t>
   </si>
@@ -329,18 +329,6 @@
 2) Click on 'SIGN UP' button </t>
   </si>
   <si>
-    <t>1) Enter value in numbers which is in between 8-32 characters 
-2) Click on 'SIGN UP' button</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1) Enter value which is alphanumeric but more than 32 characters 
-2) Click on 'SIGN UP' button </t>
-  </si>
-  <si>
-    <t>1) Enter value in alphanumeric which is in between 8-32 characters 
-2) Click on 'SIGN UP' button</t>
-  </si>
-  <si>
     <t>1) Enter alphanumeric data in contact number field 
 2) Click on 'SIGN UP' button</t>
   </si>
@@ -416,16 +404,57 @@
     <t>1. click the three line icon on the lefty hand corner of the screen (toolbar)</t>
   </si>
   <si>
-    <t>1.  Click the location search icon on the right corner of toolbar</t>
-  </si>
-  <si>
     <t>The menu should be inflated from the left hand side</t>
   </si>
   <si>
     <t>The location search should be infalted on the tool bar.</t>
   </si>
   <si>
-    <t>1.  On loading the screen there should be 3</t>
+    <t xml:space="preserve">Signed up successfully </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) Enter value which is alphanumeric but more than 12 characters 
+2) Click on 'SIGN UP' button </t>
+  </si>
+  <si>
+    <t>1) Enter value in alphanumeric which is in between 8-12 characters 
+2) Click on 'SIGN UP' button</t>
+  </si>
+  <si>
+    <t>Goes to congirmation page, but the user will not recive the confirmation code hence signup fail</t>
+  </si>
+  <si>
+    <t>Invalid input error message</t>
+  </si>
+  <si>
+    <t>1412 hrs</t>
+  </si>
+  <si>
+    <t>User is notified that there is no connectivity</t>
+  </si>
+  <si>
+    <t>Yes the location reset while walking around</t>
+  </si>
+  <si>
+    <t>The menu slides in from left</t>
+  </si>
+  <si>
+    <t>The location search gives suggestions and moves the map to the searched location on clicking</t>
+  </si>
+  <si>
+    <t>1.  Click the location search icon on the right corner of toolbar.                                         2. Search for a added location</t>
+  </si>
+  <si>
+    <t>On loading the screen there should be 3 floating action button at the bottom right hand corner</t>
+  </si>
+  <si>
+    <t>1.  Load home page</t>
+  </si>
+  <si>
+    <t>The button apear at the bottom right hand corner</t>
+  </si>
+  <si>
+    <t>1439 hrs</t>
   </si>
 </sst>
 </file>
@@ -745,7 +774,7 @@
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -813,30 +842,62 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -844,21 +905,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -877,17 +923,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="6" xfId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -895,11 +941,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="7" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="8" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="12" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="13" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -922,27 +971,6 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="7" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="8" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="12" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -951,6 +979,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -2017,10 +2051,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I73"/>
+  <dimension ref="A1:I72"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A61" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B69" sqref="B69:C69"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2037,15 +2071,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="40.799999999999997" customHeight="1">
-      <c r="A1" s="64" t="s">
+      <c r="A1" s="60" t="s">
         <v>64</v>
       </c>
-      <c r="B1" s="65"/>
-      <c r="C1" s="65"/>
-      <c r="D1" s="65"/>
-      <c r="E1" s="65"/>
-      <c r="F1" s="65"/>
-      <c r="G1" s="66"/>
+      <c r="B1" s="61"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="61"/>
+      <c r="F1" s="61"/>
+      <c r="G1" s="62"/>
       <c r="H1" s="16"/>
       <c r="I1" s="16"/>
     </row>
@@ -2061,15 +2095,15 @@
       <c r="I2" s="19"/>
     </row>
     <row r="3" spans="1:9" ht="31.2" customHeight="1" thickBot="1">
-      <c r="A3" s="49" t="s">
+      <c r="A3" s="55" t="s">
         <v>83</v>
       </c>
-      <c r="B3" s="49"/>
-      <c r="C3" s="49"/>
-      <c r="D3" s="49"/>
-      <c r="E3" s="49"/>
-      <c r="F3" s="49"/>
-      <c r="G3" s="49"/>
+      <c r="B3" s="55"/>
+      <c r="C3" s="55"/>
+      <c r="D3" s="55"/>
+      <c r="E3" s="55"/>
+      <c r="F3" s="55"/>
+      <c r="G3" s="55"/>
       <c r="H3" s="16"/>
       <c r="I3" s="16"/>
     </row>
@@ -2078,13 +2112,13 @@
         <v>66</v>
       </c>
       <c r="B4" s="39"/>
-      <c r="C4" s="50" t="s">
+      <c r="C4" s="40" t="s">
         <v>84</v>
       </c>
-      <c r="D4" s="51"/>
-      <c r="E4" s="51"/>
-      <c r="F4" s="51"/>
-      <c r="G4" s="52"/>
+      <c r="D4" s="41"/>
+      <c r="E4" s="41"/>
+      <c r="F4" s="41"/>
+      <c r="G4" s="42"/>
       <c r="H4" s="17"/>
       <c r="I4" s="17"/>
     </row>
@@ -2093,11 +2127,11 @@
         <v>67</v>
       </c>
       <c r="B5" s="39"/>
-      <c r="C5" s="40"/>
-      <c r="D5" s="41"/>
-      <c r="E5" s="41"/>
-      <c r="F5" s="41"/>
-      <c r="G5" s="42"/>
+      <c r="C5" s="43"/>
+      <c r="D5" s="44"/>
+      <c r="E5" s="44"/>
+      <c r="F5" s="44"/>
+      <c r="G5" s="45"/>
       <c r="H5" s="16"/>
       <c r="I5" s="16"/>
     </row>
@@ -2106,22 +2140,22 @@
         <v>68</v>
       </c>
       <c r="B6" s="39"/>
-      <c r="C6" s="43"/>
-      <c r="D6" s="44"/>
-      <c r="E6" s="44"/>
-      <c r="F6" s="44"/>
-      <c r="G6" s="45"/>
+      <c r="C6" s="48"/>
+      <c r="D6" s="49"/>
+      <c r="E6" s="49"/>
+      <c r="F6" s="49"/>
+      <c r="G6" s="50"/>
       <c r="H6" s="17"/>
       <c r="I6" s="18"/>
     </row>
     <row r="7" spans="1:9">
-      <c r="A7" s="46"/>
-      <c r="B7" s="47"/>
-      <c r="C7" s="47"/>
-      <c r="D7" s="47"/>
-      <c r="E7" s="47"/>
-      <c r="F7" s="47"/>
-      <c r="G7" s="48"/>
+      <c r="A7" s="51"/>
+      <c r="B7" s="52"/>
+      <c r="C7" s="52"/>
+      <c r="D7" s="52"/>
+      <c r="E7" s="52"/>
+      <c r="F7" s="52"/>
+      <c r="G7" s="53"/>
       <c r="H7" s="18"/>
       <c r="I7" s="18"/>
     </row>
@@ -2129,14 +2163,14 @@
       <c r="A8" s="22" t="s">
         <v>77</v>
       </c>
-      <c r="B8" s="29" t="s">
+      <c r="B8" s="37" t="s">
         <v>69</v>
       </c>
-      <c r="C8" s="30"/>
-      <c r="D8" s="29" t="s">
+      <c r="C8" s="29"/>
+      <c r="D8" s="37" t="s">
         <v>70</v>
       </c>
-      <c r="E8" s="30"/>
+      <c r="E8" s="29"/>
       <c r="F8" s="21" t="s">
         <v>71</v>
       </c>
@@ -2144,201 +2178,239 @@
         <v>73</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="34.5" customHeight="1">
+    <row r="9" spans="1:9" ht="70.2" customHeight="1">
       <c r="A9" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="36" t="s">
+      <c r="B9" s="46" t="s">
         <v>85</v>
       </c>
-      <c r="C9" s="37"/>
-      <c r="D9" s="36" t="s">
+      <c r="C9" s="47"/>
+      <c r="D9" s="46" t="s">
+        <v>122</v>
+      </c>
+      <c r="E9" s="47"/>
+      <c r="F9" s="27" t="s">
         <v>90</v>
       </c>
-      <c r="E9" s="37"/>
-      <c r="F9" s="20"/>
-      <c r="G9" s="20"/>
+      <c r="G9" s="27" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="10" spans="1:9" ht="29.4" customHeight="1">
       <c r="A10" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="36" t="s">
+      <c r="B10" s="46" t="s">
         <v>88</v>
       </c>
-      <c r="C10" s="37"/>
-      <c r="D10" s="36" t="s">
-        <v>91</v>
-      </c>
-      <c r="E10" s="53"/>
-      <c r="F10" s="20"/>
-      <c r="G10" s="20"/>
+      <c r="C10" s="47"/>
+      <c r="D10" s="46" t="s">
+        <v>119</v>
+      </c>
+      <c r="E10" s="58"/>
+      <c r="F10" s="27" t="s">
+        <v>119</v>
+      </c>
+      <c r="G10" s="27" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="11" spans="1:9" ht="40.200000000000003" customHeight="1">
       <c r="A11" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="36" t="s">
+      <c r="B11" s="46" t="s">
         <v>89</v>
       </c>
-      <c r="C11" s="37"/>
-      <c r="D11" s="36" t="s">
+      <c r="C11" s="47"/>
+      <c r="D11" s="46" t="s">
         <v>87</v>
       </c>
-      <c r="E11" s="37"/>
-      <c r="F11" s="20"/>
-      <c r="G11" s="20"/>
+      <c r="E11" s="47"/>
+      <c r="F11" s="27" t="s">
+        <v>123</v>
+      </c>
+      <c r="G11" s="27" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="12" spans="1:9" ht="58.5" customHeight="1">
       <c r="A12" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="36" t="s">
+      <c r="B12" s="46" t="s">
         <v>92</v>
       </c>
-      <c r="C12" s="53"/>
-      <c r="D12" s="36" t="s">
+      <c r="C12" s="58"/>
+      <c r="D12" s="46" t="s">
         <v>87</v>
       </c>
-      <c r="E12" s="37"/>
-      <c r="F12" s="20"/>
-      <c r="G12" s="20"/>
+      <c r="E12" s="47"/>
+      <c r="F12" s="27" t="s">
+        <v>123</v>
+      </c>
+      <c r="G12" s="27" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="13" spans="1:9" ht="57" customHeight="1">
       <c r="A13" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="B13" s="36" t="s">
+      <c r="B13" s="46" t="s">
+        <v>120</v>
+      </c>
+      <c r="C13" s="58"/>
+      <c r="D13" s="46" t="s">
+        <v>87</v>
+      </c>
+      <c r="E13" s="47"/>
+      <c r="F13" s="27" t="s">
+        <v>123</v>
+      </c>
+      <c r="G13" s="27" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="55.95" customHeight="1">
+      <c r="A14" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" s="59" t="s">
+        <v>121</v>
+      </c>
+      <c r="C14" s="59"/>
+      <c r="D14" s="46" t="s">
+        <v>91</v>
+      </c>
+      <c r="E14" s="58"/>
+      <c r="F14" s="73" t="s">
+        <v>119</v>
+      </c>
+      <c r="G14" s="27" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="45.45" customHeight="1">
+      <c r="A15" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" s="59" t="s">
+        <v>93</v>
+      </c>
+      <c r="C15" s="59"/>
+      <c r="D15" s="46" t="s">
+        <v>87</v>
+      </c>
+      <c r="E15" s="47"/>
+      <c r="F15" s="73" t="s">
+        <v>123</v>
+      </c>
+      <c r="G15" s="27" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="45.45" customHeight="1">
+      <c r="A16" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="B16" s="59" t="s">
         <v>94</v>
       </c>
-      <c r="C13" s="53"/>
-      <c r="D13" s="36" t="s">
+      <c r="C16" s="59"/>
+      <c r="D16" s="46" t="s">
         <v>87</v>
       </c>
-      <c r="E13" s="37"/>
-      <c r="F13" s="20"/>
-      <c r="G13" s="20"/>
-    </row>
-    <row r="14" spans="1:9" ht="55.95" customHeight="1">
-      <c r="A14" s="26" t="s">
-        <v>29</v>
-      </c>
-      <c r="B14" s="36" t="s">
-        <v>93</v>
-      </c>
-      <c r="C14" s="37"/>
-      <c r="D14" s="36" t="s">
-        <v>87</v>
-      </c>
-      <c r="E14" s="37"/>
-      <c r="F14" s="20"/>
-      <c r="G14" s="20"/>
-    </row>
-    <row r="15" spans="1:9" ht="55.95" customHeight="1">
-      <c r="A15" s="28" t="s">
-        <v>30</v>
-      </c>
-      <c r="B15" s="54" t="s">
+      <c r="E16" s="47"/>
+      <c r="F16" s="73" t="s">
+        <v>123</v>
+      </c>
+      <c r="G16" s="27" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="45.45" customHeight="1">
+      <c r="A17" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="B17" s="59" t="s">
         <v>95</v>
       </c>
-      <c r="C15" s="54"/>
-      <c r="D15" s="36" t="s">
+      <c r="C17" s="59"/>
+      <c r="D17" s="46" t="s">
         <v>91</v>
       </c>
-      <c r="E15" s="53"/>
-      <c r="F15" s="27"/>
-      <c r="G15" s="20"/>
-    </row>
-    <row r="16" spans="1:9" ht="45.45" customHeight="1">
-      <c r="A16" s="28" t="s">
-        <v>39</v>
-      </c>
-      <c r="B16" s="54" t="s">
-        <v>96</v>
-      </c>
-      <c r="C16" s="54"/>
-      <c r="D16" s="36" t="s">
-        <v>87</v>
-      </c>
-      <c r="E16" s="37"/>
-      <c r="F16" s="27"/>
-      <c r="G16" s="20"/>
-    </row>
-    <row r="17" spans="1:7" ht="45.45" customHeight="1">
-      <c r="A17" s="28" t="s">
-        <v>40</v>
-      </c>
-      <c r="B17" s="54" t="s">
-        <v>97</v>
-      </c>
-      <c r="C17" s="54"/>
-      <c r="D17" s="36" t="s">
-        <v>87</v>
-      </c>
-      <c r="E17" s="37"/>
-      <c r="F17" s="27"/>
-      <c r="G17" s="20"/>
-    </row>
-    <row r="18" spans="1:7" ht="45.45" customHeight="1">
-      <c r="A18" s="28" t="s">
-        <v>41</v>
-      </c>
-      <c r="B18" s="54" t="s">
-        <v>98</v>
-      </c>
-      <c r="C18" s="54"/>
-      <c r="D18" s="36" t="s">
-        <v>91</v>
-      </c>
-      <c r="E18" s="53"/>
-      <c r="F18" s="27"/>
-      <c r="G18" s="20"/>
+      <c r="E17" s="58"/>
+      <c r="F17" s="73" t="s">
+        <v>119</v>
+      </c>
+      <c r="G17" s="27" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" s="37" t="s">
+        <v>74</v>
+      </c>
+      <c r="B18" s="29"/>
+      <c r="C18" s="34" t="s">
+        <v>112</v>
+      </c>
+      <c r="D18" s="35"/>
+      <c r="E18" s="35"/>
+      <c r="F18" s="35"/>
+      <c r="G18" s="36"/>
     </row>
     <row r="19" spans="1:7">
-      <c r="A19" s="29" t="s">
-        <v>74</v>
-      </c>
-      <c r="B19" s="30"/>
-      <c r="C19" s="31"/>
-      <c r="D19" s="32"/>
-      <c r="E19" s="32"/>
-      <c r="F19" s="32"/>
-      <c r="G19" s="33"/>
+      <c r="A19" s="37" t="s">
+        <v>75</v>
+      </c>
+      <c r="B19" s="29"/>
+      <c r="C19" s="54">
+        <v>43014</v>
+      </c>
+      <c r="D19" s="35"/>
+      <c r="E19" s="35"/>
+      <c r="F19" s="35"/>
+      <c r="G19" s="36"/>
     </row>
     <row r="20" spans="1:7">
-      <c r="A20" s="29" t="s">
-        <v>75</v>
-      </c>
-      <c r="B20" s="30"/>
-      <c r="C20" s="31"/>
-      <c r="D20" s="32"/>
-      <c r="E20" s="32"/>
-      <c r="F20" s="32"/>
-      <c r="G20" s="33"/>
+      <c r="A20" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="B20" s="29"/>
+      <c r="C20" s="34" t="s">
+        <v>124</v>
+      </c>
+      <c r="D20" s="35"/>
+      <c r="E20" s="35"/>
+      <c r="F20" s="35"/>
+      <c r="G20" s="36"/>
     </row>
     <row r="21" spans="1:7">
-      <c r="A21" s="34" t="s">
-        <v>76</v>
-      </c>
-      <c r="B21" s="30"/>
-      <c r="C21" s="31"/>
-      <c r="D21" s="32"/>
-      <c r="E21" s="32"/>
-      <c r="F21" s="32"/>
-      <c r="G21" s="33"/>
-    </row>
-    <row r="22" spans="1:7">
-      <c r="A22" s="34" t="s">
+      <c r="A21" s="28" t="s">
         <v>73</v>
       </c>
-      <c r="B22" s="35"/>
-      <c r="C22" s="31"/>
-      <c r="D22" s="32"/>
-      <c r="E22" s="32"/>
-      <c r="F22" s="32"/>
-      <c r="G22" s="33"/>
-    </row>
-    <row r="23" spans="1:7" ht="26.4" customHeight="1">
+      <c r="B21" s="33"/>
+      <c r="C21" s="34" t="s">
+        <v>106</v>
+      </c>
+      <c r="D21" s="35"/>
+      <c r="E21" s="35"/>
+      <c r="F21" s="35"/>
+      <c r="G21" s="36"/>
+    </row>
+    <row r="22" spans="1:7" ht="26.4" customHeight="1">
+      <c r="A22" s="18"/>
+      <c r="B22" s="18"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="18"/>
+    </row>
+    <row r="23" spans="1:7" ht="36" customHeight="1">
       <c r="A23" s="18"/>
       <c r="B23" s="18"/>
       <c r="C23" s="18"/>
@@ -2347,7 +2419,7 @@
       <c r="F23" s="18"/>
       <c r="G23" s="18"/>
     </row>
-    <row r="24" spans="1:7" ht="36" customHeight="1">
+    <row r="24" spans="1:7" ht="25.2" customHeight="1">
       <c r="A24" s="18"/>
       <c r="B24" s="18"/>
       <c r="C24" s="18"/>
@@ -2356,7 +2428,7 @@
       <c r="F24" s="18"/>
       <c r="G24" s="18"/>
     </row>
-    <row r="25" spans="1:7" ht="25.2" customHeight="1">
+    <row r="25" spans="1:7" ht="19.8" customHeight="1">
       <c r="A25" s="18"/>
       <c r="B25" s="18"/>
       <c r="C25" s="18"/>
@@ -2365,7 +2437,7 @@
       <c r="F25" s="18"/>
       <c r="G25" s="18"/>
     </row>
-    <row r="26" spans="1:7" ht="19.8" customHeight="1">
+    <row r="26" spans="1:7">
       <c r="A26" s="18"/>
       <c r="B26" s="18"/>
       <c r="C26" s="18"/>
@@ -2374,603 +2446,617 @@
       <c r="F26" s="18"/>
       <c r="G26" s="18"/>
     </row>
-    <row r="27" spans="1:7">
-      <c r="A27" s="18"/>
-      <c r="B27" s="18"/>
-      <c r="C27" s="18"/>
-      <c r="D27" s="18"/>
-      <c r="E27" s="18"/>
-      <c r="F27" s="18"/>
-      <c r="G27" s="18"/>
-    </row>
-    <row r="28" spans="1:7" ht="25.8" customHeight="1"/>
-    <row r="29" spans="1:7" ht="20.399999999999999" thickBot="1">
-      <c r="A29" s="49" t="s">
+    <row r="27" spans="1:7" ht="25.8" customHeight="1"/>
+    <row r="28" spans="1:7" ht="20.399999999999999" thickBot="1">
+      <c r="A28" s="55" t="s">
         <v>65</v>
       </c>
-      <c r="B29" s="49"/>
-      <c r="C29" s="49"/>
-      <c r="D29" s="49"/>
-      <c r="E29" s="49"/>
-      <c r="F29" s="49"/>
-      <c r="G29" s="49"/>
-    </row>
-    <row r="30" spans="1:7" ht="15" thickTop="1">
-      <c r="A30" s="57" t="s">
+      <c r="B28" s="55"/>
+      <c r="C28" s="55"/>
+      <c r="D28" s="55"/>
+      <c r="E28" s="55"/>
+      <c r="F28" s="55"/>
+      <c r="G28" s="55"/>
+    </row>
+    <row r="29" spans="1:7" ht="15" thickTop="1">
+      <c r="A29" s="63" t="s">
         <v>66</v>
       </c>
-      <c r="B30" s="58"/>
-      <c r="C30" s="59" t="s">
+      <c r="B29" s="64"/>
+      <c r="C29" s="65" t="s">
         <v>78</v>
       </c>
-      <c r="D30" s="60"/>
-      <c r="E30" s="60"/>
-      <c r="F30" s="60"/>
-      <c r="G30" s="61"/>
+      <c r="D29" s="66"/>
+      <c r="E29" s="66"/>
+      <c r="F29" s="66"/>
+      <c r="G29" s="67"/>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="A30" s="38" t="s">
+        <v>67</v>
+      </c>
+      <c r="B30" s="39"/>
+      <c r="C30" s="43"/>
+      <c r="D30" s="44"/>
+      <c r="E30" s="44"/>
+      <c r="F30" s="44"/>
+      <c r="G30" s="45"/>
     </row>
     <row r="31" spans="1:7">
       <c r="A31" s="38" t="s">
+        <v>68</v>
+      </c>
+      <c r="B31" s="39"/>
+      <c r="C31" s="48" t="s">
+        <v>79</v>
+      </c>
+      <c r="D31" s="68"/>
+      <c r="E31" s="68"/>
+      <c r="F31" s="68"/>
+      <c r="G31" s="69"/>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="A32" s="30"/>
+      <c r="B32" s="31"/>
+      <c r="C32" s="31"/>
+      <c r="D32" s="31"/>
+      <c r="E32" s="31"/>
+      <c r="F32" s="31"/>
+      <c r="G32" s="32"/>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="A33" s="22" t="s">
+        <v>77</v>
+      </c>
+      <c r="B33" s="37" t="s">
+        <v>69</v>
+      </c>
+      <c r="C33" s="29"/>
+      <c r="D33" s="37" t="s">
+        <v>70</v>
+      </c>
+      <c r="E33" s="29"/>
+      <c r="F33" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="G33" s="22" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="18" customHeight="1">
+      <c r="A34" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="B34" s="56" t="s">
+        <v>111</v>
+      </c>
+      <c r="C34" s="57"/>
+      <c r="D34" s="34" t="s">
+        <v>72</v>
+      </c>
+      <c r="E34" s="36"/>
+      <c r="F34" s="20" t="s">
+        <v>110</v>
+      </c>
+      <c r="G34" s="20" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="46.8" customHeight="1">
+      <c r="A35" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="B35" s="56" t="s">
+        <v>50</v>
+      </c>
+      <c r="C35" s="57"/>
+      <c r="D35" s="46" t="s">
+        <v>86</v>
+      </c>
+      <c r="E35" s="58"/>
+      <c r="F35" s="20" t="s">
+        <v>108</v>
+      </c>
+      <c r="G35" s="20" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="45.6" customHeight="1">
+      <c r="A36" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="B36" s="56" t="s">
+        <v>49</v>
+      </c>
+      <c r="C36" s="57"/>
+      <c r="D36" s="46" t="s">
+        <v>80</v>
+      </c>
+      <c r="E36" s="58"/>
+      <c r="F36" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="G36" s="20" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="48" customHeight="1">
+      <c r="A37" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="B37" s="56" t="s">
+        <v>81</v>
+      </c>
+      <c r="C37" s="57"/>
+      <c r="D37" s="46" t="s">
+        <v>82</v>
+      </c>
+      <c r="E37" s="58"/>
+      <c r="F37" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="G37" s="20" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
+      <c r="A38" s="37" t="s">
+        <v>74</v>
+      </c>
+      <c r="B38" s="29"/>
+      <c r="C38" s="34" t="s">
+        <v>112</v>
+      </c>
+      <c r="D38" s="35"/>
+      <c r="E38" s="35"/>
+      <c r="F38" s="35"/>
+      <c r="G38" s="36"/>
+    </row>
+    <row r="39" spans="1:7">
+      <c r="A39" s="37" t="s">
+        <v>75</v>
+      </c>
+      <c r="B39" s="29"/>
+      <c r="C39" s="54">
+        <v>43042</v>
+      </c>
+      <c r="D39" s="35"/>
+      <c r="E39" s="35"/>
+      <c r="F39" s="35"/>
+      <c r="G39" s="36"/>
+    </row>
+    <row r="40" spans="1:7">
+      <c r="A40" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="B40" s="33"/>
+      <c r="C40" s="34" t="s">
+        <v>113</v>
+      </c>
+      <c r="D40" s="35"/>
+      <c r="E40" s="35"/>
+      <c r="F40" s="35"/>
+      <c r="G40" s="36"/>
+    </row>
+    <row r="41" spans="1:7">
+      <c r="A41" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="B41" s="33"/>
+      <c r="C41" s="34" t="s">
+        <v>106</v>
+      </c>
+      <c r="D41" s="35"/>
+      <c r="E41" s="35"/>
+      <c r="F41" s="35"/>
+      <c r="G41" s="36"/>
+    </row>
+    <row r="45" spans="1:7" ht="20.399999999999999" thickBot="1">
+      <c r="A45" s="55" t="s">
+        <v>99</v>
+      </c>
+      <c r="B45" s="55"/>
+      <c r="C45" s="55"/>
+      <c r="D45" s="55"/>
+      <c r="E45" s="55"/>
+      <c r="F45" s="55"/>
+      <c r="G45" s="55"/>
+    </row>
+    <row r="46" spans="1:7" ht="15" thickTop="1">
+      <c r="A46" s="38" t="s">
+        <v>66</v>
+      </c>
+      <c r="B46" s="39"/>
+      <c r="C46" s="40" t="s">
+        <v>96</v>
+      </c>
+      <c r="D46" s="41"/>
+      <c r="E46" s="41"/>
+      <c r="F46" s="41"/>
+      <c r="G46" s="42"/>
+    </row>
+    <row r="47" spans="1:7">
+      <c r="A47" s="38" t="s">
         <v>67</v>
       </c>
-      <c r="B31" s="39"/>
-      <c r="C31" s="40"/>
-      <c r="D31" s="41"/>
-      <c r="E31" s="41"/>
-      <c r="F31" s="41"/>
-      <c r="G31" s="42"/>
-    </row>
-    <row r="32" spans="1:7">
-      <c r="A32" s="38" t="s">
-        <v>68</v>
-      </c>
-      <c r="B32" s="39"/>
-      <c r="C32" s="43" t="s">
-        <v>79</v>
-      </c>
-      <c r="D32" s="62"/>
-      <c r="E32" s="62"/>
-      <c r="F32" s="62"/>
-      <c r="G32" s="63"/>
-    </row>
-    <row r="33" spans="1:7">
-      <c r="A33" s="31"/>
-      <c r="B33" s="32"/>
-      <c r="C33" s="32"/>
-      <c r="D33" s="32"/>
-      <c r="E33" s="32"/>
-      <c r="F33" s="32"/>
-      <c r="G33" s="33"/>
-    </row>
-    <row r="34" spans="1:7">
-      <c r="A34" s="22" t="s">
-        <v>77</v>
-      </c>
-      <c r="B34" s="29" t="s">
-        <v>69</v>
-      </c>
-      <c r="C34" s="30"/>
-      <c r="D34" s="29" t="s">
-        <v>70</v>
-      </c>
-      <c r="E34" s="30"/>
-      <c r="F34" s="21" t="s">
-        <v>71</v>
-      </c>
-      <c r="G34" s="22" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" ht="18" customHeight="1">
-      <c r="A35" s="23" t="s">
-        <v>5</v>
-      </c>
-      <c r="B35" s="55" t="s">
-        <v>114</v>
-      </c>
-      <c r="C35" s="56"/>
-      <c r="D35" s="67" t="s">
-        <v>72</v>
-      </c>
-      <c r="E35" s="68"/>
-      <c r="F35" s="20" t="s">
-        <v>113</v>
-      </c>
-      <c r="G35" s="20" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" ht="46.8" customHeight="1">
-      <c r="A36" s="26" t="s">
-        <v>6</v>
-      </c>
-      <c r="B36" s="55" t="s">
-        <v>50</v>
-      </c>
-      <c r="C36" s="56"/>
-      <c r="D36" s="36" t="s">
-        <v>86</v>
-      </c>
-      <c r="E36" s="53"/>
-      <c r="F36" s="20" t="s">
-        <v>111</v>
-      </c>
-      <c r="G36" s="20" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" ht="45.6" customHeight="1">
-      <c r="A37" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="B37" s="55" t="s">
-        <v>49</v>
-      </c>
-      <c r="C37" s="56"/>
-      <c r="D37" s="36" t="s">
-        <v>80</v>
-      </c>
-      <c r="E37" s="53"/>
-      <c r="F37" s="20" t="s">
-        <v>112</v>
-      </c>
-      <c r="G37" s="20" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" ht="48" customHeight="1">
-      <c r="A38" s="26" t="s">
-        <v>8</v>
-      </c>
-      <c r="B38" s="55" t="s">
-        <v>81</v>
-      </c>
-      <c r="C38" s="56"/>
-      <c r="D38" s="36" t="s">
-        <v>82</v>
-      </c>
-      <c r="E38" s="53"/>
-      <c r="F38" s="20" t="s">
-        <v>110</v>
-      </c>
-      <c r="G38" s="20" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7">
-      <c r="A39" s="29" t="s">
-        <v>74</v>
-      </c>
-      <c r="B39" s="30"/>
-      <c r="C39" s="67" t="s">
-        <v>115</v>
-      </c>
-      <c r="D39" s="69"/>
-      <c r="E39" s="69"/>
-      <c r="F39" s="69"/>
-      <c r="G39" s="68"/>
-    </row>
-    <row r="40" spans="1:7">
-      <c r="A40" s="29" t="s">
-        <v>75</v>
-      </c>
-      <c r="B40" s="30"/>
-      <c r="C40" s="70">
-        <v>43042</v>
-      </c>
-      <c r="D40" s="69"/>
-      <c r="E40" s="69"/>
-      <c r="F40" s="69"/>
-      <c r="G40" s="68"/>
-    </row>
-    <row r="41" spans="1:7">
-      <c r="A41" s="34" t="s">
-        <v>76</v>
-      </c>
-      <c r="B41" s="35"/>
-      <c r="C41" s="67" t="s">
-        <v>116</v>
-      </c>
-      <c r="D41" s="69"/>
-      <c r="E41" s="69"/>
-      <c r="F41" s="69"/>
-      <c r="G41" s="68"/>
-    </row>
-    <row r="42" spans="1:7">
-      <c r="A42" s="34" t="s">
-        <v>73</v>
-      </c>
-      <c r="B42" s="35"/>
-      <c r="C42" s="67" t="s">
-        <v>109</v>
-      </c>
-      <c r="D42" s="69"/>
-      <c r="E42" s="69"/>
-      <c r="F42" s="69"/>
-      <c r="G42" s="68"/>
-    </row>
-    <row r="46" spans="1:7" ht="20.399999999999999" thickBot="1">
-      <c r="A46" s="49" t="s">
-        <v>102</v>
-      </c>
-      <c r="B46" s="49"/>
-      <c r="C46" s="49"/>
-      <c r="D46" s="49"/>
-      <c r="E46" s="49"/>
-      <c r="F46" s="49"/>
-      <c r="G46" s="49"/>
-    </row>
-    <row r="47" spans="1:7" ht="15" thickTop="1">
-      <c r="A47" s="38" t="s">
-        <v>66</v>
-      </c>
       <c r="B47" s="39"/>
-      <c r="C47" s="50" t="s">
-        <v>99</v>
-      </c>
-      <c r="D47" s="51"/>
-      <c r="E47" s="51"/>
-      <c r="F47" s="51"/>
-      <c r="G47" s="52"/>
+      <c r="C47" s="43"/>
+      <c r="D47" s="44"/>
+      <c r="E47" s="44"/>
+      <c r="F47" s="44"/>
+      <c r="G47" s="45"/>
     </row>
     <row r="48" spans="1:7">
       <c r="A48" s="38" t="s">
+        <v>68</v>
+      </c>
+      <c r="B48" s="39"/>
+      <c r="C48" s="48" t="s">
+        <v>97</v>
+      </c>
+      <c r="D48" s="49"/>
+      <c r="E48" s="49"/>
+      <c r="F48" s="49"/>
+      <c r="G48" s="50"/>
+    </row>
+    <row r="49" spans="1:7" ht="16.8" customHeight="1">
+      <c r="A49" s="51"/>
+      <c r="B49" s="52"/>
+      <c r="C49" s="52"/>
+      <c r="D49" s="52"/>
+      <c r="E49" s="52"/>
+      <c r="F49" s="52"/>
+      <c r="G49" s="53"/>
+    </row>
+    <row r="50" spans="1:7" ht="63" customHeight="1">
+      <c r="A50" s="22" t="s">
+        <v>77</v>
+      </c>
+      <c r="B50" s="37" t="s">
+        <v>69</v>
+      </c>
+      <c r="C50" s="29"/>
+      <c r="D50" s="37" t="s">
+        <v>70</v>
+      </c>
+      <c r="E50" s="29"/>
+      <c r="F50" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="G50" s="22" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" ht="54" customHeight="1">
+      <c r="A51" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="B51" s="46" t="s">
+        <v>100</v>
+      </c>
+      <c r="C51" s="47"/>
+      <c r="D51" s="46" t="s">
+        <v>98</v>
+      </c>
+      <c r="E51" s="47"/>
+      <c r="F51" s="20"/>
+      <c r="G51" s="20"/>
+    </row>
+    <row r="52" spans="1:7" ht="27" customHeight="1">
+      <c r="A52" s="28" t="s">
+        <v>74</v>
+      </c>
+      <c r="B52" s="29"/>
+      <c r="C52" s="34" t="s">
+        <v>112</v>
+      </c>
+      <c r="D52" s="35"/>
+      <c r="E52" s="35"/>
+      <c r="F52" s="35"/>
+      <c r="G52" s="36"/>
+    </row>
+    <row r="53" spans="1:7" ht="34.799999999999997" customHeight="1">
+      <c r="A53" s="37" t="s">
+        <v>75</v>
+      </c>
+      <c r="B53" s="29"/>
+      <c r="C53" s="30"/>
+      <c r="D53" s="31"/>
+      <c r="E53" s="31"/>
+      <c r="F53" s="31"/>
+      <c r="G53" s="32"/>
+    </row>
+    <row r="54" spans="1:7" ht="25.2" customHeight="1">
+      <c r="A54" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="B54" s="29"/>
+      <c r="C54" s="30"/>
+      <c r="D54" s="31"/>
+      <c r="E54" s="31"/>
+      <c r="F54" s="31"/>
+      <c r="G54" s="32"/>
+    </row>
+    <row r="55" spans="1:7">
+      <c r="A55" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="B55" s="33"/>
+      <c r="C55" s="30"/>
+      <c r="D55" s="31"/>
+      <c r="E55" s="31"/>
+      <c r="F55" s="31"/>
+      <c r="G55" s="32"/>
+    </row>
+    <row r="58" spans="1:7" ht="20.399999999999999" thickBot="1">
+      <c r="A58" s="55" t="s">
+        <v>102</v>
+      </c>
+      <c r="B58" s="55"/>
+      <c r="C58" s="55"/>
+      <c r="D58" s="55"/>
+      <c r="E58" s="55"/>
+      <c r="F58" s="55"/>
+      <c r="G58" s="55"/>
+    </row>
+    <row r="59" spans="1:7" ht="15" thickTop="1">
+      <c r="A59" s="38" t="s">
+        <v>66</v>
+      </c>
+      <c r="B59" s="39"/>
+      <c r="C59" s="40" t="s">
+        <v>103</v>
+      </c>
+      <c r="D59" s="41"/>
+      <c r="E59" s="41"/>
+      <c r="F59" s="41"/>
+      <c r="G59" s="42"/>
+    </row>
+    <row r="60" spans="1:7">
+      <c r="A60" s="38" t="s">
         <v>67</v>
       </c>
-      <c r="B48" s="39"/>
-      <c r="C48" s="40"/>
-      <c r="D48" s="41"/>
-      <c r="E48" s="41"/>
-      <c r="F48" s="41"/>
-      <c r="G48" s="42"/>
-    </row>
-    <row r="49" spans="1:7">
-      <c r="A49" s="38" t="s">
-        <v>68</v>
-      </c>
-      <c r="B49" s="39"/>
-      <c r="C49" s="43" t="s">
-        <v>100</v>
-      </c>
-      <c r="D49" s="44"/>
-      <c r="E49" s="44"/>
-      <c r="F49" s="44"/>
-      <c r="G49" s="45"/>
-    </row>
-    <row r="50" spans="1:7" ht="31.8" customHeight="1">
-      <c r="A50" s="46"/>
-      <c r="B50" s="47"/>
-      <c r="C50" s="47"/>
-      <c r="D50" s="47"/>
-      <c r="E50" s="47"/>
-      <c r="F50" s="47"/>
-      <c r="G50" s="48"/>
-    </row>
-    <row r="51" spans="1:7" ht="63" customHeight="1">
-      <c r="A51" s="22" t="s">
-        <v>77</v>
-      </c>
-      <c r="B51" s="29" t="s">
-        <v>69</v>
-      </c>
-      <c r="C51" s="30"/>
-      <c r="D51" s="29" t="s">
-        <v>70</v>
-      </c>
-      <c r="E51" s="30"/>
-      <c r="F51" s="21" t="s">
-        <v>71</v>
-      </c>
-      <c r="G51" s="22" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" ht="54" customHeight="1">
-      <c r="A52" s="26" t="s">
-        <v>5</v>
-      </c>
-      <c r="B52" s="36" t="s">
-        <v>103</v>
-      </c>
-      <c r="C52" s="37"/>
-      <c r="D52" s="36" t="s">
-        <v>101</v>
-      </c>
-      <c r="E52" s="37"/>
-      <c r="F52" s="20"/>
-      <c r="G52" s="20"/>
-    </row>
-    <row r="53" spans="1:7" ht="27" customHeight="1">
-      <c r="A53" s="34" t="s">
-        <v>74</v>
-      </c>
-      <c r="B53" s="30"/>
-      <c r="C53" s="67" t="s">
-        <v>115</v>
-      </c>
-      <c r="D53" s="69"/>
-      <c r="E53" s="69"/>
-      <c r="F53" s="69"/>
-      <c r="G53" s="68"/>
-    </row>
-    <row r="54" spans="1:7" ht="34.799999999999997" customHeight="1">
-      <c r="A54" s="29" t="s">
-        <v>75</v>
-      </c>
-      <c r="B54" s="30"/>
-      <c r="C54" s="31"/>
-      <c r="D54" s="32"/>
-      <c r="E54" s="32"/>
-      <c r="F54" s="32"/>
-      <c r="G54" s="33"/>
-    </row>
-    <row r="55" spans="1:7" ht="25.2" customHeight="1">
-      <c r="A55" s="34" t="s">
-        <v>76</v>
-      </c>
-      <c r="B55" s="30"/>
-      <c r="C55" s="31"/>
-      <c r="D55" s="32"/>
-      <c r="E55" s="32"/>
-      <c r="F55" s="32"/>
-      <c r="G55" s="33"/>
-    </row>
-    <row r="56" spans="1:7">
-      <c r="A56" s="34" t="s">
-        <v>73</v>
-      </c>
-      <c r="B56" s="35"/>
-      <c r="C56" s="31"/>
-      <c r="D56" s="32"/>
-      <c r="E56" s="32"/>
-      <c r="F56" s="32"/>
-      <c r="G56" s="33"/>
-    </row>
-    <row r="59" spans="1:7" ht="20.399999999999999" thickBot="1">
-      <c r="A59" s="49" t="s">
-        <v>105</v>
-      </c>
-      <c r="B59" s="49"/>
-      <c r="C59" s="49"/>
-      <c r="D59" s="49"/>
-      <c r="E59" s="49"/>
-      <c r="F59" s="49"/>
-      <c r="G59" s="49"/>
-    </row>
-    <row r="60" spans="1:7" ht="15" thickTop="1">
-      <c r="A60" s="38" t="s">
-        <v>66</v>
-      </c>
       <c r="B60" s="39"/>
-      <c r="C60" s="50" t="s">
-        <v>106</v>
-      </c>
-      <c r="D60" s="51"/>
-      <c r="E60" s="51"/>
-      <c r="F60" s="51"/>
-      <c r="G60" s="52"/>
+      <c r="C60" s="43"/>
+      <c r="D60" s="44"/>
+      <c r="E60" s="44"/>
+      <c r="F60" s="44"/>
+      <c r="G60" s="45"/>
     </row>
     <row r="61" spans="1:7">
       <c r="A61" s="38" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B61" s="39"/>
-      <c r="C61" s="40"/>
-      <c r="D61" s="41"/>
-      <c r="E61" s="41"/>
-      <c r="F61" s="41"/>
-      <c r="G61" s="42"/>
+      <c r="C61" s="48" t="s">
+        <v>101</v>
+      </c>
+      <c r="D61" s="49"/>
+      <c r="E61" s="49"/>
+      <c r="F61" s="49"/>
+      <c r="G61" s="50"/>
     </row>
     <row r="62" spans="1:7">
-      <c r="A62" s="38" t="s">
-        <v>68</v>
-      </c>
-      <c r="B62" s="39"/>
-      <c r="C62" s="43" t="s">
+      <c r="A62" s="51"/>
+      <c r="B62" s="52"/>
+      <c r="C62" s="52"/>
+      <c r="D62" s="52"/>
+      <c r="E62" s="52"/>
+      <c r="F62" s="52"/>
+      <c r="G62" s="53"/>
+    </row>
+    <row r="63" spans="1:7">
+      <c r="A63" s="22" t="s">
+        <v>77</v>
+      </c>
+      <c r="B63" s="37" t="s">
+        <v>69</v>
+      </c>
+      <c r="C63" s="29"/>
+      <c r="D63" s="37" t="s">
+        <v>70</v>
+      </c>
+      <c r="E63" s="29"/>
+      <c r="F63" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="G63" s="22" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" ht="82.2" customHeight="1">
+      <c r="A64" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="B64" s="46" t="s">
         <v>104</v>
       </c>
-      <c r="D62" s="44"/>
-      <c r="E62" s="44"/>
-      <c r="F62" s="44"/>
-      <c r="G62" s="45"/>
-    </row>
-    <row r="63" spans="1:7">
-      <c r="A63" s="46"/>
-      <c r="B63" s="47"/>
-      <c r="C63" s="47"/>
-      <c r="D63" s="47"/>
-      <c r="E63" s="47"/>
-      <c r="F63" s="47"/>
-      <c r="G63" s="48"/>
-    </row>
-    <row r="64" spans="1:7">
-      <c r="A64" s="22" t="s">
-        <v>77</v>
-      </c>
-      <c r="B64" s="29" t="s">
-        <v>69</v>
-      </c>
-      <c r="C64" s="30"/>
-      <c r="D64" s="29" t="s">
-        <v>70</v>
-      </c>
-      <c r="E64" s="30"/>
-      <c r="F64" s="21" t="s">
-        <v>71</v>
-      </c>
-      <c r="G64" s="22" t="s">
+      <c r="C64" s="47"/>
+      <c r="D64" s="46" t="s">
+        <v>105</v>
+      </c>
+      <c r="E64" s="47"/>
+      <c r="F64" s="74" t="s">
+        <v>125</v>
+      </c>
+      <c r="G64" s="74" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" ht="56.4" customHeight="1">
+      <c r="A65" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="B65" s="46" t="s">
+        <v>114</v>
+      </c>
+      <c r="C65" s="47"/>
+      <c r="D65" s="46" t="s">
+        <v>115</v>
+      </c>
+      <c r="E65" s="47"/>
+      <c r="F65" s="74" t="s">
+        <v>126</v>
+      </c>
+      <c r="G65" s="74" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" ht="49.8" customHeight="1">
+      <c r="A66" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="B66" s="46" t="s">
+        <v>116</v>
+      </c>
+      <c r="C66" s="47"/>
+      <c r="D66" s="46" t="s">
+        <v>117</v>
+      </c>
+      <c r="E66" s="47"/>
+      <c r="F66" s="74" t="s">
+        <v>127</v>
+      </c>
+      <c r="G66" s="74" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" ht="63.6" customHeight="1">
+      <c r="A67" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="B67" s="46" t="s">
+        <v>129</v>
+      </c>
+      <c r="C67" s="47"/>
+      <c r="D67" s="46" t="s">
+        <v>118</v>
+      </c>
+      <c r="E67" s="47"/>
+      <c r="F67" s="74" t="s">
+        <v>128</v>
+      </c>
+      <c r="G67" s="74" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" ht="79.2" customHeight="1">
+      <c r="A68" s="26" t="s">
+        <v>28</v>
+      </c>
+      <c r="B68" s="46" t="s">
+        <v>131</v>
+      </c>
+      <c r="C68" s="47"/>
+      <c r="D68" s="46" t="s">
+        <v>130</v>
+      </c>
+      <c r="E68" s="47"/>
+      <c r="F68" s="74" t="s">
+        <v>132</v>
+      </c>
+      <c r="G68" s="74" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7">
+      <c r="A69" s="28" t="s">
+        <v>74</v>
+      </c>
+      <c r="B69" s="29"/>
+      <c r="C69" s="34" t="s">
+        <v>112</v>
+      </c>
+      <c r="D69" s="35"/>
+      <c r="E69" s="35"/>
+      <c r="F69" s="35"/>
+      <c r="G69" s="36"/>
+    </row>
+    <row r="70" spans="1:7">
+      <c r="A70" s="37" t="s">
+        <v>75</v>
+      </c>
+      <c r="B70" s="29"/>
+      <c r="C70" s="54">
+        <v>43014</v>
+      </c>
+      <c r="D70" s="35"/>
+      <c r="E70" s="35"/>
+      <c r="F70" s="35"/>
+      <c r="G70" s="36"/>
+    </row>
+    <row r="71" spans="1:7">
+      <c r="A71" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="B71" s="29"/>
+      <c r="C71" s="34" t="s">
+        <v>133</v>
+      </c>
+      <c r="D71" s="35"/>
+      <c r="E71" s="35"/>
+      <c r="F71" s="35"/>
+      <c r="G71" s="36"/>
+    </row>
+    <row r="72" spans="1:7">
+      <c r="A72" s="28" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="65" spans="1:7" ht="82.2" customHeight="1">
-      <c r="A65" s="26" t="s">
-        <v>5</v>
-      </c>
-      <c r="B65" s="36" t="s">
-        <v>107</v>
-      </c>
-      <c r="C65" s="37"/>
-      <c r="D65" s="36" t="s">
-        <v>108</v>
-      </c>
-      <c r="E65" s="37"/>
-      <c r="F65" s="20"/>
-      <c r="G65" s="20"/>
-    </row>
-    <row r="66" spans="1:7" ht="56.4" customHeight="1">
-      <c r="A66" s="26" t="s">
-        <v>6</v>
-      </c>
-      <c r="B66" s="36" t="s">
-        <v>117</v>
-      </c>
-      <c r="C66" s="37"/>
-      <c r="D66" s="36" t="s">
-        <v>118</v>
-      </c>
-      <c r="E66" s="37"/>
-      <c r="F66" s="20"/>
-      <c r="G66" s="20"/>
-    </row>
-    <row r="67" spans="1:7" ht="49.8" customHeight="1">
-      <c r="A67" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="B67" s="36" t="s">
-        <v>119</v>
-      </c>
-      <c r="C67" s="37"/>
-      <c r="D67" s="36" t="s">
-        <v>121</v>
-      </c>
-      <c r="E67" s="37"/>
-      <c r="F67" s="20"/>
-      <c r="G67" s="20"/>
-    </row>
-    <row r="68" spans="1:7" ht="41.4" customHeight="1">
-      <c r="A68" s="26" t="s">
-        <v>8</v>
-      </c>
-      <c r="B68" s="36" t="s">
-        <v>120</v>
-      </c>
-      <c r="C68" s="37"/>
-      <c r="D68" s="36" t="s">
-        <v>122</v>
-      </c>
-      <c r="E68" s="37"/>
-      <c r="F68" s="20"/>
-      <c r="G68" s="20"/>
-    </row>
-    <row r="69" spans="1:7" ht="46.8" customHeight="1">
-      <c r="A69" s="26" t="s">
-        <v>28</v>
-      </c>
-      <c r="B69" s="36" t="s">
-        <v>123</v>
-      </c>
-      <c r="C69" s="37"/>
-      <c r="D69" s="36" t="s">
-        <v>122</v>
-      </c>
-      <c r="E69" s="37"/>
-      <c r="F69" s="20"/>
-      <c r="G69" s="20"/>
-    </row>
-    <row r="70" spans="1:7">
-      <c r="A70" s="34" t="s">
-        <v>74</v>
-      </c>
-      <c r="B70" s="30"/>
-      <c r="C70" s="31"/>
-      <c r="D70" s="32"/>
-      <c r="E70" s="32"/>
-      <c r="F70" s="32"/>
-      <c r="G70" s="33"/>
-    </row>
-    <row r="71" spans="1:7">
-      <c r="A71" s="29" t="s">
-        <v>75</v>
-      </c>
-      <c r="B71" s="30"/>
-      <c r="C71" s="31"/>
-      <c r="D71" s="32"/>
-      <c r="E71" s="32"/>
-      <c r="F71" s="32"/>
-      <c r="G71" s="33"/>
-    </row>
-    <row r="72" spans="1:7">
-      <c r="A72" s="34" t="s">
-        <v>76</v>
-      </c>
-      <c r="B72" s="30"/>
-      <c r="C72" s="31"/>
-      <c r="D72" s="32"/>
-      <c r="E72" s="32"/>
-      <c r="F72" s="32"/>
-      <c r="G72" s="33"/>
-    </row>
-    <row r="73" spans="1:7">
-      <c r="A73" s="34" t="s">
-        <v>73</v>
-      </c>
-      <c r="B73" s="35"/>
-      <c r="C73" s="31"/>
-      <c r="D73" s="32"/>
-      <c r="E73" s="32"/>
-      <c r="F73" s="32"/>
-      <c r="G73" s="33"/>
+      <c r="B72" s="33"/>
+      <c r="C72" s="34" t="s">
+        <v>106</v>
+      </c>
+      <c r="D72" s="35"/>
+      <c r="E72" s="35"/>
+      <c r="F72" s="35"/>
+      <c r="G72" s="36"/>
     </row>
   </sheetData>
-  <mergeCells count="113">
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="C55:G55"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="C56:G56"/>
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="C53:G53"/>
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="C54:G54"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="C47:G47"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="C48:G48"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="D52:E52"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="C49:G49"/>
-    <mergeCell ref="A50:G50"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="D51:E51"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="C39:G39"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="C40:G40"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="C41:G41"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="C42:G42"/>
-    <mergeCell ref="A46:G46"/>
-    <mergeCell ref="A33:G33"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="D34:E34"/>
+  <mergeCells count="111">
+    <mergeCell ref="A70:B70"/>
+    <mergeCell ref="C70:G70"/>
+    <mergeCell ref="A71:B71"/>
+    <mergeCell ref="C71:G71"/>
+    <mergeCell ref="A72:B72"/>
+    <mergeCell ref="C72:G72"/>
+    <mergeCell ref="B63:C63"/>
+    <mergeCell ref="D63:E63"/>
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="D64:E64"/>
+    <mergeCell ref="A69:B69"/>
+    <mergeCell ref="C69:G69"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="D65:E65"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="D66:E66"/>
+    <mergeCell ref="B67:C67"/>
+    <mergeCell ref="D67:E67"/>
+    <mergeCell ref="B68:C68"/>
+    <mergeCell ref="D68:E68"/>
+    <mergeCell ref="A60:B60"/>
+    <mergeCell ref="C60:G60"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="C61:G61"/>
+    <mergeCell ref="A62:G62"/>
+    <mergeCell ref="A58:G58"/>
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="C59:G59"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="C21:G21"/>
     <mergeCell ref="B35:C35"/>
     <mergeCell ref="D35:E35"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="C20:G20"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="A28:G28"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="C29:G29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="C30:G30"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="C31:G31"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="B13:C13"/>
     <mergeCell ref="B12:C12"/>
@@ -2991,50 +3077,53 @@
     <mergeCell ref="D10:E10"/>
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="D11:E11"/>
-    <mergeCell ref="A61:B61"/>
-    <mergeCell ref="C61:G61"/>
-    <mergeCell ref="A62:B62"/>
-    <mergeCell ref="C62:G62"/>
-    <mergeCell ref="A63:G63"/>
-    <mergeCell ref="A59:G59"/>
-    <mergeCell ref="A60:B60"/>
-    <mergeCell ref="C60:G60"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="C21:G21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="C22:G22"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="A32:G32"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="D34:E34"/>
     <mergeCell ref="B36:C36"/>
     <mergeCell ref="D36:E36"/>
-    <mergeCell ref="A29:G29"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="C30:G30"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="C31:G31"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="C32:G32"/>
-    <mergeCell ref="A71:B71"/>
-    <mergeCell ref="C71:G71"/>
-    <mergeCell ref="A72:B72"/>
-    <mergeCell ref="C72:G72"/>
-    <mergeCell ref="A73:B73"/>
-    <mergeCell ref="C73:G73"/>
-    <mergeCell ref="B64:C64"/>
-    <mergeCell ref="D64:E64"/>
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="D65:E65"/>
-    <mergeCell ref="A70:B70"/>
-    <mergeCell ref="C70:G70"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="D66:E66"/>
-    <mergeCell ref="B67:C67"/>
-    <mergeCell ref="D67:E67"/>
-    <mergeCell ref="B68:C68"/>
-    <mergeCell ref="D68:E68"/>
-    <mergeCell ref="B69:C69"/>
-    <mergeCell ref="D69:E69"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="C38:G38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="C39:G39"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="C40:G40"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="C41:G41"/>
+    <mergeCell ref="A45:G45"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="C54:G54"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="C55:G55"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="C52:G52"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="C53:G53"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="C46:G46"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="C47:G47"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="D51:E51"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="C48:G48"/>
+    <mergeCell ref="A49:G49"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="D50:E50"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
@@ -3045,7 +3134,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A4:I24"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
@@ -3064,17 +3153,17 @@
   </cols>
   <sheetData>
     <row r="4" spans="1:9" ht="18">
-      <c r="A4" s="71" t="s">
+      <c r="A4" s="70" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="72"/>
-      <c r="C4" s="72"/>
-      <c r="D4" s="72"/>
-      <c r="E4" s="72"/>
-      <c r="F4" s="72"/>
-      <c r="G4" s="72"/>
-      <c r="H4" s="72"/>
-      <c r="I4" s="73"/>
+      <c r="B4" s="71"/>
+      <c r="C4" s="71"/>
+      <c r="D4" s="71"/>
+      <c r="E4" s="71"/>
+      <c r="F4" s="71"/>
+      <c r="G4" s="71"/>
+      <c r="H4" s="71"/>
+      <c r="I4" s="72"/>
     </row>
     <row r="5" spans="1:9" s="4" customFormat="1">
       <c r="A5" s="2" t="s">
@@ -3194,17 +3283,17 @@
       <c r="I9" s="9"/>
     </row>
     <row r="13" spans="1:9" ht="18">
-      <c r="A13" s="71" t="s">
+      <c r="A13" s="70" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="72"/>
-      <c r="C13" s="72"/>
-      <c r="D13" s="72"/>
-      <c r="E13" s="72"/>
-      <c r="F13" s="72"/>
-      <c r="G13" s="72"/>
-      <c r="H13" s="72"/>
-      <c r="I13" s="73"/>
+      <c r="B13" s="71"/>
+      <c r="C13" s="71"/>
+      <c r="D13" s="71"/>
+      <c r="E13" s="71"/>
+      <c r="F13" s="71"/>
+      <c r="G13" s="71"/>
+      <c r="H13" s="71"/>
+      <c r="I13" s="72"/>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="2" t="s">

</xml_diff>

<commit_message>
Made small changes to homepage
</commit_message>
<xml_diff>
--- a/FYP documentation/FYP_Test_Plan.xlsx
+++ b/FYP documentation/FYP_Test_Plan.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="137">
   <si>
     <t>Expected Result</t>
   </si>
@@ -455,6 +455,15 @@
   </si>
   <si>
     <t>1439 hrs</t>
+  </si>
+  <si>
+    <t>File operation</t>
+  </si>
+  <si>
+    <t>Test if file operation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add area 1 and area 2. Area 2 should have file 1 and file 2 </t>
   </si>
 </sst>
 </file>
@@ -845,11 +854,128 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="6" xfId="3" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="13" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="15" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="7" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="8" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="12" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -860,117 +986,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="6" xfId="3" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="7" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="8" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="12" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="13" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="15" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -979,12 +994,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -2051,10 +2060,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I72"/>
+  <dimension ref="A1:I90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView tabSelected="1" topLeftCell="A73" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C79" sqref="C79:G79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2071,15 +2080,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="40.799999999999997" customHeight="1">
-      <c r="A1" s="60" t="s">
+      <c r="A1" s="66" t="s">
         <v>64</v>
       </c>
-      <c r="B1" s="61"/>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="61"/>
-      <c r="F1" s="61"/>
-      <c r="G1" s="62"/>
+      <c r="B1" s="67"/>
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
+      <c r="F1" s="67"/>
+      <c r="G1" s="68"/>
       <c r="H1" s="16"/>
       <c r="I1" s="16"/>
     </row>
@@ -2095,67 +2104,67 @@
       <c r="I2" s="19"/>
     </row>
     <row r="3" spans="1:9" ht="31.2" customHeight="1" thickBot="1">
-      <c r="A3" s="55" t="s">
+      <c r="A3" s="51" t="s">
         <v>83</v>
       </c>
-      <c r="B3" s="55"/>
-      <c r="C3" s="55"/>
-      <c r="D3" s="55"/>
-      <c r="E3" s="55"/>
-      <c r="F3" s="55"/>
-      <c r="G3" s="55"/>
+      <c r="B3" s="51"/>
+      <c r="C3" s="51"/>
+      <c r="D3" s="51"/>
+      <c r="E3" s="51"/>
+      <c r="F3" s="51"/>
+      <c r="G3" s="51"/>
       <c r="H3" s="16"/>
       <c r="I3" s="16"/>
     </row>
     <row r="4" spans="1:9" ht="18.600000000000001" customHeight="1" thickTop="1">
-      <c r="A4" s="38" t="s">
+      <c r="A4" s="40" t="s">
         <v>66</v>
       </c>
-      <c r="B4" s="39"/>
-      <c r="C4" s="40" t="s">
+      <c r="B4" s="41"/>
+      <c r="C4" s="52" t="s">
         <v>84</v>
       </c>
-      <c r="D4" s="41"/>
-      <c r="E4" s="41"/>
-      <c r="F4" s="41"/>
-      <c r="G4" s="42"/>
+      <c r="D4" s="53"/>
+      <c r="E4" s="53"/>
+      <c r="F4" s="53"/>
+      <c r="G4" s="54"/>
       <c r="H4" s="17"/>
       <c r="I4" s="17"/>
     </row>
     <row r="5" spans="1:9" ht="14.4" customHeight="1">
-      <c r="A5" s="38" t="s">
+      <c r="A5" s="40" t="s">
         <v>67</v>
       </c>
-      <c r="B5" s="39"/>
-      <c r="C5" s="43"/>
-      <c r="D5" s="44"/>
-      <c r="E5" s="44"/>
-      <c r="F5" s="44"/>
-      <c r="G5" s="45"/>
+      <c r="B5" s="41"/>
+      <c r="C5" s="42"/>
+      <c r="D5" s="43"/>
+      <c r="E5" s="43"/>
+      <c r="F5" s="43"/>
+      <c r="G5" s="44"/>
       <c r="H5" s="16"/>
       <c r="I5" s="16"/>
     </row>
     <row r="6" spans="1:9" ht="14.4" customHeight="1">
-      <c r="A6" s="38" t="s">
+      <c r="A6" s="40" t="s">
         <v>68</v>
       </c>
-      <c r="B6" s="39"/>
-      <c r="C6" s="48"/>
-      <c r="D6" s="49"/>
-      <c r="E6" s="49"/>
-      <c r="F6" s="49"/>
-      <c r="G6" s="50"/>
+      <c r="B6" s="41"/>
+      <c r="C6" s="45"/>
+      <c r="D6" s="46"/>
+      <c r="E6" s="46"/>
+      <c r="F6" s="46"/>
+      <c r="G6" s="47"/>
       <c r="H6" s="17"/>
       <c r="I6" s="18"/>
     </row>
     <row r="7" spans="1:9">
-      <c r="A7" s="51"/>
-      <c r="B7" s="52"/>
-      <c r="C7" s="52"/>
-      <c r="D7" s="52"/>
-      <c r="E7" s="52"/>
-      <c r="F7" s="52"/>
-      <c r="G7" s="53"/>
+      <c r="A7" s="48"/>
+      <c r="B7" s="49"/>
+      <c r="C7" s="49"/>
+      <c r="D7" s="49"/>
+      <c r="E7" s="49"/>
+      <c r="F7" s="49"/>
+      <c r="G7" s="50"/>
       <c r="H7" s="18"/>
       <c r="I7" s="18"/>
     </row>
@@ -2163,14 +2172,14 @@
       <c r="A8" s="22" t="s">
         <v>77</v>
       </c>
-      <c r="B8" s="37" t="s">
+      <c r="B8" s="30" t="s">
         <v>69</v>
       </c>
-      <c r="C8" s="29"/>
-      <c r="D8" s="37" t="s">
+      <c r="C8" s="31"/>
+      <c r="D8" s="30" t="s">
         <v>70</v>
       </c>
-      <c r="E8" s="29"/>
+      <c r="E8" s="31"/>
       <c r="F8" s="21" t="s">
         <v>71</v>
       </c>
@@ -2182,14 +2191,14 @@
       <c r="A9" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="46" t="s">
+      <c r="B9" s="38" t="s">
         <v>85</v>
       </c>
-      <c r="C9" s="47"/>
-      <c r="D9" s="46" t="s">
+      <c r="C9" s="39"/>
+      <c r="D9" s="38" t="s">
         <v>122</v>
       </c>
-      <c r="E9" s="47"/>
+      <c r="E9" s="39"/>
       <c r="F9" s="27" t="s">
         <v>90</v>
       </c>
@@ -2201,14 +2210,14 @@
       <c r="A10" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="46" t="s">
+      <c r="B10" s="38" t="s">
         <v>88</v>
       </c>
-      <c r="C10" s="47"/>
-      <c r="D10" s="46" t="s">
+      <c r="C10" s="39"/>
+      <c r="D10" s="38" t="s">
         <v>119</v>
       </c>
-      <c r="E10" s="58"/>
+      <c r="E10" s="55"/>
       <c r="F10" s="27" t="s">
         <v>119</v>
       </c>
@@ -2220,14 +2229,14 @@
       <c r="A11" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="46" t="s">
+      <c r="B11" s="38" t="s">
         <v>89</v>
       </c>
-      <c r="C11" s="47"/>
-      <c r="D11" s="46" t="s">
+      <c r="C11" s="39"/>
+      <c r="D11" s="38" t="s">
         <v>87</v>
       </c>
-      <c r="E11" s="47"/>
+      <c r="E11" s="39"/>
       <c r="F11" s="27" t="s">
         <v>123</v>
       </c>
@@ -2239,14 +2248,14 @@
       <c r="A12" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="46" t="s">
+      <c r="B12" s="38" t="s">
         <v>92</v>
       </c>
-      <c r="C12" s="58"/>
-      <c r="D12" s="46" t="s">
+      <c r="C12" s="55"/>
+      <c r="D12" s="38" t="s">
         <v>87</v>
       </c>
-      <c r="E12" s="47"/>
+      <c r="E12" s="39"/>
       <c r="F12" s="27" t="s">
         <v>123</v>
       </c>
@@ -2258,14 +2267,14 @@
       <c r="A13" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="B13" s="46" t="s">
+      <c r="B13" s="38" t="s">
         <v>120</v>
       </c>
-      <c r="C13" s="58"/>
-      <c r="D13" s="46" t="s">
+      <c r="C13" s="55"/>
+      <c r="D13" s="38" t="s">
         <v>87</v>
       </c>
-      <c r="E13" s="47"/>
+      <c r="E13" s="39"/>
       <c r="F13" s="27" t="s">
         <v>123</v>
       </c>
@@ -2277,15 +2286,15 @@
       <c r="A14" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="B14" s="59" t="s">
+      <c r="B14" s="56" t="s">
         <v>121</v>
       </c>
-      <c r="C14" s="59"/>
-      <c r="D14" s="46" t="s">
+      <c r="C14" s="56"/>
+      <c r="D14" s="38" t="s">
         <v>91</v>
       </c>
-      <c r="E14" s="58"/>
-      <c r="F14" s="73" t="s">
+      <c r="E14" s="55"/>
+      <c r="F14" s="28" t="s">
         <v>119</v>
       </c>
       <c r="G14" s="27" t="s">
@@ -2296,15 +2305,15 @@
       <c r="A15" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="B15" s="59" t="s">
+      <c r="B15" s="56" t="s">
         <v>93</v>
       </c>
-      <c r="C15" s="59"/>
-      <c r="D15" s="46" t="s">
+      <c r="C15" s="56"/>
+      <c r="D15" s="38" t="s">
         <v>87</v>
       </c>
-      <c r="E15" s="47"/>
-      <c r="F15" s="73" t="s">
+      <c r="E15" s="39"/>
+      <c r="F15" s="28" t="s">
         <v>123</v>
       </c>
       <c r="G15" s="27" t="s">
@@ -2315,15 +2324,15 @@
       <c r="A16" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="B16" s="59" t="s">
+      <c r="B16" s="56" t="s">
         <v>94</v>
       </c>
-      <c r="C16" s="59"/>
-      <c r="D16" s="46" t="s">
+      <c r="C16" s="56"/>
+      <c r="D16" s="38" t="s">
         <v>87</v>
       </c>
-      <c r="E16" s="47"/>
-      <c r="F16" s="73" t="s">
+      <c r="E16" s="39"/>
+      <c r="F16" s="28" t="s">
         <v>123</v>
       </c>
       <c r="G16" s="27" t="s">
@@ -2334,15 +2343,15 @@
       <c r="A17" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="B17" s="59" t="s">
+      <c r="B17" s="56" t="s">
         <v>95</v>
       </c>
-      <c r="C17" s="59"/>
-      <c r="D17" s="46" t="s">
+      <c r="C17" s="56"/>
+      <c r="D17" s="38" t="s">
         <v>91</v>
       </c>
-      <c r="E17" s="58"/>
-      <c r="F17" s="73" t="s">
+      <c r="E17" s="55"/>
+      <c r="F17" s="28" t="s">
         <v>119</v>
       </c>
       <c r="G17" s="27" t="s">
@@ -2350,58 +2359,58 @@
       </c>
     </row>
     <row r="18" spans="1:7">
-      <c r="A18" s="37" t="s">
+      <c r="A18" s="30" t="s">
         <v>74</v>
       </c>
-      <c r="B18" s="29"/>
-      <c r="C18" s="34" t="s">
+      <c r="B18" s="31"/>
+      <c r="C18" s="36" t="s">
         <v>112</v>
       </c>
-      <c r="D18" s="35"/>
-      <c r="E18" s="35"/>
-      <c r="F18" s="35"/>
-      <c r="G18" s="36"/>
+      <c r="D18" s="33"/>
+      <c r="E18" s="33"/>
+      <c r="F18" s="33"/>
+      <c r="G18" s="34"/>
     </row>
     <row r="19" spans="1:7">
-      <c r="A19" s="37" t="s">
+      <c r="A19" s="30" t="s">
         <v>75</v>
       </c>
-      <c r="B19" s="29"/>
-      <c r="C19" s="54">
+      <c r="B19" s="31"/>
+      <c r="C19" s="32">
         <v>43014</v>
       </c>
-      <c r="D19" s="35"/>
-      <c r="E19" s="35"/>
-      <c r="F19" s="35"/>
-      <c r="G19" s="36"/>
+      <c r="D19" s="33"/>
+      <c r="E19" s="33"/>
+      <c r="F19" s="33"/>
+      <c r="G19" s="34"/>
     </row>
     <row r="20" spans="1:7">
-      <c r="A20" s="28" t="s">
+      <c r="A20" s="35" t="s">
         <v>76</v>
       </c>
-      <c r="B20" s="29"/>
-      <c r="C20" s="34" t="s">
+      <c r="B20" s="31"/>
+      <c r="C20" s="36" t="s">
         <v>124</v>
       </c>
-      <c r="D20" s="35"/>
-      <c r="E20" s="35"/>
-      <c r="F20" s="35"/>
-      <c r="G20" s="36"/>
+      <c r="D20" s="33"/>
+      <c r="E20" s="33"/>
+      <c r="F20" s="33"/>
+      <c r="G20" s="34"/>
     </row>
     <row r="21" spans="1:7">
-      <c r="A21" s="28" t="s">
+      <c r="A21" s="35" t="s">
         <v>73</v>
       </c>
-      <c r="B21" s="33"/>
-      <c r="C21" s="34" t="s">
+      <c r="B21" s="37"/>
+      <c r="C21" s="36" t="s">
         <v>106</v>
       </c>
-      <c r="D21" s="35"/>
-      <c r="E21" s="35"/>
-      <c r="F21" s="35"/>
-      <c r="G21" s="36"/>
-    </row>
-    <row r="22" spans="1:7" ht="26.4" customHeight="1">
+      <c r="D21" s="33"/>
+      <c r="E21" s="33"/>
+      <c r="F21" s="33"/>
+      <c r="G21" s="34"/>
+    </row>
+    <row r="22" spans="1:7" ht="14.4" customHeight="1">
       <c r="A22" s="18"/>
       <c r="B22" s="18"/>
       <c r="C22" s="18"/>
@@ -2410,7 +2419,7 @@
       <c r="F22" s="18"/>
       <c r="G22" s="18"/>
     </row>
-    <row r="23" spans="1:7" ht="36" customHeight="1">
+    <row r="23" spans="1:7" ht="10.8" customHeight="1">
       <c r="A23" s="18"/>
       <c r="B23" s="18"/>
       <c r="C23" s="18"/>
@@ -2419,7 +2428,7 @@
       <c r="F23" s="18"/>
       <c r="G23" s="18"/>
     </row>
-    <row r="24" spans="1:7" ht="25.2" customHeight="1">
+    <row r="24" spans="1:7" ht="15.6" customHeight="1">
       <c r="A24" s="18"/>
       <c r="B24" s="18"/>
       <c r="C24" s="18"/>
@@ -2428,7 +2437,7 @@
       <c r="F24" s="18"/>
       <c r="G24" s="18"/>
     </row>
-    <row r="25" spans="1:7" ht="19.8" customHeight="1">
+    <row r="25" spans="1:7" ht="14.4" customHeight="1">
       <c r="A25" s="18"/>
       <c r="B25" s="18"/>
       <c r="C25" s="18"/>
@@ -2446,76 +2455,76 @@
       <c r="F26" s="18"/>
       <c r="G26" s="18"/>
     </row>
-    <row r="27" spans="1:7" ht="25.8" customHeight="1"/>
+    <row r="27" spans="1:7" ht="12" customHeight="1"/>
     <row r="28" spans="1:7" ht="20.399999999999999" thickBot="1">
-      <c r="A28" s="55" t="s">
+      <c r="A28" s="51" t="s">
         <v>65</v>
       </c>
-      <c r="B28" s="55"/>
-      <c r="C28" s="55"/>
-      <c r="D28" s="55"/>
-      <c r="E28" s="55"/>
-      <c r="F28" s="55"/>
-      <c r="G28" s="55"/>
+      <c r="B28" s="51"/>
+      <c r="C28" s="51"/>
+      <c r="D28" s="51"/>
+      <c r="E28" s="51"/>
+      <c r="F28" s="51"/>
+      <c r="G28" s="51"/>
     </row>
     <row r="29" spans="1:7" ht="15" thickTop="1">
-      <c r="A29" s="63" t="s">
+      <c r="A29" s="59" t="s">
         <v>66</v>
       </c>
-      <c r="B29" s="64"/>
-      <c r="C29" s="65" t="s">
+      <c r="B29" s="60"/>
+      <c r="C29" s="61" t="s">
         <v>78</v>
       </c>
-      <c r="D29" s="66"/>
-      <c r="E29" s="66"/>
-      <c r="F29" s="66"/>
-      <c r="G29" s="67"/>
+      <c r="D29" s="62"/>
+      <c r="E29" s="62"/>
+      <c r="F29" s="62"/>
+      <c r="G29" s="63"/>
     </row>
     <row r="30" spans="1:7">
-      <c r="A30" s="38" t="s">
+      <c r="A30" s="40" t="s">
         <v>67</v>
       </c>
-      <c r="B30" s="39"/>
-      <c r="C30" s="43"/>
-      <c r="D30" s="44"/>
-      <c r="E30" s="44"/>
-      <c r="F30" s="44"/>
-      <c r="G30" s="45"/>
+      <c r="B30" s="41"/>
+      <c r="C30" s="42"/>
+      <c r="D30" s="43"/>
+      <c r="E30" s="43"/>
+      <c r="F30" s="43"/>
+      <c r="G30" s="44"/>
     </row>
     <row r="31" spans="1:7">
-      <c r="A31" s="38" t="s">
+      <c r="A31" s="40" t="s">
         <v>68</v>
       </c>
-      <c r="B31" s="39"/>
-      <c r="C31" s="48" t="s">
+      <c r="B31" s="41"/>
+      <c r="C31" s="45" t="s">
         <v>79</v>
       </c>
-      <c r="D31" s="68"/>
-      <c r="E31" s="68"/>
-      <c r="F31" s="68"/>
-      <c r="G31" s="69"/>
+      <c r="D31" s="64"/>
+      <c r="E31" s="64"/>
+      <c r="F31" s="64"/>
+      <c r="G31" s="65"/>
     </row>
     <row r="32" spans="1:7">
-      <c r="A32" s="30"/>
-      <c r="B32" s="31"/>
-      <c r="C32" s="31"/>
-      <c r="D32" s="31"/>
-      <c r="E32" s="31"/>
-      <c r="F32" s="31"/>
-      <c r="G32" s="32"/>
+      <c r="A32" s="69"/>
+      <c r="B32" s="70"/>
+      <c r="C32" s="70"/>
+      <c r="D32" s="70"/>
+      <c r="E32" s="70"/>
+      <c r="F32" s="70"/>
+      <c r="G32" s="71"/>
     </row>
     <row r="33" spans="1:7">
       <c r="A33" s="22" t="s">
         <v>77</v>
       </c>
-      <c r="B33" s="37" t="s">
+      <c r="B33" s="30" t="s">
         <v>69</v>
       </c>
-      <c r="C33" s="29"/>
-      <c r="D33" s="37" t="s">
+      <c r="C33" s="31"/>
+      <c r="D33" s="30" t="s">
         <v>70</v>
       </c>
-      <c r="E33" s="29"/>
+      <c r="E33" s="31"/>
       <c r="F33" s="21" t="s">
         <v>71</v>
       </c>
@@ -2527,14 +2536,14 @@
       <c r="A34" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="B34" s="56" t="s">
+      <c r="B34" s="57" t="s">
         <v>111</v>
       </c>
-      <c r="C34" s="57"/>
-      <c r="D34" s="34" t="s">
+      <c r="C34" s="58"/>
+      <c r="D34" s="36" t="s">
         <v>72</v>
       </c>
-      <c r="E34" s="36"/>
+      <c r="E34" s="34"/>
       <c r="F34" s="20" t="s">
         <v>110</v>
       </c>
@@ -2546,14 +2555,14 @@
       <c r="A35" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="B35" s="56" t="s">
+      <c r="B35" s="57" t="s">
         <v>50</v>
       </c>
-      <c r="C35" s="57"/>
-      <c r="D35" s="46" t="s">
+      <c r="C35" s="58"/>
+      <c r="D35" s="38" t="s">
         <v>86</v>
       </c>
-      <c r="E35" s="58"/>
+      <c r="E35" s="55"/>
       <c r="F35" s="20" t="s">
         <v>108</v>
       </c>
@@ -2565,14 +2574,14 @@
       <c r="A36" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="B36" s="56" t="s">
+      <c r="B36" s="57" t="s">
         <v>49</v>
       </c>
-      <c r="C36" s="57"/>
-      <c r="D36" s="46" t="s">
+      <c r="C36" s="58"/>
+      <c r="D36" s="38" t="s">
         <v>80</v>
       </c>
-      <c r="E36" s="58"/>
+      <c r="E36" s="55"/>
       <c r="F36" s="20" t="s">
         <v>109</v>
       </c>
@@ -2584,14 +2593,14 @@
       <c r="A37" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="B37" s="56" t="s">
+      <c r="B37" s="57" t="s">
         <v>81</v>
       </c>
-      <c r="C37" s="57"/>
-      <c r="D37" s="46" t="s">
+      <c r="C37" s="58"/>
+      <c r="D37" s="38" t="s">
         <v>82</v>
       </c>
-      <c r="E37" s="58"/>
+      <c r="E37" s="55"/>
       <c r="F37" s="20" t="s">
         <v>107</v>
       </c>
@@ -2600,126 +2609,126 @@
       </c>
     </row>
     <row r="38" spans="1:7">
-      <c r="A38" s="37" t="s">
+      <c r="A38" s="30" t="s">
         <v>74</v>
       </c>
-      <c r="B38" s="29"/>
-      <c r="C38" s="34" t="s">
+      <c r="B38" s="31"/>
+      <c r="C38" s="36" t="s">
         <v>112</v>
       </c>
-      <c r="D38" s="35"/>
-      <c r="E38" s="35"/>
-      <c r="F38" s="35"/>
-      <c r="G38" s="36"/>
+      <c r="D38" s="33"/>
+      <c r="E38" s="33"/>
+      <c r="F38" s="33"/>
+      <c r="G38" s="34"/>
     </row>
     <row r="39" spans="1:7">
-      <c r="A39" s="37" t="s">
+      <c r="A39" s="30" t="s">
         <v>75</v>
       </c>
-      <c r="B39" s="29"/>
-      <c r="C39" s="54">
+      <c r="B39" s="31"/>
+      <c r="C39" s="32">
         <v>43042</v>
       </c>
-      <c r="D39" s="35"/>
-      <c r="E39" s="35"/>
-      <c r="F39" s="35"/>
-      <c r="G39" s="36"/>
+      <c r="D39" s="33"/>
+      <c r="E39" s="33"/>
+      <c r="F39" s="33"/>
+      <c r="G39" s="34"/>
     </row>
     <row r="40" spans="1:7">
-      <c r="A40" s="28" t="s">
+      <c r="A40" s="35" t="s">
         <v>76</v>
       </c>
-      <c r="B40" s="33"/>
-      <c r="C40" s="34" t="s">
+      <c r="B40" s="37"/>
+      <c r="C40" s="36" t="s">
         <v>113</v>
       </c>
-      <c r="D40" s="35"/>
-      <c r="E40" s="35"/>
-      <c r="F40" s="35"/>
-      <c r="G40" s="36"/>
+      <c r="D40" s="33"/>
+      <c r="E40" s="33"/>
+      <c r="F40" s="33"/>
+      <c r="G40" s="34"/>
     </row>
     <row r="41" spans="1:7">
-      <c r="A41" s="28" t="s">
+      <c r="A41" s="35" t="s">
         <v>73</v>
       </c>
-      <c r="B41" s="33"/>
-      <c r="C41" s="34" t="s">
+      <c r="B41" s="37"/>
+      <c r="C41" s="36" t="s">
         <v>106</v>
       </c>
-      <c r="D41" s="35"/>
-      <c r="E41" s="35"/>
-      <c r="F41" s="35"/>
-      <c r="G41" s="36"/>
+      <c r="D41" s="33"/>
+      <c r="E41" s="33"/>
+      <c r="F41" s="33"/>
+      <c r="G41" s="34"/>
     </row>
     <row r="45" spans="1:7" ht="20.399999999999999" thickBot="1">
-      <c r="A45" s="55" t="s">
+      <c r="A45" s="51" t="s">
         <v>99</v>
       </c>
-      <c r="B45" s="55"/>
-      <c r="C45" s="55"/>
-      <c r="D45" s="55"/>
-      <c r="E45" s="55"/>
-      <c r="F45" s="55"/>
-      <c r="G45" s="55"/>
+      <c r="B45" s="51"/>
+      <c r="C45" s="51"/>
+      <c r="D45" s="51"/>
+      <c r="E45" s="51"/>
+      <c r="F45" s="51"/>
+      <c r="G45" s="51"/>
     </row>
     <row r="46" spans="1:7" ht="15" thickTop="1">
-      <c r="A46" s="38" t="s">
+      <c r="A46" s="40" t="s">
         <v>66</v>
       </c>
-      <c r="B46" s="39"/>
-      <c r="C46" s="40" t="s">
+      <c r="B46" s="41"/>
+      <c r="C46" s="52" t="s">
         <v>96</v>
       </c>
-      <c r="D46" s="41"/>
-      <c r="E46" s="41"/>
-      <c r="F46" s="41"/>
-      <c r="G46" s="42"/>
+      <c r="D46" s="53"/>
+      <c r="E46" s="53"/>
+      <c r="F46" s="53"/>
+      <c r="G46" s="54"/>
     </row>
     <row r="47" spans="1:7">
-      <c r="A47" s="38" t="s">
+      <c r="A47" s="40" t="s">
         <v>67</v>
       </c>
-      <c r="B47" s="39"/>
-      <c r="C47" s="43"/>
-      <c r="D47" s="44"/>
-      <c r="E47" s="44"/>
-      <c r="F47" s="44"/>
-      <c r="G47" s="45"/>
+      <c r="B47" s="41"/>
+      <c r="C47" s="42"/>
+      <c r="D47" s="43"/>
+      <c r="E47" s="43"/>
+      <c r="F47" s="43"/>
+      <c r="G47" s="44"/>
     </row>
     <row r="48" spans="1:7">
-      <c r="A48" s="38" t="s">
+      <c r="A48" s="40" t="s">
         <v>68</v>
       </c>
-      <c r="B48" s="39"/>
-      <c r="C48" s="48" t="s">
+      <c r="B48" s="41"/>
+      <c r="C48" s="45" t="s">
         <v>97</v>
       </c>
-      <c r="D48" s="49"/>
-      <c r="E48" s="49"/>
-      <c r="F48" s="49"/>
-      <c r="G48" s="50"/>
+      <c r="D48" s="46"/>
+      <c r="E48" s="46"/>
+      <c r="F48" s="46"/>
+      <c r="G48" s="47"/>
     </row>
     <row r="49" spans="1:7" ht="16.8" customHeight="1">
-      <c r="A49" s="51"/>
-      <c r="B49" s="52"/>
-      <c r="C49" s="52"/>
-      <c r="D49" s="52"/>
-      <c r="E49" s="52"/>
-      <c r="F49" s="52"/>
-      <c r="G49" s="53"/>
+      <c r="A49" s="48"/>
+      <c r="B49" s="49"/>
+      <c r="C49" s="49"/>
+      <c r="D49" s="49"/>
+      <c r="E49" s="49"/>
+      <c r="F49" s="49"/>
+      <c r="G49" s="50"/>
     </row>
     <row r="50" spans="1:7" ht="63" customHeight="1">
       <c r="A50" s="22" t="s">
         <v>77</v>
       </c>
-      <c r="B50" s="37" t="s">
+      <c r="B50" s="30" t="s">
         <v>69</v>
       </c>
-      <c r="C50" s="29"/>
-      <c r="D50" s="37" t="s">
+      <c r="C50" s="31"/>
+      <c r="D50" s="30" t="s">
         <v>70</v>
       </c>
-      <c r="E50" s="29"/>
+      <c r="E50" s="31"/>
       <c r="F50" s="21" t="s">
         <v>71</v>
       </c>
@@ -2731,132 +2740,132 @@
       <c r="A51" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="B51" s="46" t="s">
+      <c r="B51" s="38" t="s">
         <v>100</v>
       </c>
-      <c r="C51" s="47"/>
-      <c r="D51" s="46" t="s">
+      <c r="C51" s="39"/>
+      <c r="D51" s="38" t="s">
         <v>98</v>
       </c>
-      <c r="E51" s="47"/>
+      <c r="E51" s="39"/>
       <c r="F51" s="20"/>
       <c r="G51" s="20"/>
     </row>
     <row r="52" spans="1:7" ht="27" customHeight="1">
-      <c r="A52" s="28" t="s">
+      <c r="A52" s="35" t="s">
         <v>74</v>
       </c>
-      <c r="B52" s="29"/>
-      <c r="C52" s="34" t="s">
+      <c r="B52" s="31"/>
+      <c r="C52" s="36" t="s">
         <v>112</v>
       </c>
-      <c r="D52" s="35"/>
-      <c r="E52" s="35"/>
-      <c r="F52" s="35"/>
-      <c r="G52" s="36"/>
+      <c r="D52" s="33"/>
+      <c r="E52" s="33"/>
+      <c r="F52" s="33"/>
+      <c r="G52" s="34"/>
     </row>
     <row r="53" spans="1:7" ht="34.799999999999997" customHeight="1">
-      <c r="A53" s="37" t="s">
+      <c r="A53" s="30" t="s">
         <v>75</v>
       </c>
-      <c r="B53" s="29"/>
-      <c r="C53" s="30"/>
-      <c r="D53" s="31"/>
-      <c r="E53" s="31"/>
-      <c r="F53" s="31"/>
-      <c r="G53" s="32"/>
+      <c r="B53" s="31"/>
+      <c r="C53" s="69"/>
+      <c r="D53" s="70"/>
+      <c r="E53" s="70"/>
+      <c r="F53" s="70"/>
+      <c r="G53" s="71"/>
     </row>
     <row r="54" spans="1:7" ht="25.2" customHeight="1">
-      <c r="A54" s="28" t="s">
+      <c r="A54" s="35" t="s">
         <v>76</v>
       </c>
-      <c r="B54" s="29"/>
-      <c r="C54" s="30"/>
-      <c r="D54" s="31"/>
-      <c r="E54" s="31"/>
-      <c r="F54" s="31"/>
-      <c r="G54" s="32"/>
+      <c r="B54" s="31"/>
+      <c r="C54" s="69"/>
+      <c r="D54" s="70"/>
+      <c r="E54" s="70"/>
+      <c r="F54" s="70"/>
+      <c r="G54" s="71"/>
     </row>
     <row r="55" spans="1:7">
-      <c r="A55" s="28" t="s">
+      <c r="A55" s="35" t="s">
         <v>73</v>
       </c>
-      <c r="B55" s="33"/>
-      <c r="C55" s="30"/>
-      <c r="D55" s="31"/>
-      <c r="E55" s="31"/>
-      <c r="F55" s="31"/>
-      <c r="G55" s="32"/>
+      <c r="B55" s="37"/>
+      <c r="C55" s="69"/>
+      <c r="D55" s="70"/>
+      <c r="E55" s="70"/>
+      <c r="F55" s="70"/>
+      <c r="G55" s="71"/>
     </row>
     <row r="58" spans="1:7" ht="20.399999999999999" thickBot="1">
-      <c r="A58" s="55" t="s">
+      <c r="A58" s="51" t="s">
         <v>102</v>
       </c>
-      <c r="B58" s="55"/>
-      <c r="C58" s="55"/>
-      <c r="D58" s="55"/>
-      <c r="E58" s="55"/>
-      <c r="F58" s="55"/>
-      <c r="G58" s="55"/>
+      <c r="B58" s="51"/>
+      <c r="C58" s="51"/>
+      <c r="D58" s="51"/>
+      <c r="E58" s="51"/>
+      <c r="F58" s="51"/>
+      <c r="G58" s="51"/>
     </row>
     <row r="59" spans="1:7" ht="15" thickTop="1">
-      <c r="A59" s="38" t="s">
+      <c r="A59" s="40" t="s">
         <v>66</v>
       </c>
-      <c r="B59" s="39"/>
-      <c r="C59" s="40" t="s">
+      <c r="B59" s="41"/>
+      <c r="C59" s="52" t="s">
         <v>103</v>
       </c>
-      <c r="D59" s="41"/>
-      <c r="E59" s="41"/>
-      <c r="F59" s="41"/>
-      <c r="G59" s="42"/>
+      <c r="D59" s="53"/>
+      <c r="E59" s="53"/>
+      <c r="F59" s="53"/>
+      <c r="G59" s="54"/>
     </row>
     <row r="60" spans="1:7">
-      <c r="A60" s="38" t="s">
+      <c r="A60" s="40" t="s">
         <v>67</v>
       </c>
-      <c r="B60" s="39"/>
-      <c r="C60" s="43"/>
-      <c r="D60" s="44"/>
-      <c r="E60" s="44"/>
-      <c r="F60" s="44"/>
-      <c r="G60" s="45"/>
+      <c r="B60" s="41"/>
+      <c r="C60" s="42"/>
+      <c r="D60" s="43"/>
+      <c r="E60" s="43"/>
+      <c r="F60" s="43"/>
+      <c r="G60" s="44"/>
     </row>
     <row r="61" spans="1:7">
-      <c r="A61" s="38" t="s">
+      <c r="A61" s="40" t="s">
         <v>68</v>
       </c>
-      <c r="B61" s="39"/>
-      <c r="C61" s="48" t="s">
+      <c r="B61" s="41"/>
+      <c r="C61" s="45" t="s">
         <v>101</v>
       </c>
-      <c r="D61" s="49"/>
-      <c r="E61" s="49"/>
-      <c r="F61" s="49"/>
-      <c r="G61" s="50"/>
+      <c r="D61" s="46"/>
+      <c r="E61" s="46"/>
+      <c r="F61" s="46"/>
+      <c r="G61" s="47"/>
     </row>
     <row r="62" spans="1:7">
-      <c r="A62" s="51"/>
-      <c r="B62" s="52"/>
-      <c r="C62" s="52"/>
-      <c r="D62" s="52"/>
-      <c r="E62" s="52"/>
-      <c r="F62" s="52"/>
-      <c r="G62" s="53"/>
+      <c r="A62" s="48"/>
+      <c r="B62" s="49"/>
+      <c r="C62" s="49"/>
+      <c r="D62" s="49"/>
+      <c r="E62" s="49"/>
+      <c r="F62" s="49"/>
+      <c r="G62" s="50"/>
     </row>
     <row r="63" spans="1:7">
       <c r="A63" s="22" t="s">
         <v>77</v>
       </c>
-      <c r="B63" s="37" t="s">
+      <c r="B63" s="30" t="s">
         <v>69</v>
       </c>
-      <c r="C63" s="29"/>
-      <c r="D63" s="37" t="s">
+      <c r="C63" s="31"/>
+      <c r="D63" s="30" t="s">
         <v>70</v>
       </c>
-      <c r="E63" s="29"/>
+      <c r="E63" s="31"/>
       <c r="F63" s="21" t="s">
         <v>71</v>
       </c>
@@ -2868,18 +2877,18 @@
       <c r="A64" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="B64" s="46" t="s">
+      <c r="B64" s="38" t="s">
         <v>104</v>
       </c>
-      <c r="C64" s="47"/>
-      <c r="D64" s="46" t="s">
+      <c r="C64" s="39"/>
+      <c r="D64" s="38" t="s">
         <v>105</v>
       </c>
-      <c r="E64" s="47"/>
-      <c r="F64" s="74" t="s">
+      <c r="E64" s="39"/>
+      <c r="F64" s="29" t="s">
         <v>125</v>
       </c>
-      <c r="G64" s="74" t="s">
+      <c r="G64" s="29" t="s">
         <v>106</v>
       </c>
     </row>
@@ -2887,18 +2896,18 @@
       <c r="A65" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="B65" s="46" t="s">
+      <c r="B65" s="38" t="s">
         <v>114</v>
       </c>
-      <c r="C65" s="47"/>
-      <c r="D65" s="46" t="s">
+      <c r="C65" s="39"/>
+      <c r="D65" s="38" t="s">
         <v>115</v>
       </c>
-      <c r="E65" s="47"/>
-      <c r="F65" s="74" t="s">
+      <c r="E65" s="39"/>
+      <c r="F65" s="29" t="s">
         <v>126</v>
       </c>
-      <c r="G65" s="74" t="s">
+      <c r="G65" s="29" t="s">
         <v>106</v>
       </c>
     </row>
@@ -2906,18 +2915,18 @@
       <c r="A66" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="B66" s="46" t="s">
+      <c r="B66" s="38" t="s">
         <v>116</v>
       </c>
-      <c r="C66" s="47"/>
-      <c r="D66" s="46" t="s">
+      <c r="C66" s="39"/>
+      <c r="D66" s="38" t="s">
         <v>117</v>
       </c>
-      <c r="E66" s="47"/>
-      <c r="F66" s="74" t="s">
+      <c r="E66" s="39"/>
+      <c r="F66" s="29" t="s">
         <v>127</v>
       </c>
-      <c r="G66" s="74" t="s">
+      <c r="G66" s="29" t="s">
         <v>106</v>
       </c>
     </row>
@@ -2925,18 +2934,18 @@
       <c r="A67" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="B67" s="46" t="s">
+      <c r="B67" s="38" t="s">
         <v>129</v>
       </c>
-      <c r="C67" s="47"/>
-      <c r="D67" s="46" t="s">
+      <c r="C67" s="39"/>
+      <c r="D67" s="38" t="s">
         <v>118</v>
       </c>
-      <c r="E67" s="47"/>
-      <c r="F67" s="74" t="s">
+      <c r="E67" s="39"/>
+      <c r="F67" s="29" t="s">
         <v>128</v>
       </c>
-      <c r="G67" s="74" t="s">
+      <c r="G67" s="29" t="s">
         <v>106</v>
       </c>
     </row>
@@ -2944,95 +2953,393 @@
       <c r="A68" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="B68" s="46" t="s">
+      <c r="B68" s="38" t="s">
         <v>131</v>
       </c>
-      <c r="C68" s="47"/>
-      <c r="D68" s="46" t="s">
+      <c r="C68" s="39"/>
+      <c r="D68" s="38" t="s">
         <v>130</v>
       </c>
-      <c r="E68" s="47"/>
-      <c r="F68" s="74" t="s">
+      <c r="E68" s="39"/>
+      <c r="F68" s="29" t="s">
         <v>132</v>
       </c>
-      <c r="G68" s="74" t="s">
+      <c r="G68" s="29" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="69" spans="1:7">
-      <c r="A69" s="28" t="s">
+      <c r="A69" s="35" t="s">
         <v>74</v>
       </c>
-      <c r="B69" s="29"/>
-      <c r="C69" s="34" t="s">
+      <c r="B69" s="31"/>
+      <c r="C69" s="36" t="s">
         <v>112</v>
       </c>
-      <c r="D69" s="35"/>
-      <c r="E69" s="35"/>
-      <c r="F69" s="35"/>
-      <c r="G69" s="36"/>
+      <c r="D69" s="33"/>
+      <c r="E69" s="33"/>
+      <c r="F69" s="33"/>
+      <c r="G69" s="34"/>
     </row>
     <row r="70" spans="1:7">
-      <c r="A70" s="37" t="s">
+      <c r="A70" s="30" t="s">
         <v>75</v>
       </c>
-      <c r="B70" s="29"/>
-      <c r="C70" s="54">
+      <c r="B70" s="31"/>
+      <c r="C70" s="32">
         <v>43014</v>
       </c>
-      <c r="D70" s="35"/>
-      <c r="E70" s="35"/>
-      <c r="F70" s="35"/>
-      <c r="G70" s="36"/>
+      <c r="D70" s="33"/>
+      <c r="E70" s="33"/>
+      <c r="F70" s="33"/>
+      <c r="G70" s="34"/>
     </row>
     <row r="71" spans="1:7">
-      <c r="A71" s="28" t="s">
+      <c r="A71" s="35" t="s">
         <v>76</v>
       </c>
-      <c r="B71" s="29"/>
-      <c r="C71" s="34" t="s">
+      <c r="B71" s="31"/>
+      <c r="C71" s="36" t="s">
         <v>133</v>
       </c>
-      <c r="D71" s="35"/>
-      <c r="E71" s="35"/>
-      <c r="F71" s="35"/>
-      <c r="G71" s="36"/>
+      <c r="D71" s="33"/>
+      <c r="E71" s="33"/>
+      <c r="F71" s="33"/>
+      <c r="G71" s="34"/>
     </row>
     <row r="72" spans="1:7">
-      <c r="A72" s="28" t="s">
+      <c r="A72" s="35" t="s">
         <v>73</v>
       </c>
-      <c r="B72" s="33"/>
-      <c r="C72" s="34" t="s">
+      <c r="B72" s="37"/>
+      <c r="C72" s="36" t="s">
         <v>106</v>
       </c>
-      <c r="D72" s="35"/>
-      <c r="E72" s="35"/>
-      <c r="F72" s="35"/>
-      <c r="G72" s="36"/>
+      <c r="D72" s="33"/>
+      <c r="E72" s="33"/>
+      <c r="F72" s="33"/>
+      <c r="G72" s="34"/>
+    </row>
+    <row r="76" spans="1:7" ht="20.399999999999999" thickBot="1">
+      <c r="A76" s="51" t="s">
+        <v>134</v>
+      </c>
+      <c r="B76" s="51"/>
+      <c r="C76" s="51"/>
+      <c r="D76" s="51"/>
+      <c r="E76" s="51"/>
+      <c r="F76" s="51"/>
+      <c r="G76" s="51"/>
+    </row>
+    <row r="77" spans="1:7" ht="15" thickTop="1">
+      <c r="A77" s="40" t="s">
+        <v>66</v>
+      </c>
+      <c r="B77" s="41"/>
+      <c r="C77" s="52" t="s">
+        <v>135</v>
+      </c>
+      <c r="D77" s="53"/>
+      <c r="E77" s="53"/>
+      <c r="F77" s="53"/>
+      <c r="G77" s="54"/>
+    </row>
+    <row r="78" spans="1:7">
+      <c r="A78" s="40" t="s">
+        <v>67</v>
+      </c>
+      <c r="B78" s="41"/>
+      <c r="C78" s="42"/>
+      <c r="D78" s="43"/>
+      <c r="E78" s="43"/>
+      <c r="F78" s="43"/>
+      <c r="G78" s="44"/>
+    </row>
+    <row r="79" spans="1:7">
+      <c r="A79" s="40" t="s">
+        <v>68</v>
+      </c>
+      <c r="B79" s="41"/>
+      <c r="C79" s="45" t="s">
+        <v>136</v>
+      </c>
+      <c r="D79" s="46"/>
+      <c r="E79" s="46"/>
+      <c r="F79" s="46"/>
+      <c r="G79" s="47"/>
+    </row>
+    <row r="80" spans="1:7">
+      <c r="A80" s="48"/>
+      <c r="B80" s="49"/>
+      <c r="C80" s="49"/>
+      <c r="D80" s="49"/>
+      <c r="E80" s="49"/>
+      <c r="F80" s="49"/>
+      <c r="G80" s="50"/>
+    </row>
+    <row r="81" spans="1:7">
+      <c r="A81" s="22" t="s">
+        <v>77</v>
+      </c>
+      <c r="B81" s="30" t="s">
+        <v>69</v>
+      </c>
+      <c r="C81" s="31"/>
+      <c r="D81" s="30" t="s">
+        <v>70</v>
+      </c>
+      <c r="E81" s="31"/>
+      <c r="F81" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="G81" s="22" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7">
+      <c r="A82" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="B82" s="38" t="s">
+        <v>104</v>
+      </c>
+      <c r="C82" s="39"/>
+      <c r="D82" s="38" t="s">
+        <v>105</v>
+      </c>
+      <c r="E82" s="39"/>
+      <c r="F82" s="29" t="s">
+        <v>125</v>
+      </c>
+      <c r="G82" s="29" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7">
+      <c r="A83" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="B83" s="38" t="s">
+        <v>114</v>
+      </c>
+      <c r="C83" s="39"/>
+      <c r="D83" s="38" t="s">
+        <v>115</v>
+      </c>
+      <c r="E83" s="39"/>
+      <c r="F83" s="29" t="s">
+        <v>126</v>
+      </c>
+      <c r="G83" s="29" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7">
+      <c r="A84" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="B84" s="38" t="s">
+        <v>116</v>
+      </c>
+      <c r="C84" s="39"/>
+      <c r="D84" s="38" t="s">
+        <v>117</v>
+      </c>
+      <c r="E84" s="39"/>
+      <c r="F84" s="29" t="s">
+        <v>127</v>
+      </c>
+      <c r="G84" s="29" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" ht="28.8">
+      <c r="A85" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="B85" s="38" t="s">
+        <v>129</v>
+      </c>
+      <c r="C85" s="39"/>
+      <c r="D85" s="38" t="s">
+        <v>118</v>
+      </c>
+      <c r="E85" s="39"/>
+      <c r="F85" s="29" t="s">
+        <v>128</v>
+      </c>
+      <c r="G85" s="29" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" ht="28.8">
+      <c r="A86" s="26" t="s">
+        <v>28</v>
+      </c>
+      <c r="B86" s="38" t="s">
+        <v>131</v>
+      </c>
+      <c r="C86" s="39"/>
+      <c r="D86" s="38" t="s">
+        <v>130</v>
+      </c>
+      <c r="E86" s="39"/>
+      <c r="F86" s="29" t="s">
+        <v>132</v>
+      </c>
+      <c r="G86" s="29" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7">
+      <c r="A87" s="35" t="s">
+        <v>74</v>
+      </c>
+      <c r="B87" s="31"/>
+      <c r="C87" s="36" t="s">
+        <v>112</v>
+      </c>
+      <c r="D87" s="33"/>
+      <c r="E87" s="33"/>
+      <c r="F87" s="33"/>
+      <c r="G87" s="34"/>
+    </row>
+    <row r="88" spans="1:7">
+      <c r="A88" s="30" t="s">
+        <v>75</v>
+      </c>
+      <c r="B88" s="31"/>
+      <c r="C88" s="32">
+        <v>43014</v>
+      </c>
+      <c r="D88" s="33"/>
+      <c r="E88" s="33"/>
+      <c r="F88" s="33"/>
+      <c r="G88" s="34"/>
+    </row>
+    <row r="89" spans="1:7">
+      <c r="A89" s="35" t="s">
+        <v>76</v>
+      </c>
+      <c r="B89" s="31"/>
+      <c r="C89" s="36" t="s">
+        <v>133</v>
+      </c>
+      <c r="D89" s="33"/>
+      <c r="E89" s="33"/>
+      <c r="F89" s="33"/>
+      <c r="G89" s="34"/>
+    </row>
+    <row r="90" spans="1:7">
+      <c r="A90" s="35" t="s">
+        <v>73</v>
+      </c>
+      <c r="B90" s="37"/>
+      <c r="C90" s="36" t="s">
+        <v>106</v>
+      </c>
+      <c r="D90" s="33"/>
+      <c r="E90" s="33"/>
+      <c r="F90" s="33"/>
+      <c r="G90" s="34"/>
     </row>
   </sheetData>
-  <mergeCells count="111">
-    <mergeCell ref="A70:B70"/>
-    <mergeCell ref="C70:G70"/>
-    <mergeCell ref="A71:B71"/>
-    <mergeCell ref="C71:G71"/>
-    <mergeCell ref="A72:B72"/>
-    <mergeCell ref="C72:G72"/>
-    <mergeCell ref="B63:C63"/>
-    <mergeCell ref="D63:E63"/>
-    <mergeCell ref="B64:C64"/>
-    <mergeCell ref="D64:E64"/>
-    <mergeCell ref="A69:B69"/>
-    <mergeCell ref="C69:G69"/>
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="D65:E65"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="D66:E66"/>
-    <mergeCell ref="B67:C67"/>
-    <mergeCell ref="D67:E67"/>
-    <mergeCell ref="B68:C68"/>
-    <mergeCell ref="D68:E68"/>
+  <mergeCells count="139">
+    <mergeCell ref="A87:B87"/>
+    <mergeCell ref="C87:G87"/>
+    <mergeCell ref="A88:B88"/>
+    <mergeCell ref="C88:G88"/>
+    <mergeCell ref="A89:B89"/>
+    <mergeCell ref="C89:G89"/>
+    <mergeCell ref="A90:B90"/>
+    <mergeCell ref="C90:G90"/>
+    <mergeCell ref="B82:C82"/>
+    <mergeCell ref="D82:E82"/>
+    <mergeCell ref="B83:C83"/>
+    <mergeCell ref="D83:E83"/>
+    <mergeCell ref="B84:C84"/>
+    <mergeCell ref="D84:E84"/>
+    <mergeCell ref="B85:C85"/>
+    <mergeCell ref="D85:E85"/>
+    <mergeCell ref="B86:C86"/>
+    <mergeCell ref="D86:E86"/>
+    <mergeCell ref="A76:G76"/>
+    <mergeCell ref="A77:B77"/>
+    <mergeCell ref="C77:G77"/>
+    <mergeCell ref="A78:B78"/>
+    <mergeCell ref="C78:G78"/>
+    <mergeCell ref="A79:B79"/>
+    <mergeCell ref="C79:G79"/>
+    <mergeCell ref="A80:G80"/>
+    <mergeCell ref="B81:C81"/>
+    <mergeCell ref="D81:E81"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="C54:G54"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="C55:G55"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="C52:G52"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="C53:G53"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="C46:G46"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="C47:G47"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="D51:E51"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="C48:G48"/>
+    <mergeCell ref="A49:G49"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="D50:E50"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="C38:G38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="C39:G39"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="C40:G40"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="C41:G41"/>
+    <mergeCell ref="A45:G45"/>
+    <mergeCell ref="A32:G32"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A3:G3"/>
+    <mergeCell ref="A7:G7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:G6"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:G4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:G5"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="D13:E13"/>
     <mergeCell ref="A60:B60"/>
     <mergeCell ref="C60:G60"/>
     <mergeCell ref="A61:B61"/>
@@ -3057,73 +3364,26 @@
     <mergeCell ref="C30:G30"/>
     <mergeCell ref="A31:B31"/>
     <mergeCell ref="C31:G31"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A3:G3"/>
-    <mergeCell ref="A7:G7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:G6"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:G4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:G5"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="A32:G32"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="C38:G38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="C39:G39"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="C40:G40"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="C41:G41"/>
-    <mergeCell ref="A45:G45"/>
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="C54:G54"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="C55:G55"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="C52:G52"/>
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="C53:G53"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="C46:G46"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="C47:G47"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="D51:E51"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="C48:G48"/>
-    <mergeCell ref="A49:G49"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="D50:E50"/>
+    <mergeCell ref="A70:B70"/>
+    <mergeCell ref="C70:G70"/>
+    <mergeCell ref="A71:B71"/>
+    <mergeCell ref="C71:G71"/>
+    <mergeCell ref="A72:B72"/>
+    <mergeCell ref="C72:G72"/>
+    <mergeCell ref="B63:C63"/>
+    <mergeCell ref="D63:E63"/>
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="D64:E64"/>
+    <mergeCell ref="A69:B69"/>
+    <mergeCell ref="C69:G69"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="D65:E65"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="D66:E66"/>
+    <mergeCell ref="B67:C67"/>
+    <mergeCell ref="D67:E67"/>
+    <mergeCell ref="B68:C68"/>
+    <mergeCell ref="D68:E68"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
@@ -3134,7 +3394,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A4:I24"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
@@ -3153,17 +3413,17 @@
   </cols>
   <sheetData>
     <row r="4" spans="1:9" ht="18">
-      <c r="A4" s="70" t="s">
+      <c r="A4" s="72" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="71"/>
-      <c r="C4" s="71"/>
-      <c r="D4" s="71"/>
-      <c r="E4" s="71"/>
-      <c r="F4" s="71"/>
-      <c r="G4" s="71"/>
-      <c r="H4" s="71"/>
-      <c r="I4" s="72"/>
+      <c r="B4" s="73"/>
+      <c r="C4" s="73"/>
+      <c r="D4" s="73"/>
+      <c r="E4" s="73"/>
+      <c r="F4" s="73"/>
+      <c r="G4" s="73"/>
+      <c r="H4" s="73"/>
+      <c r="I4" s="74"/>
     </row>
     <row r="5" spans="1:9" s="4" customFormat="1">
       <c r="A5" s="2" t="s">
@@ -3283,17 +3543,17 @@
       <c r="I9" s="9"/>
     </row>
     <row r="13" spans="1:9" ht="18">
-      <c r="A13" s="70" t="s">
+      <c r="A13" s="72" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="71"/>
-      <c r="C13" s="71"/>
-      <c r="D13" s="71"/>
-      <c r="E13" s="71"/>
-      <c r="F13" s="71"/>
-      <c r="G13" s="71"/>
-      <c r="H13" s="71"/>
-      <c r="I13" s="72"/>
+      <c r="B13" s="73"/>
+      <c r="C13" s="73"/>
+      <c r="D13" s="73"/>
+      <c r="E13" s="73"/>
+      <c r="F13" s="73"/>
+      <c r="G13" s="73"/>
+      <c r="H13" s="73"/>
+      <c r="I13" s="74"/>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="2" t="s">

</xml_diff>

<commit_message>
added pdf viewer test
</commit_message>
<xml_diff>
--- a/FYP documentation/FYP_Test_Plan.xlsx
+++ b/FYP documentation/FYP_Test_Plan.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="161">
   <si>
     <t>Expected Result</t>
   </si>
@@ -463,7 +463,82 @@
     <t>Test if file operation</t>
   </si>
   <si>
-    <t xml:space="preserve">Add area 1 and area 2. Area 2 should have file 1 and file 2 </t>
+    <t>The first device logout when we login to second device</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1423hrs </t>
+  </si>
+  <si>
+    <t>Add area 1 and area 2. Area 2 should have file 1 and file 2 and Area 1 should be empty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. navigate to area 2 click on file 1 option.
+2. choose are 1 and copy                                         </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. navigate to area 2 click on file 1 option.
+2. choose are 1 and move </t>
+  </si>
+  <si>
+    <t>A copy of file 1 should be created in Area 1 and Area 2 has a copy.</t>
+  </si>
+  <si>
+    <t>A copy of file 1 is created in area 1 and Area 2 has a copy.</t>
+  </si>
+  <si>
+    <t>A copy of file 2 should be created in Area 1 . Area 2 should not have a copy.</t>
+  </si>
+  <si>
+    <t>A copy of file 2 should be created in Area 1 . Area 2 does not have a copy.</t>
+  </si>
+  <si>
+    <t>1. Delete all file from area 1</t>
+  </si>
+  <si>
+    <t>All files should be deleted</t>
+  </si>
+  <si>
+    <t>All files are delete</t>
+  </si>
+  <si>
+    <t>PDF Viewer</t>
+  </si>
+  <si>
+    <t>Test if file operation works as per requirement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Navigate to the file and open it.                                       </t>
+  </si>
+  <si>
+    <t>The pdf file should open in the pdf viewer and all pages can be viewed.</t>
+  </si>
+  <si>
+    <t>The file open and all pages can be viewed</t>
+  </si>
+  <si>
+    <t>A area with 10 meter radius and a file.</t>
+  </si>
+  <si>
+    <t>1. Open the pdf document
+2.  Walk more than 10m from the point of creation</t>
+  </si>
+  <si>
+    <t>The pdf document should close</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the pdf document closes </t>
+  </si>
+  <si>
+    <t>1600 hrs</t>
+  </si>
+  <si>
+    <t>1. Switch screen off</t>
+  </si>
+  <si>
+    <t>The pdf viewer should close and logout</t>
+  </si>
+  <si>
+    <t>the pdf viewer close and logout</t>
   </si>
 </sst>
 </file>
@@ -860,27 +935,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -890,12 +965,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="6" xfId="3" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -923,17 +1010,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="6" xfId="3" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -941,11 +1031,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="7" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="8" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="12" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="13" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -967,24 +1060,6 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="7" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="8" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="12" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2060,35 +2135,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I90"/>
+  <dimension ref="A1:I104"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A73" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C79" sqref="C79:G79"/>
+      <selection activeCell="I65" sqref="I65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="9.88671875" customWidth="1"/>
     <col min="2" max="2" width="13.5546875" customWidth="1"/>
-    <col min="3" max="3" width="13.109375" customWidth="1"/>
+    <col min="3" max="3" width="12.88671875" customWidth="1"/>
     <col min="4" max="4" width="15.109375" customWidth="1"/>
     <col min="5" max="5" width="8.6640625" customWidth="1"/>
-    <col min="6" max="6" width="41.6640625" customWidth="1"/>
-    <col min="7" max="7" width="15.44140625" customWidth="1"/>
+    <col min="6" max="6" width="38.109375" customWidth="1"/>
+    <col min="7" max="7" width="15.77734375" customWidth="1"/>
     <col min="8" max="8" width="10.5546875" customWidth="1"/>
     <col min="9" max="9" width="7.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="40.799999999999997" customHeight="1">
-      <c r="A1" s="66" t="s">
+      <c r="A1" s="62" t="s">
         <v>64</v>
       </c>
-      <c r="B1" s="67"/>
-      <c r="C1" s="67"/>
-      <c r="D1" s="67"/>
-      <c r="E1" s="67"/>
-      <c r="F1" s="67"/>
-      <c r="G1" s="68"/>
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
+      <c r="F1" s="63"/>
+      <c r="G1" s="64"/>
       <c r="H1" s="16"/>
       <c r="I1" s="16"/>
     </row>
@@ -2104,67 +2179,67 @@
       <c r="I2" s="19"/>
     </row>
     <row r="3" spans="1:9" ht="31.2" customHeight="1" thickBot="1">
-      <c r="A3" s="51" t="s">
+      <c r="A3" s="40" t="s">
         <v>83</v>
       </c>
-      <c r="B3" s="51"/>
-      <c r="C3" s="51"/>
-      <c r="D3" s="51"/>
-      <c r="E3" s="51"/>
-      <c r="F3" s="51"/>
-      <c r="G3" s="51"/>
+      <c r="B3" s="40"/>
+      <c r="C3" s="40"/>
+      <c r="D3" s="40"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="40"/>
+      <c r="G3" s="40"/>
       <c r="H3" s="16"/>
       <c r="I3" s="16"/>
     </row>
     <row r="4" spans="1:9" ht="18.600000000000001" customHeight="1" thickTop="1">
-      <c r="A4" s="40" t="s">
+      <c r="A4" s="41" t="s">
         <v>66</v>
       </c>
-      <c r="B4" s="41"/>
-      <c r="C4" s="52" t="s">
+      <c r="B4" s="42"/>
+      <c r="C4" s="43" t="s">
         <v>84</v>
       </c>
-      <c r="D4" s="53"/>
-      <c r="E4" s="53"/>
-      <c r="F4" s="53"/>
-      <c r="G4" s="54"/>
+      <c r="D4" s="44"/>
+      <c r="E4" s="44"/>
+      <c r="F4" s="44"/>
+      <c r="G4" s="45"/>
       <c r="H4" s="17"/>
       <c r="I4" s="17"/>
     </row>
     <row r="5" spans="1:9" ht="14.4" customHeight="1">
-      <c r="A5" s="40" t="s">
+      <c r="A5" s="41" t="s">
         <v>67</v>
       </c>
-      <c r="B5" s="41"/>
-      <c r="C5" s="42"/>
-      <c r="D5" s="43"/>
-      <c r="E5" s="43"/>
-      <c r="F5" s="43"/>
-      <c r="G5" s="44"/>
+      <c r="B5" s="42"/>
+      <c r="C5" s="46"/>
+      <c r="D5" s="47"/>
+      <c r="E5" s="47"/>
+      <c r="F5" s="47"/>
+      <c r="G5" s="48"/>
       <c r="H5" s="16"/>
       <c r="I5" s="16"/>
     </row>
     <row r="6" spans="1:9" ht="14.4" customHeight="1">
-      <c r="A6" s="40" t="s">
+      <c r="A6" s="41" t="s">
         <v>68</v>
       </c>
-      <c r="B6" s="41"/>
-      <c r="C6" s="45"/>
-      <c r="D6" s="46"/>
-      <c r="E6" s="46"/>
-      <c r="F6" s="46"/>
-      <c r="G6" s="47"/>
+      <c r="B6" s="42"/>
+      <c r="C6" s="49"/>
+      <c r="D6" s="50"/>
+      <c r="E6" s="50"/>
+      <c r="F6" s="50"/>
+      <c r="G6" s="51"/>
       <c r="H6" s="17"/>
       <c r="I6" s="18"/>
     </row>
     <row r="7" spans="1:9">
-      <c r="A7" s="48"/>
-      <c r="B7" s="49"/>
-      <c r="C7" s="49"/>
-      <c r="D7" s="49"/>
-      <c r="E7" s="49"/>
-      <c r="F7" s="49"/>
-      <c r="G7" s="50"/>
+      <c r="A7" s="52"/>
+      <c r="B7" s="53"/>
+      <c r="C7" s="53"/>
+      <c r="D7" s="53"/>
+      <c r="E7" s="53"/>
+      <c r="F7" s="53"/>
+      <c r="G7" s="54"/>
       <c r="H7" s="18"/>
       <c r="I7" s="18"/>
     </row>
@@ -2172,11 +2247,11 @@
       <c r="A8" s="22" t="s">
         <v>77</v>
       </c>
-      <c r="B8" s="30" t="s">
+      <c r="B8" s="35" t="s">
         <v>69</v>
       </c>
       <c r="C8" s="31"/>
-      <c r="D8" s="30" t="s">
+      <c r="D8" s="35" t="s">
         <v>70</v>
       </c>
       <c r="E8" s="31"/>
@@ -2206,7 +2281,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="29.4" customHeight="1">
+    <row r="10" spans="1:9" ht="41.4" customHeight="1">
       <c r="A10" s="26" t="s">
         <v>6</v>
       </c>
@@ -2217,7 +2292,7 @@
       <c r="D10" s="38" t="s">
         <v>119</v>
       </c>
-      <c r="E10" s="55"/>
+      <c r="E10" s="60"/>
       <c r="F10" s="27" t="s">
         <v>119</v>
       </c>
@@ -2225,7 +2300,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="40.200000000000003" customHeight="1">
+    <row r="11" spans="1:9" ht="67.8" customHeight="1">
       <c r="A11" s="26" t="s">
         <v>7</v>
       </c>
@@ -2244,14 +2319,14 @@
         <v>106</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="58.5" customHeight="1">
+    <row r="12" spans="1:9" ht="73.2" customHeight="1">
       <c r="A12" s="26" t="s">
         <v>8</v>
       </c>
       <c r="B12" s="38" t="s">
         <v>92</v>
       </c>
-      <c r="C12" s="55"/>
+      <c r="C12" s="60"/>
       <c r="D12" s="38" t="s">
         <v>87</v>
       </c>
@@ -2270,7 +2345,7 @@
       <c r="B13" s="38" t="s">
         <v>120</v>
       </c>
-      <c r="C13" s="55"/>
+      <c r="C13" s="60"/>
       <c r="D13" s="38" t="s">
         <v>87</v>
       </c>
@@ -2286,14 +2361,14 @@
       <c r="A14" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="B14" s="56" t="s">
+      <c r="B14" s="61" t="s">
         <v>121</v>
       </c>
-      <c r="C14" s="56"/>
+      <c r="C14" s="61"/>
       <c r="D14" s="38" t="s">
         <v>91</v>
       </c>
-      <c r="E14" s="55"/>
+      <c r="E14" s="60"/>
       <c r="F14" s="28" t="s">
         <v>119</v>
       </c>
@@ -2301,14 +2376,14 @@
         <v>106</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="45.45" customHeight="1">
+    <row r="15" spans="1:9" ht="92.4" customHeight="1">
       <c r="A15" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="B15" s="56" t="s">
+      <c r="B15" s="61" t="s">
         <v>93</v>
       </c>
-      <c r="C15" s="56"/>
+      <c r="C15" s="61"/>
       <c r="D15" s="38" t="s">
         <v>87</v>
       </c>
@@ -2320,14 +2395,14 @@
         <v>106</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="45.45" customHeight="1">
+    <row r="16" spans="1:9" ht="84.6" customHeight="1">
       <c r="A16" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="B16" s="56" t="s">
+      <c r="B16" s="61" t="s">
         <v>94</v>
       </c>
-      <c r="C16" s="56"/>
+      <c r="C16" s="61"/>
       <c r="D16" s="38" t="s">
         <v>87</v>
       </c>
@@ -2339,18 +2414,18 @@
         <v>106</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="45.45" customHeight="1">
+    <row r="17" spans="1:7" ht="94.8" customHeight="1">
       <c r="A17" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="B17" s="56" t="s">
+      <c r="B17" s="61" t="s">
         <v>95</v>
       </c>
-      <c r="C17" s="56"/>
+      <c r="C17" s="61"/>
       <c r="D17" s="38" t="s">
         <v>91</v>
       </c>
-      <c r="E17" s="55"/>
+      <c r="E17" s="60"/>
       <c r="F17" s="28" t="s">
         <v>119</v>
       </c>
@@ -2359,11 +2434,11 @@
       </c>
     </row>
     <row r="18" spans="1:7">
-      <c r="A18" s="30" t="s">
+      <c r="A18" s="35" t="s">
         <v>74</v>
       </c>
       <c r="B18" s="31"/>
-      <c r="C18" s="36" t="s">
+      <c r="C18" s="32" t="s">
         <v>112</v>
       </c>
       <c r="D18" s="33"/>
@@ -2372,11 +2447,11 @@
       <c r="G18" s="34"/>
     </row>
     <row r="19" spans="1:7">
-      <c r="A19" s="30" t="s">
+      <c r="A19" s="35" t="s">
         <v>75</v>
       </c>
       <c r="B19" s="31"/>
-      <c r="C19" s="32">
+      <c r="C19" s="36">
         <v>43014</v>
       </c>
       <c r="D19" s="33"/>
@@ -2385,11 +2460,11 @@
       <c r="G19" s="34"/>
     </row>
     <row r="20" spans="1:7">
-      <c r="A20" s="35" t="s">
+      <c r="A20" s="30" t="s">
         <v>76</v>
       </c>
       <c r="B20" s="31"/>
-      <c r="C20" s="36" t="s">
+      <c r="C20" s="32" t="s">
         <v>124</v>
       </c>
       <c r="D20" s="33"/>
@@ -2398,11 +2473,11 @@
       <c r="G20" s="34"/>
     </row>
     <row r="21" spans="1:7">
-      <c r="A21" s="35" t="s">
+      <c r="A21" s="30" t="s">
         <v>73</v>
       </c>
       <c r="B21" s="37"/>
-      <c r="C21" s="36" t="s">
+      <c r="C21" s="32" t="s">
         <v>106</v>
       </c>
       <c r="D21" s="33"/>
@@ -2457,71 +2532,71 @@
     </row>
     <row r="27" spans="1:7" ht="12" customHeight="1"/>
     <row r="28" spans="1:7" ht="20.399999999999999" thickBot="1">
-      <c r="A28" s="51" t="s">
+      <c r="A28" s="40" t="s">
         <v>65</v>
       </c>
-      <c r="B28" s="51"/>
-      <c r="C28" s="51"/>
-      <c r="D28" s="51"/>
-      <c r="E28" s="51"/>
-      <c r="F28" s="51"/>
-      <c r="G28" s="51"/>
+      <c r="B28" s="40"/>
+      <c r="C28" s="40"/>
+      <c r="D28" s="40"/>
+      <c r="E28" s="40"/>
+      <c r="F28" s="40"/>
+      <c r="G28" s="40"/>
     </row>
     <row r="29" spans="1:7" ht="15" thickTop="1">
-      <c r="A29" s="59" t="s">
+      <c r="A29" s="65" t="s">
         <v>66</v>
       </c>
-      <c r="B29" s="60"/>
-      <c r="C29" s="61" t="s">
+      <c r="B29" s="66"/>
+      <c r="C29" s="67" t="s">
         <v>78</v>
       </c>
-      <c r="D29" s="62"/>
-      <c r="E29" s="62"/>
-      <c r="F29" s="62"/>
-      <c r="G29" s="63"/>
+      <c r="D29" s="68"/>
+      <c r="E29" s="68"/>
+      <c r="F29" s="68"/>
+      <c r="G29" s="69"/>
     </row>
     <row r="30" spans="1:7">
-      <c r="A30" s="40" t="s">
+      <c r="A30" s="41" t="s">
         <v>67</v>
       </c>
-      <c r="B30" s="41"/>
-      <c r="C30" s="42"/>
-      <c r="D30" s="43"/>
-      <c r="E30" s="43"/>
-      <c r="F30" s="43"/>
-      <c r="G30" s="44"/>
+      <c r="B30" s="42"/>
+      <c r="C30" s="46"/>
+      <c r="D30" s="47"/>
+      <c r="E30" s="47"/>
+      <c r="F30" s="47"/>
+      <c r="G30" s="48"/>
     </row>
     <row r="31" spans="1:7">
-      <c r="A31" s="40" t="s">
+      <c r="A31" s="41" t="s">
         <v>68</v>
       </c>
-      <c r="B31" s="41"/>
-      <c r="C31" s="45" t="s">
+      <c r="B31" s="42"/>
+      <c r="C31" s="49" t="s">
         <v>79</v>
       </c>
-      <c r="D31" s="64"/>
-      <c r="E31" s="64"/>
-      <c r="F31" s="64"/>
-      <c r="G31" s="65"/>
+      <c r="D31" s="70"/>
+      <c r="E31" s="70"/>
+      <c r="F31" s="70"/>
+      <c r="G31" s="71"/>
     </row>
     <row r="32" spans="1:7">
-      <c r="A32" s="69"/>
-      <c r="B32" s="70"/>
-      <c r="C32" s="70"/>
-      <c r="D32" s="70"/>
-      <c r="E32" s="70"/>
-      <c r="F32" s="70"/>
-      <c r="G32" s="71"/>
+      <c r="A32" s="55"/>
+      <c r="B32" s="56"/>
+      <c r="C32" s="56"/>
+      <c r="D32" s="56"/>
+      <c r="E32" s="56"/>
+      <c r="F32" s="56"/>
+      <c r="G32" s="57"/>
     </row>
     <row r="33" spans="1:7">
       <c r="A33" s="22" t="s">
         <v>77</v>
       </c>
-      <c r="B33" s="30" t="s">
+      <c r="B33" s="35" t="s">
         <v>69</v>
       </c>
       <c r="C33" s="31"/>
-      <c r="D33" s="30" t="s">
+      <c r="D33" s="35" t="s">
         <v>70</v>
       </c>
       <c r="E33" s="31"/>
@@ -2536,11 +2611,11 @@
       <c r="A34" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="B34" s="57" t="s">
+      <c r="B34" s="58" t="s">
         <v>111</v>
       </c>
-      <c r="C34" s="58"/>
-      <c r="D34" s="36" t="s">
+      <c r="C34" s="59"/>
+      <c r="D34" s="32" t="s">
         <v>72</v>
       </c>
       <c r="E34" s="34"/>
@@ -2555,14 +2630,14 @@
       <c r="A35" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="B35" s="57" t="s">
+      <c r="B35" s="58" t="s">
         <v>50</v>
       </c>
-      <c r="C35" s="58"/>
+      <c r="C35" s="59"/>
       <c r="D35" s="38" t="s">
         <v>86</v>
       </c>
-      <c r="E35" s="55"/>
+      <c r="E35" s="60"/>
       <c r="F35" s="20" t="s">
         <v>108</v>
       </c>
@@ -2574,14 +2649,14 @@
       <c r="A36" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="B36" s="57" t="s">
+      <c r="B36" s="58" t="s">
         <v>49</v>
       </c>
-      <c r="C36" s="58"/>
+      <c r="C36" s="59"/>
       <c r="D36" s="38" t="s">
         <v>80</v>
       </c>
-      <c r="E36" s="55"/>
+      <c r="E36" s="60"/>
       <c r="F36" s="20" t="s">
         <v>109</v>
       </c>
@@ -2593,14 +2668,14 @@
       <c r="A37" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="B37" s="57" t="s">
+      <c r="B37" s="58" t="s">
         <v>81</v>
       </c>
-      <c r="C37" s="58"/>
+      <c r="C37" s="59"/>
       <c r="D37" s="38" t="s">
         <v>82</v>
       </c>
-      <c r="E37" s="55"/>
+      <c r="E37" s="60"/>
       <c r="F37" s="20" t="s">
         <v>107</v>
       </c>
@@ -2609,11 +2684,11 @@
       </c>
     </row>
     <row r="38" spans="1:7">
-      <c r="A38" s="30" t="s">
+      <c r="A38" s="35" t="s">
         <v>74</v>
       </c>
       <c r="B38" s="31"/>
-      <c r="C38" s="36" t="s">
+      <c r="C38" s="32" t="s">
         <v>112</v>
       </c>
       <c r="D38" s="33"/>
@@ -2622,11 +2697,11 @@
       <c r="G38" s="34"/>
     </row>
     <row r="39" spans="1:7">
-      <c r="A39" s="30" t="s">
+      <c r="A39" s="35" t="s">
         <v>75</v>
       </c>
       <c r="B39" s="31"/>
-      <c r="C39" s="32">
+      <c r="C39" s="36">
         <v>43042</v>
       </c>
       <c r="D39" s="33"/>
@@ -2635,11 +2710,11 @@
       <c r="G39" s="34"/>
     </row>
     <row r="40" spans="1:7">
-      <c r="A40" s="35" t="s">
+      <c r="A40" s="30" t="s">
         <v>76</v>
       </c>
       <c r="B40" s="37"/>
-      <c r="C40" s="36" t="s">
+      <c r="C40" s="32" t="s">
         <v>113</v>
       </c>
       <c r="D40" s="33"/>
@@ -2648,11 +2723,11 @@
       <c r="G40" s="34"/>
     </row>
     <row r="41" spans="1:7">
-      <c r="A41" s="35" t="s">
+      <c r="A41" s="30" t="s">
         <v>73</v>
       </c>
       <c r="B41" s="37"/>
-      <c r="C41" s="36" t="s">
+      <c r="C41" s="32" t="s">
         <v>106</v>
       </c>
       <c r="D41" s="33"/>
@@ -2661,71 +2736,71 @@
       <c r="G41" s="34"/>
     </row>
     <row r="45" spans="1:7" ht="20.399999999999999" thickBot="1">
-      <c r="A45" s="51" t="s">
+      <c r="A45" s="40" t="s">
         <v>99</v>
       </c>
-      <c r="B45" s="51"/>
-      <c r="C45" s="51"/>
-      <c r="D45" s="51"/>
-      <c r="E45" s="51"/>
-      <c r="F45" s="51"/>
-      <c r="G45" s="51"/>
+      <c r="B45" s="40"/>
+      <c r="C45" s="40"/>
+      <c r="D45" s="40"/>
+      <c r="E45" s="40"/>
+      <c r="F45" s="40"/>
+      <c r="G45" s="40"/>
     </row>
     <row r="46" spans="1:7" ht="15" thickTop="1">
-      <c r="A46" s="40" t="s">
+      <c r="A46" s="41" t="s">
         <v>66</v>
       </c>
-      <c r="B46" s="41"/>
-      <c r="C46" s="52" t="s">
+      <c r="B46" s="42"/>
+      <c r="C46" s="43" t="s">
         <v>96</v>
       </c>
-      <c r="D46" s="53"/>
-      <c r="E46" s="53"/>
-      <c r="F46" s="53"/>
-      <c r="G46" s="54"/>
+      <c r="D46" s="44"/>
+      <c r="E46" s="44"/>
+      <c r="F46" s="44"/>
+      <c r="G46" s="45"/>
     </row>
     <row r="47" spans="1:7">
-      <c r="A47" s="40" t="s">
+      <c r="A47" s="41" t="s">
         <v>67</v>
       </c>
-      <c r="B47" s="41"/>
-      <c r="C47" s="42"/>
-      <c r="D47" s="43"/>
-      <c r="E47" s="43"/>
-      <c r="F47" s="43"/>
-      <c r="G47" s="44"/>
+      <c r="B47" s="42"/>
+      <c r="C47" s="46"/>
+      <c r="D47" s="47"/>
+      <c r="E47" s="47"/>
+      <c r="F47" s="47"/>
+      <c r="G47" s="48"/>
     </row>
     <row r="48" spans="1:7">
-      <c r="A48" s="40" t="s">
+      <c r="A48" s="41" t="s">
         <v>68</v>
       </c>
-      <c r="B48" s="41"/>
-      <c r="C48" s="45" t="s">
+      <c r="B48" s="42"/>
+      <c r="C48" s="49" t="s">
         <v>97</v>
       </c>
-      <c r="D48" s="46"/>
-      <c r="E48" s="46"/>
-      <c r="F48" s="46"/>
-      <c r="G48" s="47"/>
+      <c r="D48" s="50"/>
+      <c r="E48" s="50"/>
+      <c r="F48" s="50"/>
+      <c r="G48" s="51"/>
     </row>
     <row r="49" spans="1:7" ht="16.8" customHeight="1">
-      <c r="A49" s="48"/>
-      <c r="B49" s="49"/>
-      <c r="C49" s="49"/>
-      <c r="D49" s="49"/>
-      <c r="E49" s="49"/>
-      <c r="F49" s="49"/>
-      <c r="G49" s="50"/>
+      <c r="A49" s="52"/>
+      <c r="B49" s="53"/>
+      <c r="C49" s="53"/>
+      <c r="D49" s="53"/>
+      <c r="E49" s="53"/>
+      <c r="F49" s="53"/>
+      <c r="G49" s="54"/>
     </row>
     <row r="50" spans="1:7" ht="63" customHeight="1">
       <c r="A50" s="22" t="s">
         <v>77</v>
       </c>
-      <c r="B50" s="30" t="s">
+      <c r="B50" s="35" t="s">
         <v>69</v>
       </c>
       <c r="C50" s="31"/>
-      <c r="D50" s="30" t="s">
+      <c r="D50" s="35" t="s">
         <v>70</v>
       </c>
       <c r="E50" s="31"/>
@@ -2736,7 +2811,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="51" spans="1:7" ht="54" customHeight="1">
+    <row r="51" spans="1:7" ht="74.400000000000006" customHeight="1">
       <c r="A51" s="26" t="s">
         <v>5</v>
       </c>
@@ -2748,15 +2823,19 @@
         <v>98</v>
       </c>
       <c r="E51" s="39"/>
-      <c r="F51" s="20"/>
-      <c r="G51" s="20"/>
+      <c r="F51" s="29" t="s">
+        <v>136</v>
+      </c>
+      <c r="G51" s="27" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="52" spans="1:7" ht="27" customHeight="1">
-      <c r="A52" s="35" t="s">
+      <c r="A52" s="30" t="s">
         <v>74</v>
       </c>
       <c r="B52" s="31"/>
-      <c r="C52" s="36" t="s">
+      <c r="C52" s="32" t="s">
         <v>112</v>
       </c>
       <c r="D52" s="33"/>
@@ -2764,105 +2843,111 @@
       <c r="F52" s="33"/>
       <c r="G52" s="34"/>
     </row>
-    <row r="53" spans="1:7" ht="34.799999999999997" customHeight="1">
-      <c r="A53" s="30" t="s">
+    <row r="53" spans="1:7" ht="22.8" customHeight="1">
+      <c r="A53" s="35" t="s">
         <v>75</v>
       </c>
       <c r="B53" s="31"/>
-      <c r="C53" s="69"/>
-      <c r="D53" s="70"/>
-      <c r="E53" s="70"/>
-      <c r="F53" s="70"/>
-      <c r="G53" s="71"/>
-    </row>
-    <row r="54" spans="1:7" ht="25.2" customHeight="1">
-      <c r="A54" s="35" t="s">
+      <c r="C53" s="36">
+        <v>43046</v>
+      </c>
+      <c r="D53" s="33"/>
+      <c r="E53" s="33"/>
+      <c r="F53" s="33"/>
+      <c r="G53" s="34"/>
+    </row>
+    <row r="54" spans="1:7" ht="15.6" customHeight="1">
+      <c r="A54" s="30" t="s">
         <v>76</v>
       </c>
       <c r="B54" s="31"/>
-      <c r="C54" s="69"/>
-      <c r="D54" s="70"/>
-      <c r="E54" s="70"/>
-      <c r="F54" s="70"/>
-      <c r="G54" s="71"/>
+      <c r="C54" s="32" t="s">
+        <v>137</v>
+      </c>
+      <c r="D54" s="33"/>
+      <c r="E54" s="33"/>
+      <c r="F54" s="33"/>
+      <c r="G54" s="34"/>
     </row>
     <row r="55" spans="1:7">
-      <c r="A55" s="35" t="s">
+      <c r="A55" s="30" t="s">
         <v>73</v>
       </c>
       <c r="B55" s="37"/>
-      <c r="C55" s="69"/>
-      <c r="D55" s="70"/>
-      <c r="E55" s="70"/>
-      <c r="F55" s="70"/>
-      <c r="G55" s="71"/>
+      <c r="C55" s="32" t="s">
+        <v>106</v>
+      </c>
+      <c r="D55" s="33"/>
+      <c r="E55" s="33"/>
+      <c r="F55" s="33"/>
+      <c r="G55" s="34"/>
     </row>
     <row r="58" spans="1:7" ht="20.399999999999999" thickBot="1">
-      <c r="A58" s="51" t="s">
+      <c r="A58" s="40" t="s">
         <v>102</v>
       </c>
-      <c r="B58" s="51"/>
-      <c r="C58" s="51"/>
-      <c r="D58" s="51"/>
-      <c r="E58" s="51"/>
-      <c r="F58" s="51"/>
-      <c r="G58" s="51"/>
+      <c r="B58" s="40"/>
+      <c r="C58" s="40"/>
+      <c r="D58" s="40"/>
+      <c r="E58" s="40"/>
+      <c r="F58" s="40"/>
+      <c r="G58" s="40"/>
     </row>
     <row r="59" spans="1:7" ht="15" thickTop="1">
-      <c r="A59" s="40" t="s">
+      <c r="A59" s="41" t="s">
         <v>66</v>
       </c>
-      <c r="B59" s="41"/>
-      <c r="C59" s="52" t="s">
+      <c r="B59" s="42"/>
+      <c r="C59" s="43" t="s">
         <v>103</v>
       </c>
-      <c r="D59" s="53"/>
-      <c r="E59" s="53"/>
-      <c r="F59" s="53"/>
-      <c r="G59" s="54"/>
+      <c r="D59" s="44"/>
+      <c r="E59" s="44"/>
+      <c r="F59" s="44"/>
+      <c r="G59" s="45"/>
     </row>
     <row r="60" spans="1:7">
-      <c r="A60" s="40" t="s">
+      <c r="A60" s="41" t="s">
         <v>67</v>
       </c>
-      <c r="B60" s="41"/>
-      <c r="C60" s="42"/>
-      <c r="D60" s="43"/>
-      <c r="E60" s="43"/>
-      <c r="F60" s="43"/>
-      <c r="G60" s="44"/>
+      <c r="B60" s="42"/>
+      <c r="C60" s="46"/>
+      <c r="D60" s="47"/>
+      <c r="E60" s="47"/>
+      <c r="F60" s="47"/>
+      <c r="G60" s="48"/>
     </row>
     <row r="61" spans="1:7">
-      <c r="A61" s="40" t="s">
+      <c r="A61" s="41" t="s">
         <v>68</v>
       </c>
-      <c r="B61" s="41"/>
-      <c r="C61" s="45" t="s">
+      <c r="B61" s="42"/>
+      <c r="C61" s="49" t="s">
         <v>101</v>
       </c>
-      <c r="D61" s="46"/>
-      <c r="E61" s="46"/>
-      <c r="F61" s="46"/>
-      <c r="G61" s="47"/>
+      <c r="D61" s="50"/>
+      <c r="E61" s="50"/>
+      <c r="F61" s="50"/>
+      <c r="G61" s="51"/>
     </row>
     <row r="62" spans="1:7">
-      <c r="A62" s="48"/>
-      <c r="B62" s="49"/>
-      <c r="C62" s="49"/>
-      <c r="D62" s="49"/>
-      <c r="E62" s="49"/>
-      <c r="F62" s="49"/>
-      <c r="G62" s="50"/>
+      <c r="A62" s="52"/>
+      <c r="B62" s="53"/>
+      <c r="C62" s="53"/>
+      <c r="D62" s="53"/>
+      <c r="E62" s="53"/>
+      <c r="F62" s="53"/>
+      <c r="G62" s="54"/>
     </row>
     <row r="63" spans="1:7">
       <c r="A63" s="22" t="s">
         <v>77</v>
       </c>
-      <c r="B63" s="30" t="s">
+      <c r="B63" s="35" t="s">
         <v>69</v>
       </c>
       <c r="C63" s="31"/>
-      <c r="D63" s="30" t="s">
+      <c r="D63" s="35" t="s">
         <v>70</v>
       </c>
       <c r="E63" s="31"/>
@@ -2969,11 +3054,11 @@
       </c>
     </row>
     <row r="69" spans="1:7">
-      <c r="A69" s="35" t="s">
+      <c r="A69" s="30" t="s">
         <v>74</v>
       </c>
       <c r="B69" s="31"/>
-      <c r="C69" s="36" t="s">
+      <c r="C69" s="32" t="s">
         <v>112</v>
       </c>
       <c r="D69" s="33"/>
@@ -2982,12 +3067,12 @@
       <c r="G69" s="34"/>
     </row>
     <row r="70" spans="1:7">
-      <c r="A70" s="30" t="s">
+      <c r="A70" s="35" t="s">
         <v>75</v>
       </c>
       <c r="B70" s="31"/>
-      <c r="C70" s="32">
-        <v>43014</v>
+      <c r="C70" s="36">
+        <v>43045</v>
       </c>
       <c r="D70" s="33"/>
       <c r="E70" s="33"/>
@@ -2995,11 +3080,11 @@
       <c r="G70" s="34"/>
     </row>
     <row r="71" spans="1:7">
-      <c r="A71" s="35" t="s">
+      <c r="A71" s="30" t="s">
         <v>76</v>
       </c>
       <c r="B71" s="31"/>
-      <c r="C71" s="36" t="s">
+      <c r="C71" s="32" t="s">
         <v>133</v>
       </c>
       <c r="D71" s="33"/>
@@ -3008,11 +3093,11 @@
       <c r="G71" s="34"/>
     </row>
     <row r="72" spans="1:7">
-      <c r="A72" s="35" t="s">
+      <c r="A72" s="30" t="s">
         <v>73</v>
       </c>
       <c r="B72" s="37"/>
-      <c r="C72" s="36" t="s">
+      <c r="C72" s="32" t="s">
         <v>106</v>
       </c>
       <c r="D72" s="33"/>
@@ -3021,71 +3106,71 @@
       <c r="G72" s="34"/>
     </row>
     <row r="76" spans="1:7" ht="20.399999999999999" thickBot="1">
-      <c r="A76" s="51" t="s">
+      <c r="A76" s="40" t="s">
         <v>134</v>
       </c>
-      <c r="B76" s="51"/>
-      <c r="C76" s="51"/>
-      <c r="D76" s="51"/>
-      <c r="E76" s="51"/>
-      <c r="F76" s="51"/>
-      <c r="G76" s="51"/>
+      <c r="B76" s="40"/>
+      <c r="C76" s="40"/>
+      <c r="D76" s="40"/>
+      <c r="E76" s="40"/>
+      <c r="F76" s="40"/>
+      <c r="G76" s="40"/>
     </row>
     <row r="77" spans="1:7" ht="15" thickTop="1">
-      <c r="A77" s="40" t="s">
+      <c r="A77" s="41" t="s">
         <v>66</v>
       </c>
-      <c r="B77" s="41"/>
-      <c r="C77" s="52" t="s">
-        <v>135</v>
-      </c>
-      <c r="D77" s="53"/>
-      <c r="E77" s="53"/>
-      <c r="F77" s="53"/>
-      <c r="G77" s="54"/>
+      <c r="B77" s="42"/>
+      <c r="C77" s="43" t="s">
+        <v>149</v>
+      </c>
+      <c r="D77" s="44"/>
+      <c r="E77" s="44"/>
+      <c r="F77" s="44"/>
+      <c r="G77" s="45"/>
     </row>
     <row r="78" spans="1:7">
-      <c r="A78" s="40" t="s">
+      <c r="A78" s="41" t="s">
         <v>67</v>
       </c>
-      <c r="B78" s="41"/>
-      <c r="C78" s="42"/>
-      <c r="D78" s="43"/>
-      <c r="E78" s="43"/>
-      <c r="F78" s="43"/>
-      <c r="G78" s="44"/>
+      <c r="B78" s="42"/>
+      <c r="C78" s="46"/>
+      <c r="D78" s="47"/>
+      <c r="E78" s="47"/>
+      <c r="F78" s="47"/>
+      <c r="G78" s="48"/>
     </row>
     <row r="79" spans="1:7">
-      <c r="A79" s="40" t="s">
+      <c r="A79" s="41" t="s">
         <v>68</v>
       </c>
-      <c r="B79" s="41"/>
-      <c r="C79" s="45" t="s">
-        <v>136</v>
-      </c>
-      <c r="D79" s="46"/>
-      <c r="E79" s="46"/>
-      <c r="F79" s="46"/>
-      <c r="G79" s="47"/>
+      <c r="B79" s="42"/>
+      <c r="C79" s="49" t="s">
+        <v>138</v>
+      </c>
+      <c r="D79" s="50"/>
+      <c r="E79" s="50"/>
+      <c r="F79" s="50"/>
+      <c r="G79" s="51"/>
     </row>
     <row r="80" spans="1:7">
-      <c r="A80" s="48"/>
-      <c r="B80" s="49"/>
-      <c r="C80" s="49"/>
-      <c r="D80" s="49"/>
-      <c r="E80" s="49"/>
-      <c r="F80" s="49"/>
-      <c r="G80" s="50"/>
+      <c r="A80" s="52"/>
+      <c r="B80" s="53"/>
+      <c r="C80" s="53"/>
+      <c r="D80" s="53"/>
+      <c r="E80" s="53"/>
+      <c r="F80" s="53"/>
+      <c r="G80" s="54"/>
     </row>
     <row r="81" spans="1:7">
       <c r="A81" s="22" t="s">
         <v>77</v>
       </c>
-      <c r="B81" s="30" t="s">
+      <c r="B81" s="35" t="s">
         <v>69</v>
       </c>
       <c r="C81" s="31"/>
-      <c r="D81" s="30" t="s">
+      <c r="D81" s="35" t="s">
         <v>70</v>
       </c>
       <c r="E81" s="31"/>
@@ -3096,108 +3181,96 @@
         <v>73</v>
       </c>
     </row>
-    <row r="82" spans="1:7">
+    <row r="82" spans="1:7" ht="53.4" customHeight="1">
       <c r="A82" s="26" t="s">
         <v>5</v>
       </c>
       <c r="B82" s="38" t="s">
-        <v>104</v>
+        <v>139</v>
       </c>
       <c r="C82" s="39"/>
       <c r="D82" s="38" t="s">
-        <v>105</v>
+        <v>141</v>
       </c>
       <c r="E82" s="39"/>
       <c r="F82" s="29" t="s">
-        <v>125</v>
+        <v>142</v>
       </c>
       <c r="G82" s="29" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="83" spans="1:7">
+    <row r="83" spans="1:7" ht="49.2" customHeight="1">
       <c r="A83" s="26" t="s">
         <v>6</v>
       </c>
       <c r="B83" s="38" t="s">
-        <v>114</v>
+        <v>140</v>
       </c>
       <c r="C83" s="39"/>
       <c r="D83" s="38" t="s">
-        <v>115</v>
+        <v>143</v>
       </c>
       <c r="E83" s="39"/>
       <c r="F83" s="29" t="s">
-        <v>126</v>
+        <v>144</v>
       </c>
       <c r="G83" s="29" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="84" spans="1:7">
+    <row r="84" spans="1:7" ht="49.2" customHeight="1">
       <c r="A84" s="26" t="s">
         <v>7</v>
       </c>
       <c r="B84" s="38" t="s">
-        <v>116</v>
+        <v>145</v>
       </c>
       <c r="C84" s="39"/>
       <c r="D84" s="38" t="s">
-        <v>117</v>
+        <v>146</v>
       </c>
       <c r="E84" s="39"/>
       <c r="F84" s="29" t="s">
-        <v>127</v>
+        <v>147</v>
       </c>
       <c r="G84" s="29" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="85" spans="1:7" ht="28.8">
-      <c r="A85" s="26" t="s">
-        <v>8</v>
-      </c>
-      <c r="B85" s="38" t="s">
-        <v>129</v>
-      </c>
-      <c r="C85" s="39"/>
-      <c r="D85" s="38" t="s">
-        <v>118</v>
-      </c>
-      <c r="E85" s="39"/>
-      <c r="F85" s="29" t="s">
-        <v>128</v>
-      </c>
-      <c r="G85" s="29" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="86" spans="1:7" ht="28.8">
-      <c r="A86" s="26" t="s">
-        <v>28</v>
-      </c>
-      <c r="B86" s="38" t="s">
-        <v>131</v>
-      </c>
-      <c r="C86" s="39"/>
-      <c r="D86" s="38" t="s">
-        <v>130</v>
-      </c>
-      <c r="E86" s="39"/>
-      <c r="F86" s="29" t="s">
-        <v>132</v>
-      </c>
-      <c r="G86" s="29" t="s">
-        <v>106</v>
-      </c>
+    <row r="85" spans="1:7">
+      <c r="A85" s="30" t="s">
+        <v>74</v>
+      </c>
+      <c r="B85" s="31"/>
+      <c r="C85" s="32" t="s">
+        <v>112</v>
+      </c>
+      <c r="D85" s="33"/>
+      <c r="E85" s="33"/>
+      <c r="F85" s="33"/>
+      <c r="G85" s="34"/>
+    </row>
+    <row r="86" spans="1:7">
+      <c r="A86" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="B86" s="31"/>
+      <c r="C86" s="36">
+        <v>43046</v>
+      </c>
+      <c r="D86" s="33"/>
+      <c r="E86" s="33"/>
+      <c r="F86" s="33"/>
+      <c r="G86" s="34"/>
     </row>
     <row r="87" spans="1:7">
-      <c r="A87" s="35" t="s">
-        <v>74</v>
+      <c r="A87" s="30" t="s">
+        <v>76</v>
       </c>
       <c r="B87" s="31"/>
-      <c r="C87" s="36" t="s">
-        <v>112</v>
+      <c r="C87" s="32" t="s">
+        <v>133</v>
       </c>
       <c r="D87" s="33"/>
       <c r="E87" s="33"/>
@@ -3206,140 +3279,248 @@
     </row>
     <row r="88" spans="1:7">
       <c r="A88" s="30" t="s">
-        <v>75</v>
-      </c>
-      <c r="B88" s="31"/>
-      <c r="C88" s="32">
-        <v>43014</v>
+        <v>73</v>
+      </c>
+      <c r="B88" s="37"/>
+      <c r="C88" s="32" t="s">
+        <v>106</v>
       </c>
       <c r="D88" s="33"/>
       <c r="E88" s="33"/>
       <c r="F88" s="33"/>
       <c r="G88" s="34"/>
     </row>
-    <row r="89" spans="1:7">
-      <c r="A89" s="35" t="s">
+    <row r="92" spans="1:7" ht="20.399999999999999" thickBot="1">
+      <c r="A92" s="40" t="s">
+        <v>148</v>
+      </c>
+      <c r="B92" s="40"/>
+      <c r="C92" s="40"/>
+      <c r="D92" s="40"/>
+      <c r="E92" s="40"/>
+      <c r="F92" s="40"/>
+      <c r="G92" s="40"/>
+    </row>
+    <row r="93" spans="1:7" ht="15" thickTop="1">
+      <c r="A93" s="41" t="s">
+        <v>66</v>
+      </c>
+      <c r="B93" s="42"/>
+      <c r="C93" s="43" t="s">
+        <v>135</v>
+      </c>
+      <c r="D93" s="44"/>
+      <c r="E93" s="44"/>
+      <c r="F93" s="44"/>
+      <c r="G93" s="45"/>
+    </row>
+    <row r="94" spans="1:7">
+      <c r="A94" s="41" t="s">
+        <v>67</v>
+      </c>
+      <c r="B94" s="42"/>
+      <c r="C94" s="46"/>
+      <c r="D94" s="47"/>
+      <c r="E94" s="47"/>
+      <c r="F94" s="47"/>
+      <c r="G94" s="48"/>
+    </row>
+    <row r="95" spans="1:7">
+      <c r="A95" s="41" t="s">
+        <v>68</v>
+      </c>
+      <c r="B95" s="42"/>
+      <c r="C95" s="49" t="s">
+        <v>153</v>
+      </c>
+      <c r="D95" s="50"/>
+      <c r="E95" s="50"/>
+      <c r="F95" s="50"/>
+      <c r="G95" s="51"/>
+    </row>
+    <row r="96" spans="1:7">
+      <c r="A96" s="52"/>
+      <c r="B96" s="53"/>
+      <c r="C96" s="53"/>
+      <c r="D96" s="53"/>
+      <c r="E96" s="53"/>
+      <c r="F96" s="53"/>
+      <c r="G96" s="54"/>
+    </row>
+    <row r="97" spans="1:7">
+      <c r="A97" s="22" t="s">
+        <v>77</v>
+      </c>
+      <c r="B97" s="35" t="s">
+        <v>69</v>
+      </c>
+      <c r="C97" s="31"/>
+      <c r="D97" s="35" t="s">
+        <v>70</v>
+      </c>
+      <c r="E97" s="31"/>
+      <c r="F97" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="G97" s="22" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" ht="53.4" customHeight="1">
+      <c r="A98" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="B98" s="38" t="s">
+        <v>150</v>
+      </c>
+      <c r="C98" s="39"/>
+      <c r="D98" s="38" t="s">
+        <v>151</v>
+      </c>
+      <c r="E98" s="39"/>
+      <c r="F98" s="29" t="s">
+        <v>152</v>
+      </c>
+      <c r="G98" s="29" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" ht="54" customHeight="1">
+      <c r="A99" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="B99" s="38" t="s">
+        <v>154</v>
+      </c>
+      <c r="C99" s="39"/>
+      <c r="D99" s="38" t="s">
+        <v>155</v>
+      </c>
+      <c r="E99" s="39"/>
+      <c r="F99" s="29" t="s">
+        <v>156</v>
+      </c>
+      <c r="G99" s="29" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" ht="40.799999999999997" customHeight="1">
+      <c r="A100" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="B100" s="38" t="s">
+        <v>158</v>
+      </c>
+      <c r="C100" s="39"/>
+      <c r="D100" s="38" t="s">
+        <v>159</v>
+      </c>
+      <c r="E100" s="39"/>
+      <c r="F100" s="29" t="s">
+        <v>160</v>
+      </c>
+      <c r="G100" s="29" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7">
+      <c r="A101" s="30" t="s">
+        <v>74</v>
+      </c>
+      <c r="B101" s="31"/>
+      <c r="C101" s="32" t="s">
+        <v>112</v>
+      </c>
+      <c r="D101" s="33"/>
+      <c r="E101" s="33"/>
+      <c r="F101" s="33"/>
+      <c r="G101" s="34"/>
+    </row>
+    <row r="102" spans="1:7">
+      <c r="A102" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="B102" s="31"/>
+      <c r="C102" s="36">
+        <v>43046</v>
+      </c>
+      <c r="D102" s="33"/>
+      <c r="E102" s="33"/>
+      <c r="F102" s="33"/>
+      <c r="G102" s="34"/>
+    </row>
+    <row r="103" spans="1:7">
+      <c r="A103" s="30" t="s">
         <v>76</v>
       </c>
-      <c r="B89" s="31"/>
-      <c r="C89" s="36" t="s">
-        <v>133</v>
-      </c>
-      <c r="D89" s="33"/>
-      <c r="E89" s="33"/>
-      <c r="F89" s="33"/>
-      <c r="G89" s="34"/>
-    </row>
-    <row r="90" spans="1:7">
-      <c r="A90" s="35" t="s">
+      <c r="B103" s="31"/>
+      <c r="C103" s="32" t="s">
+        <v>157</v>
+      </c>
+      <c r="D103" s="33"/>
+      <c r="E103" s="33"/>
+      <c r="F103" s="33"/>
+      <c r="G103" s="34"/>
+    </row>
+    <row r="104" spans="1:7">
+      <c r="A104" s="30" t="s">
         <v>73</v>
       </c>
-      <c r="B90" s="37"/>
-      <c r="C90" s="36" t="s">
+      <c r="B104" s="37"/>
+      <c r="C104" s="32" t="s">
         <v>106</v>
       </c>
-      <c r="D90" s="33"/>
-      <c r="E90" s="33"/>
-      <c r="F90" s="33"/>
-      <c r="G90" s="34"/>
+      <c r="D104" s="33"/>
+      <c r="E104" s="33"/>
+      <c r="F104" s="33"/>
+      <c r="G104" s="34"/>
     </row>
   </sheetData>
-  <mergeCells count="139">
-    <mergeCell ref="A87:B87"/>
-    <mergeCell ref="C87:G87"/>
-    <mergeCell ref="A88:B88"/>
-    <mergeCell ref="C88:G88"/>
-    <mergeCell ref="A89:B89"/>
-    <mergeCell ref="C89:G89"/>
-    <mergeCell ref="A90:B90"/>
-    <mergeCell ref="C90:G90"/>
-    <mergeCell ref="B82:C82"/>
-    <mergeCell ref="D82:E82"/>
-    <mergeCell ref="B83:C83"/>
-    <mergeCell ref="D83:E83"/>
-    <mergeCell ref="B84:C84"/>
-    <mergeCell ref="D84:E84"/>
-    <mergeCell ref="B85:C85"/>
-    <mergeCell ref="D85:E85"/>
-    <mergeCell ref="B86:C86"/>
-    <mergeCell ref="D86:E86"/>
-    <mergeCell ref="A76:G76"/>
-    <mergeCell ref="A77:B77"/>
-    <mergeCell ref="C77:G77"/>
-    <mergeCell ref="A78:B78"/>
-    <mergeCell ref="C78:G78"/>
-    <mergeCell ref="A79:B79"/>
-    <mergeCell ref="C79:G79"/>
-    <mergeCell ref="A80:G80"/>
-    <mergeCell ref="B81:C81"/>
-    <mergeCell ref="D81:E81"/>
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="C54:G54"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="C55:G55"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="C52:G52"/>
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="C53:G53"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="C46:G46"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="C47:G47"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="D51:E51"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="C48:G48"/>
-    <mergeCell ref="A49:G49"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="D50:E50"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="C38:G38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="C39:G39"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="C40:G40"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="C41:G41"/>
-    <mergeCell ref="A45:G45"/>
-    <mergeCell ref="A32:G32"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A3:G3"/>
-    <mergeCell ref="A7:G7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:G6"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:G4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:G5"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="D13:E13"/>
+  <mergeCells count="159">
+    <mergeCell ref="A103:B103"/>
+    <mergeCell ref="C103:G103"/>
+    <mergeCell ref="A104:B104"/>
+    <mergeCell ref="C104:G104"/>
+    <mergeCell ref="B100:C100"/>
+    <mergeCell ref="D100:E100"/>
+    <mergeCell ref="B98:C98"/>
+    <mergeCell ref="D98:E98"/>
+    <mergeCell ref="B99:C99"/>
+    <mergeCell ref="D99:E99"/>
+    <mergeCell ref="A101:B101"/>
+    <mergeCell ref="C101:G101"/>
+    <mergeCell ref="A102:B102"/>
+    <mergeCell ref="C102:G102"/>
+    <mergeCell ref="A92:G92"/>
+    <mergeCell ref="A93:B93"/>
+    <mergeCell ref="C93:G93"/>
+    <mergeCell ref="A94:B94"/>
+    <mergeCell ref="C94:G94"/>
+    <mergeCell ref="A95:B95"/>
+    <mergeCell ref="C95:G95"/>
+    <mergeCell ref="A96:G96"/>
+    <mergeCell ref="B97:C97"/>
+    <mergeCell ref="D97:E97"/>
+    <mergeCell ref="A70:B70"/>
+    <mergeCell ref="C70:G70"/>
+    <mergeCell ref="A71:B71"/>
+    <mergeCell ref="C71:G71"/>
+    <mergeCell ref="A72:B72"/>
+    <mergeCell ref="C72:G72"/>
+    <mergeCell ref="B63:C63"/>
+    <mergeCell ref="D63:E63"/>
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="D64:E64"/>
+    <mergeCell ref="A69:B69"/>
+    <mergeCell ref="C69:G69"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="D65:E65"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="D66:E66"/>
+    <mergeCell ref="B67:C67"/>
+    <mergeCell ref="D67:E67"/>
+    <mergeCell ref="B68:C68"/>
+    <mergeCell ref="D68:E68"/>
     <mergeCell ref="A60:B60"/>
     <mergeCell ref="C60:G60"/>
     <mergeCell ref="A61:B61"/>
@@ -3364,26 +3545,97 @@
     <mergeCell ref="C30:G30"/>
     <mergeCell ref="A31:B31"/>
     <mergeCell ref="C31:G31"/>
-    <mergeCell ref="A70:B70"/>
-    <mergeCell ref="C70:G70"/>
-    <mergeCell ref="A71:B71"/>
-    <mergeCell ref="C71:G71"/>
-    <mergeCell ref="A72:B72"/>
-    <mergeCell ref="C72:G72"/>
-    <mergeCell ref="B63:C63"/>
-    <mergeCell ref="D63:E63"/>
-    <mergeCell ref="B64:C64"/>
-    <mergeCell ref="D64:E64"/>
-    <mergeCell ref="A69:B69"/>
-    <mergeCell ref="C69:G69"/>
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="D65:E65"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="D66:E66"/>
-    <mergeCell ref="B67:C67"/>
-    <mergeCell ref="D67:E67"/>
-    <mergeCell ref="B68:C68"/>
-    <mergeCell ref="D68:E68"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A3:G3"/>
+    <mergeCell ref="A7:G7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:G6"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:G4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:G5"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="A32:G32"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="C38:G38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="C39:G39"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="C40:G40"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="C41:G41"/>
+    <mergeCell ref="A45:G45"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="C54:G54"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="C55:G55"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="C52:G52"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="C53:G53"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="C46:G46"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="C47:G47"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="D51:E51"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="C48:G48"/>
+    <mergeCell ref="A49:G49"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="D50:E50"/>
+    <mergeCell ref="A76:G76"/>
+    <mergeCell ref="A77:B77"/>
+    <mergeCell ref="C77:G77"/>
+    <mergeCell ref="A78:B78"/>
+    <mergeCell ref="C78:G78"/>
+    <mergeCell ref="A79:B79"/>
+    <mergeCell ref="C79:G79"/>
+    <mergeCell ref="A80:G80"/>
+    <mergeCell ref="B81:C81"/>
+    <mergeCell ref="D81:E81"/>
+    <mergeCell ref="A85:B85"/>
+    <mergeCell ref="C85:G85"/>
+    <mergeCell ref="A86:B86"/>
+    <mergeCell ref="C86:G86"/>
+    <mergeCell ref="A87:B87"/>
+    <mergeCell ref="C87:G87"/>
+    <mergeCell ref="A88:B88"/>
+    <mergeCell ref="C88:G88"/>
+    <mergeCell ref="B82:C82"/>
+    <mergeCell ref="D82:E82"/>
+    <mergeCell ref="B83:C83"/>
+    <mergeCell ref="D83:E83"/>
+    <mergeCell ref="B84:C84"/>
+    <mergeCell ref="D84:E84"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Added list of test in test report
</commit_message>
<xml_diff>
--- a/FYP documentation/FYP_Test_Plan.xlsx
+++ b/FYP documentation/FYP_Test_Plan.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="165">
   <si>
     <t>Expected Result</t>
   </si>
@@ -539,6 +539,18 @@
   </si>
   <si>
     <t>the pdf viewer close and logout</t>
+  </si>
+  <si>
+    <t>Cloud storage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Import files larger than 1GB                                     </t>
+  </si>
+  <si>
+    <t>The application should stop uploading files larger than 1 GB or if total space used is greater than 1GB</t>
+  </si>
+  <si>
+    <t>2. Check S3 if the importad files are binging added to cloud</t>
   </si>
 </sst>
 </file>
@@ -950,21 +962,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="6" xfId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1010,6 +1022,48 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="13" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="15" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="7" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="8" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="12" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1018,48 +1072,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="7" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="8" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="12" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="13" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="15" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2135,10 +2147,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I104"/>
+  <dimension ref="A1:I121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I65" sqref="I65"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2155,15 +2167,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="40.799999999999997" customHeight="1">
-      <c r="A1" s="62" t="s">
+      <c r="A1" s="66" t="s">
         <v>64</v>
       </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
-      <c r="F1" s="63"/>
-      <c r="G1" s="64"/>
+      <c r="B1" s="67"/>
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
+      <c r="F1" s="67"/>
+      <c r="G1" s="68"/>
       <c r="H1" s="16"/>
       <c r="I1" s="16"/>
     </row>
@@ -2247,11 +2259,11 @@
       <c r="A8" s="22" t="s">
         <v>77</v>
       </c>
-      <c r="B8" s="35" t="s">
+      <c r="B8" s="38" t="s">
         <v>69</v>
       </c>
       <c r="C8" s="31"/>
-      <c r="D8" s="35" t="s">
+      <c r="D8" s="38" t="s">
         <v>70</v>
       </c>
       <c r="E8" s="31"/>
@@ -2266,14 +2278,14 @@
       <c r="A9" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="38" t="s">
+      <c r="B9" s="36" t="s">
         <v>85</v>
       </c>
-      <c r="C9" s="39"/>
-      <c r="D9" s="38" t="s">
+      <c r="C9" s="37"/>
+      <c r="D9" s="36" t="s">
         <v>122</v>
       </c>
-      <c r="E9" s="39"/>
+      <c r="E9" s="37"/>
       <c r="F9" s="27" t="s">
         <v>90</v>
       </c>
@@ -2285,14 +2297,14 @@
       <c r="A10" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="38" t="s">
+      <c r="B10" s="36" t="s">
         <v>88</v>
       </c>
-      <c r="C10" s="39"/>
-      <c r="D10" s="38" t="s">
+      <c r="C10" s="37"/>
+      <c r="D10" s="36" t="s">
         <v>119</v>
       </c>
-      <c r="E10" s="60"/>
+      <c r="E10" s="55"/>
       <c r="F10" s="27" t="s">
         <v>119</v>
       </c>
@@ -2304,14 +2316,14 @@
       <c r="A11" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="38" t="s">
+      <c r="B11" s="36" t="s">
         <v>89</v>
       </c>
-      <c r="C11" s="39"/>
-      <c r="D11" s="38" t="s">
+      <c r="C11" s="37"/>
+      <c r="D11" s="36" t="s">
         <v>87</v>
       </c>
-      <c r="E11" s="39"/>
+      <c r="E11" s="37"/>
       <c r="F11" s="27" t="s">
         <v>123</v>
       </c>
@@ -2323,14 +2335,14 @@
       <c r="A12" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="38" t="s">
+      <c r="B12" s="36" t="s">
         <v>92</v>
       </c>
-      <c r="C12" s="60"/>
-      <c r="D12" s="38" t="s">
+      <c r="C12" s="55"/>
+      <c r="D12" s="36" t="s">
         <v>87</v>
       </c>
-      <c r="E12" s="39"/>
+      <c r="E12" s="37"/>
       <c r="F12" s="27" t="s">
         <v>123</v>
       </c>
@@ -2342,14 +2354,14 @@
       <c r="A13" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="B13" s="38" t="s">
+      <c r="B13" s="36" t="s">
         <v>120</v>
       </c>
-      <c r="C13" s="60"/>
-      <c r="D13" s="38" t="s">
+      <c r="C13" s="55"/>
+      <c r="D13" s="36" t="s">
         <v>87</v>
       </c>
-      <c r="E13" s="39"/>
+      <c r="E13" s="37"/>
       <c r="F13" s="27" t="s">
         <v>123</v>
       </c>
@@ -2361,14 +2373,14 @@
       <c r="A14" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="B14" s="61" t="s">
+      <c r="B14" s="56" t="s">
         <v>121</v>
       </c>
-      <c r="C14" s="61"/>
-      <c r="D14" s="38" t="s">
+      <c r="C14" s="56"/>
+      <c r="D14" s="36" t="s">
         <v>91</v>
       </c>
-      <c r="E14" s="60"/>
+      <c r="E14" s="55"/>
       <c r="F14" s="28" t="s">
         <v>119</v>
       </c>
@@ -2380,14 +2392,14 @@
       <c r="A15" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="B15" s="61" t="s">
+      <c r="B15" s="56" t="s">
         <v>93</v>
       </c>
-      <c r="C15" s="61"/>
-      <c r="D15" s="38" t="s">
+      <c r="C15" s="56"/>
+      <c r="D15" s="36" t="s">
         <v>87</v>
       </c>
-      <c r="E15" s="39"/>
+      <c r="E15" s="37"/>
       <c r="F15" s="28" t="s">
         <v>123</v>
       </c>
@@ -2399,14 +2411,14 @@
       <c r="A16" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="B16" s="61" t="s">
+      <c r="B16" s="56" t="s">
         <v>94</v>
       </c>
-      <c r="C16" s="61"/>
-      <c r="D16" s="38" t="s">
+      <c r="C16" s="56"/>
+      <c r="D16" s="36" t="s">
         <v>87</v>
       </c>
-      <c r="E16" s="39"/>
+      <c r="E16" s="37"/>
       <c r="F16" s="28" t="s">
         <v>123</v>
       </c>
@@ -2418,14 +2430,14 @@
       <c r="A17" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="B17" s="61" t="s">
+      <c r="B17" s="56" t="s">
         <v>95</v>
       </c>
-      <c r="C17" s="61"/>
-      <c r="D17" s="38" t="s">
+      <c r="C17" s="56"/>
+      <c r="D17" s="36" t="s">
         <v>91</v>
       </c>
-      <c r="E17" s="60"/>
+      <c r="E17" s="55"/>
       <c r="F17" s="28" t="s">
         <v>119</v>
       </c>
@@ -2434,7 +2446,7 @@
       </c>
     </row>
     <row r="18" spans="1:7">
-      <c r="A18" s="35" t="s">
+      <c r="A18" s="38" t="s">
         <v>74</v>
       </c>
       <c r="B18" s="31"/>
@@ -2447,11 +2459,11 @@
       <c r="G18" s="34"/>
     </row>
     <row r="19" spans="1:7">
-      <c r="A19" s="35" t="s">
+      <c r="A19" s="38" t="s">
         <v>75</v>
       </c>
       <c r="B19" s="31"/>
-      <c r="C19" s="36">
+      <c r="C19" s="39">
         <v>43014</v>
       </c>
       <c r="D19" s="33"/>
@@ -2476,7 +2488,7 @@
       <c r="A21" s="30" t="s">
         <v>73</v>
       </c>
-      <c r="B21" s="37"/>
+      <c r="B21" s="35"/>
       <c r="C21" s="32" t="s">
         <v>106</v>
       </c>
@@ -2543,17 +2555,17 @@
       <c r="G28" s="40"/>
     </row>
     <row r="29" spans="1:7" ht="15" thickTop="1">
-      <c r="A29" s="65" t="s">
+      <c r="A29" s="59" t="s">
         <v>66</v>
       </c>
-      <c r="B29" s="66"/>
-      <c r="C29" s="67" t="s">
+      <c r="B29" s="60"/>
+      <c r="C29" s="61" t="s">
         <v>78</v>
       </c>
-      <c r="D29" s="68"/>
-      <c r="E29" s="68"/>
-      <c r="F29" s="68"/>
-      <c r="G29" s="69"/>
+      <c r="D29" s="62"/>
+      <c r="E29" s="62"/>
+      <c r="F29" s="62"/>
+      <c r="G29" s="63"/>
     </row>
     <row r="30" spans="1:7">
       <c r="A30" s="41" t="s">
@@ -2574,29 +2586,29 @@
       <c r="C31" s="49" t="s">
         <v>79</v>
       </c>
-      <c r="D31" s="70"/>
-      <c r="E31" s="70"/>
-      <c r="F31" s="70"/>
-      <c r="G31" s="71"/>
+      <c r="D31" s="64"/>
+      <c r="E31" s="64"/>
+      <c r="F31" s="64"/>
+      <c r="G31" s="65"/>
     </row>
     <row r="32" spans="1:7">
-      <c r="A32" s="55"/>
-      <c r="B32" s="56"/>
-      <c r="C32" s="56"/>
-      <c r="D32" s="56"/>
-      <c r="E32" s="56"/>
-      <c r="F32" s="56"/>
-      <c r="G32" s="57"/>
+      <c r="A32" s="69"/>
+      <c r="B32" s="70"/>
+      <c r="C32" s="70"/>
+      <c r="D32" s="70"/>
+      <c r="E32" s="70"/>
+      <c r="F32" s="70"/>
+      <c r="G32" s="71"/>
     </row>
     <row r="33" spans="1:7">
       <c r="A33" s="22" t="s">
         <v>77</v>
       </c>
-      <c r="B33" s="35" t="s">
+      <c r="B33" s="38" t="s">
         <v>69</v>
       </c>
       <c r="C33" s="31"/>
-      <c r="D33" s="35" t="s">
+      <c r="D33" s="38" t="s">
         <v>70</v>
       </c>
       <c r="E33" s="31"/>
@@ -2611,10 +2623,10 @@
       <c r="A34" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="B34" s="58" t="s">
+      <c r="B34" s="57" t="s">
         <v>111</v>
       </c>
-      <c r="C34" s="59"/>
+      <c r="C34" s="58"/>
       <c r="D34" s="32" t="s">
         <v>72</v>
       </c>
@@ -2630,14 +2642,14 @@
       <c r="A35" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="B35" s="58" t="s">
+      <c r="B35" s="57" t="s">
         <v>50</v>
       </c>
-      <c r="C35" s="59"/>
-      <c r="D35" s="38" t="s">
+      <c r="C35" s="58"/>
+      <c r="D35" s="36" t="s">
         <v>86</v>
       </c>
-      <c r="E35" s="60"/>
+      <c r="E35" s="55"/>
       <c r="F35" s="20" t="s">
         <v>108</v>
       </c>
@@ -2649,14 +2661,14 @@
       <c r="A36" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="B36" s="58" t="s">
+      <c r="B36" s="57" t="s">
         <v>49</v>
       </c>
-      <c r="C36" s="59"/>
-      <c r="D36" s="38" t="s">
+      <c r="C36" s="58"/>
+      <c r="D36" s="36" t="s">
         <v>80</v>
       </c>
-      <c r="E36" s="60"/>
+      <c r="E36" s="55"/>
       <c r="F36" s="20" t="s">
         <v>109</v>
       </c>
@@ -2668,14 +2680,14 @@
       <c r="A37" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="B37" s="58" t="s">
+      <c r="B37" s="57" t="s">
         <v>81</v>
       </c>
-      <c r="C37" s="59"/>
-      <c r="D37" s="38" t="s">
+      <c r="C37" s="58"/>
+      <c r="D37" s="36" t="s">
         <v>82</v>
       </c>
-      <c r="E37" s="60"/>
+      <c r="E37" s="55"/>
       <c r="F37" s="20" t="s">
         <v>107</v>
       </c>
@@ -2684,7 +2696,7 @@
       </c>
     </row>
     <row r="38" spans="1:7">
-      <c r="A38" s="35" t="s">
+      <c r="A38" s="38" t="s">
         <v>74</v>
       </c>
       <c r="B38" s="31"/>
@@ -2697,11 +2709,11 @@
       <c r="G38" s="34"/>
     </row>
     <row r="39" spans="1:7">
-      <c r="A39" s="35" t="s">
+      <c r="A39" s="38" t="s">
         <v>75</v>
       </c>
       <c r="B39" s="31"/>
-      <c r="C39" s="36">
+      <c r="C39" s="39">
         <v>43042</v>
       </c>
       <c r="D39" s="33"/>
@@ -2713,7 +2725,7 @@
       <c r="A40" s="30" t="s">
         <v>76</v>
       </c>
-      <c r="B40" s="37"/>
+      <c r="B40" s="35"/>
       <c r="C40" s="32" t="s">
         <v>113</v>
       </c>
@@ -2726,7 +2738,7 @@
       <c r="A41" s="30" t="s">
         <v>73</v>
       </c>
-      <c r="B41" s="37"/>
+      <c r="B41" s="35"/>
       <c r="C41" s="32" t="s">
         <v>106</v>
       </c>
@@ -2796,11 +2808,11 @@
       <c r="A50" s="22" t="s">
         <v>77</v>
       </c>
-      <c r="B50" s="35" t="s">
+      <c r="B50" s="38" t="s">
         <v>69</v>
       </c>
       <c r="C50" s="31"/>
-      <c r="D50" s="35" t="s">
+      <c r="D50" s="38" t="s">
         <v>70</v>
       </c>
       <c r="E50" s="31"/>
@@ -2815,14 +2827,14 @@
       <c r="A51" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="B51" s="38" t="s">
+      <c r="B51" s="36" t="s">
         <v>100</v>
       </c>
-      <c r="C51" s="39"/>
-      <c r="D51" s="38" t="s">
+      <c r="C51" s="37"/>
+      <c r="D51" s="36" t="s">
         <v>98</v>
       </c>
-      <c r="E51" s="39"/>
+      <c r="E51" s="37"/>
       <c r="F51" s="29" t="s">
         <v>136</v>
       </c>
@@ -2844,11 +2856,11 @@
       <c r="G52" s="34"/>
     </row>
     <row r="53" spans="1:7" ht="22.8" customHeight="1">
-      <c r="A53" s="35" t="s">
+      <c r="A53" s="38" t="s">
         <v>75</v>
       </c>
       <c r="B53" s="31"/>
-      <c r="C53" s="36">
+      <c r="C53" s="39">
         <v>43046</v>
       </c>
       <c r="D53" s="33"/>
@@ -2873,7 +2885,7 @@
       <c r="A55" s="30" t="s">
         <v>73</v>
       </c>
-      <c r="B55" s="37"/>
+      <c r="B55" s="35"/>
       <c r="C55" s="32" t="s">
         <v>106</v>
       </c>
@@ -2943,11 +2955,11 @@
       <c r="A63" s="22" t="s">
         <v>77</v>
       </c>
-      <c r="B63" s="35" t="s">
+      <c r="B63" s="38" t="s">
         <v>69</v>
       </c>
       <c r="C63" s="31"/>
-      <c r="D63" s="35" t="s">
+      <c r="D63" s="38" t="s">
         <v>70</v>
       </c>
       <c r="E63" s="31"/>
@@ -2962,14 +2974,14 @@
       <c r="A64" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="B64" s="38" t="s">
+      <c r="B64" s="36" t="s">
         <v>104</v>
       </c>
-      <c r="C64" s="39"/>
-      <c r="D64" s="38" t="s">
+      <c r="C64" s="37"/>
+      <c r="D64" s="36" t="s">
         <v>105</v>
       </c>
-      <c r="E64" s="39"/>
+      <c r="E64" s="37"/>
       <c r="F64" s="29" t="s">
         <v>125</v>
       </c>
@@ -2981,14 +2993,14 @@
       <c r="A65" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="B65" s="38" t="s">
+      <c r="B65" s="36" t="s">
         <v>114</v>
       </c>
-      <c r="C65" s="39"/>
-      <c r="D65" s="38" t="s">
+      <c r="C65" s="37"/>
+      <c r="D65" s="36" t="s">
         <v>115</v>
       </c>
-      <c r="E65" s="39"/>
+      <c r="E65" s="37"/>
       <c r="F65" s="29" t="s">
         <v>126</v>
       </c>
@@ -3000,14 +3012,14 @@
       <c r="A66" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="B66" s="38" t="s">
+      <c r="B66" s="36" t="s">
         <v>116</v>
       </c>
-      <c r="C66" s="39"/>
-      <c r="D66" s="38" t="s">
+      <c r="C66" s="37"/>
+      <c r="D66" s="36" t="s">
         <v>117</v>
       </c>
-      <c r="E66" s="39"/>
+      <c r="E66" s="37"/>
       <c r="F66" s="29" t="s">
         <v>127</v>
       </c>
@@ -3019,14 +3031,14 @@
       <c r="A67" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="B67" s="38" t="s">
+      <c r="B67" s="36" t="s">
         <v>129</v>
       </c>
-      <c r="C67" s="39"/>
-      <c r="D67" s="38" t="s">
+      <c r="C67" s="37"/>
+      <c r="D67" s="36" t="s">
         <v>118</v>
       </c>
-      <c r="E67" s="39"/>
+      <c r="E67" s="37"/>
       <c r="F67" s="29" t="s">
         <v>128</v>
       </c>
@@ -3038,14 +3050,14 @@
       <c r="A68" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="B68" s="38" t="s">
+      <c r="B68" s="36" t="s">
         <v>131</v>
       </c>
-      <c r="C68" s="39"/>
-      <c r="D68" s="38" t="s">
+      <c r="C68" s="37"/>
+      <c r="D68" s="36" t="s">
         <v>130</v>
       </c>
-      <c r="E68" s="39"/>
+      <c r="E68" s="37"/>
       <c r="F68" s="29" t="s">
         <v>132</v>
       </c>
@@ -3067,11 +3079,11 @@
       <c r="G69" s="34"/>
     </row>
     <row r="70" spans="1:7">
-      <c r="A70" s="35" t="s">
+      <c r="A70" s="38" t="s">
         <v>75</v>
       </c>
       <c r="B70" s="31"/>
-      <c r="C70" s="36">
+      <c r="C70" s="39">
         <v>43045</v>
       </c>
       <c r="D70" s="33"/>
@@ -3096,7 +3108,7 @@
       <c r="A72" s="30" t="s">
         <v>73</v>
       </c>
-      <c r="B72" s="37"/>
+      <c r="B72" s="35"/>
       <c r="C72" s="32" t="s">
         <v>106</v>
       </c>
@@ -3166,11 +3178,11 @@
       <c r="A81" s="22" t="s">
         <v>77</v>
       </c>
-      <c r="B81" s="35" t="s">
+      <c r="B81" s="38" t="s">
         <v>69</v>
       </c>
       <c r="C81" s="31"/>
-      <c r="D81" s="35" t="s">
+      <c r="D81" s="38" t="s">
         <v>70</v>
       </c>
       <c r="E81" s="31"/>
@@ -3185,14 +3197,14 @@
       <c r="A82" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="B82" s="38" t="s">
+      <c r="B82" s="36" t="s">
         <v>139</v>
       </c>
-      <c r="C82" s="39"/>
-      <c r="D82" s="38" t="s">
+      <c r="C82" s="37"/>
+      <c r="D82" s="36" t="s">
         <v>141</v>
       </c>
-      <c r="E82" s="39"/>
+      <c r="E82" s="37"/>
       <c r="F82" s="29" t="s">
         <v>142</v>
       </c>
@@ -3204,14 +3216,14 @@
       <c r="A83" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="B83" s="38" t="s">
+      <c r="B83" s="36" t="s">
         <v>140</v>
       </c>
-      <c r="C83" s="39"/>
-      <c r="D83" s="38" t="s">
+      <c r="C83" s="37"/>
+      <c r="D83" s="36" t="s">
         <v>143</v>
       </c>
-      <c r="E83" s="39"/>
+      <c r="E83" s="37"/>
       <c r="F83" s="29" t="s">
         <v>144</v>
       </c>
@@ -3223,14 +3235,14 @@
       <c r="A84" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="B84" s="38" t="s">
+      <c r="B84" s="36" t="s">
         <v>145</v>
       </c>
-      <c r="C84" s="39"/>
-      <c r="D84" s="38" t="s">
+      <c r="C84" s="37"/>
+      <c r="D84" s="36" t="s">
         <v>146</v>
       </c>
-      <c r="E84" s="39"/>
+      <c r="E84" s="37"/>
       <c r="F84" s="29" t="s">
         <v>147</v>
       </c>
@@ -3252,11 +3264,11 @@
       <c r="G85" s="34"/>
     </row>
     <row r="86" spans="1:7">
-      <c r="A86" s="35" t="s">
+      <c r="A86" s="38" t="s">
         <v>75</v>
       </c>
       <c r="B86" s="31"/>
-      <c r="C86" s="36">
+      <c r="C86" s="39">
         <v>43046</v>
       </c>
       <c r="D86" s="33"/>
@@ -3281,7 +3293,7 @@
       <c r="A88" s="30" t="s">
         <v>73</v>
       </c>
-      <c r="B88" s="37"/>
+      <c r="B88" s="35"/>
       <c r="C88" s="32" t="s">
         <v>106</v>
       </c>
@@ -3351,11 +3363,11 @@
       <c r="A97" s="22" t="s">
         <v>77</v>
       </c>
-      <c r="B97" s="35" t="s">
+      <c r="B97" s="38" t="s">
         <v>69</v>
       </c>
       <c r="C97" s="31"/>
-      <c r="D97" s="35" t="s">
+      <c r="D97" s="38" t="s">
         <v>70</v>
       </c>
       <c r="E97" s="31"/>
@@ -3370,14 +3382,14 @@
       <c r="A98" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="B98" s="38" t="s">
+      <c r="B98" s="36" t="s">
         <v>150</v>
       </c>
-      <c r="C98" s="39"/>
-      <c r="D98" s="38" t="s">
+      <c r="C98" s="37"/>
+      <c r="D98" s="36" t="s">
         <v>151</v>
       </c>
-      <c r="E98" s="39"/>
+      <c r="E98" s="37"/>
       <c r="F98" s="29" t="s">
         <v>152</v>
       </c>
@@ -3389,14 +3401,14 @@
       <c r="A99" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="B99" s="38" t="s">
+      <c r="B99" s="36" t="s">
         <v>154</v>
       </c>
-      <c r="C99" s="39"/>
-      <c r="D99" s="38" t="s">
+      <c r="C99" s="37"/>
+      <c r="D99" s="36" t="s">
         <v>155</v>
       </c>
-      <c r="E99" s="39"/>
+      <c r="E99" s="37"/>
       <c r="F99" s="29" t="s">
         <v>156</v>
       </c>
@@ -3408,14 +3420,14 @@
       <c r="A100" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="B100" s="38" t="s">
+      <c r="B100" s="36" t="s">
         <v>158</v>
       </c>
-      <c r="C100" s="39"/>
-      <c r="D100" s="38" t="s">
+      <c r="C100" s="37"/>
+      <c r="D100" s="36" t="s">
         <v>159</v>
       </c>
-      <c r="E100" s="39"/>
+      <c r="E100" s="37"/>
       <c r="F100" s="29" t="s">
         <v>160</v>
       </c>
@@ -3437,11 +3449,11 @@
       <c r="G101" s="34"/>
     </row>
     <row r="102" spans="1:7">
-      <c r="A102" s="35" t="s">
+      <c r="A102" s="38" t="s">
         <v>75</v>
       </c>
       <c r="B102" s="31"/>
-      <c r="C102" s="36">
+      <c r="C102" s="39">
         <v>43046</v>
       </c>
       <c r="D102" s="33"/>
@@ -3466,7 +3478,7 @@
       <c r="A104" s="30" t="s">
         <v>73</v>
       </c>
-      <c r="B104" s="37"/>
+      <c r="B104" s="35"/>
       <c r="C104" s="32" t="s">
         <v>106</v>
       </c>
@@ -3475,52 +3487,306 @@
       <c r="F104" s="33"/>
       <c r="G104" s="34"/>
     </row>
+    <row r="109" spans="1:7" ht="20.399999999999999" thickBot="1">
+      <c r="A109" s="40" t="s">
+        <v>161</v>
+      </c>
+      <c r="B109" s="40"/>
+      <c r="C109" s="40"/>
+      <c r="D109" s="40"/>
+      <c r="E109" s="40"/>
+      <c r="F109" s="40"/>
+      <c r="G109" s="40"/>
+    </row>
+    <row r="110" spans="1:7" ht="15" thickTop="1">
+      <c r="A110" s="41" t="s">
+        <v>66</v>
+      </c>
+      <c r="B110" s="42"/>
+      <c r="C110" s="43" t="s">
+        <v>135</v>
+      </c>
+      <c r="D110" s="44"/>
+      <c r="E110" s="44"/>
+      <c r="F110" s="44"/>
+      <c r="G110" s="45"/>
+    </row>
+    <row r="111" spans="1:7">
+      <c r="A111" s="41" t="s">
+        <v>67</v>
+      </c>
+      <c r="B111" s="42"/>
+      <c r="C111" s="46"/>
+      <c r="D111" s="47"/>
+      <c r="E111" s="47"/>
+      <c r="F111" s="47"/>
+      <c r="G111" s="48"/>
+    </row>
+    <row r="112" spans="1:7">
+      <c r="A112" s="41" t="s">
+        <v>68</v>
+      </c>
+      <c r="B112" s="42"/>
+      <c r="C112" s="49"/>
+      <c r="D112" s="50"/>
+      <c r="E112" s="50"/>
+      <c r="F112" s="50"/>
+      <c r="G112" s="51"/>
+    </row>
+    <row r="113" spans="1:7">
+      <c r="A113" s="52"/>
+      <c r="B113" s="53"/>
+      <c r="C113" s="53"/>
+      <c r="D113" s="53"/>
+      <c r="E113" s="53"/>
+      <c r="F113" s="53"/>
+      <c r="G113" s="54"/>
+    </row>
+    <row r="114" spans="1:7">
+      <c r="A114" s="22" t="s">
+        <v>77</v>
+      </c>
+      <c r="B114" s="38" t="s">
+        <v>69</v>
+      </c>
+      <c r="C114" s="31"/>
+      <c r="D114" s="38" t="s">
+        <v>70</v>
+      </c>
+      <c r="E114" s="31"/>
+      <c r="F114" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="G114" s="22" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" ht="61.2" customHeight="1">
+      <c r="A115" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="B115" s="36" t="s">
+        <v>162</v>
+      </c>
+      <c r="C115" s="37"/>
+      <c r="D115" s="36" t="s">
+        <v>163</v>
+      </c>
+      <c r="E115" s="37"/>
+      <c r="F115" s="29" t="s">
+        <v>152</v>
+      </c>
+      <c r="G115" s="29" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" ht="34.799999999999997" customHeight="1">
+      <c r="A116" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="B116" s="36" t="s">
+        <v>164</v>
+      </c>
+      <c r="C116" s="37"/>
+      <c r="D116" s="36" t="s">
+        <v>155</v>
+      </c>
+      <c r="E116" s="37"/>
+      <c r="F116" s="29" t="s">
+        <v>156</v>
+      </c>
+      <c r="G116" s="29" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7">
+      <c r="A117" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="B117" s="36" t="s">
+        <v>158</v>
+      </c>
+      <c r="C117" s="37"/>
+      <c r="D117" s="36" t="s">
+        <v>159</v>
+      </c>
+      <c r="E117" s="37"/>
+      <c r="F117" s="29" t="s">
+        <v>160</v>
+      </c>
+      <c r="G117" s="29" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7">
+      <c r="A118" s="30" t="s">
+        <v>74</v>
+      </c>
+      <c r="B118" s="31"/>
+      <c r="C118" s="32" t="s">
+        <v>112</v>
+      </c>
+      <c r="D118" s="33"/>
+      <c r="E118" s="33"/>
+      <c r="F118" s="33"/>
+      <c r="G118" s="34"/>
+    </row>
+    <row r="119" spans="1:7">
+      <c r="A119" s="38" t="s">
+        <v>75</v>
+      </c>
+      <c r="B119" s="31"/>
+      <c r="C119" s="39">
+        <v>43046</v>
+      </c>
+      <c r="D119" s="33"/>
+      <c r="E119" s="33"/>
+      <c r="F119" s="33"/>
+      <c r="G119" s="34"/>
+    </row>
+    <row r="120" spans="1:7">
+      <c r="A120" s="30" t="s">
+        <v>76</v>
+      </c>
+      <c r="B120" s="31"/>
+      <c r="C120" s="32" t="s">
+        <v>157</v>
+      </c>
+      <c r="D120" s="33"/>
+      <c r="E120" s="33"/>
+      <c r="F120" s="33"/>
+      <c r="G120" s="34"/>
+    </row>
+    <row r="121" spans="1:7">
+      <c r="A121" s="30" t="s">
+        <v>73</v>
+      </c>
+      <c r="B121" s="35"/>
+      <c r="C121" s="32" t="s">
+        <v>106</v>
+      </c>
+      <c r="D121" s="33"/>
+      <c r="E121" s="33"/>
+      <c r="F121" s="33"/>
+      <c r="G121" s="34"/>
+    </row>
   </sheetData>
-  <mergeCells count="159">
-    <mergeCell ref="A103:B103"/>
-    <mergeCell ref="C103:G103"/>
-    <mergeCell ref="A104:B104"/>
-    <mergeCell ref="C104:G104"/>
-    <mergeCell ref="B100:C100"/>
-    <mergeCell ref="D100:E100"/>
-    <mergeCell ref="B98:C98"/>
-    <mergeCell ref="D98:E98"/>
-    <mergeCell ref="B99:C99"/>
-    <mergeCell ref="D99:E99"/>
-    <mergeCell ref="A101:B101"/>
-    <mergeCell ref="C101:G101"/>
-    <mergeCell ref="A102:B102"/>
-    <mergeCell ref="C102:G102"/>
-    <mergeCell ref="A92:G92"/>
-    <mergeCell ref="A93:B93"/>
-    <mergeCell ref="C93:G93"/>
-    <mergeCell ref="A94:B94"/>
-    <mergeCell ref="C94:G94"/>
-    <mergeCell ref="A95:B95"/>
-    <mergeCell ref="C95:G95"/>
-    <mergeCell ref="A96:G96"/>
-    <mergeCell ref="B97:C97"/>
-    <mergeCell ref="D97:E97"/>
-    <mergeCell ref="A70:B70"/>
-    <mergeCell ref="C70:G70"/>
-    <mergeCell ref="A71:B71"/>
-    <mergeCell ref="C71:G71"/>
-    <mergeCell ref="A72:B72"/>
-    <mergeCell ref="C72:G72"/>
-    <mergeCell ref="B63:C63"/>
-    <mergeCell ref="D63:E63"/>
-    <mergeCell ref="B64:C64"/>
-    <mergeCell ref="D64:E64"/>
-    <mergeCell ref="A69:B69"/>
-    <mergeCell ref="C69:G69"/>
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="D65:E65"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="D66:E66"/>
-    <mergeCell ref="B67:C67"/>
-    <mergeCell ref="D67:E67"/>
-    <mergeCell ref="B68:C68"/>
-    <mergeCell ref="D68:E68"/>
+  <mergeCells count="183">
+    <mergeCell ref="A120:B120"/>
+    <mergeCell ref="C120:G120"/>
+    <mergeCell ref="A121:B121"/>
+    <mergeCell ref="C121:G121"/>
+    <mergeCell ref="B115:C115"/>
+    <mergeCell ref="D115:E115"/>
+    <mergeCell ref="B116:C116"/>
+    <mergeCell ref="D116:E116"/>
+    <mergeCell ref="B117:C117"/>
+    <mergeCell ref="D117:E117"/>
+    <mergeCell ref="A118:B118"/>
+    <mergeCell ref="C118:G118"/>
+    <mergeCell ref="A119:B119"/>
+    <mergeCell ref="C119:G119"/>
+    <mergeCell ref="A109:G109"/>
+    <mergeCell ref="A110:B110"/>
+    <mergeCell ref="C110:G110"/>
+    <mergeCell ref="A111:B111"/>
+    <mergeCell ref="C111:G111"/>
+    <mergeCell ref="A112:B112"/>
+    <mergeCell ref="C112:G112"/>
+    <mergeCell ref="A113:G113"/>
+    <mergeCell ref="B114:C114"/>
+    <mergeCell ref="D114:E114"/>
+    <mergeCell ref="A85:B85"/>
+    <mergeCell ref="C85:G85"/>
+    <mergeCell ref="A86:B86"/>
+    <mergeCell ref="C86:G86"/>
+    <mergeCell ref="A87:B87"/>
+    <mergeCell ref="C87:G87"/>
+    <mergeCell ref="A88:B88"/>
+    <mergeCell ref="C88:G88"/>
+    <mergeCell ref="B82:C82"/>
+    <mergeCell ref="D82:E82"/>
+    <mergeCell ref="B83:C83"/>
+    <mergeCell ref="D83:E83"/>
+    <mergeCell ref="B84:C84"/>
+    <mergeCell ref="D84:E84"/>
+    <mergeCell ref="A76:G76"/>
+    <mergeCell ref="A77:B77"/>
+    <mergeCell ref="C77:G77"/>
+    <mergeCell ref="A78:B78"/>
+    <mergeCell ref="C78:G78"/>
+    <mergeCell ref="A79:B79"/>
+    <mergeCell ref="C79:G79"/>
+    <mergeCell ref="A80:G80"/>
+    <mergeCell ref="B81:C81"/>
+    <mergeCell ref="D81:E81"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="C54:G54"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="C55:G55"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="C52:G52"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="C53:G53"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="C46:G46"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="C47:G47"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="D51:E51"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="C48:G48"/>
+    <mergeCell ref="A49:G49"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="D50:E50"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="C38:G38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="C39:G39"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="C40:G40"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="C41:G41"/>
+    <mergeCell ref="A45:G45"/>
+    <mergeCell ref="A32:G32"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A3:G3"/>
+    <mergeCell ref="A7:G7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:G6"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:G4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:G5"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="D13:E13"/>
     <mergeCell ref="A60:B60"/>
     <mergeCell ref="C60:G60"/>
     <mergeCell ref="A61:B61"/>
@@ -3545,97 +3811,50 @@
     <mergeCell ref="C30:G30"/>
     <mergeCell ref="A31:B31"/>
     <mergeCell ref="C31:G31"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A3:G3"/>
-    <mergeCell ref="A7:G7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:G6"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:G4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:G5"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="A32:G32"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="C38:G38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="C39:G39"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="C40:G40"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="C41:G41"/>
-    <mergeCell ref="A45:G45"/>
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="C54:G54"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="C55:G55"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="C52:G52"/>
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="C53:G53"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="C46:G46"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="C47:G47"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="D51:E51"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="C48:G48"/>
-    <mergeCell ref="A49:G49"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="D50:E50"/>
-    <mergeCell ref="A76:G76"/>
-    <mergeCell ref="A77:B77"/>
-    <mergeCell ref="C77:G77"/>
-    <mergeCell ref="A78:B78"/>
-    <mergeCell ref="C78:G78"/>
-    <mergeCell ref="A79:B79"/>
-    <mergeCell ref="C79:G79"/>
-    <mergeCell ref="A80:G80"/>
-    <mergeCell ref="B81:C81"/>
-    <mergeCell ref="D81:E81"/>
-    <mergeCell ref="A85:B85"/>
-    <mergeCell ref="C85:G85"/>
-    <mergeCell ref="A86:B86"/>
-    <mergeCell ref="C86:G86"/>
-    <mergeCell ref="A87:B87"/>
-    <mergeCell ref="C87:G87"/>
-    <mergeCell ref="A88:B88"/>
-    <mergeCell ref="C88:G88"/>
-    <mergeCell ref="B82:C82"/>
-    <mergeCell ref="D82:E82"/>
-    <mergeCell ref="B83:C83"/>
-    <mergeCell ref="D83:E83"/>
-    <mergeCell ref="B84:C84"/>
-    <mergeCell ref="D84:E84"/>
+    <mergeCell ref="A70:B70"/>
+    <mergeCell ref="C70:G70"/>
+    <mergeCell ref="A71:B71"/>
+    <mergeCell ref="C71:G71"/>
+    <mergeCell ref="A72:B72"/>
+    <mergeCell ref="C72:G72"/>
+    <mergeCell ref="B63:C63"/>
+    <mergeCell ref="D63:E63"/>
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="D64:E64"/>
+    <mergeCell ref="A69:B69"/>
+    <mergeCell ref="C69:G69"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="D65:E65"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="D66:E66"/>
+    <mergeCell ref="B67:C67"/>
+    <mergeCell ref="D67:E67"/>
+    <mergeCell ref="B68:C68"/>
+    <mergeCell ref="D68:E68"/>
+    <mergeCell ref="A92:G92"/>
+    <mergeCell ref="A93:B93"/>
+    <mergeCell ref="C93:G93"/>
+    <mergeCell ref="A94:B94"/>
+    <mergeCell ref="C94:G94"/>
+    <mergeCell ref="A95:B95"/>
+    <mergeCell ref="C95:G95"/>
+    <mergeCell ref="A96:G96"/>
+    <mergeCell ref="B97:C97"/>
+    <mergeCell ref="D97:E97"/>
+    <mergeCell ref="A103:B103"/>
+    <mergeCell ref="C103:G103"/>
+    <mergeCell ref="A104:B104"/>
+    <mergeCell ref="C104:G104"/>
+    <mergeCell ref="B100:C100"/>
+    <mergeCell ref="D100:E100"/>
+    <mergeCell ref="B98:C98"/>
+    <mergeCell ref="D98:E98"/>
+    <mergeCell ref="B99:C99"/>
+    <mergeCell ref="D99:E99"/>
+    <mergeCell ref="A101:B101"/>
+    <mergeCell ref="C101:G101"/>
+    <mergeCell ref="A102:B102"/>
+    <mergeCell ref="C102:G102"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Fixed error in signup and added more test caseses
</commit_message>
<xml_diff>
--- a/FYP documentation/FYP_Test_Plan.xlsx
+++ b/FYP documentation/FYP_Test_Plan.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="226">
   <si>
     <t>Expected Result</t>
   </si>
@@ -239,9 +239,6 @@
     <t>Test Plan</t>
   </si>
   <si>
-    <t>Login</t>
-  </si>
-  <si>
     <t>Objective</t>
   </si>
   <si>
@@ -294,9 +291,6 @@
     <t>Login fail</t>
   </si>
   <si>
-    <t>Sign up</t>
-  </si>
-  <si>
     <t>Test plan for Signup</t>
   </si>
   <si>
@@ -350,16 +344,10 @@
     <t>The first device should log out</t>
   </si>
   <si>
-    <t>Instance ID Verification</t>
-  </si>
-  <si>
     <t>1. Login to first device.               2. Login to second device</t>
   </si>
   <si>
     <t>The user should have previously signed up</t>
-  </si>
-  <si>
-    <t>Home page</t>
   </si>
   <si>
     <t>Test if home page is functional</t>
@@ -457,9 +445,6 @@
     <t>1439 hrs</t>
   </si>
   <si>
-    <t>File operation</t>
-  </si>
-  <si>
     <t>Test if file operation</t>
   </si>
   <si>
@@ -501,9 +486,6 @@
     <t>All files are delete</t>
   </si>
   <si>
-    <t>PDF Viewer</t>
-  </si>
-  <si>
     <t>Test if file operation works as per requirement</t>
   </si>
   <si>
@@ -541,16 +523,225 @@
     <t>the pdf viewer close and logout</t>
   </si>
   <si>
-    <t>Cloud storage</t>
-  </si>
-  <si>
     <t xml:space="preserve">1. Import files larger than 1GB                                     </t>
   </si>
   <si>
     <t>The application should stop uploading files larger than 1 GB or if total space used is greater than 1GB</t>
   </si>
   <si>
-    <t>2. Check S3 if the importad files are binging added to cloud</t>
+    <t xml:space="preserve"> A error message is printed and upload fail</t>
+  </si>
+  <si>
+    <t>The afile is uploaded to S3</t>
+  </si>
+  <si>
+    <t>The file is visible in S3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Enter password 4 times  </t>
+  </si>
+  <si>
+    <t>A delay timee of 10 second should starts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. After timer stops in previous test case and enter another invalid password.
+2. Close the app while the timer is running.
+3. Open the app 
+</t>
+  </si>
+  <si>
+    <t>The timer should run for 20 sec and on reopening the app the timer should continue from where it left off.</t>
+  </si>
+  <si>
+    <t>The delay run for 20 sec and on reopening it continue form the 12 sec (where it left off).</t>
+  </si>
+  <si>
+    <t>1730 hrs</t>
+  </si>
+  <si>
+    <t>The user should have logged in to the system</t>
+  </si>
+  <si>
+    <t>1. Sign up</t>
+  </si>
+  <si>
+    <t>TC1-001</t>
+  </si>
+  <si>
+    <t>TC2-002</t>
+  </si>
+  <si>
+    <t>TC1-002</t>
+  </si>
+  <si>
+    <t>TC1-003</t>
+  </si>
+  <si>
+    <t>TC1-004</t>
+  </si>
+  <si>
+    <t>TC1-005</t>
+  </si>
+  <si>
+    <t>TC1-006</t>
+  </si>
+  <si>
+    <t>TC1-007</t>
+  </si>
+  <si>
+    <t>TC1-008</t>
+  </si>
+  <si>
+    <t>TC1-009</t>
+  </si>
+  <si>
+    <t>TC2-001</t>
+  </si>
+  <si>
+    <t>2. Login</t>
+  </si>
+  <si>
+    <t>TC2-003</t>
+  </si>
+  <si>
+    <t>TC2-004</t>
+  </si>
+  <si>
+    <t>TC2-005</t>
+  </si>
+  <si>
+    <t>TC2-006</t>
+  </si>
+  <si>
+    <t>TC3-001</t>
+  </si>
+  <si>
+    <t>3. Instance ID Verification</t>
+  </si>
+  <si>
+    <t>TC4-001</t>
+  </si>
+  <si>
+    <t>TC4-002</t>
+  </si>
+  <si>
+    <t>TC4-003</t>
+  </si>
+  <si>
+    <t>TC4-004</t>
+  </si>
+  <si>
+    <t>TC4-005</t>
+  </si>
+  <si>
+    <t>4. Home page</t>
+  </si>
+  <si>
+    <t>TC6-001</t>
+  </si>
+  <si>
+    <t>TC6-002</t>
+  </si>
+  <si>
+    <t>TC6-003</t>
+  </si>
+  <si>
+    <t>5. PDF Viewer</t>
+  </si>
+  <si>
+    <t>9. File operation</t>
+  </si>
+  <si>
+    <t>TC9-001</t>
+  </si>
+  <si>
+    <t>TC9-002</t>
+  </si>
+  <si>
+    <t>TC9-003</t>
+  </si>
+  <si>
+    <t>13. Cloud storage</t>
+  </si>
+  <si>
+    <t>TC13-001</t>
+  </si>
+  <si>
+    <t>TC13-002</t>
+  </si>
+  <si>
+    <t>14. Change user</t>
+  </si>
+  <si>
+    <t>Test if cloud storage function properly</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Add area and a file 
+2. Logout and click on change user.                                </t>
+  </si>
+  <si>
+    <t>The change user button should dissapear and signup button and email field should be editable.</t>
+  </si>
+  <si>
+    <t>The result is as expected.</t>
+  </si>
+  <si>
+    <t>1.Upload a 30mb file and S3 should display the file in cloud.</t>
+  </si>
+  <si>
+    <t>TC14-001</t>
+  </si>
+  <si>
+    <t>TC14-002</t>
+  </si>
+  <si>
+    <t>1. Login using another account</t>
+  </si>
+  <si>
+    <t>On login the file previously created in the other account should not be visible.</t>
+  </si>
+  <si>
+    <t>The file is not visible and the state of the app is set to what the new user should see.</t>
+  </si>
+  <si>
+    <t>1756 hrs</t>
+  </si>
+  <si>
+    <t>Need 2 devices to test this feature and a user account</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Login to device 1
+2. Add a area and file 
+3. Logout from devise 1 and login to device 2.
+4. Navigate to area explorer
+</t>
+  </si>
+  <si>
+    <t>The file added in device 1 should appear in devise 2.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Do the same test with 3 device </t>
+  </si>
+  <si>
+    <t>A three devises should show same same area and files</t>
+  </si>
+  <si>
+    <t>the files and data are consistant over multiple devises</t>
+  </si>
+  <si>
+    <t>2030 hrs</t>
+  </si>
+  <si>
+    <t>16. File and data synchronization</t>
+  </si>
+  <si>
+    <t>Test to check if the database and files are synchronised over multiple device</t>
+  </si>
+  <si>
+    <t>TC16-001</t>
+  </si>
+  <si>
+    <t>TC16-002</t>
   </si>
 </sst>
 </file>
@@ -1022,17 +1213,35 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="7" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="8" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="12" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="13" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1054,24 +1263,6 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="7" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="8" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="12" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2147,10 +2338,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I121"/>
+  <dimension ref="A1:I188"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F37" sqref="F37"/>
+    <sheetView tabSelected="1" topLeftCell="A193" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A184" sqref="A184"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2167,15 +2358,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="40.799999999999997" customHeight="1">
-      <c r="A1" s="66" t="s">
+      <c r="A1" s="62" t="s">
         <v>64</v>
       </c>
-      <c r="B1" s="67"/>
-      <c r="C1" s="67"/>
-      <c r="D1" s="67"/>
-      <c r="E1" s="67"/>
-      <c r="F1" s="67"/>
-      <c r="G1" s="68"/>
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
+      <c r="F1" s="63"/>
+      <c r="G1" s="64"/>
       <c r="H1" s="16"/>
       <c r="I1" s="16"/>
     </row>
@@ -2192,7 +2383,7 @@
     </row>
     <row r="3" spans="1:9" ht="31.2" customHeight="1" thickBot="1">
       <c r="A3" s="40" t="s">
-        <v>83</v>
+        <v>167</v>
       </c>
       <c r="B3" s="40"/>
       <c r="C3" s="40"/>
@@ -2205,11 +2396,11 @@
     </row>
     <row r="4" spans="1:9" ht="18.600000000000001" customHeight="1" thickTop="1">
       <c r="A4" s="41" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B4" s="42"/>
       <c r="C4" s="43" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D4" s="44"/>
       <c r="E4" s="44"/>
@@ -2220,7 +2411,7 @@
     </row>
     <row r="5" spans="1:9" ht="14.4" customHeight="1">
       <c r="A5" s="41" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B5" s="42"/>
       <c r="C5" s="46"/>
@@ -2233,7 +2424,7 @@
     </row>
     <row r="6" spans="1:9" ht="14.4" customHeight="1">
       <c r="A6" s="41" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B6" s="42"/>
       <c r="C6" s="49"/>
@@ -2257,201 +2448,201 @@
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="22" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B8" s="38" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C8" s="31"/>
       <c r="D8" s="38" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E8" s="31"/>
       <c r="F8" s="21" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G8" s="22" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="70.2" customHeight="1">
       <c r="A9" s="26" t="s">
-        <v>5</v>
+        <v>168</v>
       </c>
       <c r="B9" s="36" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C9" s="37"/>
       <c r="D9" s="36" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="E9" s="37"/>
       <c r="F9" s="27" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="G9" s="27" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="41.4" customHeight="1">
       <c r="A10" s="26" t="s">
-        <v>6</v>
+        <v>170</v>
       </c>
       <c r="B10" s="36" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C10" s="37"/>
       <c r="D10" s="36" t="s">
-        <v>119</v>
-      </c>
-      <c r="E10" s="55"/>
+        <v>115</v>
+      </c>
+      <c r="E10" s="60"/>
       <c r="F10" s="27" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="G10" s="27" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="67.8" customHeight="1">
       <c r="A11" s="26" t="s">
-        <v>7</v>
+        <v>171</v>
       </c>
       <c r="B11" s="36" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C11" s="37"/>
       <c r="D11" s="36" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E11" s="37"/>
       <c r="F11" s="27" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="G11" s="27" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="73.2" customHeight="1">
       <c r="A12" s="26" t="s">
-        <v>8</v>
+        <v>172</v>
       </c>
       <c r="B12" s="36" t="s">
-        <v>92</v>
-      </c>
-      <c r="C12" s="55"/>
+        <v>90</v>
+      </c>
+      <c r="C12" s="60"/>
       <c r="D12" s="36" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E12" s="37"/>
       <c r="F12" s="27" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="G12" s="27" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="57" customHeight="1">
       <c r="A13" s="26" t="s">
-        <v>28</v>
+        <v>173</v>
       </c>
       <c r="B13" s="36" t="s">
-        <v>120</v>
-      </c>
-      <c r="C13" s="55"/>
+        <v>116</v>
+      </c>
+      <c r="C13" s="60"/>
       <c r="D13" s="36" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E13" s="37"/>
       <c r="F13" s="27" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="G13" s="27" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="55.95" customHeight="1">
       <c r="A14" s="27" t="s">
-        <v>29</v>
-      </c>
-      <c r="B14" s="56" t="s">
-        <v>121</v>
-      </c>
-      <c r="C14" s="56"/>
+        <v>174</v>
+      </c>
+      <c r="B14" s="61" t="s">
+        <v>117</v>
+      </c>
+      <c r="C14" s="61"/>
       <c r="D14" s="36" t="s">
-        <v>91</v>
-      </c>
-      <c r="E14" s="55"/>
+        <v>89</v>
+      </c>
+      <c r="E14" s="60"/>
       <c r="F14" s="28" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="G14" s="27" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="92.4" customHeight="1">
       <c r="A15" s="27" t="s">
-        <v>30</v>
-      </c>
-      <c r="B15" s="56" t="s">
-        <v>93</v>
-      </c>
-      <c r="C15" s="56"/>
+        <v>175</v>
+      </c>
+      <c r="B15" s="61" t="s">
+        <v>91</v>
+      </c>
+      <c r="C15" s="61"/>
       <c r="D15" s="36" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E15" s="37"/>
       <c r="F15" s="28" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="G15" s="27" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="84.6" customHeight="1">
       <c r="A16" s="27" t="s">
-        <v>39</v>
-      </c>
-      <c r="B16" s="56" t="s">
-        <v>94</v>
-      </c>
-      <c r="C16" s="56"/>
+        <v>176</v>
+      </c>
+      <c r="B16" s="61" t="s">
+        <v>92</v>
+      </c>
+      <c r="C16" s="61"/>
       <c r="D16" s="36" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E16" s="37"/>
       <c r="F16" s="28" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="G16" s="27" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="94.8" customHeight="1">
       <c r="A17" s="27" t="s">
-        <v>40</v>
-      </c>
-      <c r="B17" s="56" t="s">
-        <v>95</v>
-      </c>
-      <c r="C17" s="56"/>
+        <v>177</v>
+      </c>
+      <c r="B17" s="61" t="s">
+        <v>93</v>
+      </c>
+      <c r="C17" s="61"/>
       <c r="D17" s="36" t="s">
-        <v>91</v>
-      </c>
-      <c r="E17" s="55"/>
+        <v>89</v>
+      </c>
+      <c r="E17" s="60"/>
       <c r="F17" s="28" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="G17" s="27" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="18" spans="1:7">
       <c r="A18" s="38" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B18" s="31"/>
       <c r="C18" s="32" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="D18" s="33"/>
       <c r="E18" s="33"/>
@@ -2460,7 +2651,7 @@
     </row>
     <row r="19" spans="1:7">
       <c r="A19" s="38" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B19" s="31"/>
       <c r="C19" s="39">
@@ -2473,11 +2664,11 @@
     </row>
     <row r="20" spans="1:7">
       <c r="A20" s="30" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B20" s="31"/>
       <c r="C20" s="32" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="D20" s="33"/>
       <c r="E20" s="33"/>
@@ -2486,11 +2677,11 @@
     </row>
     <row r="21" spans="1:7">
       <c r="A21" s="30" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B21" s="35"/>
       <c r="C21" s="32" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="D21" s="33"/>
       <c r="E21" s="33"/>
@@ -2545,7 +2736,7 @@
     <row r="27" spans="1:7" ht="12" customHeight="1"/>
     <row r="28" spans="1:7" ht="20.399999999999999" thickBot="1">
       <c r="A28" s="40" t="s">
-        <v>65</v>
+        <v>179</v>
       </c>
       <c r="B28" s="40"/>
       <c r="C28" s="40"/>
@@ -2555,21 +2746,21 @@
       <c r="G28" s="40"/>
     </row>
     <row r="29" spans="1:7" ht="15" thickTop="1">
-      <c r="A29" s="59" t="s">
-        <v>66</v>
-      </c>
-      <c r="B29" s="60"/>
-      <c r="C29" s="61" t="s">
-        <v>78</v>
-      </c>
-      <c r="D29" s="62"/>
-      <c r="E29" s="62"/>
-      <c r="F29" s="62"/>
-      <c r="G29" s="63"/>
+      <c r="A29" s="65" t="s">
+        <v>65</v>
+      </c>
+      <c r="B29" s="66"/>
+      <c r="C29" s="67" t="s">
+        <v>77</v>
+      </c>
+      <c r="D29" s="68"/>
+      <c r="E29" s="68"/>
+      <c r="F29" s="68"/>
+      <c r="G29" s="69"/>
     </row>
     <row r="30" spans="1:7">
       <c r="A30" s="41" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B30" s="42"/>
       <c r="C30" s="46"/>
@@ -2580,154 +2771,166 @@
     </row>
     <row r="31" spans="1:7">
       <c r="A31" s="41" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B31" s="42"/>
       <c r="C31" s="49" t="s">
-        <v>79</v>
-      </c>
-      <c r="D31" s="64"/>
-      <c r="E31" s="64"/>
-      <c r="F31" s="64"/>
-      <c r="G31" s="65"/>
+        <v>78</v>
+      </c>
+      <c r="D31" s="70"/>
+      <c r="E31" s="70"/>
+      <c r="F31" s="70"/>
+      <c r="G31" s="71"/>
     </row>
     <row r="32" spans="1:7">
-      <c r="A32" s="69"/>
-      <c r="B32" s="70"/>
-      <c r="C32" s="70"/>
-      <c r="D32" s="70"/>
-      <c r="E32" s="70"/>
-      <c r="F32" s="70"/>
-      <c r="G32" s="71"/>
+      <c r="A32" s="55"/>
+      <c r="B32" s="56"/>
+      <c r="C32" s="56"/>
+      <c r="D32" s="56"/>
+      <c r="E32" s="56"/>
+      <c r="F32" s="56"/>
+      <c r="G32" s="57"/>
     </row>
     <row r="33" spans="1:7">
       <c r="A33" s="22" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B33" s="38" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C33" s="31"/>
       <c r="D33" s="38" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E33" s="31"/>
       <c r="F33" s="21" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G33" s="22" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="18" customHeight="1">
       <c r="A34" s="23" t="s">
-        <v>5</v>
-      </c>
-      <c r="B34" s="57" t="s">
-        <v>111</v>
-      </c>
-      <c r="C34" s="58"/>
+        <v>178</v>
+      </c>
+      <c r="B34" s="58" t="s">
+        <v>107</v>
+      </c>
+      <c r="C34" s="59"/>
       <c r="D34" s="32" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E34" s="34"/>
       <c r="F34" s="20" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="G34" s="20" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="46.8" customHeight="1">
       <c r="A35" s="26" t="s">
-        <v>6</v>
-      </c>
-      <c r="B35" s="57" t="s">
+        <v>169</v>
+      </c>
+      <c r="B35" s="58" t="s">
         <v>50</v>
       </c>
-      <c r="C35" s="58"/>
+      <c r="C35" s="59"/>
       <c r="D35" s="36" t="s">
-        <v>86</v>
-      </c>
-      <c r="E35" s="55"/>
+        <v>84</v>
+      </c>
+      <c r="E35" s="60"/>
       <c r="F35" s="20" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="G35" s="20" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="45.6" customHeight="1">
       <c r="A36" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="B36" s="57" t="s">
+        <v>180</v>
+      </c>
+      <c r="B36" s="58" t="s">
         <v>49</v>
       </c>
-      <c r="C36" s="58"/>
+      <c r="C36" s="59"/>
       <c r="D36" s="36" t="s">
-        <v>80</v>
-      </c>
-      <c r="E36" s="55"/>
+        <v>79</v>
+      </c>
+      <c r="E36" s="60"/>
       <c r="F36" s="20" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="G36" s="20" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="48" customHeight="1">
       <c r="A37" s="26" t="s">
-        <v>8</v>
-      </c>
-      <c r="B37" s="57" t="s">
+        <v>181</v>
+      </c>
+      <c r="B37" s="58" t="s">
+        <v>80</v>
+      </c>
+      <c r="C37" s="59"/>
+      <c r="D37" s="36" t="s">
         <v>81</v>
       </c>
-      <c r="C37" s="58"/>
-      <c r="D37" s="36" t="s">
-        <v>82</v>
-      </c>
-      <c r="E37" s="55"/>
+      <c r="E37" s="60"/>
       <c r="F37" s="20" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="G37" s="20" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7">
-      <c r="A38" s="38" t="s">
-        <v>74</v>
-      </c>
-      <c r="B38" s="31"/>
-      <c r="C38" s="32" t="s">
-        <v>112</v>
-      </c>
-      <c r="D38" s="33"/>
-      <c r="E38" s="33"/>
-      <c r="F38" s="33"/>
-      <c r="G38" s="34"/>
-    </row>
-    <row r="39" spans="1:7">
-      <c r="A39" s="38" t="s">
-        <v>75</v>
-      </c>
-      <c r="B39" s="31"/>
-      <c r="C39" s="39">
-        <v>43042</v>
-      </c>
-      <c r="D39" s="33"/>
-      <c r="E39" s="33"/>
-      <c r="F39" s="33"/>
-      <c r="G39" s="34"/>
+        <v>102</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="64.2" customHeight="1">
+      <c r="A38" s="26" t="s">
+        <v>182</v>
+      </c>
+      <c r="B38" s="36" t="s">
+        <v>160</v>
+      </c>
+      <c r="C38" s="60"/>
+      <c r="D38" s="36" t="s">
+        <v>161</v>
+      </c>
+      <c r="E38" s="60"/>
+      <c r="F38" s="27" t="s">
+        <v>161</v>
+      </c>
+      <c r="G38" s="27" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="83.4" customHeight="1">
+      <c r="A39" s="26" t="s">
+        <v>183</v>
+      </c>
+      <c r="B39" s="36" t="s">
+        <v>162</v>
+      </c>
+      <c r="C39" s="60"/>
+      <c r="D39" s="36" t="s">
+        <v>163</v>
+      </c>
+      <c r="E39" s="60"/>
+      <c r="F39" s="29" t="s">
+        <v>164</v>
+      </c>
+      <c r="G39" s="27" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="40" spans="1:7">
-      <c r="A40" s="30" t="s">
-        <v>76</v>
-      </c>
-      <c r="B40" s="35"/>
+      <c r="A40" s="38" t="s">
+        <v>73</v>
+      </c>
+      <c r="B40" s="31"/>
       <c r="C40" s="32" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="D40" s="33"/>
       <c r="E40" s="33"/>
@@ -2735,146 +2938,146 @@
       <c r="G40" s="34"/>
     </row>
     <row r="41" spans="1:7">
-      <c r="A41" s="30" t="s">
-        <v>73</v>
-      </c>
-      <c r="B41" s="35"/>
-      <c r="C41" s="32" t="s">
-        <v>106</v>
+      <c r="A41" s="38" t="s">
+        <v>74</v>
+      </c>
+      <c r="B41" s="31"/>
+      <c r="C41" s="39">
+        <v>43042</v>
       </c>
       <c r="D41" s="33"/>
       <c r="E41" s="33"/>
       <c r="F41" s="33"/>
       <c r="G41" s="34"/>
     </row>
-    <row r="45" spans="1:7" ht="20.399999999999999" thickBot="1">
-      <c r="A45" s="40" t="s">
-        <v>99</v>
-      </c>
-      <c r="B45" s="40"/>
-      <c r="C45" s="40"/>
-      <c r="D45" s="40"/>
-      <c r="E45" s="40"/>
-      <c r="F45" s="40"/>
-      <c r="G45" s="40"/>
-    </row>
-    <row r="46" spans="1:7" ht="15" thickTop="1">
-      <c r="A46" s="41" t="s">
+    <row r="42" spans="1:7">
+      <c r="A42" s="30" t="s">
+        <v>75</v>
+      </c>
+      <c r="B42" s="35"/>
+      <c r="C42" s="32" t="s">
+        <v>109</v>
+      </c>
+      <c r="D42" s="33"/>
+      <c r="E42" s="33"/>
+      <c r="F42" s="33"/>
+      <c r="G42" s="34"/>
+    </row>
+    <row r="43" spans="1:7">
+      <c r="A43" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="B43" s="35"/>
+      <c r="C43" s="32" t="s">
+        <v>102</v>
+      </c>
+      <c r="D43" s="33"/>
+      <c r="E43" s="33"/>
+      <c r="F43" s="33"/>
+      <c r="G43" s="34"/>
+    </row>
+    <row r="47" spans="1:7" ht="20.399999999999999" thickBot="1">
+      <c r="A47" s="40" t="s">
+        <v>185</v>
+      </c>
+      <c r="B47" s="40"/>
+      <c r="C47" s="40"/>
+      <c r="D47" s="40"/>
+      <c r="E47" s="40"/>
+      <c r="F47" s="40"/>
+      <c r="G47" s="40"/>
+    </row>
+    <row r="48" spans="1:7" ht="15" thickTop="1">
+      <c r="A48" s="41" t="s">
+        <v>65</v>
+      </c>
+      <c r="B48" s="42"/>
+      <c r="C48" s="43" t="s">
+        <v>94</v>
+      </c>
+      <c r="D48" s="44"/>
+      <c r="E48" s="44"/>
+      <c r="F48" s="44"/>
+      <c r="G48" s="45"/>
+    </row>
+    <row r="49" spans="1:7" ht="16.8" customHeight="1">
+      <c r="A49" s="41" t="s">
         <v>66</v>
       </c>
-      <c r="B46" s="42"/>
-      <c r="C46" s="43" t="s">
+      <c r="B49" s="42"/>
+      <c r="C49" s="46"/>
+      <c r="D49" s="47"/>
+      <c r="E49" s="47"/>
+      <c r="F49" s="47"/>
+      <c r="G49" s="48"/>
+    </row>
+    <row r="50" spans="1:7" ht="26.4" customHeight="1">
+      <c r="A50" s="41" t="s">
+        <v>67</v>
+      </c>
+      <c r="B50" s="42"/>
+      <c r="C50" s="49" t="s">
+        <v>95</v>
+      </c>
+      <c r="D50" s="50"/>
+      <c r="E50" s="50"/>
+      <c r="F50" s="50"/>
+      <c r="G50" s="51"/>
+    </row>
+    <row r="51" spans="1:7" ht="15.6" customHeight="1">
+      <c r="A51" s="52"/>
+      <c r="B51" s="53"/>
+      <c r="C51" s="53"/>
+      <c r="D51" s="53"/>
+      <c r="E51" s="53"/>
+      <c r="F51" s="53"/>
+      <c r="G51" s="54"/>
+    </row>
+    <row r="52" spans="1:7" ht="27" customHeight="1">
+      <c r="A52" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="B52" s="38" t="s">
+        <v>68</v>
+      </c>
+      <c r="C52" s="31"/>
+      <c r="D52" s="38" t="s">
+        <v>69</v>
+      </c>
+      <c r="E52" s="31"/>
+      <c r="F52" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="G52" s="22" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" ht="35.4" customHeight="1">
+      <c r="A53" s="26" t="s">
+        <v>184</v>
+      </c>
+      <c r="B53" s="36" t="s">
+        <v>97</v>
+      </c>
+      <c r="C53" s="37"/>
+      <c r="D53" s="36" t="s">
         <v>96</v>
       </c>
-      <c r="D46" s="44"/>
-      <c r="E46" s="44"/>
-      <c r="F46" s="44"/>
-      <c r="G46" s="45"/>
-    </row>
-    <row r="47" spans="1:7">
-      <c r="A47" s="41" t="s">
-        <v>67</v>
-      </c>
-      <c r="B47" s="42"/>
-      <c r="C47" s="46"/>
-      <c r="D47" s="47"/>
-      <c r="E47" s="47"/>
-      <c r="F47" s="47"/>
-      <c r="G47" s="48"/>
-    </row>
-    <row r="48" spans="1:7">
-      <c r="A48" s="41" t="s">
-        <v>68</v>
-      </c>
-      <c r="B48" s="42"/>
-      <c r="C48" s="49" t="s">
-        <v>97</v>
-      </c>
-      <c r="D48" s="50"/>
-      <c r="E48" s="50"/>
-      <c r="F48" s="50"/>
-      <c r="G48" s="51"/>
-    </row>
-    <row r="49" spans="1:7" ht="16.8" customHeight="1">
-      <c r="A49" s="52"/>
-      <c r="B49" s="53"/>
-      <c r="C49" s="53"/>
-      <c r="D49" s="53"/>
-      <c r="E49" s="53"/>
-      <c r="F49" s="53"/>
-      <c r="G49" s="54"/>
-    </row>
-    <row r="50" spans="1:7" ht="63" customHeight="1">
-      <c r="A50" s="22" t="s">
-        <v>77</v>
-      </c>
-      <c r="B50" s="38" t="s">
-        <v>69</v>
-      </c>
-      <c r="C50" s="31"/>
-      <c r="D50" s="38" t="s">
-        <v>70</v>
-      </c>
-      <c r="E50" s="31"/>
-      <c r="F50" s="21" t="s">
-        <v>71</v>
-      </c>
-      <c r="G50" s="22" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" ht="74.400000000000006" customHeight="1">
-      <c r="A51" s="26" t="s">
-        <v>5</v>
-      </c>
-      <c r="B51" s="36" t="s">
-        <v>100</v>
-      </c>
-      <c r="C51" s="37"/>
-      <c r="D51" s="36" t="s">
-        <v>98</v>
-      </c>
-      <c r="E51" s="37"/>
-      <c r="F51" s="29" t="s">
-        <v>136</v>
-      </c>
-      <c r="G51" s="27" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" ht="27" customHeight="1">
-      <c r="A52" s="30" t="s">
-        <v>74</v>
-      </c>
-      <c r="B52" s="31"/>
-      <c r="C52" s="32" t="s">
-        <v>112</v>
-      </c>
-      <c r="D52" s="33"/>
-      <c r="E52" s="33"/>
-      <c r="F52" s="33"/>
-      <c r="G52" s="34"/>
-    </row>
-    <row r="53" spans="1:7" ht="22.8" customHeight="1">
-      <c r="A53" s="38" t="s">
-        <v>75</v>
-      </c>
-      <c r="B53" s="31"/>
-      <c r="C53" s="39">
-        <v>43046</v>
-      </c>
-      <c r="D53" s="33"/>
-      <c r="E53" s="33"/>
-      <c r="F53" s="33"/>
-      <c r="G53" s="34"/>
+      <c r="E53" s="37"/>
+      <c r="F53" s="29" t="s">
+        <v>131</v>
+      </c>
+      <c r="G53" s="27" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="54" spans="1:7" ht="15.6" customHeight="1">
       <c r="A54" s="30" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B54" s="31"/>
       <c r="C54" s="32" t="s">
-        <v>137</v>
+        <v>108</v>
       </c>
       <c r="D54" s="33"/>
       <c r="E54" s="33"/>
@@ -2882,222 +3085,222 @@
       <c r="G54" s="34"/>
     </row>
     <row r="55" spans="1:7">
-      <c r="A55" s="30" t="s">
-        <v>73</v>
-      </c>
-      <c r="B55" s="35"/>
-      <c r="C55" s="32" t="s">
-        <v>106</v>
+      <c r="A55" s="38" t="s">
+        <v>74</v>
+      </c>
+      <c r="B55" s="31"/>
+      <c r="C55" s="39">
+        <v>43046</v>
       </c>
       <c r="D55" s="33"/>
       <c r="E55" s="33"/>
       <c r="F55" s="33"/>
       <c r="G55" s="34"/>
     </row>
-    <row r="58" spans="1:7" ht="20.399999999999999" thickBot="1">
-      <c r="A58" s="40" t="s">
+    <row r="56" spans="1:7">
+      <c r="A56" s="30" t="s">
+        <v>75</v>
+      </c>
+      <c r="B56" s="31"/>
+      <c r="C56" s="32" t="s">
+        <v>132</v>
+      </c>
+      <c r="D56" s="33"/>
+      <c r="E56" s="33"/>
+      <c r="F56" s="33"/>
+      <c r="G56" s="34"/>
+    </row>
+    <row r="57" spans="1:7">
+      <c r="A57" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="B57" s="35"/>
+      <c r="C57" s="32" t="s">
         <v>102</v>
       </c>
-      <c r="B58" s="40"/>
-      <c r="C58" s="40"/>
-      <c r="D58" s="40"/>
-      <c r="E58" s="40"/>
-      <c r="F58" s="40"/>
-      <c r="G58" s="40"/>
-    </row>
-    <row r="59" spans="1:7" ht="15" thickTop="1">
-      <c r="A59" s="41" t="s">
+      <c r="D57" s="33"/>
+      <c r="E57" s="33"/>
+      <c r="F57" s="33"/>
+      <c r="G57" s="34"/>
+    </row>
+    <row r="60" spans="1:7" ht="20.399999999999999" thickBot="1">
+      <c r="A60" s="40" t="s">
+        <v>191</v>
+      </c>
+      <c r="B60" s="40"/>
+      <c r="C60" s="40"/>
+      <c r="D60" s="40"/>
+      <c r="E60" s="40"/>
+      <c r="F60" s="40"/>
+      <c r="G60" s="40"/>
+    </row>
+    <row r="61" spans="1:7" ht="15" thickTop="1">
+      <c r="A61" s="41" t="s">
+        <v>65</v>
+      </c>
+      <c r="B61" s="42"/>
+      <c r="C61" s="43" t="s">
+        <v>99</v>
+      </c>
+      <c r="D61" s="44"/>
+      <c r="E61" s="44"/>
+      <c r="F61" s="44"/>
+      <c r="G61" s="45"/>
+    </row>
+    <row r="62" spans="1:7">
+      <c r="A62" s="41" t="s">
         <v>66</v>
       </c>
-      <c r="B59" s="42"/>
-      <c r="C59" s="43" t="s">
-        <v>103</v>
-      </c>
-      <c r="D59" s="44"/>
-      <c r="E59" s="44"/>
-      <c r="F59" s="44"/>
-      <c r="G59" s="45"/>
-    </row>
-    <row r="60" spans="1:7">
-      <c r="A60" s="41" t="s">
+      <c r="B62" s="42"/>
+      <c r="C62" s="46"/>
+      <c r="D62" s="47"/>
+      <c r="E62" s="47"/>
+      <c r="F62" s="47"/>
+      <c r="G62" s="48"/>
+    </row>
+    <row r="63" spans="1:7">
+      <c r="A63" s="41" t="s">
         <v>67</v>
       </c>
-      <c r="B60" s="42"/>
-      <c r="C60" s="46"/>
-      <c r="D60" s="47"/>
-      <c r="E60" s="47"/>
-      <c r="F60" s="47"/>
-      <c r="G60" s="48"/>
-    </row>
-    <row r="61" spans="1:7">
-      <c r="A61" s="41" t="s">
+      <c r="B63" s="42"/>
+      <c r="C63" s="49" t="s">
+        <v>98</v>
+      </c>
+      <c r="D63" s="50"/>
+      <c r="E63" s="50"/>
+      <c r="F63" s="50"/>
+      <c r="G63" s="51"/>
+    </row>
+    <row r="64" spans="1:7" ht="21" customHeight="1">
+      <c r="A64" s="52"/>
+      <c r="B64" s="53"/>
+      <c r="C64" s="53"/>
+      <c r="D64" s="53"/>
+      <c r="E64" s="53"/>
+      <c r="F64" s="53"/>
+      <c r="G64" s="54"/>
+    </row>
+    <row r="65" spans="1:7" ht="56.4" customHeight="1">
+      <c r="A65" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="B65" s="38" t="s">
         <v>68</v>
       </c>
-      <c r="B61" s="42"/>
-      <c r="C61" s="49" t="s">
-        <v>101</v>
-      </c>
-      <c r="D61" s="50"/>
-      <c r="E61" s="50"/>
-      <c r="F61" s="50"/>
-      <c r="G61" s="51"/>
-    </row>
-    <row r="62" spans="1:7">
-      <c r="A62" s="52"/>
-      <c r="B62" s="53"/>
-      <c r="C62" s="53"/>
-      <c r="D62" s="53"/>
-      <c r="E62" s="53"/>
-      <c r="F62" s="53"/>
-      <c r="G62" s="54"/>
-    </row>
-    <row r="63" spans="1:7">
-      <c r="A63" s="22" t="s">
-        <v>77</v>
-      </c>
-      <c r="B63" s="38" t="s">
+      <c r="C65" s="31"/>
+      <c r="D65" s="38" t="s">
         <v>69</v>
       </c>
-      <c r="C63" s="31"/>
-      <c r="D63" s="38" t="s">
+      <c r="E65" s="31"/>
+      <c r="F65" s="21" t="s">
         <v>70</v>
       </c>
-      <c r="E63" s="31"/>
-      <c r="F63" s="21" t="s">
-        <v>71</v>
-      </c>
-      <c r="G63" s="22" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" ht="82.2" customHeight="1">
-      <c r="A64" s="26" t="s">
-        <v>5</v>
-      </c>
-      <c r="B64" s="36" t="s">
-        <v>104</v>
-      </c>
-      <c r="C64" s="37"/>
-      <c r="D64" s="36" t="s">
-        <v>105</v>
-      </c>
-      <c r="E64" s="37"/>
-      <c r="F64" s="29" t="s">
-        <v>125</v>
-      </c>
-      <c r="G64" s="29" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" ht="56.4" customHeight="1">
-      <c r="A65" s="26" t="s">
-        <v>6</v>
-      </c>
-      <c r="B65" s="36" t="s">
-        <v>114</v>
-      </c>
-      <c r="C65" s="37"/>
-      <c r="D65" s="36" t="s">
-        <v>115</v>
-      </c>
-      <c r="E65" s="37"/>
-      <c r="F65" s="29" t="s">
-        <v>126</v>
-      </c>
-      <c r="G65" s="29" t="s">
-        <v>106</v>
+      <c r="G65" s="22" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="66" spans="1:7" ht="49.8" customHeight="1">
       <c r="A66" s="26" t="s">
-        <v>7</v>
+        <v>186</v>
       </c>
       <c r="B66" s="36" t="s">
-        <v>116</v>
+        <v>100</v>
       </c>
       <c r="C66" s="37"/>
       <c r="D66" s="36" t="s">
-        <v>117</v>
+        <v>101</v>
       </c>
       <c r="E66" s="37"/>
       <c r="F66" s="29" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="G66" s="29" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="67" spans="1:7" ht="63.6" customHeight="1">
       <c r="A67" s="26" t="s">
-        <v>8</v>
+        <v>187</v>
       </c>
       <c r="B67" s="36" t="s">
-        <v>129</v>
+        <v>110</v>
       </c>
       <c r="C67" s="37"/>
       <c r="D67" s="36" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="E67" s="37"/>
       <c r="F67" s="29" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="G67" s="29" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="68" spans="1:7" ht="79.2" customHeight="1">
       <c r="A68" s="26" t="s">
-        <v>28</v>
+        <v>188</v>
       </c>
       <c r="B68" s="36" t="s">
-        <v>131</v>
+        <v>112</v>
       </c>
       <c r="C68" s="37"/>
       <c r="D68" s="36" t="s">
-        <v>130</v>
+        <v>113</v>
       </c>
       <c r="E68" s="37"/>
       <c r="F68" s="29" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="G68" s="29" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7">
-      <c r="A69" s="30" t="s">
-        <v>74</v>
-      </c>
-      <c r="B69" s="31"/>
-      <c r="C69" s="32" t="s">
-        <v>112</v>
-      </c>
-      <c r="D69" s="33"/>
-      <c r="E69" s="33"/>
-      <c r="F69" s="33"/>
-      <c r="G69" s="34"/>
-    </row>
-    <row r="70" spans="1:7">
-      <c r="A70" s="38" t="s">
-        <v>75</v>
-      </c>
-      <c r="B70" s="31"/>
-      <c r="C70" s="39">
-        <v>43045</v>
-      </c>
-      <c r="D70" s="33"/>
-      <c r="E70" s="33"/>
-      <c r="F70" s="33"/>
-      <c r="G70" s="34"/>
+        <v>102</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" ht="43.2">
+      <c r="A69" s="26" t="s">
+        <v>189</v>
+      </c>
+      <c r="B69" s="36" t="s">
+        <v>125</v>
+      </c>
+      <c r="C69" s="37"/>
+      <c r="D69" s="36" t="s">
+        <v>114</v>
+      </c>
+      <c r="E69" s="37"/>
+      <c r="F69" s="29" t="s">
+        <v>124</v>
+      </c>
+      <c r="G69" s="29" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" ht="28.8">
+      <c r="A70" s="26" t="s">
+        <v>190</v>
+      </c>
+      <c r="B70" s="36" t="s">
+        <v>127</v>
+      </c>
+      <c r="C70" s="37"/>
+      <c r="D70" s="36" t="s">
+        <v>126</v>
+      </c>
+      <c r="E70" s="37"/>
+      <c r="F70" s="29" t="s">
+        <v>128</v>
+      </c>
+      <c r="G70" s="29" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="71" spans="1:7">
       <c r="A71" s="30" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B71" s="31"/>
       <c r="C71" s="32" t="s">
-        <v>133</v>
+        <v>108</v>
       </c>
       <c r="D71" s="33"/>
       <c r="E71" s="33"/>
@@ -3105,369 +3308,187 @@
       <c r="G71" s="34"/>
     </row>
     <row r="72" spans="1:7">
-      <c r="A72" s="30" t="s">
-        <v>73</v>
-      </c>
-      <c r="B72" s="35"/>
-      <c r="C72" s="32" t="s">
-        <v>106</v>
+      <c r="A72" s="38" t="s">
+        <v>74</v>
+      </c>
+      <c r="B72" s="31"/>
+      <c r="C72" s="39">
+        <v>43045</v>
       </c>
       <c r="D72" s="33"/>
       <c r="E72" s="33"/>
       <c r="F72" s="33"/>
       <c r="G72" s="34"/>
     </row>
-    <row r="76" spans="1:7" ht="20.399999999999999" thickBot="1">
-      <c r="A76" s="40" t="s">
-        <v>134</v>
-      </c>
-      <c r="B76" s="40"/>
-      <c r="C76" s="40"/>
-      <c r="D76" s="40"/>
-      <c r="E76" s="40"/>
-      <c r="F76" s="40"/>
-      <c r="G76" s="40"/>
-    </row>
-    <row r="77" spans="1:7" ht="15" thickTop="1">
-      <c r="A77" s="41" t="s">
+    <row r="73" spans="1:7">
+      <c r="A73" s="30" t="s">
+        <v>75</v>
+      </c>
+      <c r="B73" s="31"/>
+      <c r="C73" s="32" t="s">
+        <v>129</v>
+      </c>
+      <c r="D73" s="33"/>
+      <c r="E73" s="33"/>
+      <c r="F73" s="33"/>
+      <c r="G73" s="34"/>
+    </row>
+    <row r="74" spans="1:7">
+      <c r="A74" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="B74" s="35"/>
+      <c r="C74" s="32" t="s">
+        <v>102</v>
+      </c>
+      <c r="D74" s="33"/>
+      <c r="E74" s="33"/>
+      <c r="F74" s="33"/>
+      <c r="G74" s="34"/>
+    </row>
+    <row r="82" spans="1:7" ht="53.4" customHeight="1"/>
+    <row r="83" spans="1:7" ht="49.2" customHeight="1"/>
+    <row r="84" spans="1:7" ht="49.2" customHeight="1"/>
+    <row r="94" spans="1:7" ht="20.399999999999999" thickBot="1">
+      <c r="A94" s="40" t="s">
+        <v>195</v>
+      </c>
+      <c r="B94" s="40"/>
+      <c r="C94" s="40"/>
+      <c r="D94" s="40"/>
+      <c r="E94" s="40"/>
+      <c r="F94" s="40"/>
+      <c r="G94" s="40"/>
+    </row>
+    <row r="95" spans="1:7" ht="15" thickTop="1">
+      <c r="A95" s="41" t="s">
+        <v>65</v>
+      </c>
+      <c r="B95" s="42"/>
+      <c r="C95" s="43" t="s">
+        <v>130</v>
+      </c>
+      <c r="D95" s="44"/>
+      <c r="E95" s="44"/>
+      <c r="F95" s="44"/>
+      <c r="G95" s="45"/>
+    </row>
+    <row r="96" spans="1:7">
+      <c r="A96" s="41" t="s">
         <v>66</v>
       </c>
-      <c r="B77" s="42"/>
-      <c r="C77" s="43" t="s">
-        <v>149</v>
-      </c>
-      <c r="D77" s="44"/>
-      <c r="E77" s="44"/>
-      <c r="F77" s="44"/>
-      <c r="G77" s="45"/>
-    </row>
-    <row r="78" spans="1:7">
-      <c r="A78" s="41" t="s">
+      <c r="B96" s="42"/>
+      <c r="C96" s="46"/>
+      <c r="D96" s="47"/>
+      <c r="E96" s="47"/>
+      <c r="F96" s="47"/>
+      <c r="G96" s="48"/>
+    </row>
+    <row r="97" spans="1:7">
+      <c r="A97" s="41" t="s">
         <v>67</v>
       </c>
-      <c r="B78" s="42"/>
-      <c r="C78" s="46"/>
-      <c r="D78" s="47"/>
-      <c r="E78" s="47"/>
-      <c r="F78" s="47"/>
-      <c r="G78" s="48"/>
-    </row>
-    <row r="79" spans="1:7">
-      <c r="A79" s="41" t="s">
+      <c r="B97" s="42"/>
+      <c r="C97" s="49" t="s">
+        <v>147</v>
+      </c>
+      <c r="D97" s="50"/>
+      <c r="E97" s="50"/>
+      <c r="F97" s="50"/>
+      <c r="G97" s="51"/>
+    </row>
+    <row r="98" spans="1:7" ht="53.4" customHeight="1">
+      <c r="A98" s="52"/>
+      <c r="B98" s="53"/>
+      <c r="C98" s="53"/>
+      <c r="D98" s="53"/>
+      <c r="E98" s="53"/>
+      <c r="F98" s="53"/>
+      <c r="G98" s="54"/>
+    </row>
+    <row r="99" spans="1:7" ht="54" customHeight="1">
+      <c r="A99" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="B99" s="38" t="s">
         <v>68</v>
       </c>
-      <c r="B79" s="42"/>
-      <c r="C79" s="49" t="s">
-        <v>138</v>
-      </c>
-      <c r="D79" s="50"/>
-      <c r="E79" s="50"/>
-      <c r="F79" s="50"/>
-      <c r="G79" s="51"/>
-    </row>
-    <row r="80" spans="1:7">
-      <c r="A80" s="52"/>
-      <c r="B80" s="53"/>
-      <c r="C80" s="53"/>
-      <c r="D80" s="53"/>
-      <c r="E80" s="53"/>
-      <c r="F80" s="53"/>
-      <c r="G80" s="54"/>
-    </row>
-    <row r="81" spans="1:7">
-      <c r="A81" s="22" t="s">
-        <v>77</v>
-      </c>
-      <c r="B81" s="38" t="s">
+      <c r="C99" s="31"/>
+      <c r="D99" s="38" t="s">
         <v>69</v>
       </c>
-      <c r="C81" s="31"/>
-      <c r="D81" s="38" t="s">
+      <c r="E99" s="31"/>
+      <c r="F99" s="21" t="s">
         <v>70</v>
       </c>
-      <c r="E81" s="31"/>
-      <c r="F81" s="21" t="s">
-        <v>71</v>
-      </c>
-      <c r="G81" s="22" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="82" spans="1:7" ht="53.4" customHeight="1">
-      <c r="A82" s="26" t="s">
-        <v>5</v>
-      </c>
-      <c r="B82" s="36" t="s">
-        <v>139</v>
-      </c>
-      <c r="C82" s="37"/>
-      <c r="D82" s="36" t="s">
-        <v>141</v>
-      </c>
-      <c r="E82" s="37"/>
-      <c r="F82" s="29" t="s">
-        <v>142</v>
-      </c>
-      <c r="G82" s="29" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="83" spans="1:7" ht="49.2" customHeight="1">
-      <c r="A83" s="26" t="s">
-        <v>6</v>
-      </c>
-      <c r="B83" s="36" t="s">
-        <v>140</v>
-      </c>
-      <c r="C83" s="37"/>
-      <c r="D83" s="36" t="s">
-        <v>143</v>
-      </c>
-      <c r="E83" s="37"/>
-      <c r="F83" s="29" t="s">
+      <c r="G99" s="22" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" ht="47.4" customHeight="1">
+      <c r="A100" s="26" t="s">
+        <v>192</v>
+      </c>
+      <c r="B100" s="36" t="s">
         <v>144</v>
-      </c>
-      <c r="G83" s="29" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="84" spans="1:7" ht="49.2" customHeight="1">
-      <c r="A84" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="B84" s="36" t="s">
-        <v>145</v>
-      </c>
-      <c r="C84" s="37"/>
-      <c r="D84" s="36" t="s">
-        <v>146</v>
-      </c>
-      <c r="E84" s="37"/>
-      <c r="F84" s="29" t="s">
-        <v>147</v>
-      </c>
-      <c r="G84" s="29" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="85" spans="1:7">
-      <c r="A85" s="30" t="s">
-        <v>74</v>
-      </c>
-      <c r="B85" s="31"/>
-      <c r="C85" s="32" t="s">
-        <v>112</v>
-      </c>
-      <c r="D85" s="33"/>
-      <c r="E85" s="33"/>
-      <c r="F85" s="33"/>
-      <c r="G85" s="34"/>
-    </row>
-    <row r="86" spans="1:7">
-      <c r="A86" s="38" t="s">
-        <v>75</v>
-      </c>
-      <c r="B86" s="31"/>
-      <c r="C86" s="39">
-        <v>43046</v>
-      </c>
-      <c r="D86" s="33"/>
-      <c r="E86" s="33"/>
-      <c r="F86" s="33"/>
-      <c r="G86" s="34"/>
-    </row>
-    <row r="87" spans="1:7">
-      <c r="A87" s="30" t="s">
-        <v>76</v>
-      </c>
-      <c r="B87" s="31"/>
-      <c r="C87" s="32" t="s">
-        <v>133</v>
-      </c>
-      <c r="D87" s="33"/>
-      <c r="E87" s="33"/>
-      <c r="F87" s="33"/>
-      <c r="G87" s="34"/>
-    </row>
-    <row r="88" spans="1:7">
-      <c r="A88" s="30" t="s">
-        <v>73</v>
-      </c>
-      <c r="B88" s="35"/>
-      <c r="C88" s="32" t="s">
-        <v>106</v>
-      </c>
-      <c r="D88" s="33"/>
-      <c r="E88" s="33"/>
-      <c r="F88" s="33"/>
-      <c r="G88" s="34"/>
-    </row>
-    <row r="92" spans="1:7" ht="20.399999999999999" thickBot="1">
-      <c r="A92" s="40" t="s">
-        <v>148</v>
-      </c>
-      <c r="B92" s="40"/>
-      <c r="C92" s="40"/>
-      <c r="D92" s="40"/>
-      <c r="E92" s="40"/>
-      <c r="F92" s="40"/>
-      <c r="G92" s="40"/>
-    </row>
-    <row r="93" spans="1:7" ht="15" thickTop="1">
-      <c r="A93" s="41" t="s">
-        <v>66</v>
-      </c>
-      <c r="B93" s="42"/>
-      <c r="C93" s="43" t="s">
-        <v>135</v>
-      </c>
-      <c r="D93" s="44"/>
-      <c r="E93" s="44"/>
-      <c r="F93" s="44"/>
-      <c r="G93" s="45"/>
-    </row>
-    <row r="94" spans="1:7">
-      <c r="A94" s="41" t="s">
-        <v>67</v>
-      </c>
-      <c r="B94" s="42"/>
-      <c r="C94" s="46"/>
-      <c r="D94" s="47"/>
-      <c r="E94" s="47"/>
-      <c r="F94" s="47"/>
-      <c r="G94" s="48"/>
-    </row>
-    <row r="95" spans="1:7">
-      <c r="A95" s="41" t="s">
-        <v>68</v>
-      </c>
-      <c r="B95" s="42"/>
-      <c r="C95" s="49" t="s">
-        <v>153</v>
-      </c>
-      <c r="D95" s="50"/>
-      <c r="E95" s="50"/>
-      <c r="F95" s="50"/>
-      <c r="G95" s="51"/>
-    </row>
-    <row r="96" spans="1:7">
-      <c r="A96" s="52"/>
-      <c r="B96" s="53"/>
-      <c r="C96" s="53"/>
-      <c r="D96" s="53"/>
-      <c r="E96" s="53"/>
-      <c r="F96" s="53"/>
-      <c r="G96" s="54"/>
-    </row>
-    <row r="97" spans="1:7">
-      <c r="A97" s="22" t="s">
-        <v>77</v>
-      </c>
-      <c r="B97" s="38" t="s">
-        <v>69</v>
-      </c>
-      <c r="C97" s="31"/>
-      <c r="D97" s="38" t="s">
-        <v>70</v>
-      </c>
-      <c r="E97" s="31"/>
-      <c r="F97" s="21" t="s">
-        <v>71</v>
-      </c>
-      <c r="G97" s="22" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="98" spans="1:7" ht="53.4" customHeight="1">
-      <c r="A98" s="26" t="s">
-        <v>5</v>
-      </c>
-      <c r="B98" s="36" t="s">
-        <v>150</v>
-      </c>
-      <c r="C98" s="37"/>
-      <c r="D98" s="36" t="s">
-        <v>151</v>
-      </c>
-      <c r="E98" s="37"/>
-      <c r="F98" s="29" t="s">
-        <v>152</v>
-      </c>
-      <c r="G98" s="29" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="99" spans="1:7" ht="54" customHeight="1">
-      <c r="A99" s="26" t="s">
-        <v>6</v>
-      </c>
-      <c r="B99" s="36" t="s">
-        <v>154</v>
-      </c>
-      <c r="C99" s="37"/>
-      <c r="D99" s="36" t="s">
-        <v>155</v>
-      </c>
-      <c r="E99" s="37"/>
-      <c r="F99" s="29" t="s">
-        <v>156</v>
-      </c>
-      <c r="G99" s="29" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="100" spans="1:7" ht="40.799999999999997" customHeight="1">
-      <c r="A100" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="B100" s="36" t="s">
-        <v>158</v>
       </c>
       <c r="C100" s="37"/>
       <c r="D100" s="36" t="s">
-        <v>159</v>
+        <v>145</v>
       </c>
       <c r="E100" s="37"/>
       <c r="F100" s="29" t="s">
-        <v>160</v>
+        <v>146</v>
       </c>
       <c r="G100" s="29" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="101" spans="1:7">
-      <c r="A101" s="30" t="s">
-        <v>74</v>
-      </c>
-      <c r="B101" s="31"/>
-      <c r="C101" s="32" t="s">
-        <v>112</v>
-      </c>
-      <c r="D101" s="33"/>
-      <c r="E101" s="33"/>
-      <c r="F101" s="33"/>
-      <c r="G101" s="34"/>
-    </row>
-    <row r="102" spans="1:7">
-      <c r="A102" s="38" t="s">
-        <v>75</v>
-      </c>
-      <c r="B102" s="31"/>
-      <c r="C102" s="39">
-        <v>43046</v>
-      </c>
-      <c r="D102" s="33"/>
-      <c r="E102" s="33"/>
-      <c r="F102" s="33"/>
-      <c r="G102" s="34"/>
+        <v>102</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" ht="44.4" customHeight="1">
+      <c r="A101" s="26" t="s">
+        <v>193</v>
+      </c>
+      <c r="B101" s="36" t="s">
+        <v>148</v>
+      </c>
+      <c r="C101" s="37"/>
+      <c r="D101" s="36" t="s">
+        <v>149</v>
+      </c>
+      <c r="E101" s="37"/>
+      <c r="F101" s="29" t="s">
+        <v>150</v>
+      </c>
+      <c r="G101" s="29" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" ht="22.2" customHeight="1">
+      <c r="A102" s="26" t="s">
+        <v>194</v>
+      </c>
+      <c r="B102" s="36" t="s">
+        <v>152</v>
+      </c>
+      <c r="C102" s="37"/>
+      <c r="D102" s="36" t="s">
+        <v>153</v>
+      </c>
+      <c r="E102" s="37"/>
+      <c r="F102" s="29" t="s">
+        <v>154</v>
+      </c>
+      <c r="G102" s="29" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="103" spans="1:7">
       <c r="A103" s="30" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B103" s="31"/>
       <c r="C103" s="32" t="s">
-        <v>157</v>
+        <v>108</v>
       </c>
       <c r="D103" s="33"/>
       <c r="E103" s="33"/>
@@ -3475,297 +3496,849 @@
       <c r="G103" s="34"/>
     </row>
     <row r="104" spans="1:7">
-      <c r="A104" s="30" t="s">
-        <v>73</v>
-      </c>
-      <c r="B104" s="35"/>
-      <c r="C104" s="32" t="s">
-        <v>106</v>
+      <c r="A104" s="38" t="s">
+        <v>74</v>
+      </c>
+      <c r="B104" s="31"/>
+      <c r="C104" s="39">
+        <v>43046</v>
       </c>
       <c r="D104" s="33"/>
       <c r="E104" s="33"/>
       <c r="F104" s="33"/>
       <c r="G104" s="34"/>
     </row>
-    <row r="109" spans="1:7" ht="20.399999999999999" thickBot="1">
-      <c r="A109" s="40" t="s">
-        <v>161</v>
-      </c>
-      <c r="B109" s="40"/>
-      <c r="C109" s="40"/>
-      <c r="D109" s="40"/>
-      <c r="E109" s="40"/>
-      <c r="F109" s="40"/>
-      <c r="G109" s="40"/>
-    </row>
-    <row r="110" spans="1:7" ht="15" thickTop="1">
-      <c r="A110" s="41" t="s">
+    <row r="105" spans="1:7">
+      <c r="A105" s="30" t="s">
+        <v>75</v>
+      </c>
+      <c r="B105" s="31"/>
+      <c r="C105" s="32" t="s">
+        <v>151</v>
+      </c>
+      <c r="D105" s="33"/>
+      <c r="E105" s="33"/>
+      <c r="F105" s="33"/>
+      <c r="G105" s="34"/>
+    </row>
+    <row r="106" spans="1:7">
+      <c r="A106" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="B106" s="35"/>
+      <c r="C106" s="32" t="s">
+        <v>102</v>
+      </c>
+      <c r="D106" s="33"/>
+      <c r="E106" s="33"/>
+      <c r="F106" s="33"/>
+      <c r="G106" s="34"/>
+    </row>
+    <row r="115" spans="1:7" ht="16.8" customHeight="1"/>
+    <row r="116" spans="1:7" ht="34.799999999999997" customHeight="1"/>
+    <row r="117" spans="1:7" ht="27" customHeight="1"/>
+    <row r="118" spans="1:7" ht="35.4" customHeight="1"/>
+    <row r="126" spans="1:7" ht="20.399999999999999" thickBot="1">
+      <c r="A126" s="40" t="s">
+        <v>196</v>
+      </c>
+      <c r="B126" s="40"/>
+      <c r="C126" s="40"/>
+      <c r="D126" s="40"/>
+      <c r="E126" s="40"/>
+      <c r="F126" s="40"/>
+      <c r="G126" s="40"/>
+    </row>
+    <row r="127" spans="1:7" ht="15" thickTop="1">
+      <c r="A127" s="41" t="s">
+        <v>65</v>
+      </c>
+      <c r="B127" s="42"/>
+      <c r="C127" s="43" t="s">
+        <v>143</v>
+      </c>
+      <c r="D127" s="44"/>
+      <c r="E127" s="44"/>
+      <c r="F127" s="44"/>
+      <c r="G127" s="45"/>
+    </row>
+    <row r="128" spans="1:7">
+      <c r="A128" s="41" t="s">
         <v>66</v>
       </c>
-      <c r="B110" s="42"/>
-      <c r="C110" s="43" t="s">
+      <c r="B128" s="42"/>
+      <c r="C128" s="46"/>
+      <c r="D128" s="47"/>
+      <c r="E128" s="47"/>
+      <c r="F128" s="47"/>
+      <c r="G128" s="48"/>
+    </row>
+    <row r="129" spans="1:7">
+      <c r="A129" s="41" t="s">
+        <v>67</v>
+      </c>
+      <c r="B129" s="42"/>
+      <c r="C129" s="49" t="s">
+        <v>133</v>
+      </c>
+      <c r="D129" s="50"/>
+      <c r="E129" s="50"/>
+      <c r="F129" s="50"/>
+      <c r="G129" s="51"/>
+    </row>
+    <row r="130" spans="1:7">
+      <c r="A130" s="52"/>
+      <c r="B130" s="53"/>
+      <c r="C130" s="53"/>
+      <c r="D130" s="53"/>
+      <c r="E130" s="53"/>
+      <c r="F130" s="53"/>
+      <c r="G130" s="54"/>
+    </row>
+    <row r="131" spans="1:7">
+      <c r="A131" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="B131" s="38" t="s">
+        <v>68</v>
+      </c>
+      <c r="C131" s="31"/>
+      <c r="D131" s="38" t="s">
+        <v>69</v>
+      </c>
+      <c r="E131" s="31"/>
+      <c r="F131" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="G131" s="22" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7" ht="57.6" customHeight="1">
+      <c r="A132" s="26" t="s">
+        <v>197</v>
+      </c>
+      <c r="B132" s="36" t="s">
+        <v>134</v>
+      </c>
+      <c r="C132" s="37"/>
+      <c r="D132" s="36" t="s">
+        <v>136</v>
+      </c>
+      <c r="E132" s="37"/>
+      <c r="F132" s="29" t="s">
+        <v>137</v>
+      </c>
+      <c r="G132" s="29" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="133" spans="1:7" ht="49.2" customHeight="1">
+      <c r="A133" s="26" t="s">
+        <v>198</v>
+      </c>
+      <c r="B133" s="36" t="s">
         <v>135</v>
       </c>
-      <c r="D110" s="44"/>
-      <c r="E110" s="44"/>
-      <c r="F110" s="44"/>
-      <c r="G110" s="45"/>
-    </row>
-    <row r="111" spans="1:7">
-      <c r="A111" s="41" t="s">
+      <c r="C133" s="37"/>
+      <c r="D133" s="36" t="s">
+        <v>138</v>
+      </c>
+      <c r="E133" s="37"/>
+      <c r="F133" s="29" t="s">
+        <v>139</v>
+      </c>
+      <c r="G133" s="29" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="134" spans="1:7" ht="31.2" customHeight="1">
+      <c r="A134" s="26" t="s">
+        <v>199</v>
+      </c>
+      <c r="B134" s="36" t="s">
+        <v>140</v>
+      </c>
+      <c r="C134" s="37"/>
+      <c r="D134" s="36" t="s">
+        <v>141</v>
+      </c>
+      <c r="E134" s="37"/>
+      <c r="F134" s="29" t="s">
+        <v>142</v>
+      </c>
+      <c r="G134" s="29" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="135" spans="1:7">
+      <c r="A135" s="30" t="s">
+        <v>73</v>
+      </c>
+      <c r="B135" s="31"/>
+      <c r="C135" s="32" t="s">
+        <v>108</v>
+      </c>
+      <c r="D135" s="33"/>
+      <c r="E135" s="33"/>
+      <c r="F135" s="33"/>
+      <c r="G135" s="34"/>
+    </row>
+    <row r="136" spans="1:7">
+      <c r="A136" s="38" t="s">
+        <v>74</v>
+      </c>
+      <c r="B136" s="31"/>
+      <c r="C136" s="39">
+        <v>43046</v>
+      </c>
+      <c r="D136" s="33"/>
+      <c r="E136" s="33"/>
+      <c r="F136" s="33"/>
+      <c r="G136" s="34"/>
+    </row>
+    <row r="137" spans="1:7">
+      <c r="A137" s="30" t="s">
+        <v>75</v>
+      </c>
+      <c r="B137" s="31"/>
+      <c r="C137" s="32" t="s">
+        <v>129</v>
+      </c>
+      <c r="D137" s="33"/>
+      <c r="E137" s="33"/>
+      <c r="F137" s="33"/>
+      <c r="G137" s="34"/>
+    </row>
+    <row r="138" spans="1:7">
+      <c r="A138" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="B138" s="35"/>
+      <c r="C138" s="32" t="s">
+        <v>102</v>
+      </c>
+      <c r="D138" s="33"/>
+      <c r="E138" s="33"/>
+      <c r="F138" s="33"/>
+      <c r="G138" s="34"/>
+    </row>
+    <row r="142" spans="1:7" ht="20.399999999999999" thickBot="1">
+      <c r="A142" s="40" t="s">
+        <v>200</v>
+      </c>
+      <c r="B142" s="40"/>
+      <c r="C142" s="40"/>
+      <c r="D142" s="40"/>
+      <c r="E142" s="40"/>
+      <c r="F142" s="40"/>
+      <c r="G142" s="40"/>
+    </row>
+    <row r="143" spans="1:7" ht="15" thickTop="1">
+      <c r="A143" s="41" t="s">
+        <v>65</v>
+      </c>
+      <c r="B143" s="42"/>
+      <c r="C143" s="43" t="s">
+        <v>204</v>
+      </c>
+      <c r="D143" s="44"/>
+      <c r="E143" s="44"/>
+      <c r="F143" s="44"/>
+      <c r="G143" s="45"/>
+    </row>
+    <row r="144" spans="1:7">
+      <c r="A144" s="41" t="s">
+        <v>66</v>
+      </c>
+      <c r="B144" s="42"/>
+      <c r="C144" s="46"/>
+      <c r="D144" s="47"/>
+      <c r="E144" s="47"/>
+      <c r="F144" s="47"/>
+      <c r="G144" s="48"/>
+    </row>
+    <row r="145" spans="1:7">
+      <c r="A145" s="41" t="s">
         <v>67</v>
       </c>
-      <c r="B111" s="42"/>
-      <c r="C111" s="46"/>
-      <c r="D111" s="47"/>
-      <c r="E111" s="47"/>
-      <c r="F111" s="47"/>
-      <c r="G111" s="48"/>
-    </row>
-    <row r="112" spans="1:7">
-      <c r="A112" s="41" t="s">
+      <c r="B145" s="42"/>
+      <c r="C145" s="49" t="s">
+        <v>166</v>
+      </c>
+      <c r="D145" s="50"/>
+      <c r="E145" s="50"/>
+      <c r="F145" s="50"/>
+      <c r="G145" s="51"/>
+    </row>
+    <row r="146" spans="1:7">
+      <c r="A146" s="52"/>
+      <c r="B146" s="53"/>
+      <c r="C146" s="53"/>
+      <c r="D146" s="53"/>
+      <c r="E146" s="53"/>
+      <c r="F146" s="53"/>
+      <c r="G146" s="54"/>
+    </row>
+    <row r="147" spans="1:7">
+      <c r="A147" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="B147" s="38" t="s">
         <v>68</v>
       </c>
-      <c r="B112" s="42"/>
-      <c r="C112" s="49"/>
-      <c r="D112" s="50"/>
-      <c r="E112" s="50"/>
-      <c r="F112" s="50"/>
-      <c r="G112" s="51"/>
-    </row>
-    <row r="113" spans="1:7">
-      <c r="A113" s="52"/>
-      <c r="B113" s="53"/>
-      <c r="C113" s="53"/>
-      <c r="D113" s="53"/>
-      <c r="E113" s="53"/>
-      <c r="F113" s="53"/>
-      <c r="G113" s="54"/>
-    </row>
-    <row r="114" spans="1:7">
-      <c r="A114" s="22" t="s">
-        <v>77</v>
-      </c>
-      <c r="B114" s="38" t="s">
+      <c r="C147" s="31"/>
+      <c r="D147" s="38" t="s">
         <v>69</v>
       </c>
-      <c r="C114" s="31"/>
-      <c r="D114" s="38" t="s">
+      <c r="E147" s="31"/>
+      <c r="F147" s="21" t="s">
         <v>70</v>
       </c>
-      <c r="E114" s="31"/>
-      <c r="F114" s="21" t="s">
-        <v>71</v>
-      </c>
-      <c r="G114" s="22" t="s">
+      <c r="G147" s="22" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="148" spans="1:7" ht="63" customHeight="1">
+      <c r="A148" s="26" t="s">
+        <v>201</v>
+      </c>
+      <c r="B148" s="36" t="s">
+        <v>155</v>
+      </c>
+      <c r="C148" s="37"/>
+      <c r="D148" s="36" t="s">
+        <v>156</v>
+      </c>
+      <c r="E148" s="37"/>
+      <c r="F148" s="29" t="s">
+        <v>157</v>
+      </c>
+      <c r="G148" s="29" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="149" spans="1:7" ht="57" customHeight="1">
+      <c r="A149" s="26" t="s">
+        <v>202</v>
+      </c>
+      <c r="B149" s="36" t="s">
+        <v>208</v>
+      </c>
+      <c r="C149" s="37"/>
+      <c r="D149" s="36" t="s">
+        <v>158</v>
+      </c>
+      <c r="E149" s="37"/>
+      <c r="F149" s="29" t="s">
+        <v>159</v>
+      </c>
+      <c r="G149" s="29" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="150" spans="1:7">
+      <c r="A150" s="30" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="115" spans="1:7" ht="61.2" customHeight="1">
-      <c r="A115" s="26" t="s">
-        <v>5</v>
-      </c>
-      <c r="B115" s="36" t="s">
-        <v>162</v>
-      </c>
-      <c r="C115" s="37"/>
-      <c r="D115" s="36" t="s">
-        <v>163</v>
-      </c>
-      <c r="E115" s="37"/>
-      <c r="F115" s="29" t="s">
-        <v>152</v>
-      </c>
-      <c r="G115" s="29" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="116" spans="1:7" ht="34.799999999999997" customHeight="1">
-      <c r="A116" s="26" t="s">
-        <v>6</v>
-      </c>
-      <c r="B116" s="36" t="s">
-        <v>164</v>
-      </c>
-      <c r="C116" s="37"/>
-      <c r="D116" s="36" t="s">
-        <v>155</v>
-      </c>
-      <c r="E116" s="37"/>
-      <c r="F116" s="29" t="s">
-        <v>156</v>
-      </c>
-      <c r="G116" s="29" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="117" spans="1:7">
-      <c r="A117" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="B117" s="36" t="s">
-        <v>158</v>
-      </c>
-      <c r="C117" s="37"/>
-      <c r="D117" s="36" t="s">
-        <v>159</v>
-      </c>
-      <c r="E117" s="37"/>
-      <c r="F117" s="29" t="s">
-        <v>160</v>
-      </c>
-      <c r="G117" s="29" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="118" spans="1:7">
-      <c r="A118" s="30" t="s">
+      <c r="B150" s="31"/>
+      <c r="C150" s="32" t="s">
+        <v>108</v>
+      </c>
+      <c r="D150" s="33"/>
+      <c r="E150" s="33"/>
+      <c r="F150" s="33"/>
+      <c r="G150" s="34"/>
+    </row>
+    <row r="151" spans="1:7">
+      <c r="A151" s="38" t="s">
         <v>74</v>
       </c>
-      <c r="B118" s="31"/>
-      <c r="C118" s="32" t="s">
-        <v>112</v>
-      </c>
-      <c r="D118" s="33"/>
-      <c r="E118" s="33"/>
-      <c r="F118" s="33"/>
-      <c r="G118" s="34"/>
-    </row>
-    <row r="119" spans="1:7">
-      <c r="A119" s="38" t="s">
+      <c r="B151" s="31"/>
+      <c r="C151" s="39">
+        <v>43047</v>
+      </c>
+      <c r="D151" s="33"/>
+      <c r="E151" s="33"/>
+      <c r="F151" s="33"/>
+      <c r="G151" s="34"/>
+    </row>
+    <row r="152" spans="1:7">
+      <c r="A152" s="30" t="s">
         <v>75</v>
       </c>
-      <c r="B119" s="31"/>
-      <c r="C119" s="39">
-        <v>43046</v>
-      </c>
-      <c r="D119" s="33"/>
-      <c r="E119" s="33"/>
-      <c r="F119" s="33"/>
-      <c r="G119" s="34"/>
-    </row>
-    <row r="120" spans="1:7">
-      <c r="A120" s="30" t="s">
+      <c r="B152" s="31"/>
+      <c r="C152" s="32" t="s">
+        <v>165</v>
+      </c>
+      <c r="D152" s="33"/>
+      <c r="E152" s="33"/>
+      <c r="F152" s="33"/>
+      <c r="G152" s="34"/>
+    </row>
+    <row r="153" spans="1:7">
+      <c r="A153" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="B153" s="35"/>
+      <c r="C153" s="32" t="s">
+        <v>102</v>
+      </c>
+      <c r="D153" s="33"/>
+      <c r="E153" s="33"/>
+      <c r="F153" s="33"/>
+      <c r="G153" s="34"/>
+    </row>
+    <row r="157" spans="1:7" ht="20.399999999999999" thickBot="1">
+      <c r="A157" s="40" t="s">
+        <v>203</v>
+      </c>
+      <c r="B157" s="40"/>
+      <c r="C157" s="40"/>
+      <c r="D157" s="40"/>
+      <c r="E157" s="40"/>
+      <c r="F157" s="40"/>
+      <c r="G157" s="40"/>
+    </row>
+    <row r="158" spans="1:7" ht="15" thickTop="1">
+      <c r="A158" s="41" t="s">
+        <v>65</v>
+      </c>
+      <c r="B158" s="42"/>
+      <c r="C158" s="43" t="s">
+        <v>130</v>
+      </c>
+      <c r="D158" s="44"/>
+      <c r="E158" s="44"/>
+      <c r="F158" s="44"/>
+      <c r="G158" s="45"/>
+    </row>
+    <row r="159" spans="1:7">
+      <c r="A159" s="41" t="s">
+        <v>66</v>
+      </c>
+      <c r="B159" s="42"/>
+      <c r="C159" s="46"/>
+      <c r="D159" s="47"/>
+      <c r="E159" s="47"/>
+      <c r="F159" s="47"/>
+      <c r="G159" s="48"/>
+    </row>
+    <row r="160" spans="1:7">
+      <c r="A160" s="41" t="s">
+        <v>67</v>
+      </c>
+      <c r="B160" s="42"/>
+      <c r="C160" s="49" t="s">
+        <v>166</v>
+      </c>
+      <c r="D160" s="50"/>
+      <c r="E160" s="50"/>
+      <c r="F160" s="50"/>
+      <c r="G160" s="51"/>
+    </row>
+    <row r="161" spans="1:7">
+      <c r="A161" s="52"/>
+      <c r="B161" s="53"/>
+      <c r="C161" s="53"/>
+      <c r="D161" s="53"/>
+      <c r="E161" s="53"/>
+      <c r="F161" s="53"/>
+      <c r="G161" s="54"/>
+    </row>
+    <row r="162" spans="1:7">
+      <c r="A162" s="22" t="s">
         <v>76</v>
       </c>
-      <c r="B120" s="31"/>
-      <c r="C120" s="32" t="s">
-        <v>157</v>
-      </c>
-      <c r="D120" s="33"/>
-      <c r="E120" s="33"/>
-      <c r="F120" s="33"/>
-      <c r="G120" s="34"/>
-    </row>
-    <row r="121" spans="1:7">
-      <c r="A121" s="30" t="s">
+      <c r="B162" s="38" t="s">
+        <v>68</v>
+      </c>
+      <c r="C162" s="31"/>
+      <c r="D162" s="38" t="s">
+        <v>69</v>
+      </c>
+      <c r="E162" s="31"/>
+      <c r="F162" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="G162" s="22" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="163" spans="1:7" ht="70.8" customHeight="1">
+      <c r="A163" s="26" t="s">
+        <v>209</v>
+      </c>
+      <c r="B163" s="36" t="s">
+        <v>205</v>
+      </c>
+      <c r="C163" s="37"/>
+      <c r="D163" s="36" t="s">
+        <v>206</v>
+      </c>
+      <c r="E163" s="37"/>
+      <c r="F163" s="29" t="s">
+        <v>207</v>
+      </c>
+      <c r="G163" s="29" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="164" spans="1:7" ht="66.599999999999994" customHeight="1">
+      <c r="A164" s="26" t="s">
+        <v>210</v>
+      </c>
+      <c r="B164" s="36" t="s">
+        <v>211</v>
+      </c>
+      <c r="C164" s="37"/>
+      <c r="D164" s="36" t="s">
+        <v>212</v>
+      </c>
+      <c r="E164" s="37"/>
+      <c r="F164" s="29" t="s">
+        <v>213</v>
+      </c>
+      <c r="G164" s="29" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="165" spans="1:7">
+      <c r="A165" s="30" t="s">
         <v>73</v>
       </c>
-      <c r="B121" s="35"/>
-      <c r="C121" s="32" t="s">
-        <v>106</v>
-      </c>
-      <c r="D121" s="33"/>
-      <c r="E121" s="33"/>
-      <c r="F121" s="33"/>
-      <c r="G121" s="34"/>
+      <c r="B165" s="31"/>
+      <c r="C165" s="32" t="s">
+        <v>108</v>
+      </c>
+      <c r="D165" s="33"/>
+      <c r="E165" s="33"/>
+      <c r="F165" s="33"/>
+      <c r="G165" s="34"/>
+    </row>
+    <row r="166" spans="1:7">
+      <c r="A166" s="38" t="s">
+        <v>74</v>
+      </c>
+      <c r="B166" s="31"/>
+      <c r="C166" s="39">
+        <v>43047</v>
+      </c>
+      <c r="D166" s="33"/>
+      <c r="E166" s="33"/>
+      <c r="F166" s="33"/>
+      <c r="G166" s="34"/>
+    </row>
+    <row r="167" spans="1:7">
+      <c r="A167" s="30" t="s">
+        <v>75</v>
+      </c>
+      <c r="B167" s="31"/>
+      <c r="C167" s="32" t="s">
+        <v>214</v>
+      </c>
+      <c r="D167" s="33"/>
+      <c r="E167" s="33"/>
+      <c r="F167" s="33"/>
+      <c r="G167" s="34"/>
+    </row>
+    <row r="168" spans="1:7">
+      <c r="A168" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="B168" s="35"/>
+      <c r="C168" s="32" t="s">
+        <v>102</v>
+      </c>
+      <c r="D168" s="33"/>
+      <c r="E168" s="33"/>
+      <c r="F168" s="33"/>
+      <c r="G168" s="34"/>
+    </row>
+    <row r="177" spans="1:7" ht="20.399999999999999" thickBot="1">
+      <c r="A177" s="40" t="s">
+        <v>222</v>
+      </c>
+      <c r="B177" s="40"/>
+      <c r="C177" s="40"/>
+      <c r="D177" s="40"/>
+      <c r="E177" s="40"/>
+      <c r="F177" s="40"/>
+      <c r="G177" s="40"/>
+    </row>
+    <row r="178" spans="1:7" ht="15" thickTop="1">
+      <c r="A178" s="41" t="s">
+        <v>65</v>
+      </c>
+      <c r="B178" s="42"/>
+      <c r="C178" s="43" t="s">
+        <v>223</v>
+      </c>
+      <c r="D178" s="44"/>
+      <c r="E178" s="44"/>
+      <c r="F178" s="44"/>
+      <c r="G178" s="45"/>
+    </row>
+    <row r="179" spans="1:7">
+      <c r="A179" s="41" t="s">
+        <v>66</v>
+      </c>
+      <c r="B179" s="42"/>
+      <c r="C179" s="46"/>
+      <c r="D179" s="47"/>
+      <c r="E179" s="47"/>
+      <c r="F179" s="47"/>
+      <c r="G179" s="48"/>
+    </row>
+    <row r="180" spans="1:7">
+      <c r="A180" s="41" t="s">
+        <v>67</v>
+      </c>
+      <c r="B180" s="42"/>
+      <c r="C180" s="49" t="s">
+        <v>215</v>
+      </c>
+      <c r="D180" s="50"/>
+      <c r="E180" s="50"/>
+      <c r="F180" s="50"/>
+      <c r="G180" s="51"/>
+    </row>
+    <row r="181" spans="1:7">
+      <c r="A181" s="52"/>
+      <c r="B181" s="53"/>
+      <c r="C181" s="53"/>
+      <c r="D181" s="53"/>
+      <c r="E181" s="53"/>
+      <c r="F181" s="53"/>
+      <c r="G181" s="54"/>
+    </row>
+    <row r="182" spans="1:7">
+      <c r="A182" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="B182" s="38" t="s">
+        <v>68</v>
+      </c>
+      <c r="C182" s="31"/>
+      <c r="D182" s="38" t="s">
+        <v>69</v>
+      </c>
+      <c r="E182" s="31"/>
+      <c r="F182" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="G182" s="22" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="183" spans="1:7" ht="111" customHeight="1">
+      <c r="A183" s="26" t="s">
+        <v>224</v>
+      </c>
+      <c r="B183" s="36" t="s">
+        <v>216</v>
+      </c>
+      <c r="C183" s="37"/>
+      <c r="D183" s="36" t="s">
+        <v>217</v>
+      </c>
+      <c r="E183" s="37"/>
+      <c r="F183" s="29" t="s">
+        <v>207</v>
+      </c>
+      <c r="G183" s="29" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="184" spans="1:7" ht="43.2" customHeight="1">
+      <c r="A184" s="26" t="s">
+        <v>225</v>
+      </c>
+      <c r="B184" s="36" t="s">
+        <v>218</v>
+      </c>
+      <c r="C184" s="37"/>
+      <c r="D184" s="36" t="s">
+        <v>219</v>
+      </c>
+      <c r="E184" s="37"/>
+      <c r="F184" s="29" t="s">
+        <v>220</v>
+      </c>
+      <c r="G184" s="29" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="185" spans="1:7">
+      <c r="A185" s="30" t="s">
+        <v>73</v>
+      </c>
+      <c r="B185" s="31"/>
+      <c r="C185" s="32" t="s">
+        <v>108</v>
+      </c>
+      <c r="D185" s="33"/>
+      <c r="E185" s="33"/>
+      <c r="F185" s="33"/>
+      <c r="G185" s="34"/>
+    </row>
+    <row r="186" spans="1:7">
+      <c r="A186" s="38" t="s">
+        <v>74</v>
+      </c>
+      <c r="B186" s="31"/>
+      <c r="C186" s="39">
+        <v>43047</v>
+      </c>
+      <c r="D186" s="33"/>
+      <c r="E186" s="33"/>
+      <c r="F186" s="33"/>
+      <c r="G186" s="34"/>
+    </row>
+    <row r="187" spans="1:7">
+      <c r="A187" s="30" t="s">
+        <v>75</v>
+      </c>
+      <c r="B187" s="31"/>
+      <c r="C187" s="32" t="s">
+        <v>221</v>
+      </c>
+      <c r="D187" s="33"/>
+      <c r="E187" s="33"/>
+      <c r="F187" s="33"/>
+      <c r="G187" s="34"/>
+    </row>
+    <row r="188" spans="1:7">
+      <c r="A188" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="B188" s="35"/>
+      <c r="C188" s="32" t="s">
+        <v>102</v>
+      </c>
+      <c r="D188" s="33"/>
+      <c r="E188" s="33"/>
+      <c r="F188" s="33"/>
+      <c r="G188" s="34"/>
     </row>
   </sheetData>
-  <mergeCells count="183">
-    <mergeCell ref="A120:B120"/>
-    <mergeCell ref="C120:G120"/>
-    <mergeCell ref="A121:B121"/>
-    <mergeCell ref="C121:G121"/>
-    <mergeCell ref="B115:C115"/>
-    <mergeCell ref="D115:E115"/>
-    <mergeCell ref="B116:C116"/>
-    <mergeCell ref="D116:E116"/>
-    <mergeCell ref="B117:C117"/>
-    <mergeCell ref="D117:E117"/>
-    <mergeCell ref="A118:B118"/>
-    <mergeCell ref="C118:G118"/>
-    <mergeCell ref="A119:B119"/>
-    <mergeCell ref="C119:G119"/>
-    <mergeCell ref="A109:G109"/>
-    <mergeCell ref="A110:B110"/>
-    <mergeCell ref="C110:G110"/>
-    <mergeCell ref="A111:B111"/>
-    <mergeCell ref="C111:G111"/>
-    <mergeCell ref="A112:B112"/>
-    <mergeCell ref="C112:G112"/>
-    <mergeCell ref="A113:G113"/>
-    <mergeCell ref="B114:C114"/>
-    <mergeCell ref="D114:E114"/>
-    <mergeCell ref="A85:B85"/>
-    <mergeCell ref="C85:G85"/>
-    <mergeCell ref="A86:B86"/>
-    <mergeCell ref="C86:G86"/>
-    <mergeCell ref="A87:B87"/>
-    <mergeCell ref="C87:G87"/>
-    <mergeCell ref="A88:B88"/>
-    <mergeCell ref="C88:G88"/>
-    <mergeCell ref="B82:C82"/>
-    <mergeCell ref="D82:E82"/>
-    <mergeCell ref="B83:C83"/>
-    <mergeCell ref="D83:E83"/>
-    <mergeCell ref="B84:C84"/>
-    <mergeCell ref="D84:E84"/>
-    <mergeCell ref="A76:G76"/>
-    <mergeCell ref="A77:B77"/>
-    <mergeCell ref="C77:G77"/>
-    <mergeCell ref="A78:B78"/>
-    <mergeCell ref="C78:G78"/>
-    <mergeCell ref="A79:B79"/>
-    <mergeCell ref="C79:G79"/>
-    <mergeCell ref="A80:G80"/>
-    <mergeCell ref="B81:C81"/>
-    <mergeCell ref="D81:E81"/>
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="C54:G54"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="C55:G55"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="C52:G52"/>
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="C53:G53"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="C46:G46"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="C47:G47"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="D51:E51"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="C48:G48"/>
-    <mergeCell ref="A49:G49"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="D50:E50"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="C38:G38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="C39:G39"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="C40:G40"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="C41:G41"/>
-    <mergeCell ref="A45:G45"/>
-    <mergeCell ref="A32:G32"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="C18:G18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="C19:G19"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="B16:C16"/>
+  <mergeCells count="229">
+    <mergeCell ref="A188:B188"/>
+    <mergeCell ref="C188:G188"/>
+    <mergeCell ref="B183:C183"/>
+    <mergeCell ref="D183:E183"/>
+    <mergeCell ref="B184:C184"/>
+    <mergeCell ref="D184:E184"/>
+    <mergeCell ref="A185:B185"/>
+    <mergeCell ref="C185:G185"/>
+    <mergeCell ref="A186:B186"/>
+    <mergeCell ref="C186:G186"/>
+    <mergeCell ref="A187:B187"/>
+    <mergeCell ref="C187:G187"/>
+    <mergeCell ref="A178:B178"/>
+    <mergeCell ref="C178:G178"/>
+    <mergeCell ref="A179:B179"/>
+    <mergeCell ref="C179:G179"/>
+    <mergeCell ref="A180:B180"/>
+    <mergeCell ref="C180:G180"/>
+    <mergeCell ref="A181:G181"/>
+    <mergeCell ref="B182:C182"/>
+    <mergeCell ref="D182:E182"/>
+    <mergeCell ref="A165:B165"/>
+    <mergeCell ref="C165:G165"/>
+    <mergeCell ref="A166:B166"/>
+    <mergeCell ref="C166:G166"/>
+    <mergeCell ref="A167:B167"/>
+    <mergeCell ref="C167:G167"/>
+    <mergeCell ref="A168:B168"/>
+    <mergeCell ref="C168:G168"/>
+    <mergeCell ref="A177:G177"/>
+    <mergeCell ref="A160:B160"/>
+    <mergeCell ref="C160:G160"/>
+    <mergeCell ref="A161:G161"/>
+    <mergeCell ref="B162:C162"/>
+    <mergeCell ref="D162:E162"/>
+    <mergeCell ref="B163:C163"/>
+    <mergeCell ref="D163:E163"/>
+    <mergeCell ref="B164:C164"/>
+    <mergeCell ref="D164:E164"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="A157:G157"/>
+    <mergeCell ref="A158:B158"/>
+    <mergeCell ref="C158:G158"/>
+    <mergeCell ref="A159:B159"/>
+    <mergeCell ref="C159:G159"/>
+    <mergeCell ref="A105:B105"/>
+    <mergeCell ref="C105:G105"/>
+    <mergeCell ref="A106:B106"/>
+    <mergeCell ref="C106:G106"/>
+    <mergeCell ref="B102:C102"/>
+    <mergeCell ref="D102:E102"/>
+    <mergeCell ref="B100:C100"/>
+    <mergeCell ref="D100:E100"/>
+    <mergeCell ref="B101:C101"/>
+    <mergeCell ref="D101:E101"/>
+    <mergeCell ref="A103:B103"/>
+    <mergeCell ref="C103:G103"/>
+    <mergeCell ref="A104:B104"/>
+    <mergeCell ref="C104:G104"/>
+    <mergeCell ref="A94:G94"/>
+    <mergeCell ref="A95:B95"/>
+    <mergeCell ref="C95:G95"/>
+    <mergeCell ref="A96:B96"/>
+    <mergeCell ref="C96:G96"/>
+    <mergeCell ref="A97:B97"/>
+    <mergeCell ref="C97:G97"/>
+    <mergeCell ref="A98:G98"/>
+    <mergeCell ref="B99:C99"/>
+    <mergeCell ref="D99:E99"/>
+    <mergeCell ref="A72:B72"/>
+    <mergeCell ref="C72:G72"/>
+    <mergeCell ref="A73:B73"/>
+    <mergeCell ref="C73:G73"/>
+    <mergeCell ref="A74:B74"/>
+    <mergeCell ref="C74:G74"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="D65:E65"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="D66:E66"/>
+    <mergeCell ref="A71:B71"/>
+    <mergeCell ref="C71:G71"/>
+    <mergeCell ref="B67:C67"/>
+    <mergeCell ref="D67:E67"/>
+    <mergeCell ref="B68:C68"/>
+    <mergeCell ref="D68:E68"/>
+    <mergeCell ref="B69:C69"/>
+    <mergeCell ref="D69:E69"/>
+    <mergeCell ref="B70:C70"/>
+    <mergeCell ref="D70:E70"/>
+    <mergeCell ref="A62:B62"/>
+    <mergeCell ref="C62:G62"/>
+    <mergeCell ref="A63:B63"/>
+    <mergeCell ref="C63:G63"/>
+    <mergeCell ref="A64:G64"/>
+    <mergeCell ref="A60:G60"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="C61:G61"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="A28:G28"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="C29:G29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="C30:G30"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="C31:G31"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="B13:C13"/>
     <mergeCell ref="B12:C12"/>
@@ -3787,74 +4360,98 @@
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="D11:E11"/>
     <mergeCell ref="D13:E13"/>
-    <mergeCell ref="A60:B60"/>
-    <mergeCell ref="C60:G60"/>
-    <mergeCell ref="A61:B61"/>
-    <mergeCell ref="C61:G61"/>
-    <mergeCell ref="A62:G62"/>
-    <mergeCell ref="A58:G58"/>
-    <mergeCell ref="A59:B59"/>
-    <mergeCell ref="C59:G59"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="C20:G20"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="C21:G21"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="A28:G28"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="C29:G29"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="C30:G30"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="C31:G31"/>
-    <mergeCell ref="A70:B70"/>
-    <mergeCell ref="C70:G70"/>
-    <mergeCell ref="A71:B71"/>
-    <mergeCell ref="C71:G71"/>
-    <mergeCell ref="A72:B72"/>
-    <mergeCell ref="C72:G72"/>
-    <mergeCell ref="B63:C63"/>
-    <mergeCell ref="D63:E63"/>
-    <mergeCell ref="B64:C64"/>
-    <mergeCell ref="D64:E64"/>
-    <mergeCell ref="A69:B69"/>
-    <mergeCell ref="C69:G69"/>
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="D65:E65"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="D66:E66"/>
-    <mergeCell ref="B67:C67"/>
-    <mergeCell ref="D67:E67"/>
-    <mergeCell ref="B68:C68"/>
-    <mergeCell ref="D68:E68"/>
-    <mergeCell ref="A92:G92"/>
-    <mergeCell ref="A93:B93"/>
-    <mergeCell ref="C93:G93"/>
-    <mergeCell ref="A94:B94"/>
-    <mergeCell ref="C94:G94"/>
-    <mergeCell ref="A95:B95"/>
-    <mergeCell ref="C95:G95"/>
-    <mergeCell ref="A96:G96"/>
-    <mergeCell ref="B97:C97"/>
-    <mergeCell ref="D97:E97"/>
-    <mergeCell ref="A103:B103"/>
-    <mergeCell ref="C103:G103"/>
-    <mergeCell ref="A104:B104"/>
-    <mergeCell ref="C104:G104"/>
-    <mergeCell ref="B100:C100"/>
-    <mergeCell ref="D100:E100"/>
-    <mergeCell ref="B98:C98"/>
-    <mergeCell ref="D98:E98"/>
-    <mergeCell ref="B99:C99"/>
-    <mergeCell ref="D99:E99"/>
-    <mergeCell ref="A101:B101"/>
-    <mergeCell ref="C101:G101"/>
-    <mergeCell ref="A102:B102"/>
-    <mergeCell ref="C102:G102"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="C18:G18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="A32:G32"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="C40:G40"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="C41:G41"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="C42:G42"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="C43:G43"/>
+    <mergeCell ref="A47:G47"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="C56:G56"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="C57:G57"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="C54:G54"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="C55:G55"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="C48:G48"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="C49:G49"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="D53:E53"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="C50:G50"/>
+    <mergeCell ref="A51:G51"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="D52:E52"/>
+    <mergeCell ref="A126:G126"/>
+    <mergeCell ref="A127:B127"/>
+    <mergeCell ref="C127:G127"/>
+    <mergeCell ref="A128:B128"/>
+    <mergeCell ref="C128:G128"/>
+    <mergeCell ref="A129:B129"/>
+    <mergeCell ref="C129:G129"/>
+    <mergeCell ref="A130:G130"/>
+    <mergeCell ref="B131:C131"/>
+    <mergeCell ref="D131:E131"/>
+    <mergeCell ref="A135:B135"/>
+    <mergeCell ref="C135:G135"/>
+    <mergeCell ref="A136:B136"/>
+    <mergeCell ref="C136:G136"/>
+    <mergeCell ref="A137:B137"/>
+    <mergeCell ref="C137:G137"/>
+    <mergeCell ref="A138:B138"/>
+    <mergeCell ref="C138:G138"/>
+    <mergeCell ref="B132:C132"/>
+    <mergeCell ref="D132:E132"/>
+    <mergeCell ref="B133:C133"/>
+    <mergeCell ref="D133:E133"/>
+    <mergeCell ref="B134:C134"/>
+    <mergeCell ref="D134:E134"/>
+    <mergeCell ref="A142:G142"/>
+    <mergeCell ref="A143:B143"/>
+    <mergeCell ref="C143:G143"/>
+    <mergeCell ref="A144:B144"/>
+    <mergeCell ref="C144:G144"/>
+    <mergeCell ref="A145:B145"/>
+    <mergeCell ref="C145:G145"/>
+    <mergeCell ref="A146:G146"/>
+    <mergeCell ref="B147:C147"/>
+    <mergeCell ref="D147:E147"/>
+    <mergeCell ref="A152:B152"/>
+    <mergeCell ref="C152:G152"/>
+    <mergeCell ref="A153:B153"/>
+    <mergeCell ref="C153:G153"/>
+    <mergeCell ref="B148:C148"/>
+    <mergeCell ref="D148:E148"/>
+    <mergeCell ref="B149:C149"/>
+    <mergeCell ref="D149:E149"/>
+    <mergeCell ref="A150:B150"/>
+    <mergeCell ref="C150:G150"/>
+    <mergeCell ref="A151:B151"/>
+    <mergeCell ref="C151:G151"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Added delete user test case
</commit_message>
<xml_diff>
--- a/FYP documentation/FYP_Test_Plan.xlsx
+++ b/FYP documentation/FYP_Test_Plan.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="233">
   <si>
     <t>Expected Result</t>
   </si>
@@ -742,6 +742,29 @@
   </si>
   <si>
     <t>TC16-002</t>
+  </si>
+  <si>
+    <t>Test if delete user removes all data related to the user.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Login to the account.
+2. Go to menu and click delete account
+</t>
+  </si>
+  <si>
+    <t>15. Delete User</t>
+  </si>
+  <si>
+    <t>TC15-001</t>
+  </si>
+  <si>
+    <t>An error message will be printed out on relogin and the user related data are deleted from cloud service (Cognito,S3 and DynamoDB)</t>
+  </si>
+  <si>
+    <t>2135 hrs</t>
+  </si>
+  <si>
+    <t>All the user retated data and files are deleted and and error message is printed.</t>
   </si>
 </sst>
 </file>
@@ -2338,10 +2361,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I188"/>
+  <dimension ref="A1:I204"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A193" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A184" sqref="A184"/>
+    <sheetView tabSelected="1" topLeftCell="A178" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F209" sqref="F209"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -4221,8 +4244,173 @@
       <c r="F188" s="33"/>
       <c r="G188" s="34"/>
     </row>
+    <row r="194" spans="1:7" ht="20.399999999999999" thickBot="1">
+      <c r="A194" s="40" t="s">
+        <v>228</v>
+      </c>
+      <c r="B194" s="40"/>
+      <c r="C194" s="40"/>
+      <c r="D194" s="40"/>
+      <c r="E194" s="40"/>
+      <c r="F194" s="40"/>
+      <c r="G194" s="40"/>
+    </row>
+    <row r="195" spans="1:7" ht="15" thickTop="1">
+      <c r="A195" s="41" t="s">
+        <v>65</v>
+      </c>
+      <c r="B195" s="42"/>
+      <c r="C195" s="43" t="s">
+        <v>226</v>
+      </c>
+      <c r="D195" s="44"/>
+      <c r="E195" s="44"/>
+      <c r="F195" s="44"/>
+      <c r="G195" s="45"/>
+    </row>
+    <row r="196" spans="1:7">
+      <c r="A196" s="41" t="s">
+        <v>66</v>
+      </c>
+      <c r="B196" s="42"/>
+      <c r="C196" s="46"/>
+      <c r="D196" s="47"/>
+      <c r="E196" s="47"/>
+      <c r="F196" s="47"/>
+      <c r="G196" s="48"/>
+    </row>
+    <row r="197" spans="1:7">
+      <c r="A197" s="41" t="s">
+        <v>67</v>
+      </c>
+      <c r="B197" s="42"/>
+      <c r="C197" s="49"/>
+      <c r="D197" s="50"/>
+      <c r="E197" s="50"/>
+      <c r="F197" s="50"/>
+      <c r="G197" s="51"/>
+    </row>
+    <row r="198" spans="1:7">
+      <c r="A198" s="52"/>
+      <c r="B198" s="53"/>
+      <c r="C198" s="53"/>
+      <c r="D198" s="53"/>
+      <c r="E198" s="53"/>
+      <c r="F198" s="53"/>
+      <c r="G198" s="54"/>
+    </row>
+    <row r="199" spans="1:7">
+      <c r="A199" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="B199" s="38" t="s">
+        <v>68</v>
+      </c>
+      <c r="C199" s="31"/>
+      <c r="D199" s="38" t="s">
+        <v>69</v>
+      </c>
+      <c r="E199" s="31"/>
+      <c r="F199" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="G199" s="22" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="200" spans="1:7" ht="105.6" customHeight="1">
+      <c r="A200" s="26" t="s">
+        <v>229</v>
+      </c>
+      <c r="B200" s="36" t="s">
+        <v>227</v>
+      </c>
+      <c r="C200" s="37"/>
+      <c r="D200" s="36" t="s">
+        <v>230</v>
+      </c>
+      <c r="E200" s="37"/>
+      <c r="F200" s="29" t="s">
+        <v>232</v>
+      </c>
+      <c r="G200" s="29" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="201" spans="1:7">
+      <c r="A201" s="30" t="s">
+        <v>73</v>
+      </c>
+      <c r="B201" s="31"/>
+      <c r="C201" s="32" t="s">
+        <v>108</v>
+      </c>
+      <c r="D201" s="33"/>
+      <c r="E201" s="33"/>
+      <c r="F201" s="33"/>
+      <c r="G201" s="34"/>
+    </row>
+    <row r="202" spans="1:7">
+      <c r="A202" s="38" t="s">
+        <v>74</v>
+      </c>
+      <c r="B202" s="31"/>
+      <c r="C202" s="39">
+        <v>43047</v>
+      </c>
+      <c r="D202" s="33"/>
+      <c r="E202" s="33"/>
+      <c r="F202" s="33"/>
+      <c r="G202" s="34"/>
+    </row>
+    <row r="203" spans="1:7">
+      <c r="A203" s="30" t="s">
+        <v>75</v>
+      </c>
+      <c r="B203" s="31"/>
+      <c r="C203" s="32" t="s">
+        <v>231</v>
+      </c>
+      <c r="D203" s="33"/>
+      <c r="E203" s="33"/>
+      <c r="F203" s="33"/>
+      <c r="G203" s="34"/>
+    </row>
+    <row r="204" spans="1:7">
+      <c r="A204" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="B204" s="35"/>
+      <c r="C204" s="32" t="s">
+        <v>102</v>
+      </c>
+      <c r="D204" s="33"/>
+      <c r="E204" s="33"/>
+      <c r="F204" s="33"/>
+      <c r="G204" s="34"/>
+    </row>
   </sheetData>
-  <mergeCells count="229">
+  <mergeCells count="249">
+    <mergeCell ref="A204:B204"/>
+    <mergeCell ref="C204:G204"/>
+    <mergeCell ref="B200:C200"/>
+    <mergeCell ref="D200:E200"/>
+    <mergeCell ref="A201:B201"/>
+    <mergeCell ref="C201:G201"/>
+    <mergeCell ref="A202:B202"/>
+    <mergeCell ref="C202:G202"/>
+    <mergeCell ref="A203:B203"/>
+    <mergeCell ref="C203:G203"/>
+    <mergeCell ref="A194:G194"/>
+    <mergeCell ref="A195:B195"/>
+    <mergeCell ref="C195:G195"/>
+    <mergeCell ref="A196:B196"/>
+    <mergeCell ref="C196:G196"/>
+    <mergeCell ref="A197:B197"/>
+    <mergeCell ref="C197:G197"/>
+    <mergeCell ref="A198:G198"/>
+    <mergeCell ref="B199:C199"/>
+    <mergeCell ref="D199:E199"/>
     <mergeCell ref="A188:B188"/>
     <mergeCell ref="C188:G188"/>
     <mergeCell ref="B183:C183"/>

</xml_diff>

<commit_message>
Made changes to change name in test plan
</commit_message>
<xml_diff>
--- a/FYP documentation/FYP_Test_Plan.xlsx
+++ b/FYP documentation/FYP_Test_Plan.xlsx
@@ -1,17 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18528"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Class_notes\BSS_FYP_TEAM173D\FYP documentation\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6936"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6936" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Plan Final" sheetId="4" r:id="rId1"/>
     <sheet name="Test Plan" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="145621"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -21,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="861" uniqueCount="490">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="873" uniqueCount="496">
   <si>
     <t>Expected Result</t>
   </si>
@@ -2761,9 +2765,6 @@
     </r>
   </si>
   <si>
-    <t>No Update in Changing Name and dismiss the dialog</t>
-  </si>
-  <si>
     <t>TC12-006</t>
   </si>
   <si>
@@ -2800,11 +2801,32 @@
 2. Click "OK"</t>
     </r>
   </si>
+  <si>
+    <t>Shows first name empty error</t>
+  </si>
+  <si>
+    <t>Shows last name empty error</t>
+  </si>
+  <si>
+    <t>Shows first and last name is empty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Name is successfully chnaged </t>
+  </si>
+  <si>
+    <t>No Update in name and dismiss the dialog</t>
+  </si>
+  <si>
+    <t>there is no update in name</t>
+  </si>
+  <si>
+    <t>Error message is displayed</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="12">
     <font>
       <sz val="11"/>
@@ -3389,12 +3411,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="20% - 강조색3" xfId="5" builtinId="38"/>
-    <cellStyle name="강조색1" xfId="4" builtinId="29"/>
-    <cellStyle name="제목" xfId="2" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="제목 1" xfId="3" builtinId="16"/>
-    <cellStyle name="표준" xfId="0" builtinId="0"/>
-    <cellStyle name="하이퍼링크" xfId="1" builtinId="8"/>
+    <cellStyle name="20% - Accent3" xfId="5" builtinId="38"/>
+    <cellStyle name="Accent1" xfId="4" builtinId="29"/>
+    <cellStyle name="Heading 1" xfId="3" builtinId="16"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Title" xfId="2" builtinId="15" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -3429,7 +3451,7 @@
         <xdr:cNvPr id="2061" name="AutoShape 13">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{30BA1063-A16B-4C68-A743-4B420C5465C1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{30BA1063-A16B-4C68-A743-4B420C5465C1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3477,7 +3499,7 @@
         <xdr:cNvPr id="2060" name="Picture 12" descr="out">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{DF567FBA-98D6-41F8-887E-3AB62EFCE5E8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DF567FBA-98D6-41F8-887E-3AB62EFCE5E8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3538,7 +3560,7 @@
         <xdr:cNvPr id="2059" name="Picture 11" descr="out">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{63E93150-DA75-4658-ACF7-D189E05151A8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{63E93150-DA75-4658-ACF7-D189E05151A8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3599,7 +3621,7 @@
         <xdr:cNvPr id="2058" name="AutoShape 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{31457A75-25A1-4182-A274-BF0A57FF81ED}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{31457A75-25A1-4182-A274-BF0A57FF81ED}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3647,7 +3669,7 @@
         <xdr:cNvPr id="2057" name="AutoShape 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{FD5E9B17-BBE9-4F3F-8C7B-720ECD2D681E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FD5E9B17-BBE9-4F3F-8C7B-720ECD2D681E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3695,7 +3717,7 @@
         <xdr:cNvPr id="2056" name="AutoShape 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{ACF2AA01-B252-4B3A-A375-0E01973F5F28}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ACF2AA01-B252-4B3A-A375-0E01973F5F28}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3743,7 +3765,7 @@
         <xdr:cNvPr id="2055" name="Picture 7" descr="out">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{65879D11-6224-4C7F-89C2-EB96196F1A0F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{65879D11-6224-4C7F-89C2-EB96196F1A0F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3804,7 +3826,7 @@
         <xdr:cNvPr id="2054" name="Picture 6" descr="out">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{5CF822E1-047C-4A3B-84DC-EC8AC8269EFF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5CF822E1-047C-4A3B-84DC-EC8AC8269EFF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3865,7 +3887,7 @@
         <xdr:cNvPr id="2053" name="Picture 5" descr="out">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{04925A52-F4C6-4CD2-894B-53641F217E98}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{04925A52-F4C6-4CD2-894B-53641F217E98}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3926,7 +3948,7 @@
         <xdr:cNvPr id="2052" name="Picture 4" descr="out">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{ABFA5086-6E08-48C0-9ACC-F28827F67131}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ABFA5086-6E08-48C0-9ACC-F28827F67131}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3987,7 +4009,7 @@
         <xdr:cNvPr id="2051" name="Picture 3" descr="out">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{57E4935A-4571-48AC-8BC5-8DE7A584B4D3}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{57E4935A-4571-48AC-8BC5-8DE7A584B4D3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4048,7 +4070,7 @@
         <xdr:cNvPr id="2050" name="Picture 2" descr="out">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{73C78A6D-821A-410B-9678-567D6BA6A13D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{73C78A6D-821A-410B-9678-567D6BA6A13D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4109,7 +4131,7 @@
         <xdr:cNvPr id="2049" name="Picture 1" descr="out?google_nid=adroll5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{0583EF1F-95CC-4F68-83EF-C3E41E3B377C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0583EF1F-95CC-4F68-83EF-C3E41E3B377C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4444,18 +4466,18 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I384"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A263" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="M268" sqref="M268"/>
+    <sheetView tabSelected="1" topLeftCell="A256" zoomScale="122" zoomScaleNormal="122" workbookViewId="0">
+      <selection activeCell="G270" sqref="G270"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -7348,7 +7370,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="237" spans="1:7" ht="106.8" customHeight="1">
+    <row r="237" spans="1:7" ht="117.6" customHeight="1">
       <c r="A237" s="42" t="s">
         <v>431</v>
       </c>
@@ -7705,8 +7727,12 @@
         <v>474</v>
       </c>
       <c r="E265" s="74"/>
-      <c r="F265" s="39"/>
-      <c r="G265" s="39"/>
+      <c r="F265" s="39" t="s">
+        <v>489</v>
+      </c>
+      <c r="G265" s="39" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="266" spans="1:7" ht="43.2" customHeight="1">
       <c r="A266" s="44" t="s">
@@ -7720,8 +7746,12 @@
         <v>477</v>
       </c>
       <c r="E266" s="53"/>
-      <c r="F266" s="39"/>
-      <c r="G266" s="39"/>
+      <c r="F266" s="39" t="s">
+        <v>490</v>
+      </c>
+      <c r="G266" s="39" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="267" spans="1:7" ht="74.400000000000006" customHeight="1">
       <c r="A267" s="44" t="s">
@@ -7735,23 +7765,31 @@
         <v>480</v>
       </c>
       <c r="E267" s="53"/>
-      <c r="F267" s="39"/>
-      <c r="G267" s="39"/>
+      <c r="F267" s="39" t="s">
+        <v>491</v>
+      </c>
+      <c r="G267" s="39" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="268" spans="1:7" ht="77.400000000000006" customHeight="1">
       <c r="A268" s="44" t="s">
         <v>481</v>
       </c>
       <c r="B268" s="52" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="C268" s="74"/>
       <c r="D268" s="52" t="s">
         <v>482</v>
       </c>
       <c r="E268" s="53"/>
-      <c r="F268" s="39"/>
-      <c r="G268" s="39"/>
+      <c r="F268" s="39" t="s">
+        <v>492</v>
+      </c>
+      <c r="G268" s="39" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="269" spans="1:7" ht="55.2" customHeight="1">
       <c r="A269" s="44" t="s">
@@ -7762,26 +7800,34 @@
       </c>
       <c r="C269" s="53"/>
       <c r="D269" s="52" t="s">
-        <v>485</v>
+        <v>493</v>
       </c>
       <c r="E269" s="53"/>
-      <c r="F269" s="39"/>
-      <c r="G269" s="39"/>
+      <c r="F269" s="39" t="s">
+        <v>494</v>
+      </c>
+      <c r="G269" s="39" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="270" spans="1:7" ht="55.2" customHeight="1">
       <c r="A270" s="44" t="s">
+        <v>485</v>
+      </c>
+      <c r="B270" s="52" t="s">
         <v>486</v>
-      </c>
-      <c r="B270" s="52" t="s">
-        <v>487</v>
       </c>
       <c r="C270" s="74"/>
       <c r="D270" s="52" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="E270" s="74"/>
-      <c r="F270" s="39"/>
-      <c r="G270" s="39"/>
+      <c r="F270" s="39" t="s">
+        <v>495</v>
+      </c>
+      <c r="G270" s="39" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="271" spans="1:7">
       <c r="A271" s="50" t="s">
@@ -9101,6 +9147,21 @@
     <mergeCell ref="C262:G262"/>
     <mergeCell ref="A263:G263"/>
     <mergeCell ref="C381:G381"/>
+    <mergeCell ref="C346:G346"/>
+    <mergeCell ref="B342:C342"/>
+    <mergeCell ref="D342:E342"/>
+    <mergeCell ref="A343:B343"/>
+    <mergeCell ref="C343:G343"/>
+    <mergeCell ref="A344:B344"/>
+    <mergeCell ref="C344:G344"/>
+    <mergeCell ref="A345:B345"/>
+    <mergeCell ref="C345:G345"/>
+    <mergeCell ref="B341:C341"/>
+    <mergeCell ref="D341:E341"/>
+    <mergeCell ref="A381:B381"/>
+    <mergeCell ref="D378:E378"/>
+    <mergeCell ref="B379:C379"/>
+    <mergeCell ref="D379:E379"/>
     <mergeCell ref="C382:G382"/>
     <mergeCell ref="C383:G383"/>
     <mergeCell ref="C384:G384"/>
@@ -9125,18 +9186,6 @@
     <mergeCell ref="C339:G339"/>
     <mergeCell ref="A340:G340"/>
     <mergeCell ref="A346:B346"/>
-    <mergeCell ref="C346:G346"/>
-    <mergeCell ref="B342:C342"/>
-    <mergeCell ref="D342:E342"/>
-    <mergeCell ref="A343:B343"/>
-    <mergeCell ref="C343:G343"/>
-    <mergeCell ref="A344:B344"/>
-    <mergeCell ref="C344:G344"/>
-    <mergeCell ref="A345:B345"/>
-    <mergeCell ref="C345:G345"/>
-    <mergeCell ref="B341:C341"/>
-    <mergeCell ref="D341:E341"/>
-    <mergeCell ref="A381:B381"/>
     <mergeCell ref="A382:B382"/>
     <mergeCell ref="A383:B383"/>
     <mergeCell ref="A384:B384"/>
@@ -9161,9 +9210,6 @@
     <mergeCell ref="B377:C377"/>
     <mergeCell ref="D377:E377"/>
     <mergeCell ref="B378:C378"/>
-    <mergeCell ref="D378:E378"/>
-    <mergeCell ref="B379:C379"/>
-    <mergeCell ref="D379:E379"/>
     <mergeCell ref="B380:C380"/>
     <mergeCell ref="D380:E380"/>
     <mergeCell ref="A370:B370"/>
@@ -9672,7 +9718,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A4:I24"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
@@ -10099,8 +10145,8 @@
     <mergeCell ref="A13:I13"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="F8" r:id="rId1" display="testingfyp2017@gmail.com_x000a_testingfyp"/>
-    <hyperlink ref="F16" r:id="rId2"/>
+    <hyperlink ref="F8" r:id="rId1" display="testingfyp2017@gmail.com_x000a_testingfyp" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="F16" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId3"/>

</xml_diff>